<commit_message>
add open_24h, low_24h, high_24h, volume_24h to GDAX
</commit_message>
<xml_diff>
--- a/doc/crypto.xlsx
+++ b/doc/crypto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="p:\crypto-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F36085-27E5-4721-9D09-775F38F40AC5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7172A9A-CFD9-4C12-A336-08FBE2024CFD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12225" activeTab="1" xr2:uid="{FA204BA2-54FD-4EAD-B49B-FB8867D94DC8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12225" xr2:uid="{FA204BA2-54FD-4EAD-B49B-FB8867D94DC8}"/>
   </bookViews>
   <sheets>
     <sheet name="GDAX" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
   <si>
     <t>crypto-debug</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>1 Min</t>
+  </si>
+  <si>
+    <t>open_24h</t>
+  </si>
+  <si>
+    <t>high_24h</t>
+  </si>
+  <si>
+    <t>low_24h</t>
+  </si>
+  <si>
+    <t>volume_24h</t>
   </si>
 </sst>
 </file>
@@ -518,7 +530,79 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="86">
+  <dxfs count="90">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2804,7 +2888,7 @@
   <volType type="realTimeData">
     <main first="crypto-debug">
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -2812,7 +2896,23 @@
         <tr r="K19" s="1"/>
       </tp>
       <tp>
-        <v>8009.9</v>
+        <v>15905.412344120001</v>
+        <stp/>
+        <stp>GDAX</stp>
+        <stp>BTC-USD</stp>
+        <stp>volume_24h</stp>
+        <tr r="H4" s="2"/>
+      </tp>
+      <tp>
+        <v>215319.31700712</v>
+        <stp/>
+        <stp>GDAX</stp>
+        <stp>ETH-USD</stp>
+        <stp>volume_24h</stp>
+        <tr r="H3" s="2"/>
+      </tp>
+      <tp>
+        <v>8005.48</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -2820,7 +2920,7 @@
         <tr r="E6" s="1"/>
       </tp>
       <tp>
-        <v>128.51</v>
+        <v>128.25</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -2828,7 +2928,7 @@
         <tr r="E7" s="1"/>
       </tp>
       <tp>
-        <v>644.25</v>
+        <v>644.99</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -2870,7 +2970,7 @@
         <tr r="K16" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -2878,7 +2978,7 @@
         <tr r="K15" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -2894,7 +2994,7 @@
         <tr r="K18" s="1"/>
       </tp>
       <tp>
-        <v>0.64571999999999996</v>
+        <v>0.63848000000000005</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -2902,7 +3002,7 @@
         <tr r="E8" s="1"/>
       </tp>
       <tp>
-        <v>7.1669999999999998E-3</v>
+        <v>7.1599999999999997E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -2910,7 +3010,7 @@
         <tr r="D9" s="1"/>
       </tp>
       <tp>
-        <v>29571</v>
+        <v>29990</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -2918,7 +3018,7 @@
         <tr r="M7" s="1"/>
       </tp>
       <tp>
-        <v>199919</v>
+        <v>202926</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -2926,7 +3026,7 @@
         <tr r="M5" s="1"/>
       </tp>
       <tp>
-        <v>304507</v>
+        <v>306779</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -2934,7 +3034,7 @@
         <tr r="M6" s="1"/>
       </tp>
       <tp>
-        <v>30998</v>
+        <v>31473</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -2942,7 +3042,7 @@
         <tr r="M8" s="1"/>
       </tp>
       <tp>
-        <v>7565.86</v>
+        <v>7554</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2951,7 +3051,7 @@
         <tr r="C36" s="1"/>
       </tp>
       <tp>
-        <v>7515</v>
+        <v>7540.07</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2960,7 +3060,7 @@
         <tr r="C30" s="1"/>
       </tp>
       <tp>
-        <v>584</v>
+        <v>583</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2969,7 +3069,7 @@
         <tr r="C35" s="1"/>
       </tp>
       <tp>
-        <v>578.6</v>
+        <v>582.22</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2978,7 +3078,7 @@
         <tr r="C29" s="1"/>
       </tp>
       <tp>
-        <v>119.68</v>
+        <v>119.23</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -2987,7 +3087,7 @@
         <tr r="C37" s="1"/>
       </tp>
       <tp>
-        <v>118.71</v>
+        <v>118.74</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3014,7 +3114,7 @@
         <tr r="O30" s="1"/>
       </tp>
       <tp>
-        <v>1518580274</v>
+        <v>1521798589</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3022,7 +3122,7 @@
         <tr r="K11" s="1"/>
       </tp>
       <tp>
-        <v>41883660</v>
+        <v>41524771</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3030,7 +3130,7 @@
         <tr r="K10" s="1"/>
       </tp>
       <tp>
-        <v>372632.11</v>
+        <v>372005.87</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3064,7 +3164,7 @@
         <tr r="L21" s="1"/>
       </tp>
       <tp>
-        <v>-7.7700000000000005E-2</v>
+        <v>-7.4730000000000005E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3072,7 +3172,7 @@
         <tr r="N7" s="1"/>
       </tp>
       <tp>
-        <v>-6.2440000000000002E-2</v>
+        <v>-5.772E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3080,7 +3180,7 @@
         <tr r="N6" s="1"/>
       </tp>
       <tp>
-        <v>-0.1024</v>
+        <v>-9.5460000000000003E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3088,7 +3188,7 @@
         <tr r="N5" s="1"/>
       </tp>
       <tp>
-        <v>-7.5969999999999996E-2</v>
+        <v>-6.5369999999999998E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3096,7 +3196,7 @@
         <tr r="N8" s="1"/>
       </tp>
       <tp>
-        <v>580.64</v>
+        <v>582.16</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3105,7 +3205,7 @@
         <tr r="B35" s="1"/>
       </tp>
       <tp>
-        <v>577.82000000000005</v>
+        <v>581.96</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3114,7 +3214,7 @@
         <tr r="B29" s="1"/>
       </tp>
       <tp>
-        <v>7539.98</v>
+        <v>7543.55</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3123,7 +3223,7 @@
         <tr r="B36" s="1"/>
       </tp>
       <tp>
-        <v>7513.79</v>
+        <v>7532.15</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3132,7 +3232,7 @@
         <tr r="B30" s="1"/>
       </tp>
       <tp>
-        <v>119.39</v>
+        <v>118.93</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3141,7 +3241,7 @@
         <tr r="B37" s="1"/>
       </tp>
       <tp>
-        <v>118.71</v>
+        <v>118.74</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3182,7 +3282,7 @@
         <tr r="K21" s="1"/>
       </tp>
       <tp>
-        <v>1643.60223</v>
+        <v>160.12298999999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3191,7 +3291,7 @@
         <tr r="K37" s="1"/>
       </tp>
       <tp>
-        <v>16.262640000000001</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3200,7 +3300,7 @@
         <tr r="K31" s="1"/>
       </tp>
       <tp>
-        <v>931.01201000000003</v>
+        <v>666.99198999999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3209,7 +3309,7 @@
         <tr r="K35" s="1"/>
       </tp>
       <tp>
-        <v>3.9699999999999996E-3</v>
+        <v>11.4954</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3218,7 +3318,7 @@
         <tr r="K29" s="1"/>
       </tp>
       <tp>
-        <v>89.971158000000003</v>
+        <v>60.616477000000003</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3227,7 +3327,7 @@
         <tr r="K36" s="1"/>
       </tp>
       <tp>
-        <v>0.91675099999999998</v>
+        <v>2.9341360000000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3276,7 +3376,7 @@
         <tr r="L17" s="1"/>
       </tp>
       <tp>
-        <v>6.9280000000000001E-3</v>
+        <v>6.9340000000000001E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3284,7 +3384,7 @@
         <tr r="I9" s="1"/>
       </tp>
       <tp>
-        <v>7.9350000000000004E-5</v>
+        <v>7.9049999999999997E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3300,7 +3400,7 @@
         <tr r="I11" s="1"/>
       </tp>
       <tp>
-        <v>8.0550000000000006E-5</v>
+        <v>8.0010000000000001E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3308,7 +3408,7 @@
         <tr r="D10" s="1"/>
       </tp>
       <tp>
-        <v>9.2199999999999998E-6</v>
+        <v>9.1900000000000001E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3316,7 +3416,7 @@
         <tr r="D11" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3324,7 +3424,7 @@
         <tr r="K20" s="1"/>
       </tp>
       <tp>
-        <v>9.0499999999999997E-6</v>
+        <v>9.0599999999999997E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3332,7 +3432,7 @@
         <tr r="G11" s="1"/>
       </tp>
       <tp>
-        <v>7.9309999999999998E-5</v>
+        <v>7.894E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3340,7 +3440,7 @@
         <tr r="G10" s="1"/>
       </tp>
       <tp>
-        <v>6.9259999999999999E-3</v>
+        <v>6.9319999999999998E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3348,7 +3448,7 @@
         <tr r="G9" s="1"/>
       </tp>
       <tp>
-        <v>-4.9000000000000002E-2</v>
+        <v>-4.1759999999999999E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3356,7 +3456,7 @@
         <tr r="O8" s="1"/>
       </tp>
       <tp>
-        <v>505569</v>
+        <v>506654</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3364,7 +3464,7 @@
         <tr r="N18" s="1"/>
       </tp>
       <tp>
-        <v>1775.06377</v>
+        <v>1168.8069</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3373,7 +3473,7 @@
         <tr r="J35" s="1"/>
       </tp>
       <tp>
-        <v>1.2907299999999999</v>
+        <v>15.68529</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3382,7 +3482,7 @@
         <tr r="J29" s="1"/>
       </tp>
       <tp>
-        <v>900</v>
+        <v>6386</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3390,7 +3490,7 @@
         <tr r="F10" s="1"/>
       </tp>
       <tp>
-        <v>20826818</v>
+        <v>20828597</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3398,7 +3498,7 @@
         <tr r="M20" s="1"/>
       </tp>
       <tp>
-        <v>0.34</v>
+        <v>64.209999999999994</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3406,7 +3506,7 @@
         <tr r="J18" s="1"/>
       </tp>
       <tp>
-        <v>191</v>
+        <v>428</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3414,7 +3514,7 @@
         <tr r="J21" s="1"/>
       </tp>
       <tp>
-        <v>0.49347000000000002</v>
+        <v>0.51500000000000001</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3422,7 +3522,7 @@
         <tr r="J15" s="1"/>
       </tp>
       <tp>
-        <v>9.264E-2</v>
+        <v>3.7019899999999999</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3430,7 +3530,7 @@
         <tr r="J17" s="1"/>
       </tp>
       <tp>
-        <v>9.9999999999999995E-7</v>
+        <v>2.758E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3438,7 +3538,7 @@
         <tr r="J16" s="1"/>
       </tp>
       <tp>
-        <v>17</v>
+        <v>0.23400000000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3447,7 +3547,7 @@
         <tr r="E23" s="1"/>
       </tp>
       <tp>
-        <v>0.4</v>
+        <v>3.5999999999999997E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3456,7 +3556,7 @@
         <tr r="E24" s="1"/>
       </tp>
       <tp>
-        <v>5.8026999999999997</v>
+        <v>2.2280600000000002</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3465,7 +3565,7 @@
         <tr r="E21" s="1"/>
       </tp>
       <tp>
-        <v>1.4219999999999999</v>
+        <v>18</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3474,7 +3574,7 @@
         <tr r="E22" s="1"/>
       </tp>
       <tp>
-        <v>0.219</v>
+        <v>1.4</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3483,7 +3583,7 @@
         <tr r="E19" s="1"/>
       </tp>
       <tp>
-        <v>1.8</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3492,7 +3592,7 @@
         <tr r="E20" s="1"/>
       </tp>
       <tp>
-        <v>0.06</v>
+        <v>9.8913600000000006</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3501,7 +3601,7 @@
         <tr r="E17" s="1"/>
       </tp>
       <tp>
-        <v>0.5</v>
+        <v>0.24571999999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3510,7 +3610,7 @@
         <tr r="E18" s="1"/>
       </tp>
       <tp>
-        <v>0.39602999999999999</v>
+        <v>0.51549</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3519,7 +3619,7 @@
         <tr r="E15" s="1"/>
       </tp>
       <tp>
-        <v>9</v>
+        <v>1.2547900000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -3528,7 +3628,7 @@
         <tr r="E16" s="1"/>
       </tp>
       <tp>
-        <v>-10</v>
+        <v>-9.59</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3536,7 +3636,7 @@
         <tr r="O7" s="1"/>
       </tp>
       <tp>
-        <v>-500.47</v>
+        <v>-461.59</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3544,7 +3644,7 @@
         <tr r="O6" s="1"/>
       </tp>
       <tp>
-        <v>-66.010000000000005</v>
+        <v>-61.44</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3560,7 +3660,7 @@
         <tr r="H7" s="1"/>
       </tp>
       <tp>
-        <v>0.6</v>
+        <v>0.54</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3568,7 +3668,7 @@
         <tr r="H5" s="1"/>
       </tp>
       <tp>
-        <v>2.42</v>
+        <v>5.08</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3576,7 +3676,7 @@
         <tr r="H6" s="1"/>
       </tp>
       <tp>
-        <v>7.5000000000000002E-4</v>
+        <v>2.8400000000000001E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3584,7 +3684,7 @@
         <tr r="H8" s="1"/>
       </tp>
       <tp>
-        <v>505569</v>
+        <v>506654</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3592,7 +3692,7 @@
         <tr r="M18" s="1"/>
       </tp>
       <tp>
-        <v>2000</v>
+        <v>2484</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3600,7 +3700,7 @@
         <tr r="J20" s="1"/>
       </tp>
       <tp>
-        <v>0.64600000000000002</v>
+        <v>0.64488000000000001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3608,7 +3708,7 @@
         <tr r="C8" s="1"/>
       </tp>
       <tp>
-        <v>3528.9031100000002</v>
+        <v>655.63270999999997</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3617,7 +3717,7 @@
         <tr r="J37" s="1"/>
       </tp>
       <tp>
-        <v>16.262640000000001</v>
+        <v>3.7135099999999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3626,7 +3726,7 @@
         <tr r="J31" s="1"/>
       </tp>
       <tp>
-        <v>0.94858600000000004</v>
+        <v>5.0390579999999998</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3635,7 +3735,7 @@
         <tr r="J30" s="1"/>
       </tp>
       <tp>
-        <v>238.42579499999999</v>
+        <v>158.199477</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3668,7 +3768,7 @@
         <tr r="C7" s="1"/>
       </tp>
       <tp>
-        <v>3.89</v>
+        <v>9.5399999999999991</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3676,7 +3776,7 @@
         <tr r="J9" s="1"/>
       </tp>
       <tp>
-        <v>92528</v>
+        <v>356491</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3684,7 +3784,7 @@
         <tr r="F11" s="1"/>
       </tp>
       <tp>
-        <v>28269780</v>
+        <v>28273403</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3692,7 +3792,7 @@
         <tr r="M21" s="1"/>
       </tp>
       <tp>
-        <v>7487351</v>
+        <v>7488320</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3700,7 +3800,7 @@
         <tr r="M17" s="1"/>
       </tp>
       <tp>
-        <v>45352162</v>
+        <v>45361382</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3708,7 +3808,7 @@
         <tr r="M16" s="1"/>
       </tp>
       <tp>
-        <v>26040847</v>
+        <v>26047743</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3716,7 +3816,7 @@
         <tr r="M15" s="1"/>
       </tp>
       <tp>
-        <v>13330496</v>
+        <v>13331554</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -3742,7 +3842,7 @@
         <tr r="H36" s="1"/>
       </tp>
       <tp>
-        <v>7500</v>
+        <v>7509.7</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3751,7 +3851,7 @@
         <tr r="D36" s="1"/>
       </tp>
       <tp>
-        <v>7512.57</v>
+        <v>7532.15</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3760,7 +3860,7 @@
         <tr r="D30" s="1"/>
       </tp>
       <tp>
-        <v>118.7</v>
+        <v>118.74</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3769,7 +3869,7 @@
         <tr r="D31" s="1"/>
       </tp>
       <tp>
-        <v>118.38</v>
+        <v>118.36</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3778,7 +3878,7 @@
         <tr r="D37" s="1"/>
       </tp>
       <tp>
-        <v>118.7</v>
+        <v>118.74</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3787,7 +3887,7 @@
         <tr r="E31" s="1"/>
       </tp>
       <tp>
-        <v>118.7</v>
+        <v>118.74</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3796,7 +3896,7 @@
         <tr r="E37" s="1"/>
       </tp>
       <tp>
-        <v>261</v>
+        <v>130</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3805,7 +3905,7 @@
         <tr r="N37" s="1"/>
       </tp>
       <tp>
-        <v>1966</v>
+        <v>1223</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3814,7 +3914,7 @@
         <tr r="N36" s="1"/>
       </tp>
       <tp>
-        <v>2</v>
+        <v>3</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -3823,7 +3923,7 @@
         <tr r="N31" s="1"/>
       </tp>
       <tp>
-        <v>11</v>
+        <v>52</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3832,7 +3932,7 @@
         <tr r="N30" s="1"/>
       </tp>
       <tp>
-        <v>1594</v>
+        <v>1146</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3841,7 +3941,7 @@
         <tr r="N35" s="1"/>
       </tp>
       <tp>
-        <v>4</v>
+        <v>24</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3850,7 +3950,7 @@
         <tr r="N29" s="1"/>
       </tp>
       <tp>
-        <v>458525</v>
+        <v>459548</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3858,7 +3958,7 @@
         <tr r="H18" s="1"/>
       </tp>
       <tp>
-        <v>7487351</v>
+        <v>7488321</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3866,7 +3966,7 @@
         <tr r="N17" s="1"/>
       </tp>
       <tp>
-        <v>15050999</v>
+        <v>15052222</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -3874,7 +3974,7 @@
         <tr r="M19" s="1"/>
       </tp>
       <tp>
-        <v>6593265</v>
+        <v>6594163</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3882,7 +3982,7 @@
         <tr r="H17" s="1"/>
       </tp>
       <tp>
-        <v>39447096</v>
+        <v>39455650</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3890,7 +3990,7 @@
         <tr r="H16" s="1"/>
       </tp>
       <tp>
-        <v>23115870</v>
+        <v>23121775</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3898,7 +3998,7 @@
         <tr r="H15" s="1"/>
       </tp>
       <tp>
-        <v>17543575</v>
+        <v>17545847</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3906,7 +4006,7 @@
         <tr r="H21" s="1"/>
       </tp>
       <tp>
-        <v>4.5599999999999996</v>
+        <v>1.49</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3914,7 +4014,7 @@
         <tr r="F9" s="1"/>
       </tp>
       <tp>
-        <v>235468</v>
+        <v>1963</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3940,7 +4040,7 @@
         <tr r="H29" s="1"/>
       </tp>
       <tp>
-        <v>17203563</v>
+        <v>17205151</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3948,7 +4048,7 @@
         <tr r="H20" s="1"/>
       </tp>
       <tp>
-        <v>45352162</v>
+        <v>45361382</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3956,7 +4056,7 @@
         <tr r="N16" s="1"/>
       </tp>
       <tp>
-        <v>577.64</v>
+        <v>581.45000000000005</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3965,7 +4065,7 @@
         <tr r="D29" s="1"/>
       </tp>
       <tp>
-        <v>576.29999999999995</v>
+        <v>578.88</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3974,7 +4074,7 @@
         <tr r="D35" s="1"/>
       </tp>
       <tp>
-        <v>173</v>
+        <v>1264</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3982,7 +4082,7 @@
         <tr r="J10" s="1"/>
       </tp>
       <tp>
-        <v>578</v>
+        <v>582.20000000000005</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3991,7 +4091,7 @@
         <tr r="E35" s="1"/>
       </tp>
       <tp>
-        <v>578</v>
+        <v>582.20000000000005</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4000,7 +4100,7 @@
         <tr r="E29" s="1"/>
       </tp>
       <tp>
-        <v>7515</v>
+        <v>7540.07</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4009,7 +4109,7 @@
         <tr r="E30" s="1"/>
       </tp>
       <tp>
-        <v>7515</v>
+        <v>7540.07</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4018,7 +4118,7 @@
         <tr r="E36" s="1"/>
       </tp>
       <tp>
-        <v>26040847</v>
+        <v>26047743</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4026,7 +4126,7 @@
         <tr r="N15" s="1"/>
       </tp>
       <tp>
-        <v>2.66</v>
+        <v>1.79</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4052,7 +4152,7 @@
         <tr r="H37" s="1"/>
       </tp>
       <tp>
-        <v>0.40028999999999998</v>
+        <v>0.9</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4061,7 +4161,7 @@
         <tr r="A23" s="1"/>
       </tp>
       <tp>
-        <v>12.9</v>
+        <v>2.2010000000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4070,7 +4170,7 @@
         <tr r="A24" s="1"/>
       </tp>
       <tp>
-        <v>10</v>
+        <v>1.6310100000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4079,7 +4179,7 @@
         <tr r="A21" s="1"/>
       </tp>
       <tp>
-        <v>0.5</v>
+        <v>0.30843999999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4088,7 +4188,7 @@
         <tr r="A22" s="1"/>
       </tp>
       <tp>
-        <v>1.7999999999999999E-2</v>
+        <v>1.72058</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4097,7 +4197,7 @@
         <tr r="A19" s="1"/>
       </tp>
       <tp>
-        <v>1.52519</v>
+        <v>1.00299</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4106,7 +4206,7 @@
         <tr r="A20" s="1"/>
       </tp>
       <tp>
-        <v>1.7999999999999999E-2</v>
+        <v>16.292899999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4115,7 +4215,7 @@
         <tr r="A17" s="1"/>
       </tp>
       <tp>
-        <v>1.7999999999999999E-2</v>
+        <v>6.8779999999999994E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4124,7 +4224,7 @@
         <tr r="A18" s="1"/>
       </tp>
       <tp>
-        <v>0.49347000000000002</v>
+        <v>0.51527999999999996</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4133,7 +4233,7 @@
         <tr r="A15" s="1"/>
       </tp>
       <tp>
-        <v>1.7999999999999999E-2</v>
+        <v>8.0000000000000007E-5</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4142,7 +4242,7 @@
         <tr r="A16" s="1"/>
       </tp>
       <tp>
-        <v>8.0500000000000005E-5</v>
+        <v>8.0010000000000001E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -4150,7 +4250,7 @@
         <tr r="E10" s="1"/>
       </tp>
       <tp>
-        <v>43243.799421041665</v>
+        <v>43243.828146215281</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4158,7 +4258,7 @@
         <tr r="O21" s="1"/>
       </tp>
       <tp>
-        <v>127521</v>
+        <v>128495</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4220,7 +4320,7 @@
         <tr r="M31" s="1"/>
       </tp>
       <tp>
-        <v>-1.8440000000000002E-2</v>
+        <v>-1.52E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4228,7 +4328,7 @@
         <tr r="N11" s="1"/>
       </tp>
       <tp>
-        <v>43243.799358796299</v>
+        <v>43243.828053148151</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -4236,7 +4336,7 @@
         <tr r="O20" s="1"/>
       </tp>
       <tp>
-        <v>66180</v>
+        <v>66201</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4244,7 +4344,7 @@
         <tr r="M10" s="1"/>
       </tp>
       <tp>
-        <v>-1.576E-2</v>
+        <v>-1.2E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4252,7 +4352,7 @@
         <tr r="N10" s="1"/>
       </tp>
       <tp>
-        <v>9.2199999999999998E-6</v>
+        <v>9.1900000000000001E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -4260,7 +4360,7 @@
         <tr r="E11" s="1"/>
       </tp>
       <tp>
-        <v>15051000</v>
+        <v>15052222</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4268,7 +4368,7 @@
         <tr r="N19" s="1"/>
       </tp>
       <tp>
-        <v>28269780</v>
+        <v>28273403</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4276,7 +4376,7 @@
         <tr r="N21" s="1"/>
       </tp>
       <tp>
-        <v>20826818</v>
+        <v>20828597</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -4284,7 +4384,7 @@
         <tr r="N20" s="1"/>
       </tp>
       <tp>
-        <v>43243.799348125001</v>
+        <v>43243.827995428241</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4292,7 +4392,7 @@
         <tr r="O18" s="1"/>
       </tp>
       <tp>
-        <v>43243.799419756942</v>
+        <v>43243.828132083334</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4300,7 +4400,7 @@
         <tr r="O15" s="1"/>
       </tp>
       <tp>
-        <v>43243.799415833331</v>
+        <v>43243.828134444448</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4308,7 +4408,7 @@
         <tr r="O16" s="1"/>
       </tp>
       <tp>
-        <v>43243.799404479163</v>
+        <v>43243.828064386573</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4316,7 +4416,7 @@
         <tr r="O17" s="1"/>
       </tp>
       <tp>
-        <v>-3.1300000000000001E-2</v>
+        <v>-3.0890000000000001E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -4324,7 +4424,7 @@
         <tr r="N9" s="1"/>
       </tp>
       <tp>
-        <v>43243.799420706018</v>
+        <v>43243.828137083336</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4332,7 +4432,7 @@
         <tr r="O19" s="1"/>
       </tp>
       <tp>
-        <v>52009</v>
+        <v>52096</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -4340,7 +4440,7 @@
         <tr r="M9" s="1"/>
       </tp>
       <tp>
-        <v>7.1669999999999998E-3</v>
+        <v>7.1599999999999997E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4348,7 +4448,7 @@
         <tr r="E9" s="1"/>
       </tp>
       <tp>
-        <v>7487350</v>
+        <v>7488319</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4357,7 +4457,7 @@
         <tr r="Q31" s="1"/>
       </tp>
       <tp>
-        <v>7487091</v>
+        <v>7488192</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4366,7 +4466,7 @@
         <tr r="Q37" s="1"/>
       </tp>
       <tp>
-        <v>45352149</v>
+        <v>45361328</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4375,7 +4475,7 @@
         <tr r="Q30" s="1"/>
       </tp>
       <tp>
-        <v>45350194</v>
+        <v>45360157</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4384,7 +4484,7 @@
         <tr r="Q36" s="1"/>
       </tp>
       <tp>
-        <v>26040844</v>
+        <v>26047720</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4393,7 +4493,7 @@
         <tr r="Q29" s="1"/>
       </tp>
       <tp>
-        <v>26039254</v>
+        <v>26046598</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4402,7 +4502,7 @@
         <tr r="Q35" s="1"/>
       </tp>
       <tp>
-        <v>579.55999999999995</v>
+        <v>581.9</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4410,7 +4510,7 @@
         <tr r="D3" s="2"/>
       </tp>
       <tp>
-        <v>7533.15</v>
+        <v>7542.99</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4418,7 +4518,7 @@
         <tr r="D4" s="2"/>
       </tp>
       <tp>
-        <v>43243.791666666664</v>
+        <v>43243.822916666664</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4427,7 +4527,7 @@
         <tr r="F37" s="1"/>
       </tp>
       <tp>
-        <v>43243.799305555556</v>
+        <v>43243.827777777777</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4436,7 +4536,7 @@
         <tr r="F31" s="1"/>
       </tp>
       <tp>
-        <v>118.7</v>
+        <v>118.74</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4444,7 +4544,7 @@
         <tr r="I17" s="1"/>
       </tp>
       <tp>
-        <v>7512.58</v>
+        <v>7535</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4452,7 +4552,7 @@
         <tr r="I16" s="1"/>
       </tp>
       <tp>
-        <v>-1.2699999999999999E-6</v>
+        <v>-9.5999999999999991E-7</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4460,7 +4560,7 @@
         <tr r="O10" s="1"/>
       </tp>
       <tp>
-        <v>1794793.14691304</v>
+        <v>1191563.72003854</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4469,7 +4569,7 @@
         <tr r="I36" s="1"/>
       </tp>
       <tp>
-        <v>7128.5009294299998</v>
+        <v>37969.097520559997</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4478,7 +4578,7 @@
         <tr r="I30" s="1"/>
       </tp>
       <tp>
-        <v>644.25</v>
+        <v>644.26</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4486,7 +4586,7 @@
         <tr r="D5" s="1"/>
       </tp>
       <tp>
-        <v>2E-8</v>
+        <v>1E-8</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4494,7 +4594,7 @@
         <tr r="H11" s="1"/>
       </tp>
       <tp>
-        <v>185</v>
+        <v>301.3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4510,7 +4610,7 @@
         <tr r="C11" s="1"/>
       </tp>
       <tp>
-        <v>106280.56263</v>
+        <v>106827.6857</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4518,7 +4618,7 @@
         <tr r="K7" s="1"/>
       </tp>
       <tp>
-        <v>0.59524999999999995</v>
+        <v>0.59423000000000004</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4526,7 +4626,7 @@
         <tr r="G8" s="1"/>
       </tp>
       <tp>
-        <v>12182594.599355601</v>
+        <v>12225585.756023699</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4534,7 +4634,7 @@
         <tr r="L8" s="1"/>
       </tp>
       <tp>
-        <v>43243.799999988427</v>
+        <v>43243.828472210647</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4543,7 +4643,7 @@
         <tr r="G29" s="1"/>
       </tp>
       <tp>
-        <v>43243.80208332176</v>
+        <v>43243.83333332176</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4552,7 +4652,7 @@
         <tr r="G35" s="1"/>
       </tp>
       <tp>
-        <v>43243.799999988427</v>
+        <v>43243.828472210647</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4561,7 +4661,7 @@
         <tr r="G30" s="1"/>
       </tp>
       <tp>
-        <v>43243.799999988427</v>
+        <v>43243.828472210647</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4570,7 +4670,7 @@
         <tr r="G31" s="1"/>
       </tp>
       <tp>
-        <v>43243.80208332176</v>
+        <v>43243.83333332176</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4579,7 +4679,7 @@
         <tr r="G36" s="1"/>
       </tp>
       <tp>
-        <v>43243.80208332176</v>
+        <v>43243.83333332176</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4588,7 +4688,7 @@
         <tr r="G37" s="1"/>
       </tp>
       <tp>
-        <v>745.85206400000004</v>
+        <v>9124.4314945999995</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4597,7 +4697,7 @@
         <tr r="I29" s="1"/>
       </tp>
       <tp>
-        <v>1029820.926874</v>
+        <v>678778.01629870001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4606,7 +4706,7 @@
         <tr r="I35" s="1"/>
       </tp>
       <tp>
-        <v>1.7439100000000001</v>
+        <v>7.50021</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4614,7 +4714,7 @@
         <tr r="F7" s="1"/>
       </tp>
       <tp>
-        <v>2</v>
+        <v>3.1895720000000001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4622,7 +4722,7 @@
         <tr r="F6" s="1"/>
       </tp>
       <tp>
-        <v>0.49347000000000002</v>
+        <v>0.51527999999999996</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4630,7 +4730,7 @@
         <tr r="F5" s="1"/>
       </tp>
       <tp>
-        <v>6.9259999999999999E-3</v>
+        <v>6.9329999999999999E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4638,7 +4738,7 @@
         <tr r="I19" s="1"/>
       </tp>
       <tp>
-        <v>0.59599999999999997</v>
+        <v>0.59706999999999999</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4654,7 +4754,7 @@
         <tr r="C10" s="1"/>
       </tp>
       <tp>
-        <v>43243.799305555556</v>
+        <v>43243.827777777777</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4663,7 +4763,7 @@
         <tr r="F29" s="1"/>
       </tp>
       <tp>
-        <v>43243.791666666664</v>
+        <v>43243.822916666664</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4672,7 +4772,7 @@
         <tr r="F35" s="1"/>
       </tp>
       <tp>
-        <v>578</v>
+        <v>582.20000000000005</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4680,7 +4780,7 @@
         <tr r="I15" s="1"/>
       </tp>
       <tp>
-        <v>128.44999999999999</v>
+        <v>128.15</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4688,7 +4788,7 @@
         <tr r="D7" s="1"/>
       </tp>
       <tp>
-        <v>8000</v>
+        <v>7997.61</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4696,7 +4796,7 @@
         <tr r="D6" s="1"/>
       </tp>
       <tp>
-        <v>677632.36464485002</v>
+        <v>456326.38714921998</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4705,7 +4805,7 @@
         <tr r="L36" s="1"/>
       </tp>
       <tp>
-        <v>196062.29350989999</v>
+        <v>19030.4075118</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4714,7 +4814,7 @@
         <tr r="L37" s="1"/>
       </tp>
       <tp>
-        <v>6889.3380536200002</v>
+        <v>22112.017725329999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4723,7 +4823,7 @@
         <tr r="L30" s="1"/>
       </tp>
       <tp>
-        <v>1930.5370680000001</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4732,7 +4832,7 @@
         <tr r="L31" s="1"/>
       </tp>
       <tp>
-        <v>540465.4464899</v>
+        <v>387387.3168272</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4741,7 +4841,7 @@
         <tr r="L35" s="1"/>
       </tp>
       <tp>
-        <v>2.2970419999999998</v>
+        <v>6687.1171244999996</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4750,7 +4850,7 @@
         <tr r="L29" s="1"/>
       </tp>
       <tp>
-        <v>579.11</v>
+        <v>581.89</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4758,7 +4858,7 @@
         <tr r="B3" s="2"/>
       </tp>
       <tp>
-        <v>2624.7235926899998</v>
+        <v>2618.51439093</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -4766,7 +4866,7 @@
         <tr r="L9" s="1"/>
       </tp>
       <tp>
-        <v>42435.118895</v>
+        <v>42870.260064000002</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4782,7 +4882,7 @@
         <tr r="B8" s="1"/>
       </tp>
       <tp>
-        <v>579.25</v>
+        <v>581.9</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4790,7 +4890,7 @@
         <tr r="C3" s="2"/>
       </tp>
       <tp>
-        <v>4.0000000000000001E-8</v>
+        <v>1.1000000000000001E-7</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4798,7 +4898,7 @@
         <tr r="H10" s="1"/>
       </tp>
       <tp>
-        <v>419829.58477409999</v>
+        <v>77861.828267599994</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4807,7 +4907,7 @@
         <tr r="I37" s="1"/>
       </tp>
       <tp>
-        <v>1930.5370680000001</v>
+        <v>440.94217739999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4816,7 +4916,7 @@
         <tr r="I31" s="1"/>
       </tp>
       <tp>
-        <v>254706.29717999999</v>
+        <v>256884.09805</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4824,7 +4924,7 @@
         <tr r="K5" s="1"/>
       </tp>
       <tp>
-        <v>7533.15</v>
+        <v>7543</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4832,7 +4932,7 @@
         <tr r="C4" s="2"/>
       </tp>
       <tp>
-        <v>-1.6999999999999999E-7</v>
+        <v>-1.4000000000000001E-7</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4840,7 +4940,7 @@
         <tr r="O11" s="1"/>
       </tp>
       <tp>
-        <v>7533.14</v>
+        <v>7542.99</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4848,7 +4948,7 @@
         <tr r="B4" s="2"/>
       </tp>
       <tp>
-        <v>43243.791666666664</v>
+        <v>43243.822916666664</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4857,7 +4957,7 @@
         <tr r="F36" s="1"/>
       </tp>
       <tp>
-        <v>43243.799305555556</v>
+        <v>43243.827777777777</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4866,6 +4966,22 @@
         <tr r="F30" s="1"/>
       </tp>
       <tp>
+        <v>8030.06</v>
+        <stp/>
+        <stp>GDAX</stp>
+        <stp>BTC-USD</stp>
+        <stp>high_24h</stp>
+        <tr r="F4" s="2"/>
+      </tp>
+      <tp>
+        <v>648.46</v>
+        <stp/>
+        <stp>GDAX</stp>
+        <stp>ETH-USD</stp>
+        <stp>high_24h</stp>
+        <tr r="F3" s="2"/>
+      </tp>
+      <tp>
         <v>9.0699999999999996E-6</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
@@ -4874,7 +4990,7 @@
         <tr r="I21" s="1"/>
       </tp>
       <tp>
-        <v>7.9300000000000003E-5</v>
+        <v>7.9040000000000002E-5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -4890,7 +5006,7 @@
         <tr r="B6" s="1"/>
       </tp>
       <tp>
-        <v>118.54</v>
+        <v>118.74</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4898,7 +5014,7 @@
         <tr r="G7" s="1"/>
       </tp>
       <tp>
-        <v>20037666.02</v>
+        <v>20153277.09</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4906,7 +5022,7 @@
         <tr r="K8" s="1"/>
       </tp>
       <tp>
-        <v>0.59599999999999997</v>
+        <v>0.59702999999999995</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4914,7 +5030,7 @@
         <tr r="I18" s="1"/>
       </tp>
       <tp>
-        <v>7487351</v>
+        <v>7488321</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4923,7 +5039,7 @@
         <tr r="R37" s="1"/>
       </tp>
       <tp>
-        <v>7487351</v>
+        <v>7488321</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -4932,7 +5048,7 @@
         <tr r="R31" s="1"/>
       </tp>
       <tp>
-        <v>45352159</v>
+        <v>45361379</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4941,7 +5057,7 @@
         <tr r="R30" s="1"/>
       </tp>
       <tp>
-        <v>45352159</v>
+        <v>45361379</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4950,7 +5066,7 @@
         <tr r="R36" s="1"/>
       </tp>
       <tp>
-        <v>577.44000000000005</v>
+        <v>580.67999999999995</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4959,7 +5075,7 @@
         <tr r="B24" s="1"/>
       </tp>
       <tp>
-        <v>577.5</v>
+        <v>580.73</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4968,7 +5084,7 @@
         <tr r="B23" s="1"/>
       </tp>
       <tp>
-        <v>577.99</v>
+        <v>581.63</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4977,7 +5093,7 @@
         <tr r="B16" s="1"/>
       </tp>
       <tp>
-        <v>578</v>
+        <v>581.64</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4986,7 +5102,7 @@
         <tr r="B15" s="1"/>
       </tp>
       <tp>
-        <v>577.74</v>
+        <v>581.53</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4995,7 +5111,7 @@
         <tr r="B18" s="1"/>
       </tp>
       <tp>
-        <v>577.83000000000004</v>
+        <v>581.6</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5004,7 +5120,7 @@
         <tr r="B17" s="1"/>
       </tp>
       <tp>
-        <v>577.64</v>
+        <v>581.15</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5013,7 +5129,7 @@
         <tr r="B20" s="1"/>
       </tp>
       <tp>
-        <v>577.65</v>
+        <v>581.17999999999995</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5022,7 +5138,7 @@
         <tr r="B19" s="1"/>
       </tp>
       <tp>
-        <v>577.55999999999995</v>
+        <v>580.96</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5031,7 +5147,7 @@
         <tr r="B22" s="1"/>
       </tp>
       <tp>
-        <v>577.63</v>
+        <v>581</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5040,7 +5156,7 @@
         <tr r="B21" s="1"/>
       </tp>
       <tp>
-        <v>579.02</v>
+        <v>582.70000000000005</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5049,7 +5165,7 @@
         <tr r="D21" s="1"/>
       </tp>
       <tp>
-        <v>579.26</v>
+        <v>582.77</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5058,7 +5174,7 @@
         <tr r="D22" s="1"/>
       </tp>
       <tp>
-        <v>578.96</v>
+        <v>582.59</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5067,7 +5183,7 @@
         <tr r="D19" s="1"/>
       </tp>
       <tp>
-        <v>579.01</v>
+        <v>582.6</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5076,7 +5192,7 @@
         <tr r="D20" s="1"/>
       </tp>
       <tp>
-        <v>578.87</v>
+        <v>582.21</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5085,7 +5201,7 @@
         <tr r="D17" s="1"/>
       </tp>
       <tp>
-        <v>578.95000000000005</v>
+        <v>582.22</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5094,7 +5210,7 @@
         <tr r="D18" s="1"/>
       </tp>
       <tp>
-        <v>578.6</v>
+        <v>582.17999999999995</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5103,7 +5219,7 @@
         <tr r="D15" s="1"/>
       </tp>
       <tp>
-        <v>578.82000000000005</v>
+        <v>582.19000000000005</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5112,7 +5228,7 @@
         <tr r="D16" s="1"/>
       </tp>
       <tp>
-        <v>579.27</v>
+        <v>582.9</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5121,7 +5237,7 @@
         <tr r="D23" s="1"/>
       </tp>
       <tp>
-        <v>579.29</v>
+        <v>582.92999999999995</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -5130,7 +5246,15 @@
         <tr r="D24" s="1"/>
       </tp>
       <tp>
-        <v>118.71</v>
+        <v>7433.19</v>
+        <stp/>
+        <stp>GDAX</stp>
+        <stp>BTC-USD</stp>
+        <stp>low_24h</stp>
+        <tr r="G4" s="2"/>
+      </tp>
+      <tp>
+        <v>118.91</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -5138,7 +5262,7 @@
         <tr r="I7" s="1"/>
       </tp>
       <tp>
-        <v>-2.24E-4</v>
+        <v>-2.2100000000000001E-4</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -5154,6 +5278,30 @@
         <tr r="H9" s="1"/>
       </tp>
       <tp>
+        <v>563.27</v>
+        <stp/>
+        <stp>GDAX</stp>
+        <stp>ETH-USD</stp>
+        <stp>low_24h</stp>
+        <tr r="G3" s="2"/>
+      </tp>
+      <tp>
+        <v>8001.42</v>
+        <stp/>
+        <stp>GDAX</stp>
+        <stp>BTC-USD</stp>
+        <stp>open_24h</stp>
+        <tr r="E4" s="2"/>
+      </tp>
+      <tp>
+        <v>643.34</v>
+        <stp/>
+        <stp>GDAX</stp>
+        <stp>ETH-USD</stp>
+        <stp>open_24h</stp>
+        <tr r="E3" s="2"/>
+      </tp>
+      <tp>
         <v>560</v>
         <stp/>
         <stp>BINANCE</stp>
@@ -5162,7 +5310,7 @@
         <tr r="B5" s="1"/>
       </tp>
       <tp>
-        <v>328149121.66622531</v>
+        <v>330978506.52329791</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -5170,7 +5318,7 @@
         <tr r="L6" s="1"/>
       </tp>
       <tp>
-        <v>12995945.213345701</v>
+        <v>13030528.640093099</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -5178,7 +5326,7 @@
         <tr r="L7" s="1"/>
       </tp>
       <tp>
-        <v>578</v>
+        <v>581.64</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -5186,7 +5334,7 @@
         <tr r="G5" s="1"/>
       </tp>
       <tp>
-        <v>13250</v>
+        <v>255.67</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -5194,7 +5342,7 @@
         <tr r="J8" s="1"/>
       </tp>
       <tp>
-        <v>26040847</v>
+        <v>26047743</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5203,7 +5351,7 @@
         <tr r="R35" s="1"/>
       </tp>
       <tp>
-        <v>26040847</v>
+        <v>26047743</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5212,7 +5360,7 @@
         <tr r="R29" s="1"/>
       </tp>
       <tp>
-        <v>578.6</v>
+        <v>582.17999999999995</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -5220,7 +5368,7 @@
         <tr r="I5" s="1"/>
       </tp>
       <tp>
-        <v>0.64510000000000001</v>
+        <v>0.63775000000000004</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -5228,7 +5376,7 @@
         <tr r="D8" s="1"/>
       </tp>
       <tp>
-        <v>154657317.2878904</v>
+        <v>155567039.23584211</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -5236,7 +5384,7 @@
         <tr r="L5" s="1"/>
       </tp>
       <tp>
-        <v>13743.119085259999</v>
+        <v>13766.77456217</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -5244,7 +5392,7 @@
         <tr r="L11" s="1"/>
       </tp>
       <tp>
-        <v>3304.1174867200002</v>
+        <v>3274.4077716900001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -5252,7 +5400,7 @@
         <tr r="L10" s="1"/>
       </tp>
       <tp>
-        <v>7515</v>
+        <v>7540.08</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -5268,7 +5416,7 @@
         <tr r="B7" s="1"/>
       </tp>
       <tp>
-        <v>7512.58</v>
+        <v>7535</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -5284,7 +5432,7 @@
         <tr r="C9" s="1"/>
       </tp>
       <tp>
-        <v>43243.799413310182</v>
+        <v>43243.82813209491</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5293,7 +5441,7 @@
         <tr r="P30" s="1"/>
       </tp>
       <tp>
-        <v>43243.799404513891</v>
+        <v>43243.828064409725</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -5302,7 +5450,7 @@
         <tr r="P31" s="1"/>
       </tp>
       <tp>
-        <v>43243.799413310182</v>
+        <v>43243.82813209491</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5311,7 +5459,7 @@
         <tr r="P36" s="1"/>
       </tp>
       <tp>
-        <v>43243.799404513891</v>
+        <v>43243.828064409725</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ltcusdt</stp>
@@ -5320,7 +5468,7 @@
         <tr r="P37" s="1"/>
       </tp>
       <tp>
-        <v>43243.799419791663</v>
+        <v>43243.828132118055</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5329,7 +5477,7 @@
         <tr r="P29" s="1"/>
       </tp>
       <tp>
-        <v>43243.799419791663</v>
+        <v>43243.828132129631</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5338,7 +5486,7 @@
         <tr r="P35" s="1"/>
       </tp>
       <tp>
-        <v>0.39602999999999999</v>
+        <v>0.51549</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -5346,7 +5494,7 @@
         <tr r="J5" s="1"/>
       </tp>
       <tp>
-        <v>0.2</v>
+        <v>8.1921800000000005</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -5354,7 +5502,7 @@
         <tr r="J7" s="1"/>
       </tp>
       <tp>
-        <v>2.0441069999999999</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -5367,18 +5515,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7E0BE176-951A-4CA3-A803-9256000D1161}" name="Table2" displayName="Table2" ref="A2:D4" totalsRowShown="0" dataDxfId="85" dataCellStyle="Comma">
-  <autoFilter ref="A2:D4" xr:uid="{580FE727-A11C-4ED9-9482-452D0F24BAD3}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7E0BE176-951A-4CA3-A803-9256000D1161}" name="Table2" displayName="Table2" ref="A2:H4" totalsRowShown="0" dataDxfId="89" dataCellStyle="Comma">
+  <autoFilter ref="A2:H4" xr:uid="{580FE727-A11C-4ED9-9482-452D0F24BAD3}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9C68E037-DF9F-4856-B04D-2DCDFFB4E15E}" name="Ticker"/>
-    <tableColumn id="2" xr3:uid="{8FAA28E5-F641-4937-ADD4-FAC56E0C4147}" name="BID" dataDxfId="84" dataCellStyle="Comma">
+    <tableColumn id="2" xr3:uid="{8FAA28E5-F641-4937-ADD4-FAC56E0C4147}" name="BID" dataDxfId="88" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,GDAX,$A3,B$2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{041CD0D7-D375-4B88-8B1B-CD344CCDEB4E}" name="ASK" dataDxfId="83" dataCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{041CD0D7-D375-4B88-8B1B-CD344CCDEB4E}" name="ASK" dataDxfId="87" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,GDAX,$A3,C$2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5B81F177-A71A-4810-A2A9-102CFDC4A15D}" name="LAST_PRICE" dataDxfId="82" dataCellStyle="Comma">
+    <tableColumn id="4" xr3:uid="{5B81F177-A71A-4810-A2A9-102CFDC4A15D}" name="LAST_PRICE" dataDxfId="86" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,GDAX,$A3,D$2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{88E54DB0-E57D-4C05-B81D-0BDDFCBC50D3}" name="open_24h" dataDxfId="3" dataCellStyle="Comma">
+      <calculatedColumnFormula>RTD(progId,,GDAX,$A3,E$2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{0644C03A-2092-4785-8C82-498398297E87}" name="high_24h" dataDxfId="2" dataCellStyle="Comma">
+      <calculatedColumnFormula>RTD(progId,,GDAX,$A3,F$2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{F7D7129C-1554-4D1C-AC2E-68B137E65B85}" name="low_24h" dataDxfId="1" dataCellStyle="Comma">
+      <calculatedColumnFormula>RTD(progId,,GDAX,$A3,G$2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{4BD2F6D0-F9D4-4F69-8989-8E5F76D88E95}" name="volume_24h" dataDxfId="0" dataCellStyle="Comma">
+      <calculatedColumnFormula>RTD(progId,,GDAX,$A3,H$2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5386,50 +5546,50 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4EA86895-C996-45BB-9461-8033276EAF8D}" name="Table1" displayName="Table1" ref="A4:O11" totalsRowShown="0" dataDxfId="81" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4EA86895-C996-45BB-9461-8033276EAF8D}" name="Table1" displayName="Table1" ref="A4:O11" totalsRowShown="0" dataDxfId="85" dataCellStyle="Comma">
   <autoFilter ref="A4:O11" xr:uid="{C4F49F7D-8667-4D6B-AD96-B004DDF9E1A6}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{3DCAC593-21E4-456C-93D1-EEDC8340EA91}" name="Ticker"/>
-    <tableColumn id="2" xr3:uid="{BD1F10D1-4516-437C-A019-01CE2442BC76}" name="LOW" dataDxfId="80" totalsRowDxfId="79" dataCellStyle="Comma">
+    <tableColumn id="2" xr3:uid="{BD1F10D1-4516-437C-A019-01CE2442BC76}" name="LOW" dataDxfId="84" totalsRowDxfId="83" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,B$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{91943E91-93A3-432F-90A1-9A812A7495A3}" name="HIGH" dataDxfId="78" totalsRowDxfId="77" dataCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{91943E91-93A3-432F-90A1-9A812A7495A3}" name="HIGH" dataDxfId="82" totalsRowDxfId="81" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,C$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{16B5E286-FCD6-42DD-AD70-936F5453E647}" name="CLOSE" dataDxfId="76" totalsRowDxfId="75" dataCellStyle="Comma">
+    <tableColumn id="4" xr3:uid="{16B5E286-FCD6-42DD-AD70-936F5453E647}" name="CLOSE" dataDxfId="80" totalsRowDxfId="79" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,D$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{67B2C544-857B-4123-809A-B920230BEECB}" name="OPEN" dataDxfId="74" dataCellStyle="Comma">
+    <tableColumn id="15" xr3:uid="{67B2C544-857B-4123-809A-B920230BEECB}" name="OPEN" dataDxfId="78" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,E$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{20BDBC22-B4AF-42A8-AAE5-B7ECB2022FC2}" name="BID_SIZE" dataDxfId="73" totalsRowDxfId="72" dataCellStyle="Comma">
+    <tableColumn id="9" xr3:uid="{20BDBC22-B4AF-42A8-AAE5-B7ECB2022FC2}" name="BID_SIZE" dataDxfId="77" totalsRowDxfId="76" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,F$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{ECAEA6E2-113E-4E1B-AC1E-0EC5CB822859}" name="BID" dataDxfId="71" totalsRowDxfId="70" dataCellStyle="Comma">
+    <tableColumn id="7" xr3:uid="{ECAEA6E2-113E-4E1B-AC1E-0EC5CB822859}" name="BID" dataDxfId="75" totalsRowDxfId="74" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,G$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{2B73FE2B-AD25-474E-A435-F857ECE61F97}" name="Spread" dataDxfId="69" totalsRowDxfId="68" dataCellStyle="Comma">
+    <tableColumn id="14" xr3:uid="{2B73FE2B-AD25-474E-A435-F857ECE61F97}" name="Spread" dataDxfId="73" totalsRowDxfId="72" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,H$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{01343A1D-C841-40C5-A6D2-6BD0755AEFFD}" name="ASK" dataDxfId="67" totalsRowDxfId="66" dataCellStyle="Comma">
+    <tableColumn id="8" xr3:uid="{01343A1D-C841-40C5-A6D2-6BD0755AEFFD}" name="ASK" dataDxfId="71" totalsRowDxfId="70" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,I$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7441CD62-3DE6-428D-A648-DC43FCDEC43E}" name="ASK_SIZE" dataDxfId="65" totalsRowDxfId="64" dataCellStyle="Comma">
+    <tableColumn id="6" xr3:uid="{7441CD62-3DE6-428D-A648-DC43FCDEC43E}" name="ASK_SIZE" dataDxfId="69" totalsRowDxfId="68" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,J$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5886EA1E-E3A6-4210-AA96-061D82EA05DB}" name="VOL" dataDxfId="63" totalsRowDxfId="62" dataCellStyle="Comma">
+    <tableColumn id="5" xr3:uid="{5886EA1E-E3A6-4210-AA96-061D82EA05DB}" name="VOL" dataDxfId="67" totalsRowDxfId="66" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,K$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{ED72F41F-7448-4225-8EB2-C6126D47AA45}" name="QUOTE_VOL" dataDxfId="61" totalsRowDxfId="60" dataCellStyle="Comma">
+    <tableColumn id="10" xr3:uid="{ED72F41F-7448-4225-8EB2-C6126D47AA45}" name="QUOTE_VOL" dataDxfId="65" totalsRowDxfId="64" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,L$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{6F6174C4-E63C-47F0-9019-CB5FC0BB6E18}" name="TRADES" dataDxfId="59" totalsRowDxfId="58" dataCellStyle="Comma">
+    <tableColumn id="11" xr3:uid="{6F6174C4-E63C-47F0-9019-CB5FC0BB6E18}" name="TRADES" dataDxfId="63" totalsRowDxfId="62" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,M$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{D83BB7C6-4C04-4806-AF73-A11C3BF0C421}" name="PRICE%" dataDxfId="57" totalsRowDxfId="56" dataCellStyle="Percent">
+    <tableColumn id="12" xr3:uid="{D83BB7C6-4C04-4806-AF73-A11C3BF0C421}" name="PRICE%" dataDxfId="61" totalsRowDxfId="60" dataCellStyle="Percent">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,N$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{03DEA07C-BDA4-4374-813A-6502C8EC5BD0}" name="PRICE_CHANGE" dataDxfId="55" totalsRowDxfId="54" dataCellStyle="Comma">
+    <tableColumn id="13" xr3:uid="{03DEA07C-BDA4-4374-813A-6502C8EC5BD0}" name="PRICE_CHANGE" dataDxfId="59" totalsRowDxfId="58" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE,$A5,O$4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5438,20 +5598,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{693E15AA-864E-4171-85AC-CA73EF3D952A}" name="Table3" displayName="Table3" ref="A14:E24" totalsRowShown="0" dataDxfId="53" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{693E15AA-864E-4171-85AC-CA73EF3D952A}" name="Table3" displayName="Table3" ref="A14:E24" totalsRowShown="0" dataDxfId="57" dataCellStyle="Comma">
   <autoFilter ref="A14:E24" xr:uid="{9B5750BD-A8BF-49B3-8CCE-E75F6CB95AEF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{024D3077-4CB4-423F-9919-17E1D03B62EF}" name="BID_DEPTH_SIZE" dataDxfId="52" dataCellStyle="20% - Accent6">
+    <tableColumn id="1" xr3:uid="{024D3077-4CB4-423F-9919-17E1D03B62EF}" name="BID_DEPTH_SIZE" dataDxfId="56" dataCellStyle="20% - Accent6">
       <calculatedColumnFormula>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A846FBD5-F5D1-42A6-9B15-E4F95F35D0D8}" name="BID_DEPTH" dataDxfId="51" dataCellStyle="20% - Accent6">
+    <tableColumn id="2" xr3:uid="{A846FBD5-F5D1-42A6-9B15-E4F95F35D0D8}" name="BID_DEPTH" dataDxfId="55" dataCellStyle="20% - Accent6">
       <calculatedColumnFormula>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{61C19639-7D28-4B92-A8B2-CB2407C53DA3}" name="ethusdt" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{26E73E79-2351-4AA2-B059-B8FBF5772528}" name="ASK_DEPTH" dataDxfId="49" dataCellStyle="20% - Accent2">
+    <tableColumn id="3" xr3:uid="{61C19639-7D28-4B92-A8B2-CB2407C53DA3}" name="ethusdt" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{26E73E79-2351-4AA2-B059-B8FBF5772528}" name="ASK_DEPTH" dataDxfId="53" dataCellStyle="20% - Accent2">
       <calculatedColumnFormula>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F75757B-DFD1-4B07-AFA1-EC3E611607E7}" name="ASK_DEPTH_SIZE" dataDxfId="48" dataCellStyle="20% - Accent2">
+    <tableColumn id="5" xr3:uid="{4F75757B-DFD1-4B07-AFA1-EC3E611607E7}" name="ASK_DEPTH_SIZE" dataDxfId="52" dataCellStyle="20% - Accent2">
       <calculatedColumnFormula>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C15)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5460,32 +5620,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7FA08BD9-49E7-43D9-9107-498554C9DD86}" name="Table4" displayName="Table4" ref="G14:O21" totalsRowShown="0" dataDxfId="47" tableBorderDxfId="46" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7FA08BD9-49E7-43D9-9107-498554C9DD86}" name="Table4" displayName="Table4" ref="G14:O21" totalsRowShown="0" dataDxfId="51" tableBorderDxfId="50" dataCellStyle="Comma">
   <autoFilter ref="G14:O21" xr:uid="{A420389B-2E6A-4F02-A7C2-6691F84309DB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4DF9B9E1-1E83-4EF7-84C1-2078EE821C9B}" name="SYMBOL"/>
-    <tableColumn id="2" xr3:uid="{7A9D1BD2-CDED-4716-A77F-64066BF610F2}" name="TRADE_ID" dataDxfId="45" dataCellStyle="Comma">
+    <tableColumn id="2" xr3:uid="{7A9D1BD2-CDED-4716-A77F-64066BF610F2}" name="TRADE_ID" dataDxfId="49" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINACE_TRADE,$G15,H$14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{354287B4-D1D8-44B9-86FB-9FB34A18D99C}" name="PRICE" dataDxfId="44" dataCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{354287B4-D1D8-44B9-86FB-9FB34A18D99C}" name="PRICE" dataDxfId="48" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINACE_TRADE,$G15,I$14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8697802C-B742-4C06-809E-A6FC0FE7CCD5}" name="QUANTITY" dataDxfId="43" dataCellStyle="Comma">
+    <tableColumn id="4" xr3:uid="{8697802C-B742-4C06-809E-A6FC0FE7CCD5}" name="QUANTITY" dataDxfId="47" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINACE_TRADE,$G15,J$14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4B2C6341-2C08-42AC-B29F-1942A6C5C0B8}" name="BUYER_IS_MAKER" dataDxfId="42" dataCellStyle="Comma">
+    <tableColumn id="7" xr3:uid="{4B2C6341-2C08-42AC-B29F-1942A6C5C0B8}" name="BUYER_IS_MAKER" dataDxfId="46" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINACE_TRADE,$G15,K$14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EFB18125-1C0D-4363-B531-114C2E88F054}" name="IGNORE" dataDxfId="41" dataCellStyle="Comma">
+    <tableColumn id="8" xr3:uid="{EFB18125-1C0D-4363-B531-114C2E88F054}" name="IGNORE" dataDxfId="45" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINACE_TRADE,$G15,L$14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{596DAC26-1FB0-4FA0-9F2B-2F85949317B9}" name="FIRST_ID" dataDxfId="40" dataCellStyle="Comma">
+    <tableColumn id="9" xr3:uid="{596DAC26-1FB0-4FA0-9F2B-2F85949317B9}" name="FIRST_ID" dataDxfId="44" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINACE_TRADE,$G15,M$14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{625DA386-D82A-4BD8-99A5-41F6984223F9}" name="LAST_ID" dataDxfId="39" dataCellStyle="Comma">
+    <tableColumn id="10" xr3:uid="{625DA386-D82A-4BD8-99A5-41F6984223F9}" name="LAST_ID" dataDxfId="43" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINACE_TRADE,$G15,N$14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{B43DE4EC-1073-4EE5-AFA6-29717F6887CA}" name="TRADE_TIME" dataDxfId="38" dataCellStyle="Comma">
+    <tableColumn id="11" xr3:uid="{B43DE4EC-1073-4EE5-AFA6-29717F6887CA}" name="TRADE_TIME" dataDxfId="42" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINACE_TRADE,$G15,O$14)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5494,59 +5654,59 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3449DF2E-F96A-49C0-ABBE-71A8697FFDC0}" name="Table6" displayName="Table6" ref="A28:R31" totalsRowShown="0" dataDxfId="37" tableBorderDxfId="36" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3449DF2E-F96A-49C0-ABBE-71A8697FFDC0}" name="Table6" displayName="Table6" ref="A28:R31" totalsRowShown="0" dataDxfId="41" tableBorderDxfId="40" dataCellStyle="Comma">
   <autoFilter ref="A28:R31" xr:uid="{BD9601BD-F222-4DBD-B404-C68EB6A96569}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{A75C3BB9-BD50-4A86-92A6-228C26DADEC8}" name="SYMBOL"/>
-    <tableColumn id="2" xr3:uid="{271F2E56-459C-4325-9A04-1A9F5B3B7F43}" name="OPEN" dataDxfId="35" dataCellStyle="Comma">
+    <tableColumn id="2" xr3:uid="{271F2E56-459C-4325-9A04-1A9F5B3B7F43}" name="OPEN" dataDxfId="39" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,B$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8996362D-BF62-4A19-8C47-D07BB4C877F0}" name="HIGH" dataDxfId="34" dataCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{8996362D-BF62-4A19-8C47-D07BB4C877F0}" name="HIGH" dataDxfId="38" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,C$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77448F41-FF9F-43E6-9CB3-48B1AFE42AEB}" name="LOW" dataDxfId="33" dataCellStyle="Comma">
+    <tableColumn id="4" xr3:uid="{77448F41-FF9F-43E6-9CB3-48B1AFE42AEB}" name="LOW" dataDxfId="37" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,D$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1CBFA155-B8FA-4A1A-9482-672E8069C9E1}" name="CLOSE" dataDxfId="32" dataCellStyle="Comma">
+    <tableColumn id="5" xr3:uid="{1CBFA155-B8FA-4A1A-9482-672E8069C9E1}" name="CLOSE" dataDxfId="36" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,E$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E40AE6FA-10C3-45A4-A49A-5936433E60C5}" name="OPEN_TIME" dataDxfId="31" dataCellStyle="Comma">
+    <tableColumn id="6" xr3:uid="{E40AE6FA-10C3-45A4-A49A-5936433E60C5}" name="OPEN_TIME" dataDxfId="35" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,F$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{429829C2-0F7D-49C8-AC77-925D4DCC80B5}" name="CLOSE_TIME" dataDxfId="30" dataCellStyle="Comma">
+    <tableColumn id="7" xr3:uid="{429829C2-0F7D-49C8-AC77-925D4DCC80B5}" name="CLOSE_TIME" dataDxfId="34" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,G$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{882827BB-E1D4-4F9A-A943-912E4B196B6E}" name="FINAL" dataDxfId="29" dataCellStyle="Comma">
+    <tableColumn id="8" xr3:uid="{882827BB-E1D4-4F9A-A943-912E4B196B6E}" name="FINAL" dataDxfId="33" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,H$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{190D5A98-9240-49A0-8013-C83B0A17B4AA}" name="QUOTE_VOL" dataDxfId="28" dataCellStyle="Comma">
+    <tableColumn id="12" xr3:uid="{190D5A98-9240-49A0-8013-C83B0A17B4AA}" name="QUOTE_VOL" dataDxfId="32" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,I$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D80CA8FB-9312-4FB1-81DE-39FD7E27F1CE}" name="VOL" dataDxfId="27" dataCellStyle="Comma">
+    <tableColumn id="13" xr3:uid="{D80CA8FB-9312-4FB1-81DE-39FD7E27F1CE}" name="VOL" dataDxfId="31" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,J$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{59762A20-FD1E-484A-BB6B-CEA9F72EFC92}" name="TAKE_BUY_VOL" dataDxfId="26" dataCellStyle="Comma">
+    <tableColumn id="14" xr3:uid="{59762A20-FD1E-484A-BB6B-CEA9F72EFC92}" name="TAKE_BUY_VOL" dataDxfId="30" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,K$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E8F62B9A-A83F-46A0-8F0A-0CE5786E7912}" name="TAKE_BUY_QUOTE_VOL" dataDxfId="25" dataCellStyle="Comma">
+    <tableColumn id="15" xr3:uid="{E8F62B9A-A83F-46A0-8F0A-0CE5786E7912}" name="TAKE_BUY_QUOTE_VOL" dataDxfId="29" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,L$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{ED113239-E7EA-4F6B-913B-7D90F2B103BB}" name="INTERVAL" dataDxfId="24" dataCellStyle="Comma">
+    <tableColumn id="9" xr3:uid="{ED113239-E7EA-4F6B-913B-7D90F2B103BB}" name="INTERVAL" dataDxfId="28" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,M$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{68B5E94B-07AA-4E0D-8DC9-26239ADCE6DC}" name="TRADES" dataDxfId="23" dataCellStyle="Comma">
+    <tableColumn id="16" xr3:uid="{68B5E94B-07AA-4E0D-8DC9-26239ADCE6DC}" name="TRADES" dataDxfId="27" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,N$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{11BF3445-5968-4B64-972D-05C6CECCD6DE}" name="Event" dataDxfId="22" dataCellStyle="Comma">
+    <tableColumn id="10" xr3:uid="{11BF3445-5968-4B64-972D-05C6CECCD6DE}" name="Event" dataDxfId="26" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,O$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4B94B3D0-C26F-49E3-A1F8-F4F54AEA1341}" name="Event_Time" dataDxfId="21" dataCellStyle="Comma">
+    <tableColumn id="11" xr3:uid="{4B94B3D0-C26F-49E3-A1F8-F4F54AEA1341}" name="Event_Time" dataDxfId="25" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,P$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{C421FBF6-75FF-4177-B401-9CB15DF618EC}" name="FIRST_ID" dataDxfId="20" dataCellStyle="Comma">
+    <tableColumn id="17" xr3:uid="{C421FBF6-75FF-4177-B401-9CB15DF618EC}" name="FIRST_ID" dataDxfId="24" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,Q$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{3FA40665-835F-4A52-9593-3016675D91AE}" name="LAST_ID" dataDxfId="19" dataCellStyle="Comma">
+    <tableColumn id="18" xr3:uid="{3FA40665-835F-4A52-9593-3016675D91AE}" name="LAST_ID" dataDxfId="23" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A29,R$28,$D$27)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5555,59 +5715,59 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A9543979-F06F-46F2-9BB7-92CC3F74D761}" name="Table66" displayName="Table66" ref="A34:R37" totalsRowShown="0" dataDxfId="18" tableBorderDxfId="17" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A9543979-F06F-46F2-9BB7-92CC3F74D761}" name="Table66" displayName="Table66" ref="A34:R37" totalsRowShown="0" dataDxfId="22" tableBorderDxfId="21" dataCellStyle="Comma">
   <autoFilter ref="A34:R37" xr:uid="{04787891-A2B4-4F14-ADE0-2BC3B779F519}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{CD2685D4-7653-442A-A4D2-04D1D79D1D51}" name="SYMBOL"/>
-    <tableColumn id="2" xr3:uid="{7F137C97-E79A-487B-B508-861F049FEDAC}" name="OPEN" dataDxfId="16" dataCellStyle="Comma">
+    <tableColumn id="2" xr3:uid="{7F137C97-E79A-487B-B508-861F049FEDAC}" name="OPEN" dataDxfId="20" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,B$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4354B8F2-F3BC-4A63-9256-CE5D89BD7C2B}" name="HIGH" dataDxfId="15" dataCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{4354B8F2-F3BC-4A63-9256-CE5D89BD7C2B}" name="HIGH" dataDxfId="19" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,C$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D69F9FDB-4C2B-4CCA-8F57-7B2DFB93739C}" name="LOW" dataDxfId="14" dataCellStyle="Comma">
+    <tableColumn id="4" xr3:uid="{D69F9FDB-4C2B-4CCA-8F57-7B2DFB93739C}" name="LOW" dataDxfId="18" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,D$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{82A6E250-BACF-4151-A155-4791DB06A39C}" name="CLOSE" dataDxfId="13" dataCellStyle="Comma">
+    <tableColumn id="5" xr3:uid="{82A6E250-BACF-4151-A155-4791DB06A39C}" name="CLOSE" dataDxfId="17" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,E$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D574DD0D-6DFB-4B48-9B1B-B8EE63D45B4B}" name="OPEN_TIME" dataDxfId="12" dataCellStyle="Comma">
+    <tableColumn id="6" xr3:uid="{D574DD0D-6DFB-4B48-9B1B-B8EE63D45B4B}" name="OPEN_TIME" dataDxfId="16" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,F$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{10BFDF65-DE5F-4E2B-89F8-F8584D7D2860}" name="CLOSE_TIME" dataDxfId="11" dataCellStyle="Comma">
+    <tableColumn id="7" xr3:uid="{10BFDF65-DE5F-4E2B-89F8-F8584D7D2860}" name="CLOSE_TIME" dataDxfId="15" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,G$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CB0B768D-7853-490A-9ADF-4CE8C41E4DBB}" name="FINAL" dataDxfId="10" dataCellStyle="Comma">
+    <tableColumn id="8" xr3:uid="{CB0B768D-7853-490A-9ADF-4CE8C41E4DBB}" name="FINAL" dataDxfId="14" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,H$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{6A5EC966-BE44-4A64-9534-F53DCC5D84E7}" name="QUOTE_VOL" dataDxfId="9" dataCellStyle="Comma">
+    <tableColumn id="12" xr3:uid="{6A5EC966-BE44-4A64-9534-F53DCC5D84E7}" name="QUOTE_VOL" dataDxfId="13" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,I$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{1F63118F-B624-4D66-86EC-A2D0140A6209}" name="VOL" dataDxfId="8" dataCellStyle="Comma">
+    <tableColumn id="13" xr3:uid="{1F63118F-B624-4D66-86EC-A2D0140A6209}" name="VOL" dataDxfId="12" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,J$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{8AA416CC-EC2D-4AC5-B0F5-BF89B4BDC1DF}" name="TAKE_BUY_VOL" dataDxfId="7" dataCellStyle="Comma">
+    <tableColumn id="14" xr3:uid="{8AA416CC-EC2D-4AC5-B0F5-BF89B4BDC1DF}" name="TAKE_BUY_VOL" dataDxfId="11" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,K$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{05EB0F9B-698C-48B7-8FD2-F4F6E81B4DAA}" name="TAKE_BUY_QUOTE_VOL" dataDxfId="6" dataCellStyle="Comma">
+    <tableColumn id="15" xr3:uid="{05EB0F9B-698C-48B7-8FD2-F4F6E81B4DAA}" name="TAKE_BUY_QUOTE_VOL" dataDxfId="10" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,L$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7A11E2BE-98B4-44A3-A99A-F72BED6FCF64}" name="INTERVAL" dataDxfId="5" dataCellStyle="Comma">
+    <tableColumn id="9" xr3:uid="{7A11E2BE-98B4-44A3-A99A-F72BED6FCF64}" name="INTERVAL" dataDxfId="9" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,M$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{FAC045CA-037C-43CE-8DA6-5B4FA60C5466}" name="TRADES" dataDxfId="4" dataCellStyle="Comma">
+    <tableColumn id="16" xr3:uid="{FAC045CA-037C-43CE-8DA6-5B4FA60C5466}" name="TRADES" dataDxfId="8" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,N$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{528B6C8B-64D5-45B1-8F49-30BB75CB0054}" name="Event" dataDxfId="3" dataCellStyle="Comma">
+    <tableColumn id="10" xr3:uid="{528B6C8B-64D5-45B1-8F49-30BB75CB0054}" name="Event" dataDxfId="7" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,O$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{C1FF08F6-0AC6-46A7-8E2A-7C66E43876F2}" name="Event_Time" dataDxfId="2" dataCellStyle="Comma">
+    <tableColumn id="11" xr3:uid="{C1FF08F6-0AC6-46A7-8E2A-7C66E43876F2}" name="Event_Time" dataDxfId="6" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,P$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{3FA7F86A-4BF7-405A-A0E0-11A0DE928556}" name="FIRST_ID" dataDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="17" xr3:uid="{3FA7F86A-4BF7-405A-A0E0-11A0DE928556}" name="FIRST_ID" dataDxfId="5" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,Q$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{39E54680-13B4-44CA-B586-9595118396B6}" name="LAST_ID" dataDxfId="0" dataCellStyle="Comma">
+    <tableColumn id="18" xr3:uid="{39E54680-13B4-44CA-B586-9595118396B6}" name="LAST_ID" dataDxfId="4" dataCellStyle="Comma">
       <calculatedColumnFormula>RTD(progId,,BINANCE_CANDLE,$A35,R$28,$D$33)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5912,19 +6072,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7470B438-0642-48A4-8F04-0651273A7466}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5932,7 +6096,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -5945,39 +6109,83 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2">
         <f>RTD(progId,,GDAX,$A3,B$2)</f>
-        <v>579.11</v>
+        <v>581.89</v>
       </c>
       <c r="C3" s="2">
         <f>RTD(progId,,GDAX,$A3,C$2)</f>
-        <v>579.25</v>
+        <v>581.9</v>
       </c>
       <c r="D3" s="2">
         <f>RTD(progId,,GDAX,$A3,D$2)</f>
-        <v>579.55999999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>581.9</v>
+      </c>
+      <c r="E3" s="2">
+        <f>RTD(progId,,GDAX,$A3,E$2)</f>
+        <v>643.34</v>
+      </c>
+      <c r="F3" s="2">
+        <f>RTD(progId,,GDAX,$A3,F$2)</f>
+        <v>648.46</v>
+      </c>
+      <c r="G3" s="2">
+        <f>RTD(progId,,GDAX,$A3,G$2)</f>
+        <v>563.27</v>
+      </c>
+      <c r="H3" s="2">
+        <f>RTD(progId,,GDAX,$A3,H$2)</f>
+        <v>215319.31700712</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2">
         <f>RTD(progId,,GDAX,$A4,B$2)</f>
-        <v>7533.14</v>
+        <v>7542.99</v>
       </c>
       <c r="C4" s="2">
         <f>RTD(progId,,GDAX,$A4,C$2)</f>
-        <v>7533.15</v>
+        <v>7543</v>
       </c>
       <c r="D4" s="2">
         <f>RTD(progId,,GDAX,$A4,D$2)</f>
-        <v>7533.15</v>
+        <v>7542.99</v>
+      </c>
+      <c r="E4" s="2">
+        <f>RTD(progId,,GDAX,$A4,E$2)</f>
+        <v>8001.42</v>
+      </c>
+      <c r="F4" s="2">
+        <f>RTD(progId,,GDAX,$A4,F$2)</f>
+        <v>8030.06</v>
+      </c>
+      <c r="G4" s="2">
+        <f>RTD(progId,,GDAX,$A4,G$2)</f>
+        <v>7433.19</v>
+      </c>
+      <c r="H4" s="2">
+        <f>RTD(progId,,GDAX,$A4,H$2)</f>
+        <v>15905.412344120001</v>
       </c>
     </row>
   </sheetData>
@@ -5993,7 +6201,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -6120,51 +6328,51 @@
       </c>
       <c r="D5" s="2">
         <f>RTD(progId,,BINANCE_24H,$A5,D$4)</f>
-        <v>644.25</v>
+        <v>644.26</v>
       </c>
       <c r="E5" s="2">
         <f>RTD(progId,,BINANCE_24H,$A5,E$4)</f>
-        <v>644.25</v>
+        <v>644.99</v>
       </c>
       <c r="F5" s="2">
         <f>RTD(progId,,BINANCE,$A5,F$4)</f>
-        <v>0.49347000000000002</v>
+        <v>0.51527999999999996</v>
       </c>
       <c r="G5" s="2">
         <f>RTD(progId,,BINANCE,$A5,G$4)</f>
-        <v>578</v>
+        <v>581.64</v>
       </c>
       <c r="H5" s="2">
         <f>RTD(progId,,BINANCE,$A5,H$4)</f>
-        <v>0.6</v>
+        <v>0.54</v>
       </c>
       <c r="I5" s="2">
         <f>RTD(progId,,BINANCE,$A5,I$4)</f>
-        <v>578.6</v>
+        <v>582.17999999999995</v>
       </c>
       <c r="J5" s="2">
         <f>RTD(progId,,BINANCE,$A5,J$4)</f>
-        <v>0.39602999999999999</v>
+        <v>0.51549</v>
       </c>
       <c r="K5" s="9">
         <f>RTD(progId,,BINANCE,$A5,K$4)</f>
-        <v>254706.29717999999</v>
+        <v>256884.09805</v>
       </c>
       <c r="L5" s="2">
         <f>RTD(progId,,BINANCE,$A5,L$4)</f>
-        <v>154657317.2878904</v>
+        <v>155567039.23584211</v>
       </c>
       <c r="M5" s="9">
         <f>RTD(progId,,BINANCE,$A5,M$4)</f>
-        <v>199919</v>
+        <v>202926</v>
       </c>
       <c r="N5" s="10">
         <f>RTD(progId,,BINANCE,$A5,N$4)</f>
-        <v>-0.1024</v>
+        <v>-9.5460000000000003E-2</v>
       </c>
       <c r="O5" s="2">
         <f>RTD(progId,,BINANCE,$A5,O$4)</f>
-        <v>-66.010000000000005</v>
+        <v>-61.44</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -6181,51 +6389,51 @@
       </c>
       <c r="D6" s="2">
         <f>RTD(progId,,BINANCE_24H,$A6,D$4)</f>
-        <v>8000</v>
+        <v>7997.61</v>
       </c>
       <c r="E6" s="2">
         <f>RTD(progId,,BINANCE_24H,$A6,E$4)</f>
-        <v>8009.9</v>
+        <v>8005.48</v>
       </c>
       <c r="F6" s="2">
         <f>RTD(progId,,BINANCE,$A6,F$4)</f>
-        <v>2</v>
+        <v>3.1895720000000001</v>
       </c>
       <c r="G6" s="2">
         <f>RTD(progId,,BINANCE,$A6,G$4)</f>
-        <v>7512.58</v>
+        <v>7535</v>
       </c>
       <c r="H6" s="2">
         <f>RTD(progId,,BINANCE,$A6,H$4)</f>
-        <v>2.42</v>
+        <v>5.08</v>
       </c>
       <c r="I6" s="2">
         <f>RTD(progId,,BINANCE,$A6,I$4)</f>
-        <v>7515</v>
+        <v>7540.08</v>
       </c>
       <c r="J6" s="2">
         <f>RTD(progId,,BINANCE,$A6,J$4)</f>
-        <v>2.0441069999999999</v>
+        <v>1</v>
       </c>
       <c r="K6" s="9">
         <f>RTD(progId,,BINANCE,$A6,K$4)</f>
-        <v>42435.118895</v>
+        <v>42870.260064000002</v>
       </c>
       <c r="L6" s="2">
         <f>RTD(progId,,BINANCE,$A6,L$4)</f>
-        <v>328149121.66622531</v>
+        <v>330978506.52329791</v>
       </c>
       <c r="M6" s="9">
         <f>RTD(progId,,BINANCE,$A6,M$4)</f>
-        <v>304507</v>
+        <v>306779</v>
       </c>
       <c r="N6" s="10">
         <f>RTD(progId,,BINANCE,$A6,N$4)</f>
-        <v>-6.2440000000000002E-2</v>
+        <v>-5.772E-2</v>
       </c>
       <c r="O6" s="2">
         <f>RTD(progId,,BINANCE,$A6,O$4)</f>
-        <v>-500.47</v>
+        <v>-461.59</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -6242,19 +6450,19 @@
       </c>
       <c r="D7" s="2">
         <f>RTD(progId,,BINANCE_24H,$A7,D$4)</f>
-        <v>128.44999999999999</v>
+        <v>128.15</v>
       </c>
       <c r="E7" s="2">
         <f>RTD(progId,,BINANCE_24H,$A7,E$4)</f>
-        <v>128.51</v>
+        <v>128.25</v>
       </c>
       <c r="F7" s="2">
         <f>RTD(progId,,BINANCE,$A7,F$4)</f>
-        <v>1.7439100000000001</v>
+        <v>7.50021</v>
       </c>
       <c r="G7" s="2">
         <f>RTD(progId,,BINANCE,$A7,G$4)</f>
-        <v>118.54</v>
+        <v>118.74</v>
       </c>
       <c r="H7" s="2">
         <f>RTD(progId,,BINANCE,$A7,H$4)</f>
@@ -6262,31 +6470,31 @@
       </c>
       <c r="I7" s="2">
         <f>RTD(progId,,BINANCE,$A7,I$4)</f>
-        <v>118.71</v>
+        <v>118.91</v>
       </c>
       <c r="J7" s="2">
         <f>RTD(progId,,BINANCE,$A7,J$4)</f>
-        <v>0.2</v>
+        <v>8.1921800000000005</v>
       </c>
       <c r="K7" s="9">
         <f>RTD(progId,,BINANCE,$A7,K$4)</f>
-        <v>106280.56263</v>
+        <v>106827.6857</v>
       </c>
       <c r="L7" s="2">
         <f>RTD(progId,,BINANCE,$A7,L$4)</f>
-        <v>12995945.213345701</v>
+        <v>13030528.640093099</v>
       </c>
       <c r="M7" s="9">
         <f>RTD(progId,,BINANCE,$A7,M$4)</f>
-        <v>29571</v>
+        <v>29990</v>
       </c>
       <c r="N7" s="10">
         <f>RTD(progId,,BINANCE,$A7,N$4)</f>
-        <v>-7.7700000000000005E-2</v>
+        <v>-7.4730000000000005E-2</v>
       </c>
       <c r="O7" s="2">
         <f>RTD(progId,,BINANCE,$A7,O$4)</f>
-        <v>-10</v>
+        <v>-9.59</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -6299,55 +6507,55 @@
       </c>
       <c r="C8" s="2">
         <f>RTD(progId,,BINANCE,$A8,C$4)</f>
-        <v>0.64600000000000002</v>
+        <v>0.64488000000000001</v>
       </c>
       <c r="D8" s="2">
         <f>RTD(progId,,BINANCE_24H,$A8,D$4)</f>
-        <v>0.64510000000000001</v>
+        <v>0.63775000000000004</v>
       </c>
       <c r="E8" s="2">
         <f>RTD(progId,,BINANCE_24H,$A8,E$4)</f>
-        <v>0.64571999999999996</v>
+        <v>0.63848000000000005</v>
       </c>
       <c r="F8" s="9">
         <f>RTD(progId,,BINANCE,$A8,F$4)</f>
-        <v>185</v>
+        <v>301.3</v>
       </c>
       <c r="G8" s="2">
         <f>RTD(progId,,BINANCE,$A8,G$4)</f>
-        <v>0.59524999999999995</v>
+        <v>0.59423000000000004</v>
       </c>
       <c r="H8" s="2">
         <f>RTD(progId,,BINANCE,$A8,H$4)</f>
-        <v>7.5000000000000002E-4</v>
+        <v>2.8400000000000001E-3</v>
       </c>
       <c r="I8" s="2">
         <f>RTD(progId,,BINANCE,$A8,I$4)</f>
-        <v>0.59599999999999997</v>
+        <v>0.59706999999999999</v>
       </c>
       <c r="J8" s="2">
         <f>RTD(progId,,BINANCE,$A8,J$4)</f>
-        <v>13250</v>
+        <v>255.67</v>
       </c>
       <c r="K8" s="9">
         <f>RTD(progId,,BINANCE,$A8,K$4)</f>
-        <v>20037666.02</v>
+        <v>20153277.09</v>
       </c>
       <c r="L8" s="2">
         <f>RTD(progId,,BINANCE,$A8,L$4)</f>
-        <v>12182594.599355601</v>
+        <v>12225585.756023699</v>
       </c>
       <c r="M8" s="9">
         <f>RTD(progId,,BINANCE,$A8,M$4)</f>
-        <v>30998</v>
+        <v>31473</v>
       </c>
       <c r="N8" s="10">
         <f>RTD(progId,,BINANCE,$A8,N$4)</f>
-        <v>-7.5969999999999996E-2</v>
+        <v>-6.5369999999999998E-2</v>
       </c>
       <c r="O8" s="2">
         <f>RTD(progId,,BINANCE,$A8,O$4)</f>
-        <v>-4.9000000000000002E-2</v>
+        <v>-4.1759999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -6364,19 +6572,19 @@
       </c>
       <c r="D9" s="2">
         <f>RTD(progId,,BINANCE_24H,$A9,D$4)</f>
-        <v>7.1669999999999998E-3</v>
+        <v>7.1599999999999997E-3</v>
       </c>
       <c r="E9" s="2">
         <f>RTD(progId,,BINANCE_24H,$A9,E$4)</f>
-        <v>7.1669999999999998E-3</v>
+        <v>7.1599999999999997E-3</v>
       </c>
       <c r="F9" s="9">
         <f>RTD(progId,,BINANCE,$A9,F$4)</f>
-        <v>4.5599999999999996</v>
+        <v>1.49</v>
       </c>
       <c r="G9" s="2">
         <f>RTD(progId,,BINANCE,$A9,G$4)</f>
-        <v>6.9259999999999999E-3</v>
+        <v>6.9319999999999998E-3</v>
       </c>
       <c r="H9" s="2">
         <f>RTD(progId,,BINANCE,$A9,H$4)</f>
@@ -6384,31 +6592,31 @@
       </c>
       <c r="I9" s="2">
         <f>RTD(progId,,BINANCE,$A9,I$4)</f>
-        <v>6.9280000000000001E-3</v>
+        <v>6.9340000000000001E-3</v>
       </c>
       <c r="J9" s="2">
         <f>RTD(progId,,BINANCE,$A9,J$4)</f>
-        <v>3.89</v>
+        <v>9.5399999999999991</v>
       </c>
       <c r="K9" s="9">
         <f>RTD(progId,,BINANCE,$A9,K$4)</f>
-        <v>372632.11</v>
+        <v>372005.87</v>
       </c>
       <c r="L9" s="2">
         <f>RTD(progId,,BINANCE,$A9,L$4)</f>
-        <v>2624.7235926899998</v>
+        <v>2618.51439093</v>
       </c>
       <c r="M9" s="9">
         <f>RTD(progId,,BINANCE,$A9,M$4)</f>
-        <v>52009</v>
+        <v>52096</v>
       </c>
       <c r="N9" s="10">
         <f>RTD(progId,,BINANCE,$A9,N$4)</f>
-        <v>-3.1300000000000001E-2</v>
+        <v>-3.0890000000000001E-2</v>
       </c>
       <c r="O9" s="2">
         <f>RTD(progId,,BINANCE,$A9,O$4)</f>
-        <v>-2.24E-4</v>
+        <v>-2.2100000000000001E-4</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6425,51 +6633,51 @@
       </c>
       <c r="D10" s="2">
         <f>RTD(progId,,BINANCE_24H,$A10,D$4)</f>
-        <v>8.0550000000000006E-5</v>
+        <v>8.0010000000000001E-5</v>
       </c>
       <c r="E10" s="2">
         <f>RTD(progId,,BINANCE_24H,$A10,E$4)</f>
-        <v>8.0500000000000005E-5</v>
+        <v>8.0010000000000001E-5</v>
       </c>
       <c r="F10" s="9">
         <f>RTD(progId,,BINANCE,$A10,F$4)</f>
-        <v>900</v>
+        <v>6386</v>
       </c>
       <c r="G10" s="2">
         <f>RTD(progId,,BINANCE,$A10,G$4)</f>
-        <v>7.9309999999999998E-5</v>
+        <v>7.894E-5</v>
       </c>
       <c r="H10" s="2">
         <f>RTD(progId,,BINANCE,$A10,H$4)</f>
-        <v>4.0000000000000001E-8</v>
+        <v>1.1000000000000001E-7</v>
       </c>
       <c r="I10" s="2">
         <f>RTD(progId,,BINANCE,$A10,I$4)</f>
-        <v>7.9350000000000004E-5</v>
+        <v>7.9049999999999997E-5</v>
       </c>
       <c r="J10" s="2">
         <f>RTD(progId,,BINANCE,$A10,J$4)</f>
-        <v>173</v>
+        <v>1264</v>
       </c>
       <c r="K10" s="9">
         <f>RTD(progId,,BINANCE,$A10,K$4)</f>
-        <v>41883660</v>
+        <v>41524771</v>
       </c>
       <c r="L10" s="2">
         <f>RTD(progId,,BINANCE,$A10,L$4)</f>
-        <v>3304.1174867200002</v>
+        <v>3274.4077716900001</v>
       </c>
       <c r="M10" s="9">
         <f>RTD(progId,,BINANCE,$A10,M$4)</f>
-        <v>66180</v>
+        <v>66201</v>
       </c>
       <c r="N10" s="10">
         <f>RTD(progId,,BINANCE,$A10,N$4)</f>
-        <v>-1.576E-2</v>
+        <v>-1.2E-2</v>
       </c>
       <c r="O10" s="2">
         <f>RTD(progId,,BINANCE,$A10,O$4)</f>
-        <v>-1.2699999999999999E-6</v>
+        <v>-9.5999999999999991E-7</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6486,23 +6694,23 @@
       </c>
       <c r="D11" s="2">
         <f>RTD(progId,,BINANCE_24H,$A11,D$4)</f>
-        <v>9.2199999999999998E-6</v>
+        <v>9.1900000000000001E-6</v>
       </c>
       <c r="E11" s="2">
         <f>RTD(progId,,BINANCE_24H,$A11,E$4)</f>
-        <v>9.2199999999999998E-6</v>
+        <v>9.1900000000000001E-6</v>
       </c>
       <c r="F11" s="9">
         <f>RTD(progId,,BINANCE,$A11,F$4)</f>
-        <v>92528</v>
+        <v>356491</v>
       </c>
       <c r="G11" s="2">
         <f>RTD(progId,,BINANCE,$A11,G$4)</f>
-        <v>9.0499999999999997E-6</v>
+        <v>9.0599999999999997E-6</v>
       </c>
       <c r="H11" s="2">
         <f>RTD(progId,,BINANCE,$A11,H$4)</f>
-        <v>2E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="I11" s="2">
         <f>RTD(progId,,BINANCE,$A11,I$4)</f>
@@ -6510,27 +6718,27 @@
       </c>
       <c r="J11" s="2">
         <f>RTD(progId,,BINANCE,$A11,J$4)</f>
-        <v>235468</v>
+        <v>1963</v>
       </c>
       <c r="K11" s="9">
         <f>RTD(progId,,BINANCE,$A11,K$4)</f>
-        <v>1518580274</v>
+        <v>1521798589</v>
       </c>
       <c r="L11" s="2">
         <f>RTD(progId,,BINANCE,$A11,L$4)</f>
-        <v>13743.119085259999</v>
+        <v>13766.77456217</v>
       </c>
       <c r="M11" s="9">
         <f>RTD(progId,,BINANCE,$A11,M$4)</f>
-        <v>127521</v>
+        <v>128495</v>
       </c>
       <c r="N11" s="10">
         <f>RTD(progId,,BINANCE,$A11,N$4)</f>
-        <v>-1.8440000000000002E-2</v>
+        <v>-1.52E-2</v>
       </c>
       <c r="O11" s="2">
         <f>RTD(progId,,BINANCE,$A11,O$4)</f>
-        <v>-1.6999999999999999E-7</v>
+        <v>-1.4000000000000001E-7</v>
       </c>
     </row>
     <row r="12" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6606,41 +6814,41 @@
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C15)</f>
-        <v>0.49347000000000002</v>
+        <v>0.51527999999999996</v>
       </c>
       <c r="B15" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C15)</f>
-        <v>578</v>
+        <v>581.64</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
       </c>
       <c r="D15" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C15)</f>
-        <v>578.6</v>
+        <v>582.17999999999995</v>
       </c>
       <c r="E15" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C15)</f>
-        <v>0.39602999999999999</v>
+        <v>0.51549</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G15,H$14)</f>
-        <v>23115870</v>
+        <v>23121775</v>
       </c>
       <c r="I15" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G15,I$14)</f>
-        <v>578</v>
+        <v>582.20000000000005</v>
       </c>
       <c r="J15" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G15,J$14)</f>
-        <v>0.49347000000000002</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="K15" s="16" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G15,K$14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="16" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G15,L$14)</f>
@@ -6648,25 +6856,25 @@
       </c>
       <c r="M15" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G15,M$14)</f>
-        <v>26040847</v>
+        <v>26047743</v>
       </c>
       <c r="N15" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G15,N$14)</f>
-        <v>26040847</v>
+        <v>26047743</v>
       </c>
       <c r="O15" s="33">
         <f>RTD(progId,,BINACE_TRADE,$G15,O$14)</f>
-        <v>43243.799419756942</v>
+        <v>43243.828132083334</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C16)</f>
-        <v>1.7999999999999999E-2</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="B16" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C16)</f>
-        <v>577.99</v>
+        <v>581.63</v>
       </c>
       <c r="C16" s="8">
         <f>C15+1</f>
@@ -6674,26 +6882,26 @@
       </c>
       <c r="D16" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C16)</f>
-        <v>578.82000000000005</v>
+        <v>582.19000000000005</v>
       </c>
       <c r="E16" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C16)</f>
-        <v>9</v>
+        <v>1.2547900000000001</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G16,H$14)</f>
-        <v>39447096</v>
+        <v>39455650</v>
       </c>
       <c r="I16" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G16,I$14)</f>
-        <v>7512.58</v>
+        <v>7535</v>
       </c>
       <c r="J16" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G16,J$14)</f>
-        <v>9.9999999999999995E-7</v>
+        <v>2.758E-3</v>
       </c>
       <c r="K16" s="16" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G16,K$14)</f>
@@ -6705,15 +6913,15 @@
       </c>
       <c r="M16" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G16,M$14)</f>
-        <v>45352162</v>
+        <v>45361382</v>
       </c>
       <c r="N16" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G16,N$14)</f>
-        <v>45352162</v>
+        <v>45361382</v>
       </c>
       <c r="O16" s="33">
         <f>RTD(progId,,BINACE_TRADE,$G16,O$14)</f>
-        <v>43243.799415833331</v>
+        <v>43243.828134444448</v>
       </c>
       <c r="Q16" s="38">
         <f>Table4[[#This Row],[PRICE]]-G6</f>
@@ -6721,17 +6929,17 @@
       </c>
       <c r="R16" s="38">
         <f>Table4[[#This Row],[PRICE]]-I6</f>
-        <v>-2.4200000000000728</v>
+        <v>-5.0799999999999272</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C17)</f>
-        <v>1.7999999999999999E-2</v>
+        <v>16.292899999999999</v>
       </c>
       <c r="B17" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C17)</f>
-        <v>577.83000000000004</v>
+        <v>581.6</v>
       </c>
       <c r="C17" s="8">
         <f t="shared" ref="C17:C24" si="0">C16+1</f>
@@ -6739,30 +6947,30 @@
       </c>
       <c r="D17" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C17)</f>
-        <v>578.87</v>
+        <v>582.21</v>
       </c>
       <c r="E17" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C17)</f>
-        <v>0.06</v>
+        <v>9.8913600000000006</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>17</v>
       </c>
       <c r="H17" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G17,H$14)</f>
-        <v>6593265</v>
+        <v>6594163</v>
       </c>
       <c r="I17" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G17,I$14)</f>
-        <v>118.7</v>
+        <v>118.74</v>
       </c>
       <c r="J17" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G17,J$14)</f>
-        <v>9.264E-2</v>
+        <v>3.7019899999999999</v>
       </c>
       <c r="K17" s="16" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G17,K$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="16" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G17,L$14)</f>
@@ -6770,26 +6978,26 @@
       </c>
       <c r="M17" s="23">
         <f>RTD(progId,,BINACE_TRADE,$G17,M$14)</f>
-        <v>7487351</v>
+        <v>7488320</v>
       </c>
       <c r="N17" s="23">
         <f>RTD(progId,,BINACE_TRADE,$G17,N$14)</f>
-        <v>7487351</v>
+        <v>7488321</v>
       </c>
       <c r="O17" s="34">
         <f>RTD(progId,,BINACE_TRADE,$G17,O$14)</f>
-        <v>43243.799404479163</v>
+        <v>43243.828064386573</v>
       </c>
       <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C18)</f>
-        <v>1.7999999999999999E-2</v>
+        <v>6.8779999999999994E-2</v>
       </c>
       <c r="B18" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C18)</f>
-        <v>577.74</v>
+        <v>581.53</v>
       </c>
       <c r="C18" s="8">
         <f t="shared" si="0"/>
@@ -6797,26 +7005,26 @@
       </c>
       <c r="D18" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C18)</f>
-        <v>578.95000000000005</v>
+        <v>582.22</v>
       </c>
       <c r="E18" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C18)</f>
-        <v>0.5</v>
+        <v>0.24571999999999999</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G18,H$14)</f>
-        <v>458525</v>
+        <v>459548</v>
       </c>
       <c r="I18" s="35">
         <f>RTD(progId,,BINACE_TRADE,$G18,I$14)</f>
-        <v>0.59599999999999997</v>
+        <v>0.59702999999999995</v>
       </c>
       <c r="J18" s="35">
         <f>RTD(progId,,BINACE_TRADE,$G18,J$14)</f>
-        <v>0.34</v>
+        <v>64.209999999999994</v>
       </c>
       <c r="K18" s="35" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G18,K$14)</f>
@@ -6828,25 +7036,25 @@
       </c>
       <c r="M18" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G18,M$14)</f>
-        <v>505569</v>
+        <v>506654</v>
       </c>
       <c r="N18" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G18,N$14)</f>
-        <v>505569</v>
+        <v>506654</v>
       </c>
       <c r="O18" s="33">
         <f>RTD(progId,,BINACE_TRADE,$G18,O$14)</f>
-        <v>43243.799348125001</v>
+        <v>43243.827995428241</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C19)</f>
-        <v>1.7999999999999999E-2</v>
+        <v>1.72058</v>
       </c>
       <c r="B19" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C19)</f>
-        <v>577.65</v>
+        <v>581.17999999999995</v>
       </c>
       <c r="C19" s="8">
         <f t="shared" si="0"/>
@@ -6854,30 +7062,30 @@
       </c>
       <c r="D19" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C19)</f>
-        <v>578.96</v>
+        <v>582.59</v>
       </c>
       <c r="E19" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C19)</f>
-        <v>0.219</v>
+        <v>1.4</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H19" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G19,H$14)</f>
-        <v>13330496</v>
+        <v>13331554</v>
       </c>
       <c r="I19" s="35">
         <f>RTD(progId,,BINACE_TRADE,$G19,I$14)</f>
-        <v>6.9259999999999999E-3</v>
+        <v>6.9329999999999999E-3</v>
       </c>
       <c r="J19" s="35">
         <f>RTD(progId,,BINACE_TRADE,$G19,J$14)</f>
-        <v>2.66</v>
+        <v>1.79</v>
       </c>
       <c r="K19" s="35" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G19,K$14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="35" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G19,L$14)</f>
@@ -6885,25 +7093,25 @@
       </c>
       <c r="M19" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G19,M$14)</f>
-        <v>15050999</v>
+        <v>15052222</v>
       </c>
       <c r="N19" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G19,N$14)</f>
-        <v>15051000</v>
+        <v>15052222</v>
       </c>
       <c r="O19" s="33">
         <f>RTD(progId,,BINACE_TRADE,$G19,O$14)</f>
-        <v>43243.799420706018</v>
+        <v>43243.828137083336</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C20)</f>
-        <v>1.52519</v>
+        <v>1.00299</v>
       </c>
       <c r="B20" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C20)</f>
-        <v>577.64</v>
+        <v>581.15</v>
       </c>
       <c r="C20" s="8">
         <f t="shared" si="0"/>
@@ -6911,30 +7119,30 @@
       </c>
       <c r="D20" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C20)</f>
-        <v>579.01</v>
+        <v>582.6</v>
       </c>
       <c r="E20" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C20)</f>
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G20,H$14)</f>
-        <v>17203563</v>
+        <v>17205151</v>
       </c>
       <c r="I20" s="35">
         <f>RTD(progId,,BINACE_TRADE,$G20,I$14)</f>
-        <v>7.9300000000000003E-5</v>
+        <v>7.9040000000000002E-5</v>
       </c>
       <c r="J20" s="35">
         <f>RTD(progId,,BINACE_TRADE,$G20,J$14)</f>
-        <v>2000</v>
+        <v>2484</v>
       </c>
       <c r="K20" s="35" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G20,K$14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="35" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G20,L$14)</f>
@@ -6942,25 +7150,25 @@
       </c>
       <c r="M20" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G20,M$14)</f>
-        <v>20826818</v>
+        <v>20828597</v>
       </c>
       <c r="N20" s="16">
         <f>RTD(progId,,BINACE_TRADE,$G20,N$14)</f>
-        <v>20826818</v>
+        <v>20828597</v>
       </c>
       <c r="O20" s="33">
         <f>RTD(progId,,BINACE_TRADE,$G20,O$14)</f>
-        <v>43243.799358796299</v>
+        <v>43243.828053148151</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C21)</f>
-        <v>10</v>
+        <v>1.6310100000000001</v>
       </c>
       <c r="B21" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C21)</f>
-        <v>577.63</v>
+        <v>581</v>
       </c>
       <c r="C21" s="8">
         <f t="shared" si="0"/>
@@ -6968,18 +7176,18 @@
       </c>
       <c r="D21" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C21)</f>
-        <v>579.02</v>
+        <v>582.70000000000005</v>
       </c>
       <c r="E21" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C21)</f>
-        <v>5.8026999999999997</v>
+        <v>2.2280600000000002</v>
       </c>
       <c r="G21" s="36" t="s">
         <v>30</v>
       </c>
       <c r="H21" s="23">
         <f>RTD(progId,,BINACE_TRADE,$G21,H$14)</f>
-        <v>17543575</v>
+        <v>17545847</v>
       </c>
       <c r="I21" s="37">
         <f>RTD(progId,,BINACE_TRADE,$G21,I$14)</f>
@@ -6987,7 +7195,7 @@
       </c>
       <c r="J21" s="37">
         <f>RTD(progId,,BINACE_TRADE,$G21,J$14)</f>
-        <v>191</v>
+        <v>428</v>
       </c>
       <c r="K21" s="37" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G21,K$14)</f>
@@ -6999,25 +7207,25 @@
       </c>
       <c r="M21" s="23">
         <f>RTD(progId,,BINACE_TRADE,$G21,M$14)</f>
-        <v>28269780</v>
+        <v>28273403</v>
       </c>
       <c r="N21" s="23">
         <f>RTD(progId,,BINACE_TRADE,$G21,N$14)</f>
-        <v>28269780</v>
+        <v>28273403</v>
       </c>
       <c r="O21" s="34">
         <f>RTD(progId,,BINACE_TRADE,$G21,O$14)</f>
-        <v>43243.799421041665</v>
+        <v>43243.828146215281</v>
       </c>
     </row>
     <row r="22" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C22)</f>
-        <v>0.5</v>
+        <v>0.30843999999999999</v>
       </c>
       <c r="B22" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C22)</f>
-        <v>577.55999999999995</v>
+        <v>580.96</v>
       </c>
       <c r="C22" s="8">
         <f t="shared" si="0"/>
@@ -7025,21 +7233,21 @@
       </c>
       <c r="D22" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C22)</f>
-        <v>579.26</v>
+        <v>582.77</v>
       </c>
       <c r="E22" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C22)</f>
-        <v>1.4219999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C23)</f>
-        <v>0.40028999999999998</v>
+        <v>0.9</v>
       </c>
       <c r="B23" s="20">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C23)</f>
-        <v>577.5</v>
+        <v>580.73</v>
       </c>
       <c r="C23" s="8">
         <f t="shared" si="0"/>
@@ -7047,21 +7255,21 @@
       </c>
       <c r="D23" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C23)</f>
-        <v>579.27</v>
+        <v>582.9</v>
       </c>
       <c r="E23" s="21">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C23)</f>
-        <v>17</v>
+        <v>0.23400000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="39">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C24)</f>
-        <v>12.9</v>
+        <v>2.2010000000000001</v>
       </c>
       <c r="B24" s="39">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C24)</f>
-        <v>577.44000000000005</v>
+        <v>580.67999999999995</v>
       </c>
       <c r="C24" s="40">
         <f t="shared" si="0"/>
@@ -7069,33 +7277,33 @@
       </c>
       <c r="D24" s="41">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C24)</f>
-        <v>579.29</v>
+        <v>582.92999999999995</v>
       </c>
       <c r="E24" s="41">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C24)</f>
-        <v>0.4</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f>SUM(Table3[BID_DEPTH_SIZE])</f>
-        <v>25.89095</v>
+        <v>24.64106</v>
       </c>
       <c r="B25" s="18">
         <f>SUMPRODUCT(Table3[[BID_DEPTH_SIZE]:[BID_DEPTH]])</f>
-        <v>5802.8709499999986</v>
+        <v>5836.7410599999994</v>
       </c>
       <c r="C25" s="19">
         <f>D25-B25</f>
-        <v>23.778780000001461</v>
+        <v>23.354360000001179</v>
       </c>
       <c r="D25" s="18">
         <f>SUMPRODUCT(Table3[[ASK_DEPTH]:[ASK_DEPTH_SIZE]])</f>
-        <v>5826.6497300000001</v>
+        <v>5860.0954200000006</v>
       </c>
       <c r="E25" s="13">
         <f>SUM(Table3[ASK_DEPTH_SIZE])</f>
-        <v>36.599730000000001</v>
+        <v>34.805420000000005</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="4"/>
@@ -7184,27 +7392,27 @@
       </c>
       <c r="B29" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,B$28,$D$27)</f>
-        <v>577.82000000000005</v>
+        <v>581.96</v>
       </c>
       <c r="C29" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,C$28,$D$27)</f>
-        <v>578.6</v>
+        <v>582.22</v>
       </c>
       <c r="D29" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,D$28,$D$27)</f>
-        <v>577.64</v>
+        <v>581.45000000000005</v>
       </c>
       <c r="E29" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,E$28,$D$27)</f>
-        <v>578</v>
+        <v>582.20000000000005</v>
       </c>
       <c r="F29" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,F$28,$D$27)</f>
-        <v>43243.799305555556</v>
+        <v>43243.827777777777</v>
       </c>
       <c r="G29" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,G$28,$D$27)</f>
-        <v>43243.799999988427</v>
+        <v>43243.828472210647</v>
       </c>
       <c r="H29" s="16" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,H$28,$D$27)</f>
@@ -7212,19 +7420,19 @@
       </c>
       <c r="I29" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,I$28,$D$27)</f>
-        <v>745.85206400000004</v>
+        <v>9124.4314945999995</v>
       </c>
       <c r="J29" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,J$28,$D$27)</f>
-        <v>1.2907299999999999</v>
+        <v>15.68529</v>
       </c>
       <c r="K29" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,K$28,$D$27)</f>
-        <v>3.9699999999999996E-3</v>
+        <v>11.4954</v>
       </c>
       <c r="L29" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,L$28,$D$27)</f>
-        <v>2.2970419999999998</v>
+        <v>6687.1171244999996</v>
       </c>
       <c r="M29" s="16" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,M$28,$D$27)</f>
@@ -7232,7 +7440,7 @@
       </c>
       <c r="N29" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,N$28,$D$27)</f>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="O29" s="16" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,O$28,$D$27)</f>
@@ -7240,15 +7448,15 @@
       </c>
       <c r="P29" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,P$28,$D$27)</f>
-        <v>43243.799419791663</v>
+        <v>43243.828132118055</v>
       </c>
       <c r="Q29" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,Q$28,$D$27)</f>
-        <v>26040844</v>
+        <v>26047720</v>
       </c>
       <c r="R29" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A29,R$28,$D$27)</f>
-        <v>26040847</v>
+        <v>26047743</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -7257,27 +7465,27 @@
       </c>
       <c r="B30" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,B$28,$D$27)</f>
-        <v>7513.79</v>
+        <v>7532.15</v>
       </c>
       <c r="C30" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,C$28,$D$27)</f>
-        <v>7515</v>
+        <v>7540.07</v>
       </c>
       <c r="D30" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,D$28,$D$27)</f>
-        <v>7512.57</v>
+        <v>7532.15</v>
       </c>
       <c r="E30" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,E$28,$D$27)</f>
-        <v>7515</v>
+        <v>7540.07</v>
       </c>
       <c r="F30" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,F$28,$D$27)</f>
-        <v>43243.799305555556</v>
+        <v>43243.827777777777</v>
       </c>
       <c r="G30" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,G$28,$D$27)</f>
-        <v>43243.799999988427</v>
+        <v>43243.828472210647</v>
       </c>
       <c r="H30" s="16" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,H$28,$D$27)</f>
@@ -7285,19 +7493,19 @@
       </c>
       <c r="I30" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,I$28,$D$27)</f>
-        <v>7128.5009294299998</v>
+        <v>37969.097520559997</v>
       </c>
       <c r="J30" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,J$28,$D$27)</f>
-        <v>0.94858600000000004</v>
+        <v>5.0390579999999998</v>
       </c>
       <c r="K30" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,K$28,$D$27)</f>
-        <v>0.91675099999999998</v>
+        <v>2.9341360000000001</v>
       </c>
       <c r="L30" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,L$28,$D$27)</f>
-        <v>6889.3380536200002</v>
+        <v>22112.017725329999</v>
       </c>
       <c r="M30" s="16" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,M$28,$D$27)</f>
@@ -7305,7 +7513,7 @@
       </c>
       <c r="N30" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,N$28,$D$27)</f>
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="O30" s="16" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,O$28,$D$27)</f>
@@ -7313,15 +7521,15 @@
       </c>
       <c r="P30" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,P$28,$D$27)</f>
-        <v>43243.799413310182</v>
+        <v>43243.82813209491</v>
       </c>
       <c r="Q30" s="31">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,Q$28,$D$27)</f>
-        <v>45352149</v>
+        <v>45361328</v>
       </c>
       <c r="R30" s="31">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,R$28,$D$27)</f>
-        <v>45352159</v>
+        <v>45361379</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -7330,27 +7538,27 @@
       </c>
       <c r="B31" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,B$28,$D$27)</f>
-        <v>118.71</v>
+        <v>118.74</v>
       </c>
       <c r="C31" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,C$28,$D$27)</f>
-        <v>118.71</v>
+        <v>118.74</v>
       </c>
       <c r="D31" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,D$28,$D$27)</f>
-        <v>118.7</v>
+        <v>118.74</v>
       </c>
       <c r="E31" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,E$28,$D$27)</f>
-        <v>118.7</v>
+        <v>118.74</v>
       </c>
       <c r="F31" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,F$28,$D$27)</f>
-        <v>43243.799305555556</v>
+        <v>43243.827777777777</v>
       </c>
       <c r="G31" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,G$28,$D$27)</f>
-        <v>43243.799999988427</v>
+        <v>43243.828472210647</v>
       </c>
       <c r="H31" s="23" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,H$28,$D$27)</f>
@@ -7358,19 +7566,19 @@
       </c>
       <c r="I31" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,I$28,$D$27)</f>
-        <v>1930.5370680000001</v>
+        <v>440.94217739999999</v>
       </c>
       <c r="J31" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,J$28,$D$27)</f>
-        <v>16.262640000000001</v>
+        <v>3.7135099999999999</v>
       </c>
       <c r="K31" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,K$28,$D$27)</f>
-        <v>16.262640000000001</v>
+        <v>0</v>
       </c>
       <c r="L31" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,L$28,$D$27)</f>
-        <v>1930.5370680000001</v>
+        <v>0</v>
       </c>
       <c r="M31" s="23" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,M$28,$D$27)</f>
@@ -7378,7 +7586,7 @@
       </c>
       <c r="N31" s="30">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,N$28,$D$27)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O31" s="23" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,O$28,$D$27)</f>
@@ -7386,15 +7594,15 @@
       </c>
       <c r="P31" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,P$28,$D$27)</f>
-        <v>43243.799404513891</v>
+        <v>43243.828064409725</v>
       </c>
       <c r="Q31" s="31">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,Q$28,$D$27)</f>
-        <v>7487350</v>
+        <v>7488319</v>
       </c>
       <c r="R31" s="31">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,R$28,$D$27)</f>
-        <v>7487351</v>
+        <v>7488321</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -7476,27 +7684,27 @@
       </c>
       <c r="B35" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,B$28,$D$33)</f>
-        <v>580.64</v>
+        <v>582.16</v>
       </c>
       <c r="C35" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,C$28,$D$33)</f>
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D35" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,D$28,$D$33)</f>
-        <v>576.29999999999995</v>
+        <v>578.88</v>
       </c>
       <c r="E35" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,E$28,$D$33)</f>
-        <v>578</v>
+        <v>582.20000000000005</v>
       </c>
       <c r="F35" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,F$28,$D$33)</f>
-        <v>43243.791666666664</v>
+        <v>43243.822916666664</v>
       </c>
       <c r="G35" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,G$28,$D$33)</f>
-        <v>43243.80208332176</v>
+        <v>43243.83333332176</v>
       </c>
       <c r="H35" s="16" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,H$28,$D$33)</f>
@@ -7504,19 +7712,19 @@
       </c>
       <c r="I35" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,I$28,$D$33)</f>
-        <v>1029820.926874</v>
+        <v>678778.01629870001</v>
       </c>
       <c r="J35" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,J$28,$D$33)</f>
-        <v>1775.06377</v>
+        <v>1168.8069</v>
       </c>
       <c r="K35" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,K$28,$D$33)</f>
-        <v>931.01201000000003</v>
+        <v>666.99198999999999</v>
       </c>
       <c r="L35" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,L$28,$D$33)</f>
-        <v>540465.4464899</v>
+        <v>387387.3168272</v>
       </c>
       <c r="M35" s="16" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,M$28,$D$33)</f>
@@ -7524,7 +7732,7 @@
       </c>
       <c r="N35" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,N$28,$D$33)</f>
-        <v>1594</v>
+        <v>1146</v>
       </c>
       <c r="O35" s="16" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,O$28,$D$33)</f>
@@ -7532,15 +7740,15 @@
       </c>
       <c r="P35" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,P$28,$D$33)</f>
-        <v>43243.799419791663</v>
+        <v>43243.828132129631</v>
       </c>
       <c r="Q35" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,Q$28,$D$33)</f>
-        <v>26039254</v>
+        <v>26046598</v>
       </c>
       <c r="R35" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A35,R$28,$D$33)</f>
-        <v>26040847</v>
+        <v>26047743</v>
       </c>
     </row>
     <row r="36" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7549,27 +7757,27 @@
       </c>
       <c r="B36" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,B$28,$D$33)</f>
-        <v>7539.98</v>
+        <v>7543.55</v>
       </c>
       <c r="C36" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,C$28,$D$33)</f>
-        <v>7565.86</v>
+        <v>7554</v>
       </c>
       <c r="D36" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,D$28,$D$33)</f>
-        <v>7500</v>
+        <v>7509.7</v>
       </c>
       <c r="E36" s="16">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,E$28,$D$33)</f>
-        <v>7515</v>
+        <v>7540.07</v>
       </c>
       <c r="F36" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,F$28,$D$33)</f>
-        <v>43243.791666666664</v>
+        <v>43243.822916666664</v>
       </c>
       <c r="G36" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,G$28,$D$33)</f>
-        <v>43243.80208332176</v>
+        <v>43243.83333332176</v>
       </c>
       <c r="H36" s="16" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,H$28,$D$33)</f>
@@ -7577,19 +7785,19 @@
       </c>
       <c r="I36" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,I$28,$D$33)</f>
-        <v>1794793.14691304</v>
+        <v>1191563.72003854</v>
       </c>
       <c r="J36" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,J$28,$D$33)</f>
-        <v>238.42579499999999</v>
+        <v>158.199477</v>
       </c>
       <c r="K36" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,K$28,$D$33)</f>
-        <v>89.971158000000003</v>
+        <v>60.616477000000003</v>
       </c>
       <c r="L36" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,L$28,$D$33)</f>
-        <v>677632.36464485002</v>
+        <v>456326.38714921998</v>
       </c>
       <c r="M36" s="16" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,M$28,$D$33)</f>
@@ -7597,7 +7805,7 @@
       </c>
       <c r="N36" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,N$28,$D$33)</f>
-        <v>1966</v>
+        <v>1223</v>
       </c>
       <c r="O36" s="16" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,O$28,$D$33)</f>
@@ -7605,15 +7813,15 @@
       </c>
       <c r="P36" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,P$28,$D$33)</f>
-        <v>43243.799413310182</v>
+        <v>43243.82813209491</v>
       </c>
       <c r="Q36" s="31">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,Q$28,$D$33)</f>
-        <v>45350194</v>
+        <v>45360157</v>
       </c>
       <c r="R36" s="31">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,R$28,$D$33)</f>
-        <v>45352159</v>
+        <v>45361379</v>
       </c>
     </row>
     <row r="37" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7622,27 +7830,27 @@
       </c>
       <c r="B37" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,B$28,$D$33)</f>
-        <v>119.39</v>
+        <v>118.93</v>
       </c>
       <c r="C37" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,C$28,$D$33)</f>
-        <v>119.68</v>
+        <v>119.23</v>
       </c>
       <c r="D37" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,D$28,$D$33)</f>
-        <v>118.38</v>
+        <v>118.36</v>
       </c>
       <c r="E37" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,E$28,$D$33)</f>
-        <v>118.7</v>
+        <v>118.74</v>
       </c>
       <c r="F37" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,F$28,$D$33)</f>
-        <v>43243.791666666664</v>
+        <v>43243.822916666664</v>
       </c>
       <c r="G37" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,G$28,$D$33)</f>
-        <v>43243.80208332176</v>
+        <v>43243.83333332176</v>
       </c>
       <c r="H37" s="23" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,H$28,$D$33)</f>
@@ -7650,19 +7858,19 @@
       </c>
       <c r="I37" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,I$28,$D$33)</f>
-        <v>419829.58477409999</v>
+        <v>77861.828267599994</v>
       </c>
       <c r="J37" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,J$28,$D$33)</f>
-        <v>3528.9031100000002</v>
+        <v>655.63270999999997</v>
       </c>
       <c r="K37" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,K$28,$D$33)</f>
-        <v>1643.60223</v>
+        <v>160.12298999999999</v>
       </c>
       <c r="L37" s="29">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,L$28,$D$33)</f>
-        <v>196062.29350989999</v>
+        <v>19030.4075118</v>
       </c>
       <c r="M37" s="23" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,M$28,$D$33)</f>
@@ -7670,7 +7878,7 @@
       </c>
       <c r="N37" s="30">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,N$28,$D$33)</f>
-        <v>261</v>
+        <v>130</v>
       </c>
       <c r="O37" s="23" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,O$28,$D$33)</f>
@@ -7678,15 +7886,15 @@
       </c>
       <c r="P37" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,P$28,$D$33)</f>
-        <v>43243.799404513891</v>
+        <v>43243.828064409725</v>
       </c>
       <c r="Q37" s="31">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,Q$28,$D$33)</f>
-        <v>7487091</v>
+        <v>7488192</v>
       </c>
       <c r="R37" s="31">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,R$28,$D$33)</f>
-        <v>7487351</v>
+        <v>7488321</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
33 millisecs for timer interval, that is cooking with gas
</commit_message>
<xml_diff>
--- a/doc/crypto.xlsx
+++ b/doc/crypto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\Crypto\crypto-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC6A323-52C9-4613-959E-A957005DF90A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3080E795-B944-48B0-942D-AD93E60F0868}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12225" tabRatio="245" xr2:uid="{FA204BA2-54FD-4EAD-B49B-FB8867D94DC8}"/>
   </bookViews>
@@ -249,12 +249,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="167" formatCode="mm:ss.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -468,7 +469,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -521,6 +522,7 @@
     <xf numFmtId="43" fontId="1" fillId="4" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent2" xfId="4" builtinId="34"/>
@@ -3427,7 +3429,7 @@
   <volType type="realTimeData">
     <main first="crypto">
       <tp>
-        <v>27338</v>
+        <v>27442</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3435,7 +3437,7 @@
         <tr r="M9" s="1"/>
       </tp>
       <tp>
-        <v>19351</v>
+        <v>19448</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3443,7 +3445,7 @@
         <tr r="M8" s="1"/>
       </tp>
       <tp>
-        <v>235000</v>
+        <v>236915</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3451,7 +3453,7 @@
         <tr r="M7" s="1"/>
       </tp>
       <tp>
-        <v>129082</v>
+        <v>129360</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3459,7 +3461,7 @@
         <tr r="M6" s="1"/>
       </tp>
       <tp>
-        <v>347.96116496000002</v>
+        <v>402.88634443000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3468,7 +3470,7 @@
         <tr r="I33" s="1"/>
       </tp>
       <tp>
-        <v>903.63612820000003</v>
+        <v>958.56130767000002</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3477,7 +3479,7 @@
         <tr r="I39" s="1"/>
       </tp>
       <tp>
-        <v>3.32</v>
+        <v>0.6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3485,7 +3487,7 @@
         <tr r="F10" s="1"/>
       </tp>
       <tp>
-        <v>124344</v>
+        <v>775560</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3493,7 +3495,7 @@
         <tr r="J12" s="1"/>
       </tp>
       <tp>
-        <v>159.16999999999999</v>
+        <v>1784.99</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3519,7 +3521,7 @@
         <tr r="F44" s="1"/>
       </tp>
       <tp>
-        <v>157839.87</v>
+        <v>157292.04999999999</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3527,7 +3529,7 @@
         <tr r="K10" s="1"/>
       </tp>
       <tp>
-        <v>1626347776</v>
+        <v>1618758548</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3535,7 +3537,7 @@
         <tr r="K12" s="1"/>
       </tp>
       <tp>
-        <v>33785487</v>
+        <v>33859109</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3615,7 +3617,7 @@
         <tr r="B38" s="1"/>
       </tp>
       <tp>
-        <v>9898</v>
+        <v>12945</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3624,7 +3626,7 @@
         <tr r="N32" s="1"/>
       </tp>
       <tp>
-        <v>27767</v>
+        <v>30814</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3633,7 +3635,7 @@
         <tr r="N38" s="1"/>
       </tp>
       <tp>
-        <v>4838</v>
+        <v>5754</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3642,7 +3644,7 @@
         <tr r="N31" s="1"/>
       </tp>
       <tp>
-        <v>13033</v>
+        <v>13949</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3651,7 +3653,7 @@
         <tr r="N37" s="1"/>
       </tp>
       <tp>
-        <v>7.9200000000000007E-2</v>
+        <v>6.8860000000000005E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3659,7 +3661,7 @@
         <tr r="N9" s="1"/>
       </tp>
       <tp>
-        <v>7.9509999999999997E-2</v>
+        <v>7.4270000000000003E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3667,7 +3669,7 @@
         <tr r="N8" s="1"/>
       </tp>
       <tp>
-        <v>9.5649999999999999E-2</v>
+        <v>8.5610000000000006E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3675,7 +3677,7 @@
         <tr r="N6" s="1"/>
       </tp>
       <tp>
-        <v>5.1819999999999998E-2</v>
+        <v>4.5539999999999997E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3683,7 +3685,7 @@
         <tr r="N7" s="1"/>
       </tp>
       <tp>
-        <v>0.53383000000000003</v>
+        <v>0.53596999999999995</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3691,7 +3693,7 @@
         <tr r="F6" s="1"/>
       </tp>
       <tp>
-        <v>1.0000000000000001E-5</v>
+        <v>0.77</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3699,7 +3701,7 @@
         <tr r="F8" s="1"/>
       </tp>
       <tp>
-        <v>8.2888000000000003E-2</v>
+        <v>0.33504499999999998</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3707,7 +3709,7 @@
         <tr r="F7" s="1"/>
       </tp>
       <tp>
-        <v>1097.7973295500001</v>
+        <v>1094.1768949100001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3715,7 +3717,7 @@
         <tr r="L10" s="1"/>
       </tp>
       <tp>
-        <v>561.86</v>
+        <v>558.61</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -3723,7 +3725,7 @@
         <tr r="C3" s="2"/>
       </tp>
       <tp>
-        <v>561.85</v>
+        <v>558.51</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -3731,7 +3733,7 @@
         <tr r="B3" s="2"/>
       </tp>
       <tp>
-        <v>52514496.026789799</v>
+        <v>53285467.580611899</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3740,7 +3742,7 @@
         <tr r="I43" s="1"/>
       </tp>
       <tp>
-        <v>129714114.66223025</v>
+        <v>132448240.77314962</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3749,7 +3751,7 @@
         <tr r="I44" s="1"/>
       </tp>
       <tp>
-        <v>7439.41</v>
+        <v>7425.81</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -3757,7 +3759,7 @@
         <tr r="B4" s="2"/>
       </tp>
       <tp>
-        <v>1088</v>
+        <v>105</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3783,7 +3785,7 @@
         <tr r="F39" s="1"/>
       </tp>
       <tp>
-        <v>245903612</v>
+        <v>247738290</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3792,7 +3794,7 @@
         <tr r="K45" s="1"/>
       </tp>
       <tp>
-        <v>7443.8</v>
+        <v>7425.82</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -3808,7 +3810,7 @@
         <tr r="G4" s="2"/>
       </tp>
       <tp>
-        <v>28850790</v>
+        <v>28851370</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3817,7 +3819,7 @@
         <tr r="Q39" s="1"/>
       </tp>
       <tp>
-        <v>28850790</v>
+        <v>28851370</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3835,7 +3837,7 @@
         <tr r="C45" s="1"/>
       </tp>
       <tp>
-        <v>2536.66786</v>
+        <v>2999.4280100000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3844,7 +3846,7 @@
         <tr r="K31" s="1"/>
       </tp>
       <tp>
-        <v>8635.5733899999996</v>
+        <v>9098.3335399999996</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3853,7 +3855,7 @@
         <tr r="K37" s="1"/>
       </tp>
       <tp>
-        <v>622.820652</v>
+        <v>823.47727199999997</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3862,7 +3864,7 @@
         <tr r="K32" s="1"/>
       </tp>
       <tp>
-        <v>2087.112353</v>
+        <v>2287.7689730000002</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3871,7 +3873,7 @@
         <tr r="K38" s="1"/>
       </tp>
       <tp>
-        <v>69718853.044642255</v>
+        <v>71208036.781617776</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3880,7 +3882,7 @@
         <tr r="L44" s="1"/>
       </tp>
       <tp>
-        <v>46725848</v>
+        <v>46728895</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3889,7 +3891,7 @@
         <tr r="Q32" s="1"/>
       </tp>
       <tp>
-        <v>46725848</v>
+        <v>46728895</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3898,7 +3900,7 @@
         <tr r="Q38" s="1"/>
       </tp>
       <tp>
-        <v>2109.96642647</v>
+        <v>2125.7351524699998</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3916,7 +3918,7 @@
         <tr r="B45" s="1"/>
       </tp>
       <tp>
-        <v>7.9900000000000004E-5</v>
+        <v>7.9789999999999993E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3924,7 +3926,7 @@
         <tr r="I11" s="1"/>
       </tp>
       <tp>
-        <v>8.6400000000000003E-6</v>
+        <v>8.6000000000000007E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3932,7 +3934,7 @@
         <tr r="I12" s="1"/>
       </tp>
       <tp>
-        <v>7.0159999999999997E-3</v>
+        <v>7.0049999999999999E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3940,7 +3942,7 @@
         <tr r="I10" s="1"/>
       </tp>
       <tp>
-        <v>7.0150000000000004E-3</v>
+        <v>6.9959999999999996E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3948,7 +3950,7 @@
         <tr r="G10" s="1"/>
       </tp>
       <tp>
-        <v>8.6300000000000004E-6</v>
+        <v>8.5900000000000008E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3956,7 +3958,7 @@
         <tr r="G12" s="1"/>
       </tp>
       <tp>
-        <v>7.9880000000000001E-5</v>
+        <v>7.9770000000000004E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3973,7 +3975,7 @@
         <tr r="G43" s="1"/>
       </tp>
       <tp>
-        <v>462</v>
+        <v>6620</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3989,7 +3991,7 @@
         <tr r="G3" s="2"/>
       </tp>
       <tp>
-        <v>26750922</v>
+        <v>26751838</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3998,7 +4000,7 @@
         <tr r="Q37" s="1"/>
       </tp>
       <tp>
-        <v>26750922</v>
+        <v>26751838</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4031,7 +4033,7 @@
         <tr r="B11" s="1"/>
       </tp>
       <tp>
-        <v>26240139.5047675</v>
+        <v>26499303.289774001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4040,7 +4042,7 @@
         <tr r="L43" s="1"/>
       </tp>
       <tp>
-        <v>3.44</v>
+        <v>1.38</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -4048,7 +4050,7 @@
         <tr r="J10" s="1"/>
       </tp>
       <tp>
-        <v>97197</v>
+        <v>181526</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4056,7 +4058,7 @@
         <tr r="F12" s="1"/>
       </tp>
       <tp>
-        <v>210.15</v>
+        <v>500</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4082,7 +4084,7 @@
         <tr r="G44" s="1"/>
       </tp>
       <tp>
-        <v>0.75</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4090,7 +4092,7 @@
         <tr r="J8" s="1"/>
       </tp>
       <tp>
-        <v>0.14785100000000001</v>
+        <v>0.29883199999999999</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4098,7 +4100,7 @@
         <tr r="J7" s="1"/>
       </tp>
       <tp>
-        <v>0.53381999999999996</v>
+        <v>0.12995999999999999</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4106,7 +4108,7 @@
         <tr r="J6" s="1"/>
       </tp>
       <tp>
-        <v>2674.6815673699998</v>
+        <v>2680.8285568000001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4114,7 +4116,7 @@
         <tr r="L11" s="1"/>
       </tp>
       <tp>
-        <v>46725848</v>
+        <v>46728895</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4123,7 +4125,7 @@
         <tr r="Q44" s="1"/>
       </tp>
       <tp>
-        <v>26750922</v>
+        <v>26751838</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4132,7 +4134,7 @@
         <tr r="Q43" s="1"/>
       </tp>
       <tp>
-        <v>13630.97249443</v>
+        <v>13568.34826689</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4140,7 +4142,7 @@
         <tr r="L12" s="1"/>
       </tp>
       <tp>
-        <v>644938</v>
+        <v>645170</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4166,7 +4168,7 @@
         <tr r="B33" s="1"/>
       </tp>
       <tp>
-        <v>1.3999999999999999E-4</v>
+        <v>1.31E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4174,7 +4176,7 @@
         <tr r="H9" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4182,7 +4184,7 @@
         <tr r="K22" s="1"/>
       </tp>
       <tp>
-        <v>0.01</v>
+        <v>0.14000000000000001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4190,7 +4192,7 @@
         <tr r="H8" s="1"/>
       </tp>
       <tp>
-        <v>4.4400000000000004</v>
+        <v>6.21</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4198,7 +4200,7 @@
         <tr r="H7" s="1"/>
       </tp>
       <tp>
-        <v>0.42</v>
+        <v>0.44</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4215,7 +4217,7 @@
         <tr r="P44" s="1"/>
       </tp>
       <tp>
-        <v>159</v>
+        <v>123</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -4223,7 +4225,7 @@
         <tr r="J21" s="1"/>
       </tp>
       <tp>
-        <v>3732</v>
+        <v>4312</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4232,7 +4234,7 @@
         <tr r="N33" s="1"/>
       </tp>
       <tp>
-        <v>9964</v>
+        <v>10544</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4250,7 +4252,7 @@
         <tr r="P43" s="1"/>
       </tp>
       <tp>
-        <v>13498381</v>
+        <v>13498492</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4267,7 +4269,7 @@
         <tr r="F45" s="1"/>
       </tp>
       <tp>
-        <v>28850790</v>
+        <v>28851371</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4275,7 +4277,7 @@
         <tr r="M22" s="1"/>
       </tp>
       <tp>
-        <v>46725857</v>
+        <v>46728899</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4283,7 +4285,7 @@
         <tr r="M17" s="1"/>
       </tp>
       <tp>
-        <v>7622844</v>
+        <v>7623019</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4291,7 +4293,7 @@
         <tr r="M18" s="1"/>
       </tp>
       <tp>
-        <v>26750925</v>
+        <v>26751838</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4317,7 +4319,7 @@
         <tr r="C33" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -4325,7 +4327,7 @@
         <tr r="K21" s="1"/>
       </tp>
       <tp>
-        <v>21103240</v>
+        <v>21103608</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -4342,7 +4344,7 @@
         <tr r="M44" s="1"/>
       </tp>
       <tp>
-        <v>4559.2420390099996</v>
+        <v>4614.16721848</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4351,7 +4353,7 @@
         <tr r="I45" s="1"/>
       </tp>
       <tp>
-        <v>2.98</v>
+        <v>250</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4359,7 +4361,7 @@
         <tr r="J19" s="1"/>
       </tp>
       <tp>
-        <v>644938</v>
+        <v>645170</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4375,7 +4377,7 @@
         <tr r="L20" s="1"/>
       </tp>
       <tp>
-        <v>1.2909200000000001</v>
+        <v>26.621500000000001</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4383,7 +4385,7 @@
         <tr r="J16" s="1"/>
       </tp>
       <tp>
-        <v>7.6188000000000006E-2</v>
+        <v>6.8230000000000001E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4391,7 +4393,7 @@
         <tr r="J17" s="1"/>
       </tp>
       <tp>
-        <v>6.6955400000000003</v>
+        <v>1E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4408,7 +4410,7 @@
         <tr r="M43" s="1"/>
       </tp>
       <tp>
-        <v>1.2243200000000001</v>
+        <v>19</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4417,7 +4419,7 @@
         <tr r="E24" s="1"/>
       </tp>
       <tp>
-        <v>3.5089999999999999</v>
+        <v>0.24099999999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4435,7 +4437,7 @@
         <tr r="E20" s="1"/>
       </tp>
       <tp>
-        <v>0.24099999999999999</v>
+        <v>2.9530699999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4444,7 +4446,7 @@
         <tr r="E21" s="1"/>
       </tp>
       <tp>
-        <v>3.3609200000000001</v>
+        <v>5.0000400000000003</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4453,7 +4455,7 @@
         <tr r="E22" s="1"/>
       </tp>
       <tp>
-        <v>0.4</v>
+        <v>3.2010000000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4462,7 +4464,7 @@
         <tr r="E23" s="1"/>
       </tp>
       <tp>
-        <v>0.53381999999999996</v>
+        <v>0.12995999999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4471,7 +4473,7 @@
         <tr r="E16" s="1"/>
       </tp>
       <tp>
-        <v>1.8919999999999999</v>
+        <v>0.75</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4480,7 +4482,7 @@
         <tr r="E17" s="1"/>
       </tp>
       <tp>
-        <v>0.38628000000000001</v>
+        <v>6.00251</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4489,7 +4491,7 @@
         <tr r="E18" s="1"/>
       </tp>
       <tp>
-        <v>2.7046800000000002</v>
+        <v>0.27856999999999998</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4498,7 +4500,7 @@
         <tr r="E19" s="1"/>
       </tp>
       <tp>
-        <v>6391</v>
+        <v>40</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4506,7 +4508,7 @@
         <tr r="J22" s="1"/>
       </tp>
       <tp>
-        <v>43249.78407371528</v>
+        <v>43249.790371134259</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4514,7 +4516,7 @@
         <tr r="O19" s="1"/>
       </tp>
       <tp>
-        <v>43249.783948402779</v>
+        <v>43249.790385069442</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4522,7 +4524,7 @@
         <tr r="O18" s="1"/>
       </tp>
       <tp>
-        <v>43249.784074039351</v>
+        <v>43249.790412187504</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4530,7 +4532,7 @@
         <tr r="O16" s="1"/>
       </tp>
       <tp>
-        <v>43249.784088125001</v>
+        <v>43249.790465729166</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4538,7 +4540,7 @@
         <tr r="O17" s="1"/>
       </tp>
       <tp>
-        <v>46725857</v>
+        <v>46728899</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4546,7 +4548,7 @@
         <tr r="N17" s="1"/>
       </tp>
       <tp>
-        <v>15246344</v>
+        <v>15246484</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4554,7 +4556,7 @@
         <tr r="N20" s="1"/>
       </tp>
       <tp>
-        <v>21103240</v>
+        <v>21103608</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -4562,7 +4564,7 @@
         <tr r="N21" s="1"/>
       </tp>
       <tp t="s">
-        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",26750741,563.00000000,5.58010000,"2018-05-29T18:46:58.024-04:00",true,true],["ETHUSDT",26750742,563.00000000,0.14228000,"2018-05-29T18:47:00.152-04:00",true,true],["ETHUSDT",26750743,563.00000000,0.13233000,"2018-05-29T18:47:00.353-04:00",true,true],["ETHUSDT",26750744,563.00000000,0.29970000,"2018-05-29T18:47:00.649-04:00",true,true],["ETHUSDT",26750745,563.01000000,0.50000000,"2018-05-29T18:47:05.632-04:00",true,false],["ETHUSDT",26750746,563.00000000,0.45987000,"2018-05-29T18:47:07.351-04:00",true,true],["ETHUSDT",26750747,563.01000000,1.13900000,"2018-05-29T18:47:07.38-04:00",true,false],["ETHUSDT",26750748,563.00000000,4.10379000,"2018-05-29T18:47:09.759-04:00",true,true],["ETHUSDT",26750749,563.01000000,0.00017000,"2018-05-29T18:47:10.643-04:00",true,false],["ETHUSDT",26750750,563.00000000,0.44356000,"2018-05-29T18:47:11.411-04:00",true,true]]</v>
+        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",26751787,558.94000000,0.99900000,"2018-05-29T18:57:50.541-04:00",true,false],["ETHUSDT",26751788,558.95000000,0.76509000,"2018-05-29T18:57:50.901-04:00",true,true],["ETHUSDT",26751789,559.35000000,0.00002000,"2018-05-29T18:57:51.915-04:00",true,false],["ETHUSDT",26751790,559.10000000,0.08702000,"2018-05-29T18:57:53.035-04:00",true,true],["ETHUSDT",26751791,559.10000000,0.08702000,"2018-05-29T18:57:53.102-04:00",true,true],["ETHUSDT",26751792,559.10000000,0.14317000,"2018-05-29T18:57:53.543-04:00",true,true],["ETHUSDT",26751793,559.35000000,0.53627000,"2018-05-29T18:57:53.896-04:00",true,false],["ETHUSDT",26751794,559.35000000,0.19734000,"2018-05-29T18:57:54.736-04:00",true,true],["ETHUSDT",26751795,559.35000000,0.33893000,"2018-05-29T18:57:54.863-04:00",true,true],["ETHUSDT",26751796,559.12000000,0.33945000,"2018-05-29T18:57:54.886-04:00",true,true]]</v>
         <stp/>
         <stp>BINANCE_HISTORY</stp>
         <stp>ETHUSDT</stp>
@@ -4571,7 +4573,7 @@
         <tr r="Q5" s="1"/>
       </tp>
       <tp>
-        <v>17445546</v>
+        <v>17445830</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -4579,7 +4581,7 @@
         <tr r="H21" s="1"/>
       </tp>
       <tp>
-        <v>28850790</v>
+        <v>28851371</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4587,7 +4589,7 @@
         <tr r="N22" s="1"/>
       </tp>
       <tp>
-        <v>561.5</v>
+        <v>559</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4596,7 +4598,7 @@
         <tr r="E31" s="1"/>
       </tp>
       <tp>
-        <v>561.5</v>
+        <v>559</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4613,7 +4615,7 @@
         <tr r="L21" s="1"/>
       </tp>
       <tp>
-        <v>1.95</v>
+        <v>0.6</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4621,7 +4623,7 @@
         <tr r="J20" s="1"/>
       </tp>
       <tp>
-        <v>7444.37</v>
+        <v>7430.54</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4630,7 +4632,7 @@
         <tr r="E38" s="1"/>
       </tp>
       <tp>
-        <v>7444.37</v>
+        <v>7430.54</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4646,14 +4648,14 @@
         <stp>BUYER_IS_MAKER</stp>
         <tr r="K20" s="1"/>
       </tp>
-      <tp t="s">
-        <v>ERROR: Expected: origin, vendor, instrument, field, [depth]</v>
+      <tp>
+        <v>43249.790466539351</v>
         <stp/>
         <stp>CLOCK</stp>
         <tr r="N2" s="1"/>
       </tp>
       <tp>
-        <v>26750925</v>
+        <v>26751838</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4661,7 +4663,7 @@
         <tr r="N16" s="1"/>
       </tp>
       <tp>
-        <v>43249.784061446757</v>
+        <v>43249.790459675925</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4670,7 +4672,7 @@
         <tr r="O45" s="1"/>
       </tp>
       <tp>
-        <v>53392516</v>
+        <v>55227194</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4679,7 +4681,7 @@
         <tr r="K39" s="1"/>
       </tp>
       <tp>
-        <v>19117125</v>
+        <v>20951803</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4688,7 +4690,7 @@
         <tr r="K33" s="1"/>
       </tp>
       <tp>
-        <v>0.46034000000000003</v>
+        <v>13</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4697,7 +4699,7 @@
         <tr r="A24" s="1"/>
       </tp>
       <tp>
-        <v>4.0000000000000002E-4</v>
+        <v>1.32884</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4706,7 +4708,7 @@
         <tr r="A25" s="1"/>
       </tp>
       <tp>
-        <v>19</v>
+        <v>4.2999999999999997E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4715,7 +4717,7 @@
         <tr r="A20" s="1"/>
       </tp>
       <tp>
-        <v>4.2999999999999997E-2</v>
+        <v>14</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4724,7 +4726,7 @@
         <tr r="A21" s="1"/>
       </tp>
       <tp>
-        <v>1</v>
+        <v>8.1999999999999993</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4733,7 +4735,7 @@
         <tr r="A22" s="1"/>
       </tp>
       <tp>
-        <v>9.7972099999999998</v>
+        <v>0.153</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4742,7 +4744,7 @@
         <tr r="A23" s="1"/>
       </tp>
       <tp>
-        <v>0.53383000000000003</v>
+        <v>0.53596999999999995</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4751,7 +4753,7 @@
         <tr r="A16" s="1"/>
       </tp>
       <tp>
-        <v>3.6420000000000001E-2</v>
+        <v>5.824E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4760,7 +4762,7 @@
         <tr r="A17" s="1"/>
       </tp>
       <tp>
-        <v>0.22222</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4769,7 +4771,7 @@
         <tr r="A18" s="1"/>
       </tp>
       <tp>
-        <v>8.8596000000000004</v>
+        <v>134.99923000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -4778,7 +4780,7 @@
         <tr r="A19" s="1"/>
       </tp>
       <tp>
-        <v>10650.18819447</v>
+        <v>10614.50775662</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4786,7 +4788,7 @@
         <tr r="H4" s="2"/>
       </tp>
       <tp>
-        <v>141081.61087484</v>
+        <v>141356.15238218001</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4794,7 +4796,7 @@
         <tr r="H3" s="2"/>
       </tp>
       <tp>
-        <v>43249.784073402778</v>
+        <v>43249.790457685187</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4821,7 +4823,7 @@
         <tr r="H32" s="1"/>
       </tp>
       <tp>
-        <v>586788</v>
+        <v>587005</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4829,7 +4831,7 @@
         <tr r="H19" s="1"/>
       </tp>
       <tp>
-        <v>28850790</v>
+        <v>28851370</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4846,7 +4848,7 @@
         <tr r="L22" s="1"/>
       </tp>
       <tp>
-        <v>40732164</v>
+        <v>40734930</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4854,7 +4856,7 @@
         <tr r="H17" s="1"/>
       </tp>
       <tp>
-        <v>6717142</v>
+        <v>6717294</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4862,7 +4864,7 @@
         <tr r="H18" s="1"/>
       </tp>
       <tp>
-        <v>23754539</v>
+        <v>23755394</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4870,7 +4872,7 @@
         <tr r="H16" s="1"/>
       </tp>
       <tp>
-        <v>43249.784061620368</v>
+        <v>43249.790412245369</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4879,7 +4881,7 @@
         <tr r="O43" s="1"/>
       </tp>
       <tp>
-        <v>17899718</v>
+        <v>17900086</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4905,7 +4907,7 @@
         <tr r="H37" s="1"/>
       </tp>
       <tp>
-        <v>7622844</v>
+        <v>7623019</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4913,7 +4915,7 @@
         <tr r="N18" s="1"/>
       </tp>
       <tp>
-        <v>15246344</v>
+        <v>15246484</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4921,7 +4923,7 @@
         <tr r="M20" s="1"/>
       </tp>
       <tp>
-        <v>50690</v>
+        <v>50816</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4946,7 +4948,7 @@
         <tr r="B6" s="1"/>
       </tp>
       <tp>
-        <v>4.36E-2</v>
+        <v>3.8159999999999999E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4954,7 +4956,7 @@
         <tr r="O9" s="1"/>
       </tp>
       <tp>
-        <v>2.5799999999999998E-4</v>
+        <v>1.9599999999999999E-4</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -4962,7 +4964,7 @@
         <tr r="O10" s="1"/>
       </tp>
       <tp>
-        <v>19355.553370000001</v>
+        <v>20732.313959999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4971,7 +4973,7 @@
         <tr r="J37" s="1"/>
       </tp>
       <tp>
-        <v>7799.1461900000004</v>
+        <v>9175.9067799999993</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4980,7 +4982,7 @@
         <tr r="J31" s="1"/>
       </tp>
       <tp>
-        <v>49.02</v>
+        <v>44.08</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4988,7 +4990,7 @@
         <tr r="O6" s="1"/>
       </tp>
       <tp>
-        <v>8.7799999999999994</v>
+        <v>8.2200000000000006</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4996,7 +4998,7 @@
         <tr r="O8" s="1"/>
       </tp>
       <tp>
-        <v>366.78</v>
+        <v>323.64999999999998</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -5004,7 +5006,7 @@
         <tr r="O7" s="1"/>
       </tp>
       <tp>
-        <v>119.21</v>
+        <v>118.89</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -5012,7 +5014,7 @@
         <tr r="I8" s="1"/>
       </tp>
       <tp>
-        <v>43032</v>
+        <v>43612</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5029,7 +5031,7 @@
         <tr r="B7" s="1"/>
       </tp>
       <tp>
-        <v>119.2</v>
+        <v>118.75</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -5037,7 +5039,7 @@
         <tr r="G8" s="1"/>
       </tp>
       <tp>
-        <v>31197315.02</v>
+        <v>31224296.57</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -5045,7 +5047,7 @@
         <tr r="K9" s="1"/>
       </tp>
       <tp>
-        <v>114326</v>
+        <v>117373</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5054,7 +5056,7 @@
         <tr r="N44" s="1"/>
       </tp>
       <tp>
-        <v>2.5149999999999999E-2</v>
+        <v>2.426E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -5062,7 +5064,7 @@
         <tr r="N11" s="1"/>
       </tp>
       <tp>
-        <v>0.59408000000000005</v>
+        <v>0.59231</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -5087,7 +5089,7 @@
         <tr r="C9" s="1"/>
       </tp>
       <tp>
-        <v>43249.784073402778</v>
+        <v>43249.790457673611</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5096,7 +5098,7 @@
         <tr r="O38" s="1"/>
       </tp>
       <tp>
-        <v>43249.784073402778</v>
+        <v>43249.790457685187</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5105,7 +5107,7 @@
         <tr r="O32" s="1"/>
       </tp>
       <tp>
-        <v>43249.784061620368</v>
+        <v>43249.790412256945</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5114,7 +5116,7 @@
         <tr r="O37" s="1"/>
       </tp>
       <tp>
-        <v>43249.784061620368</v>
+        <v>43249.790412256945</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5123,7 +5125,7 @@
         <tr r="O31" s="1"/>
       </tp>
       <tp>
-        <v>111706</v>
+        <v>111732</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -5139,7 +5141,7 @@
         <tr r="B8" s="1"/>
       </tp>
       <tp>
-        <v>1365.257846</v>
+        <v>1733.676307</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5148,7 +5150,7 @@
         <tr r="J32" s="1"/>
       </tp>
       <tp>
-        <v>3973.9061109999998</v>
+        <v>4342.3245720000004</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5157,7 +5159,7 @@
         <tr r="J38" s="1"/>
       </tp>
       <tp>
-        <v>7440.01</v>
+        <v>7424.29</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -5173,7 +5175,7 @@
         <tr r="C10" s="1"/>
       </tp>
       <tp>
-        <v>104709154</v>
+        <v>111099351</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5182,7 +5184,7 @@
         <tr r="J39" s="1"/>
       </tp>
       <tp>
-        <v>40105150</v>
+        <v>46495347</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5191,7 +5193,7 @@
         <tr r="J33" s="1"/>
       </tp>
       <tp>
-        <v>561.5</v>
+        <v>559</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5200,7 +5202,7 @@
         <tr r="E43" s="1"/>
       </tp>
       <tp>
-        <v>7444.37</v>
+        <v>7430.54</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5209,7 +5211,7 @@
         <tr r="E44" s="1"/>
       </tp>
       <tp>
-        <v>7444.45</v>
+        <v>7430.5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -5217,7 +5219,7 @@
         <tr r="I7" s="1"/>
       </tp>
       <tp>
-        <v>63241</v>
+        <v>64157</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5226,7 +5228,7 @@
         <tr r="N43" s="1"/>
       </tp>
       <tp>
-        <v>561.95000000000005</v>
+        <v>559.73</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -5294,7 +5296,7 @@
         <tr r="M37" s="1"/>
       </tp>
       <tp>
-        <v>2.494E-2</v>
+        <v>2.138E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -5311,7 +5313,7 @@
         <tr r="D43" s="1"/>
       </tp>
       <tp>
-        <v>561.53</v>
+        <v>559.29</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -5328,7 +5330,7 @@
         <tr r="D44" s="1"/>
       </tp>
       <tp>
-        <v>93478.519199999995</v>
+        <v>94855.279790000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5337,7 +5339,7 @@
         <tr r="J43" s="1"/>
       </tp>
       <tp>
-        <v>17405.573903</v>
+        <v>17773.992364000002</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5400,7 +5402,7 @@
         <tr r="P31" s="1"/>
       </tp>
       <tp>
-        <v>0.59408000000000005</v>
+        <v>0.59240000000000004</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -5452,7 +5454,7 @@
         <tr r="C12" s="1"/>
       </tp>
       <tp>
-        <v>72199.220520000003</v>
+        <v>72170.911730000007</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -5460,7 +5462,7 @@
         <tr r="K8" s="1"/>
       </tp>
       <tp>
-        <v>0.59394000000000002</v>
+        <v>0.59109</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -5468,7 +5470,7 @@
         <tr r="G9" s="1"/>
       </tp>
       <tp>
-        <v>8.6100000000000006E-6</v>
+        <v>8.5699999999999993E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5504,7 +5506,7 @@
         <tr r="H33" s="1"/>
       </tp>
       <tp>
-        <v>7435.02</v>
+        <v>7401.29</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5513,7 +5515,7 @@
         <tr r="D38" s="1"/>
       </tp>
       <tp>
-        <v>7435.02</v>
+        <v>7401.29</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5522,7 +5524,7 @@
         <tr r="D32" s="1"/>
       </tp>
       <tp>
-        <v>1.9599999999999999E-6</v>
+        <v>1.8899999999999999E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -5530,7 +5532,7 @@
         <tr r="O11" s="1"/>
       </tp>
       <tp>
-        <v>7444.82</v>
+        <v>7430.5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -5538,7 +5540,7 @@
         <tr r="I17" s="1"/>
       </tp>
       <tp>
-        <v>119.2</v>
+        <v>118.9</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -5546,7 +5548,7 @@
         <tr r="I18" s="1"/>
       </tp>
       <tp>
-        <v>3.8179999999999999E-2</v>
+        <v>2.8819999999999998E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -5554,7 +5556,7 @@
         <tr r="N10" s="1"/>
       </tp>
       <tp>
-        <v>2.1E-7</v>
+        <v>1.8E-7</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -5562,7 +5564,7 @@
         <tr r="O12" s="1"/>
       </tp>
       <tp>
-        <v>558.89</v>
+        <v>557.83000000000004</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5571,7 +5573,7 @@
         <tr r="D31" s="1"/>
       </tp>
       <tp>
-        <v>558.89</v>
+        <v>557.83000000000004</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5580,7 +5582,7 @@
         <tr r="D37" s="1"/>
       </tp>
       <tp>
-        <v>190347.42384999999</v>
+        <v>190381.1189</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -5588,7 +5590,7 @@
         <tr r="K6" s="1"/>
       </tp>
       <tp>
-        <v>39591.781053999999</v>
+        <v>39667.606401999998</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -5612,7 +5614,7 @@
         <tr r="C11" s="1"/>
       </tp>
       <tp>
-        <v>8.6300000000000004E-6</v>
+        <v>8.5900000000000008E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5621,7 +5623,7 @@
         <tr r="E39" s="1"/>
       </tp>
       <tp>
-        <v>8.6300000000000004E-6</v>
+        <v>8.5900000000000008E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5630,7 +5632,7 @@
         <tr r="E33" s="1"/>
       </tp>
       <tp>
-        <v>4651521.2728654202</v>
+        <v>6140705.0098409401</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5639,7 +5641,7 @@
         <tr r="L32" s="1"/>
       </tp>
       <tp>
-        <v>15628598.844702311</v>
+        <v>17117782.581677832</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5648,7 +5650,7 @@
         <tr r="L38" s="1"/>
       </tp>
       <tp>
-        <v>1428531.5791461</v>
+        <v>1687695.3641526001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5657,7 +5659,7 @@
         <tr r="L31" s="1"/>
       </tp>
       <tp>
-        <v>4897275.1828148998</v>
+        <v>5156438.9678213997</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5666,7 +5668,7 @@
         <tr r="L37" s="1"/>
       </tp>
       <tp>
-        <v>27101</v>
+        <v>27114</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -5674,7 +5676,7 @@
         <tr r="M10" s="1"/>
       </tp>
       <tp>
-        <v>561.52</v>
+        <v>559</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -5708,7 +5710,7 @@
         <tr r="H11" s="1"/>
       </tp>
       <tp>
-        <v>110.62</v>
+        <v>110.72</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -5716,7 +5718,7 @@
         <tr r="D8" s="1"/>
       </tp>
       <tp>
-        <v>7084</v>
+        <v>7102.46</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -5724,7 +5726,7 @@
         <tr r="D7" s="1"/>
       </tp>
       <tp>
-        <v>46723.2091</v>
+        <v>47185.969250000002</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5733,7 +5735,7 @@
         <tr r="K43" s="1"/>
       </tp>
       <tp>
-        <v>43249.784087210646</v>
+        <v>43249.790465879632</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -5741,7 +5743,7 @@
         <tr r="O20" s="1"/>
       </tp>
       <tp>
-        <v>6.7580000000000001E-3</v>
+        <v>6.7939999999999997E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -5749,7 +5751,7 @@
         <tr r="E10" s="1"/>
       </tp>
       <tp>
-        <v>512.87</v>
+        <v>514.36</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -5757,7 +5759,7 @@
         <tr r="E6" s="1"/>
       </tp>
       <tp>
-        <v>7077.65</v>
+        <v>7106.83</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -5765,7 +5767,7 @@
         <tr r="E7" s="1"/>
       </tp>
       <tp>
-        <v>110.5</v>
+        <v>110.66</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -5773,7 +5775,7 @@
         <tr r="E8" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -5821,7 +5823,7 @@
         <tr r="F4" s="2"/>
       </tp>
       <tp>
-        <v>9354.3132559999995</v>
+        <v>9554.9698759999992</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5830,7 +5832,7 @@
         <tr r="K44" s="1"/>
       </tp>
       <tp>
-        <v>0.55042000000000002</v>
+        <v>0.55318999999999996</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -5856,7 +5858,7 @@
         <tr r="F38" s="1"/>
       </tp>
       <tp>
-        <v>512.87</v>
+        <v>514.36</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -5881,7 +5883,7 @@
         <tr r="H45" s="1"/>
       </tp>
       <tp>
-        <v>6.7600000000000004E-3</v>
+        <v>6.7860000000000004E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -5898,7 +5900,7 @@
         <tr r="D45" s="1"/>
       </tp>
       <tp>
-        <v>531640512</v>
+        <v>538030709</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5925,7 +5927,7 @@
         <tr r="M33" s="1"/>
       </tp>
       <tp>
-        <v>10197293.9071803</v>
+        <v>12931420.01809966</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5934,7 +5936,7 @@
         <tr r="I32" s="1"/>
       </tp>
       <tp>
-        <v>29752099.03286355</v>
+        <v>32486225.14378291</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5943,7 +5945,7 @@
         <tr r="I38" s="1"/>
       </tp>
       <tp>
-        <v>10968944.045899499</v>
+        <v>11739915.599721599</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5952,7 +5954,7 @@
         <tr r="I37" s="1"/>
       </tp>
       <tp>
-        <v>4395155.6982738003</v>
+        <v>5166127.2520958995</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5961,7 +5963,7 @@
         <tr r="I31" s="1"/>
       </tp>
       <tp>
-        <v>8.6300000000000004E-6</v>
+        <v>8.5900000000000008E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5970,7 +5972,7 @@
         <tr r="E45" s="1"/>
       </tp>
       <tp>
-        <v>561.85</v>
+        <v>558.5</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -5978,7 +5980,7 @@
         <tr r="D3" s="2"/>
       </tp>
       <tp>
-        <v>7439.41</v>
+        <v>7425.82</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -5986,7 +5988,7 @@
         <tr r="D4" s="2"/>
       </tp>
       <tp>
-        <v>7.0150000000000004E-3</v>
+        <v>6.9959999999999996E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -5994,7 +5996,7 @@
         <tr r="I20" s="1"/>
       </tp>
       <tp>
-        <v>43249.784061435188</v>
+        <v>43249.790459687501</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -6003,7 +6005,7 @@
         <tr r="O39" s="1"/>
       </tp>
       <tp>
-        <v>43249.784061446757</v>
+        <v>43249.790459687501</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -6012,7 +6014,7 @@
         <tr r="O33" s="1"/>
       </tp>
       <tp>
-        <v>18011419.980044801</v>
+        <v>18032885.995059501</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -6020,7 +6022,7 @@
         <tr r="L9" s="1"/>
       </tp>
       <tp>
-        <v>0.55003000000000002</v>
+        <v>0.55318999999999996</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -6064,7 +6066,7 @@
         <tr r="P39" s="1"/>
       </tp>
       <tp>
-        <v>7.7960000000000006E-5</v>
+        <v>7.7929999999999994E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -6072,7 +6074,7 @@
         <tr r="E11" s="1"/>
       </tp>
       <tp>
-        <v>43249.784061412036</v>
+        <v>43249.790460972225</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -6080,7 +6082,7 @@
         <tr r="O22" s="1"/>
       </tp>
       <tp>
-        <v>103499984.5847811</v>
+        <v>103581705.32952189</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -6088,7 +6090,7 @@
         <tr r="L6" s="1"/>
       </tp>
       <tp>
-        <v>165.94695024999999</v>
+        <v>181.71567625</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -6097,7 +6099,7 @@
         <tr r="L33" s="1"/>
       </tp>
       <tp>
-        <v>460.91789722999999</v>
+        <v>476.68662323000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -6106,7 +6108,7 @@
         <tr r="L39" s="1"/>
       </tp>
       <tp>
-        <v>8.6300000000000004E-6</v>
+        <v>8.6000000000000007E-6</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -6114,7 +6116,7 @@
         <tr r="I22" s="1"/>
       </tp>
       <tp>
-        <v>561.95000000000005</v>
+        <v>559.73</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6123,7 +6125,7 @@
         <tr r="D16" s="1"/>
       </tp>
       <tp>
-        <v>561.96</v>
+        <v>559.99</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6132,7 +6134,7 @@
         <tr r="D17" s="1"/>
       </tp>
       <tp>
-        <v>561.99</v>
+        <v>560</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6141,7 +6143,7 @@
         <tr r="D18" s="1"/>
       </tp>
       <tp>
-        <v>562</v>
+        <v>560.04999999999995</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6150,7 +6152,7 @@
         <tr r="D19" s="1"/>
       </tp>
       <tp>
-        <v>562.33000000000004</v>
+        <v>560.07000000000005</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6159,7 +6161,7 @@
         <tr r="D20" s="1"/>
       </tp>
       <tp>
-        <v>562.52</v>
+        <v>560.30999999999995</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6168,7 +6170,7 @@
         <tr r="D21" s="1"/>
       </tp>
       <tp>
-        <v>562.53</v>
+        <v>560.4</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6177,7 +6179,7 @@
         <tr r="D22" s="1"/>
       </tp>
       <tp>
-        <v>562.57000000000005</v>
+        <v>560.52</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6186,7 +6188,7 @@
         <tr r="D23" s="1"/>
       </tp>
       <tp>
-        <v>562.79999999999995</v>
+        <v>560.53</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6195,7 +6197,7 @@
         <tr r="D24" s="1"/>
       </tp>
       <tp>
-        <v>563</v>
+        <v>560.72</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6204,7 +6206,7 @@
         <tr r="D25" s="1"/>
       </tp>
       <tp>
-        <v>7.9889999999999996E-5</v>
+        <v>7.9800000000000002E-5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -6221,7 +6223,7 @@
         <tr r="B43" s="1"/>
       </tp>
       <tp>
-        <v>8.3599999999999996E-6</v>
+        <v>8.3999999999999992E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -6238,7 +6240,7 @@
         <tr r="C44" s="1"/>
       </tp>
       <tp>
-        <v>560.94000000000005</v>
+        <v>558.05999999999995</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6247,7 +6249,7 @@
         <tr r="B25" s="1"/>
       </tp>
       <tp>
-        <v>561</v>
+        <v>558.25</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6256,7 +6258,7 @@
         <tr r="B24" s="1"/>
       </tp>
       <tp>
-        <v>561.02</v>
+        <v>558.28</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6265,7 +6267,7 @@
         <tr r="B23" s="1"/>
       </tp>
       <tp>
-        <v>561.05999999999995</v>
+        <v>558.44000000000005</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6274,7 +6276,7 @@
         <tr r="B22" s="1"/>
       </tp>
       <tp>
-        <v>561.12</v>
+        <v>558.69000000000005</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6283,7 +6285,7 @@
         <tr r="B21" s="1"/>
       </tp>
       <tp>
-        <v>561.24</v>
+        <v>558.88</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6292,7 +6294,7 @@
         <tr r="B20" s="1"/>
       </tp>
       <tp>
-        <v>561.25</v>
+        <v>559</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6301,7 +6303,7 @@
         <tr r="B19" s="1"/>
       </tp>
       <tp>
-        <v>561.29999999999995</v>
+        <v>559.1</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6310,7 +6312,7 @@
         <tr r="B18" s="1"/>
       </tp>
       <tp>
-        <v>561.5</v>
+        <v>559.19000000000005</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6319,7 +6321,7 @@
         <tr r="B17" s="1"/>
       </tp>
       <tp>
-        <v>561.53</v>
+        <v>559.29</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>ethusdt</stp>
@@ -6328,7 +6330,7 @@
         <tr r="B16" s="1"/>
       </tp>
       <tp>
-        <v>288938925.08285034</v>
+        <v>289597584.66202039</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -6336,7 +6338,7 @@
         <tr r="L7" s="1"/>
       </tp>
       <tp>
-        <v>8483586.2747393996</v>
+        <v>8484058.0402623005</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -6344,7 +6346,7 @@
         <tr r="L8" s="1"/>
       </tp>
       <tp>
-        <v>8.3699999999999995E-6</v>
+        <v>8.3999999999999992E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -6352,7 +6354,7 @@
         <tr r="D12" s="1"/>
       </tp>
       <tp>
-        <v>7.7899999999999996E-5</v>
+        <v>7.7799999999999994E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -6360,7 +6362,7 @@
         <tr r="D11" s="1"/>
       </tp>
       <tp>
-        <v>512.05999999999995</v>
+        <v>513.49</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -6368,7 +6370,7 @@
         <tr r="E3" s="2"/>
       </tp>
       <tp>
-        <v>7100.01</v>
+        <v>7100</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -6376,7 +6378,7 @@
         <tr r="E4" s="2"/>
       </tp>
       <tp>
-        <v>43249.783958333333</v>
+        <v>43249.790468900464</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -6425,7 +6427,7 @@
         <tr r="B44" s="1"/>
       </tp>
       <tp>
-        <v>9.9999999999999995E-7</v>
+        <v>9.0000000000000002E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -7060,7 +7062,7 @@
   <dimension ref="A1:U114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7114,9 +7116,9 @@
       <c r="M2" t="s">
         <v>67</v>
       </c>
-      <c r="N2" t="str">
+      <c r="N2" s="38">
         <f>RTD(progId,,"CLOCK")</f>
-        <v>ERROR: Expected: origin, vendor, instrument, field, [depth]</v>
+        <v>43249.790466539351</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -7196,7 +7198,7 @@
       </c>
       <c r="Q5" s="37" t="str">
         <f>RTD(progId,,BINANCE_HISTORY,S4,"a,b,c",10)</f>
-        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",26750741,563.00000000,5.58010000,"2018-05-29T18:46:58.024-04:00",true,true],["ETHUSDT",26750742,563.00000000,0.14228000,"2018-05-29T18:47:00.152-04:00",true,true],["ETHUSDT",26750743,563.00000000,0.13233000,"2018-05-29T18:47:00.353-04:00",true,true],["ETHUSDT",26750744,563.00000000,0.29970000,"2018-05-29T18:47:00.649-04:00",true,true],["ETHUSDT",26750745,563.01000000,0.50000000,"2018-05-29T18:47:05.632-04:00",true,false],["ETHUSDT",26750746,563.00000000,0.45987000,"2018-05-29T18:47:07.351-04:00",true,true],["ETHUSDT",26750747,563.01000000,1.13900000,"2018-05-29T18:47:07.38-04:00",true,false],["ETHUSDT",26750748,563.00000000,4.10379000,"2018-05-29T18:47:09.759-04:00",true,true],["ETHUSDT",26750749,563.01000000,0.00017000,"2018-05-29T18:47:10.643-04:00",true,false],["ETHUSDT",26750750,563.00000000,0.44356000,"2018-05-29T18:47:11.411-04:00",true,true]]</v>
+        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",26751787,558.94000000,0.99900000,"2018-05-29T18:57:50.541-04:00",true,false],["ETHUSDT",26751788,558.95000000,0.76509000,"2018-05-29T18:57:50.901-04:00",true,true],["ETHUSDT",26751789,559.35000000,0.00002000,"2018-05-29T18:57:51.915-04:00",true,false],["ETHUSDT",26751790,559.10000000,0.08702000,"2018-05-29T18:57:53.035-04:00",true,true],["ETHUSDT",26751791,559.10000000,0.08702000,"2018-05-29T18:57:53.102-04:00",true,true],["ETHUSDT",26751792,559.10000000,0.14317000,"2018-05-29T18:57:53.543-04:00",true,true],["ETHUSDT",26751793,559.35000000,0.53627000,"2018-05-29T18:57:53.896-04:00",true,false],["ETHUSDT",26751794,559.35000000,0.19734000,"2018-05-29T18:57:54.736-04:00",true,true],["ETHUSDT",26751795,559.35000000,0.33893000,"2018-05-29T18:57:54.863-04:00",true,true],["ETHUSDT",26751796,559.12000000,0.33945000,"2018-05-29T18:57:54.886-04:00",true,true]]</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -7213,51 +7215,51 @@
       </c>
       <c r="D6" s="2">
         <f>RTD(progId,,BINANCE_24H,$A6,D$5)</f>
-        <v>512.87</v>
+        <v>514.36</v>
       </c>
       <c r="E6" s="2">
         <f>RTD(progId,,BINANCE_24H,$A6,E$5)</f>
-        <v>512.87</v>
+        <v>514.36</v>
       </c>
       <c r="F6" s="2">
         <f>RTD(progId,,BINANCE,$A6,F$5)</f>
-        <v>0.53383000000000003</v>
+        <v>0.53596999999999995</v>
       </c>
       <c r="G6" s="2">
         <f>RTD(progId,,BINANCE,$A6,G$5)</f>
-        <v>561.53</v>
+        <v>559.29</v>
       </c>
       <c r="H6" s="2">
         <f>RTD(progId,,BINANCE,$A6,H$5)</f>
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
       <c r="I6" s="2">
         <f>RTD(progId,,BINANCE,$A6,I$5)</f>
-        <v>561.95000000000005</v>
+        <v>559.73</v>
       </c>
       <c r="J6" s="2">
         <f>RTD(progId,,BINANCE,$A6,J$5)</f>
-        <v>0.53381999999999996</v>
+        <v>0.12995999999999999</v>
       </c>
       <c r="K6" s="9">
         <f>RTD(progId,,BINANCE,$A6,K$5)</f>
-        <v>190347.42384999999</v>
+        <v>190381.1189</v>
       </c>
       <c r="L6" s="2">
         <f>RTD(progId,,BINANCE,$A6,L$5)</f>
-        <v>103499984.5847811</v>
+        <v>103581705.32952189</v>
       </c>
       <c r="M6" s="9">
         <f>RTD(progId,,BINANCE,$A6,M$5)</f>
-        <v>129082</v>
+        <v>129360</v>
       </c>
       <c r="N6" s="10">
         <f>RTD(progId,,BINANCE,$A6,N$5)</f>
-        <v>9.5649999999999999E-2</v>
+        <v>8.5610000000000006E-2</v>
       </c>
       <c r="O6" s="2">
         <f>RTD(progId,,BINANCE,$A6,O$5)</f>
-        <v>49.02</v>
+        <v>44.08</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -7274,51 +7276,51 @@
       </c>
       <c r="D7" s="2">
         <f>RTD(progId,,BINANCE_24H,$A7,D$5)</f>
-        <v>7084</v>
+        <v>7102.46</v>
       </c>
       <c r="E7" s="2">
         <f>RTD(progId,,BINANCE_24H,$A7,E$5)</f>
-        <v>7077.65</v>
+        <v>7106.83</v>
       </c>
       <c r="F7" s="2">
         <f>RTD(progId,,BINANCE,$A7,F$5)</f>
-        <v>8.2888000000000003E-2</v>
+        <v>0.33504499999999998</v>
       </c>
       <c r="G7" s="2">
         <f>RTD(progId,,BINANCE,$A7,G$5)</f>
-        <v>7440.01</v>
+        <v>7424.29</v>
       </c>
       <c r="H7" s="2">
         <f>RTD(progId,,BINANCE,$A7,H$5)</f>
-        <v>4.4400000000000004</v>
+        <v>6.21</v>
       </c>
       <c r="I7" s="2">
         <f>RTD(progId,,BINANCE,$A7,I$5)</f>
-        <v>7444.45</v>
+        <v>7430.5</v>
       </c>
       <c r="J7" s="2">
         <f>RTD(progId,,BINANCE,$A7,J$5)</f>
-        <v>0.14785100000000001</v>
+        <v>0.29883199999999999</v>
       </c>
       <c r="K7" s="9">
         <f>RTD(progId,,BINANCE,$A7,K$5)</f>
-        <v>39591.781053999999</v>
+        <v>39667.606401999998</v>
       </c>
       <c r="L7" s="2">
         <f>RTD(progId,,BINANCE,$A7,L$5)</f>
-        <v>288938925.08285034</v>
+        <v>289597584.66202039</v>
       </c>
       <c r="M7" s="9">
         <f>RTD(progId,,BINANCE,$A7,M$5)</f>
-        <v>235000</v>
+        <v>236915</v>
       </c>
       <c r="N7" s="10">
         <f>RTD(progId,,BINANCE,$A7,N$5)</f>
-        <v>5.1819999999999998E-2</v>
+        <v>4.5539999999999997E-2</v>
       </c>
       <c r="O7" s="2">
         <f>RTD(progId,,BINANCE,$A7,O$5)</f>
-        <v>366.78</v>
+        <v>323.64999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -7335,51 +7337,51 @@
       </c>
       <c r="D8" s="2">
         <f>RTD(progId,,BINANCE_24H,$A8,D$5)</f>
-        <v>110.62</v>
+        <v>110.72</v>
       </c>
       <c r="E8" s="2">
         <f>RTD(progId,,BINANCE_24H,$A8,E$5)</f>
-        <v>110.5</v>
+        <v>110.66</v>
       </c>
       <c r="F8" s="2">
         <f>RTD(progId,,BINANCE,$A8,F$5)</f>
-        <v>1.0000000000000001E-5</v>
+        <v>0.77</v>
       </c>
       <c r="G8" s="2">
         <f>RTD(progId,,BINANCE,$A8,G$5)</f>
-        <v>119.2</v>
+        <v>118.75</v>
       </c>
       <c r="H8" s="2">
         <f>RTD(progId,,BINANCE,$A8,H$5)</f>
-        <v>0.01</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I8" s="2">
         <f>RTD(progId,,BINANCE,$A8,I$5)</f>
-        <v>119.21</v>
+        <v>118.89</v>
       </c>
       <c r="J8" s="2">
         <f>RTD(progId,,BINANCE,$A8,J$5)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K8" s="9">
         <f>RTD(progId,,BINANCE,$A8,K$5)</f>
-        <v>72199.220520000003</v>
+        <v>72170.911730000007</v>
       </c>
       <c r="L8" s="2">
         <f>RTD(progId,,BINANCE,$A8,L$5)</f>
-        <v>8483586.2747393996</v>
+        <v>8484058.0402623005</v>
       </c>
       <c r="M8" s="9">
         <f>RTD(progId,,BINANCE,$A8,M$5)</f>
-        <v>19351</v>
+        <v>19448</v>
       </c>
       <c r="N8" s="10">
         <f>RTD(progId,,BINANCE,$A8,N$5)</f>
-        <v>7.9509999999999997E-2</v>
+        <v>7.4270000000000003E-2</v>
       </c>
       <c r="O8" s="2">
         <f>RTD(progId,,BINANCE,$A8,O$5)</f>
-        <v>8.7799999999999994</v>
+        <v>8.2200000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -7396,51 +7398,51 @@
       </c>
       <c r="D9" s="2">
         <f>RTD(progId,,BINANCE_24H,$A9,D$5)</f>
-        <v>0.55003000000000002</v>
+        <v>0.55318999999999996</v>
       </c>
       <c r="E9" s="2">
         <f>RTD(progId,,BINANCE_24H,$A9,E$5)</f>
-        <v>0.55042000000000002</v>
+        <v>0.55318999999999996</v>
       </c>
       <c r="F9" s="9">
         <f>RTD(progId,,BINANCE,$A9,F$5)</f>
-        <v>159.16999999999999</v>
+        <v>1784.99</v>
       </c>
       <c r="G9" s="2">
         <f>RTD(progId,,BINANCE,$A9,G$5)</f>
-        <v>0.59394000000000002</v>
+        <v>0.59109</v>
       </c>
       <c r="H9" s="2">
         <f>RTD(progId,,BINANCE,$A9,H$5)</f>
-        <v>1.3999999999999999E-4</v>
+        <v>1.31E-3</v>
       </c>
       <c r="I9" s="2">
         <f>RTD(progId,,BINANCE,$A9,I$5)</f>
-        <v>0.59408000000000005</v>
+        <v>0.59240000000000004</v>
       </c>
       <c r="J9" s="2">
         <f>RTD(progId,,BINANCE,$A9,J$5)</f>
-        <v>210.15</v>
+        <v>500</v>
       </c>
       <c r="K9" s="9">
         <f>RTD(progId,,BINANCE,$A9,K$5)</f>
-        <v>31197315.02</v>
+        <v>31224296.57</v>
       </c>
       <c r="L9" s="2">
         <f>RTD(progId,,BINANCE,$A9,L$5)</f>
-        <v>18011419.980044801</v>
+        <v>18032885.995059501</v>
       </c>
       <c r="M9" s="9">
         <f>RTD(progId,,BINANCE,$A9,M$5)</f>
-        <v>27338</v>
+        <v>27442</v>
       </c>
       <c r="N9" s="10">
         <f>RTD(progId,,BINANCE,$A9,N$5)</f>
-        <v>7.9200000000000007E-2</v>
+        <v>6.8860000000000005E-2</v>
       </c>
       <c r="O9" s="2">
         <f>RTD(progId,,BINANCE,$A9,O$5)</f>
-        <v>4.36E-2</v>
+        <v>3.8159999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -7457,51 +7459,51 @@
       </c>
       <c r="D10" s="2">
         <f>RTD(progId,,BINANCE_24H,$A10,D$5)</f>
-        <v>6.7600000000000004E-3</v>
+        <v>6.7860000000000004E-3</v>
       </c>
       <c r="E10" s="2">
         <f>RTD(progId,,BINANCE_24H,$A10,E$5)</f>
-        <v>6.7580000000000001E-3</v>
+        <v>6.7939999999999997E-3</v>
       </c>
       <c r="F10" s="9">
         <f>RTD(progId,,BINANCE,$A10,F$5)</f>
-        <v>3.32</v>
+        <v>0.6</v>
       </c>
       <c r="G10" s="2">
         <f>RTD(progId,,BINANCE,$A10,G$5)</f>
-        <v>7.0150000000000004E-3</v>
+        <v>6.9959999999999996E-3</v>
       </c>
       <c r="H10" s="2">
         <f>RTD(progId,,BINANCE,$A10,H$5)</f>
-        <v>9.9999999999999995E-7</v>
+        <v>9.0000000000000002E-6</v>
       </c>
       <c r="I10" s="2">
         <f>RTD(progId,,BINANCE,$A10,I$5)</f>
-        <v>7.0159999999999997E-3</v>
+        <v>7.0049999999999999E-3</v>
       </c>
       <c r="J10" s="2">
         <f>RTD(progId,,BINANCE,$A10,J$5)</f>
-        <v>3.44</v>
+        <v>1.38</v>
       </c>
       <c r="K10" s="9">
         <f>RTD(progId,,BINANCE,$A10,K$5)</f>
-        <v>157839.87</v>
+        <v>157292.04999999999</v>
       </c>
       <c r="L10" s="2">
         <f>RTD(progId,,BINANCE,$A10,L$5)</f>
-        <v>1097.7973295500001</v>
+        <v>1094.1768949100001</v>
       </c>
       <c r="M10" s="9">
         <f>RTD(progId,,BINANCE,$A10,M$5)</f>
-        <v>27101</v>
+        <v>27114</v>
       </c>
       <c r="N10" s="10">
         <f>RTD(progId,,BINANCE,$A10,N$5)</f>
-        <v>3.8179999999999999E-2</v>
+        <v>2.8819999999999998E-2</v>
       </c>
       <c r="O10" s="2">
         <f>RTD(progId,,BINANCE,$A10,O$5)</f>
-        <v>2.5799999999999998E-4</v>
+        <v>1.9599999999999999E-4</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -7523,19 +7525,19 @@
       </c>
       <c r="D11" s="2">
         <f>RTD(progId,,BINANCE_24H,$A11,D$5)</f>
-        <v>7.7899999999999996E-5</v>
+        <v>7.7799999999999994E-5</v>
       </c>
       <c r="E11" s="2">
         <f>RTD(progId,,BINANCE_24H,$A11,E$5)</f>
-        <v>7.7960000000000006E-5</v>
+        <v>7.7929999999999994E-5</v>
       </c>
       <c r="F11" s="9">
         <f>RTD(progId,,BINANCE,$A11,F$5)</f>
-        <v>462</v>
+        <v>6620</v>
       </c>
       <c r="G11" s="2">
         <f>RTD(progId,,BINANCE,$A11,G$5)</f>
-        <v>7.9880000000000001E-5</v>
+        <v>7.9770000000000004E-5</v>
       </c>
       <c r="H11" s="2">
         <f>RTD(progId,,BINANCE,$A11,H$5)</f>
@@ -7543,31 +7545,31 @@
       </c>
       <c r="I11" s="2">
         <f>RTD(progId,,BINANCE,$A11,I$5)</f>
-        <v>7.9900000000000004E-5</v>
+        <v>7.9789999999999993E-5</v>
       </c>
       <c r="J11" s="2">
         <f>RTD(progId,,BINANCE,$A11,J$5)</f>
-        <v>1088</v>
+        <v>105</v>
       </c>
       <c r="K11" s="9">
         <f>RTD(progId,,BINANCE,$A11,K$5)</f>
-        <v>33785487</v>
+        <v>33859109</v>
       </c>
       <c r="L11" s="2">
         <f>RTD(progId,,BINANCE,$A11,L$5)</f>
-        <v>2674.6815673699998</v>
+        <v>2680.8285568000001</v>
       </c>
       <c r="M11" s="9">
         <f>RTD(progId,,BINANCE,$A11,M$5)</f>
-        <v>50690</v>
+        <v>50816</v>
       </c>
       <c r="N11" s="10">
         <f>RTD(progId,,BINANCE,$A11,N$5)</f>
-        <v>2.5149999999999999E-2</v>
+        <v>2.426E-2</v>
       </c>
       <c r="O11" s="2">
         <f>RTD(progId,,BINANCE,$A11,O$5)</f>
-        <v>1.9599999999999999E-6</v>
+        <v>1.8899999999999999E-6</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7584,19 +7586,19 @@
       </c>
       <c r="D12" s="2">
         <f>RTD(progId,,BINANCE_24H,$A12,D$5)</f>
-        <v>8.3699999999999995E-6</v>
+        <v>8.3999999999999992E-6</v>
       </c>
       <c r="E12" s="2">
         <f>RTD(progId,,BINANCE_24H,$A12,E$5)</f>
-        <v>8.3599999999999996E-6</v>
+        <v>8.3999999999999992E-6</v>
       </c>
       <c r="F12" s="9">
         <f>RTD(progId,,BINANCE,$A12,F$5)</f>
-        <v>97197</v>
+        <v>181526</v>
       </c>
       <c r="G12" s="2">
         <f>RTD(progId,,BINANCE,$A12,G$5)</f>
-        <v>8.6300000000000004E-6</v>
+        <v>8.5900000000000008E-6</v>
       </c>
       <c r="H12" s="2">
         <f>RTD(progId,,BINANCE,$A12,H$5)</f>
@@ -7604,31 +7606,31 @@
       </c>
       <c r="I12" s="2">
         <f>RTD(progId,,BINANCE,$A12,I$5)</f>
-        <v>8.6400000000000003E-6</v>
+        <v>8.6000000000000007E-6</v>
       </c>
       <c r="J12" s="2">
         <f>RTD(progId,,BINANCE,$A12,J$5)</f>
-        <v>124344</v>
+        <v>775560</v>
       </c>
       <c r="K12" s="9">
         <f>RTD(progId,,BINANCE,$A12,K$5)</f>
-        <v>1626347776</v>
+        <v>1618758548</v>
       </c>
       <c r="L12" s="2">
         <f>RTD(progId,,BINANCE,$A12,L$5)</f>
-        <v>13630.97249443</v>
+        <v>13568.34826689</v>
       </c>
       <c r="M12" s="9">
         <f>RTD(progId,,BINANCE,$A12,M$5)</f>
-        <v>111706</v>
+        <v>111732</v>
       </c>
       <c r="N12" s="10">
         <f>RTD(progId,,BINANCE,$A12,N$5)</f>
-        <v>2.494E-2</v>
+        <v>2.138E-2</v>
       </c>
       <c r="O12" s="2">
         <f>RTD(progId,,BINANCE,$A12,O$5)</f>
-        <v>2.1E-7</v>
+        <v>1.8E-7</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7715,22 +7717,22 @@
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C16)</f>
-        <v>0.53383000000000003</v>
+        <v>0.53596999999999995</v>
       </c>
       <c r="B16" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C16)</f>
-        <v>561.53</v>
+        <v>559.29</v>
       </c>
       <c r="C16" s="8">
         <v>0</v>
       </c>
       <c r="D16" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C16)</f>
-        <v>561.95000000000005</v>
+        <v>559.73</v>
       </c>
       <c r="E16" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C16)</f>
-        <v>0.53381999999999996</v>
+        <v>0.12995999999999999</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
@@ -7738,15 +7740,15 @@
       </c>
       <c r="H16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,H$15)</f>
-        <v>23754539</v>
+        <v>23755394</v>
       </c>
       <c r="I16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,I$15)</f>
-        <v>561.52</v>
+        <v>559</v>
       </c>
       <c r="J16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,J$15)</f>
-        <v>1.2909200000000001</v>
+        <v>26.621500000000001</v>
       </c>
       <c r="K16" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G16,K$15)</f>
@@ -7758,15 +7760,15 @@
       </c>
       <c r="M16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,M$15)</f>
-        <v>26750925</v>
+        <v>26751838</v>
       </c>
       <c r="N16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,N$15)</f>
-        <v>26750925</v>
+        <v>26751838</v>
       </c>
       <c r="O16" s="30">
         <f>RTD(progId,,BINACE_TRADE,$G16,O$15)</f>
-        <v>43249.784074039351</v>
+        <v>43249.790412187504</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -7777,11 +7779,11 @@
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C17)</f>
-        <v>3.6420000000000001E-2</v>
+        <v>5.824E-2</v>
       </c>
       <c r="B17" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C17)</f>
-        <v>561.5</v>
+        <v>559.19000000000005</v>
       </c>
       <c r="C17" s="8">
         <f>C16+1</f>
@@ -7789,11 +7791,11 @@
       </c>
       <c r="D17" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C17)</f>
-        <v>561.96</v>
+        <v>559.99</v>
       </c>
       <c r="E17" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C17)</f>
-        <v>1.8919999999999999</v>
+        <v>0.75</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -7801,15 +7803,15 @@
       </c>
       <c r="H17" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G17,H$15)</f>
-        <v>40732164</v>
+        <v>40734930</v>
       </c>
       <c r="I17" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G17,I$15)</f>
-        <v>7444.82</v>
+        <v>7430.5</v>
       </c>
       <c r="J17" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G17,J$15)</f>
-        <v>7.6188000000000006E-2</v>
+        <v>6.8230000000000001E-3</v>
       </c>
       <c r="K17" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G17,K$15)</f>
@@ -7821,15 +7823,15 @@
       </c>
       <c r="M17" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G17,M$15)</f>
-        <v>46725857</v>
+        <v>46728899</v>
       </c>
       <c r="N17" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G17,N$15)</f>
-        <v>46725857</v>
+        <v>46728899</v>
       </c>
       <c r="O17" s="30">
         <f>RTD(progId,,BINACE_TRADE,$G17,O$15)</f>
-        <v>43249.784088125001</v>
+        <v>43249.790465729166</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -7840,11 +7842,11 @@
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C18)</f>
-        <v>0.22222</v>
+        <v>1</v>
       </c>
       <c r="B18" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C18)</f>
-        <v>561.29999999999995</v>
+        <v>559.1</v>
       </c>
       <c r="C18" s="8">
         <f t="shared" ref="C18:C25" si="0">C17+1</f>
@@ -7852,11 +7854,11 @@
       </c>
       <c r="D18" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C18)</f>
-        <v>561.99</v>
+        <v>560</v>
       </c>
       <c r="E18" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C18)</f>
-        <v>0.38628000000000001</v>
+        <v>6.00251</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
@@ -7864,19 +7866,19 @@
       </c>
       <c r="H18" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G18,H$15)</f>
-        <v>6717142</v>
+        <v>6717294</v>
       </c>
       <c r="I18" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G18,I$15)</f>
-        <v>119.2</v>
+        <v>118.9</v>
       </c>
       <c r="J18" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G18,J$15)</f>
-        <v>6.6955400000000003</v>
+        <v>1E-3</v>
       </c>
       <c r="K18" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G18,K$15)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G18,L$15)</f>
@@ -7884,15 +7886,15 @@
       </c>
       <c r="M18" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G18,M$15)</f>
-        <v>7622844</v>
+        <v>7623019</v>
       </c>
       <c r="N18" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G18,N$15)</f>
-        <v>7622844</v>
+        <v>7623019</v>
       </c>
       <c r="O18" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G18,O$15)</f>
-        <v>43249.783948402779</v>
+        <v>43249.790385069442</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -7903,11 +7905,11 @@
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C19)</f>
-        <v>8.8596000000000004</v>
+        <v>134.99923000000001</v>
       </c>
       <c r="B19" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C19)</f>
-        <v>561.25</v>
+        <v>559</v>
       </c>
       <c r="C19" s="8">
         <f t="shared" si="0"/>
@@ -7915,11 +7917,11 @@
       </c>
       <c r="D19" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C19)</f>
-        <v>562</v>
+        <v>560.04999999999995</v>
       </c>
       <c r="E19" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C19)</f>
-        <v>2.7046800000000002</v>
+        <v>0.27856999999999998</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
@@ -7927,15 +7929,15 @@
       </c>
       <c r="H19" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G19,H$15)</f>
-        <v>586788</v>
+        <v>587005</v>
       </c>
       <c r="I19" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G19,I$15)</f>
-        <v>0.59408000000000005</v>
+        <v>0.59231</v>
       </c>
       <c r="J19" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G19,J$15)</f>
-        <v>2.98</v>
+        <v>250</v>
       </c>
       <c r="K19" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G19,K$15)</f>
@@ -7947,25 +7949,25 @@
       </c>
       <c r="M19" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G19,M$15)</f>
-        <v>644938</v>
+        <v>645170</v>
       </c>
       <c r="N19" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G19,N$15)</f>
-        <v>644938</v>
+        <v>645170</v>
       </c>
       <c r="O19" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G19,O$15)</f>
-        <v>43249.78407371528</v>
+        <v>43249.790371134259</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C20)</f>
-        <v>19</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="B20" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C20)</f>
-        <v>561.24</v>
+        <v>558.88</v>
       </c>
       <c r="C20" s="8">
         <f t="shared" si="0"/>
@@ -7973,7 +7975,7 @@
       </c>
       <c r="D20" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C20)</f>
-        <v>562.33000000000004</v>
+        <v>560.07000000000005</v>
       </c>
       <c r="E20" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C20)</f>
@@ -7985,15 +7987,15 @@
       </c>
       <c r="H20" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G20,H$15)</f>
-        <v>13498381</v>
+        <v>13498492</v>
       </c>
       <c r="I20" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G20,I$15)</f>
-        <v>7.0150000000000004E-3</v>
+        <v>6.9959999999999996E-3</v>
       </c>
       <c r="J20" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G20,J$15)</f>
-        <v>1.95</v>
+        <v>0.6</v>
       </c>
       <c r="K20" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G20,K$15)</f>
@@ -8005,25 +8007,25 @@
       </c>
       <c r="M20" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G20,M$15)</f>
-        <v>15246344</v>
+        <v>15246484</v>
       </c>
       <c r="N20" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G20,N$15)</f>
-        <v>15246344</v>
+        <v>15246484</v>
       </c>
       <c r="O20" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G20,O$15)</f>
-        <v>43249.784087210646</v>
+        <v>43249.790465879632</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C21)</f>
-        <v>4.2999999999999997E-2</v>
+        <v>14</v>
       </c>
       <c r="B21" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C21)</f>
-        <v>561.12</v>
+        <v>558.69000000000005</v>
       </c>
       <c r="C21" s="8">
         <f t="shared" si="0"/>
@@ -8031,11 +8033,11 @@
       </c>
       <c r="D21" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C21)</f>
-        <v>562.52</v>
+        <v>560.30999999999995</v>
       </c>
       <c r="E21" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C21)</f>
-        <v>0.24099999999999999</v>
+        <v>2.9530699999999999</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
@@ -8043,19 +8045,19 @@
       </c>
       <c r="H21" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G21,H$15)</f>
-        <v>17445546</v>
+        <v>17445830</v>
       </c>
       <c r="I21" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G21,I$15)</f>
-        <v>7.9889999999999996E-5</v>
+        <v>7.9800000000000002E-5</v>
       </c>
       <c r="J21" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G21,J$15)</f>
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="K21" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G21,K$15)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G21,L$15)</f>
@@ -8063,25 +8065,25 @@
       </c>
       <c r="M21" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G21,M$15)</f>
-        <v>21103240</v>
+        <v>21103608</v>
       </c>
       <c r="N21" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G21,N$15)</f>
-        <v>21103240</v>
+        <v>21103608</v>
       </c>
       <c r="O21" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G21,O$15)</f>
-        <v>43249.783958333333</v>
+        <v>43249.790468900464</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C22)</f>
-        <v>1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="B22" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C22)</f>
-        <v>561.05999999999995</v>
+        <v>558.44000000000005</v>
       </c>
       <c r="C22" s="8">
         <f t="shared" si="0"/>
@@ -8089,11 +8091,11 @@
       </c>
       <c r="D22" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C22)</f>
-        <v>562.53</v>
+        <v>560.4</v>
       </c>
       <c r="E22" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C22)</f>
-        <v>3.3609200000000001</v>
+        <v>5.0000400000000003</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
@@ -8101,19 +8103,19 @@
       </c>
       <c r="H22" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G22,H$15)</f>
-        <v>17899718</v>
+        <v>17900086</v>
       </c>
       <c r="I22" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G22,I$15)</f>
-        <v>8.6300000000000004E-6</v>
+        <v>8.6000000000000007E-6</v>
       </c>
       <c r="J22" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G22,J$15)</f>
-        <v>6391</v>
+        <v>40</v>
       </c>
       <c r="K22" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G22,K$15)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G22,L$15)</f>
@@ -8121,25 +8123,25 @@
       </c>
       <c r="M22" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G22,M$15)</f>
-        <v>28850790</v>
+        <v>28851371</v>
       </c>
       <c r="N22" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G22,N$15)</f>
-        <v>28850790</v>
+        <v>28851371</v>
       </c>
       <c r="O22" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G22,O$15)</f>
-        <v>43249.784061412036</v>
+        <v>43249.790460972225</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C23)</f>
-        <v>9.7972099999999998</v>
+        <v>0.153</v>
       </c>
       <c r="B23" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C23)</f>
-        <v>561.02</v>
+        <v>558.28</v>
       </c>
       <c r="C23" s="8">
         <f t="shared" si="0"/>
@@ -8147,21 +8149,21 @@
       </c>
       <c r="D23" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C23)</f>
-        <v>562.57000000000005</v>
+        <v>560.52</v>
       </c>
       <c r="E23" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C23)</f>
-        <v>0.4</v>
+        <v>3.2010000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C24)</f>
-        <v>0.46034000000000003</v>
+        <v>13</v>
       </c>
       <c r="B24" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C24)</f>
-        <v>561</v>
+        <v>558.25</v>
       </c>
       <c r="C24" s="8">
         <f t="shared" si="0"/>
@@ -8169,21 +8171,21 @@
       </c>
       <c r="D24" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C24)</f>
-        <v>562.79999999999995</v>
+        <v>560.53</v>
       </c>
       <c r="E24" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C24)</f>
-        <v>1.2243200000000001</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,A$15,$C25)</f>
-        <v>4.0000000000000002E-4</v>
+        <v>1.32884</v>
       </c>
       <c r="B25" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,B$15,$C25)</f>
-        <v>560.94000000000005</v>
+        <v>558.05999999999995</v>
       </c>
       <c r="C25" s="34">
         <f t="shared" si="0"/>
@@ -8191,33 +8193,33 @@
       </c>
       <c r="D25" s="35">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,D$15,$C25)</f>
-        <v>563</v>
+        <v>560.72</v>
       </c>
       <c r="E25" s="35">
         <f>RTD(progId,,BINANCE_DEPTH,$C$15,E$15,$C25)</f>
-        <v>3.5089999999999999</v>
+        <v>0.24099999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <f>SUM(Table3[BID_DEPTH_SIZE])</f>
-        <v>39.953020000000002</v>
+        <v>173.31828000000002</v>
       </c>
       <c r="B26" s="15">
         <f>SUMPRODUCT(Table3[BID_DEPTH_SIZE],Table3[BID_DEPTH])</f>
-        <v>22421.048006099998</v>
+        <v>96865.138587300011</v>
       </c>
       <c r="C26" s="16">
         <f>D26-B26</f>
-        <v>-14380.715746299997</v>
+        <v>-75794.816730300008</v>
       </c>
       <c r="D26" s="15">
         <f>SUMPRODUCT(Table3[ASK_DEPTH_SIZE],Table3[ASK_DEPTH])</f>
-        <v>8040.3322598000004</v>
+        <v>21070.321856999999</v>
       </c>
       <c r="E26" s="13">
         <f>SUM(Table3[ASK_DEPTH_SIZE])</f>
-        <v>14.295020000000001</v>
+        <v>37.599149999999995</v>
       </c>
       <c r="F26" s="9"/>
       <c r="H26" s="1"/>
@@ -8228,14 +8230,14 @@
     <row r="27" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="32">
         <f>B16-B25</f>
-        <v>0.58999999999991815</v>
+        <v>1.2300000000000182</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>62</v>
       </c>
       <c r="D27" s="32">
         <f>D16-D25</f>
-        <v>-1.0499999999999545</v>
+        <v>-0.99000000000000909</v>
       </c>
       <c r="F27" s="9"/>
       <c r="I27" s="4"/>
@@ -8329,11 +8331,11 @@
       </c>
       <c r="D31" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,D$30,$D$29)</f>
-        <v>558.89</v>
+        <v>557.83000000000004</v>
       </c>
       <c r="E31" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,E$30,$D$29)</f>
-        <v>561.5</v>
+        <v>559</v>
       </c>
       <c r="F31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,F$30,$D$29)</f>
@@ -8349,19 +8351,19 @@
       </c>
       <c r="I31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,I$30,$D$29)</f>
-        <v>4395155.6982738003</v>
+        <v>5166127.2520958995</v>
       </c>
       <c r="J31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,J$30,$D$29)</f>
-        <v>7799.1461900000004</v>
+        <v>9175.9067799999993</v>
       </c>
       <c r="K31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,K$30,$D$29)</f>
-        <v>2536.66786</v>
+        <v>2999.4280100000001</v>
       </c>
       <c r="L31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,L$30,$D$29)</f>
-        <v>1428531.5791461</v>
+        <v>1687695.3641526001</v>
       </c>
       <c r="M31" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,M$30,$D$29)</f>
@@ -8369,11 +8371,11 @@
       </c>
       <c r="N31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,N$30,$D$29)</f>
-        <v>4838</v>
+        <v>5754</v>
       </c>
       <c r="O31" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,O$30,$D$29)</f>
-        <v>43249.784061620368</v>
+        <v>43249.790412256945</v>
       </c>
       <c r="P31" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,P$30,$D$29)</f>
@@ -8381,7 +8383,7 @@
       </c>
       <c r="Q31" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,Q$30,$D$29)</f>
-        <v>26750922</v>
+        <v>26751838</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -8398,11 +8400,11 @@
       </c>
       <c r="D32" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,D$30,$D$29)</f>
-        <v>7435.02</v>
+        <v>7401.29</v>
       </c>
       <c r="E32" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,E$30,$D$29)</f>
-        <v>7444.37</v>
+        <v>7430.54</v>
       </c>
       <c r="F32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,F$30,$D$29)</f>
@@ -8418,19 +8420,19 @@
       </c>
       <c r="I32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,I$30,$D$29)</f>
-        <v>10197293.9071803</v>
+        <v>12931420.01809966</v>
       </c>
       <c r="J32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,J$30,$D$29)</f>
-        <v>1365.257846</v>
+        <v>1733.676307</v>
       </c>
       <c r="K32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,K$30,$D$29)</f>
-        <v>622.820652</v>
+        <v>823.47727199999997</v>
       </c>
       <c r="L32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,L$30,$D$29)</f>
-        <v>4651521.2728654202</v>
+        <v>6140705.0098409401</v>
       </c>
       <c r="M32" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,M$30,$D$29)</f>
@@ -8438,11 +8440,11 @@
       </c>
       <c r="N32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,N$30,$D$29)</f>
-        <v>9898</v>
+        <v>12945</v>
       </c>
       <c r="O32" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,O$30,$D$29)</f>
-        <v>43249.784073402778</v>
+        <v>43249.790457685187</v>
       </c>
       <c r="P32" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,P$30,$D$29)</f>
@@ -8450,7 +8452,7 @@
       </c>
       <c r="Q32" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,Q$30,$D$29)</f>
-        <v>46725848</v>
+        <v>46728895</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -8467,11 +8469,11 @@
       </c>
       <c r="D33" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,D$30,$D$29)</f>
-        <v>8.6100000000000006E-6</v>
+        <v>8.5699999999999993E-6</v>
       </c>
       <c r="E33" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,E$30,$D$29)</f>
-        <v>8.6300000000000004E-6</v>
+        <v>8.5900000000000008E-6</v>
       </c>
       <c r="F33" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,F$30,$D$29)</f>
@@ -8487,19 +8489,19 @@
       </c>
       <c r="I33" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,I$30,$D$29)</f>
-        <v>347.96116496000002</v>
+        <v>402.88634443000001</v>
       </c>
       <c r="J33" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,J$30,$D$29)</f>
-        <v>40105150</v>
+        <v>46495347</v>
       </c>
       <c r="K33" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,K$30,$D$29)</f>
-        <v>19117125</v>
+        <v>20951803</v>
       </c>
       <c r="L33" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,L$30,$D$29)</f>
-        <v>165.94695024999999</v>
+        <v>181.71567625</v>
       </c>
       <c r="M33" s="20" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,M$30,$D$29)</f>
@@ -8507,11 +8509,11 @@
       </c>
       <c r="N33" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,N$30,$D$29)</f>
-        <v>3732</v>
+        <v>4312</v>
       </c>
       <c r="O33" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,O$30,$D$29)</f>
-        <v>43249.784061446757</v>
+        <v>43249.790459687501</v>
       </c>
       <c r="P33" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,P$30,$D$29)</f>
@@ -8519,7 +8521,7 @@
       </c>
       <c r="Q33" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A33,Q$30,$D$29)</f>
-        <v>28850790</v>
+        <v>28851370</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -8606,11 +8608,11 @@
       </c>
       <c r="D37" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,D$36,$D$35)</f>
-        <v>558.89</v>
+        <v>557.83000000000004</v>
       </c>
       <c r="E37" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,E$36,$D$35)</f>
-        <v>561.5</v>
+        <v>559</v>
       </c>
       <c r="F37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,F$36,$D$35)</f>
@@ -8626,19 +8628,19 @@
       </c>
       <c r="I37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,I$36,$D$35)</f>
-        <v>10968944.045899499</v>
+        <v>11739915.599721599</v>
       </c>
       <c r="J37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,J$36,$D$35)</f>
-        <v>19355.553370000001</v>
+        <v>20732.313959999999</v>
       </c>
       <c r="K37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,K$36,$D$35)</f>
-        <v>8635.5733899999996</v>
+        <v>9098.3335399999996</v>
       </c>
       <c r="L37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,L$36,$D$35)</f>
-        <v>4897275.1828148998</v>
+        <v>5156438.9678213997</v>
       </c>
       <c r="M37" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,M$36,$D$35)</f>
@@ -8646,11 +8648,11 @@
       </c>
       <c r="N37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,N$36,$D$35)</f>
-        <v>13033</v>
+        <v>13949</v>
       </c>
       <c r="O37" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,O$36,$D$35)</f>
-        <v>43249.784061620368</v>
+        <v>43249.790412256945</v>
       </c>
       <c r="P37" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,P$36,$D$35)</f>
@@ -8658,7 +8660,7 @@
       </c>
       <c r="Q37" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,Q$36,$D$35)</f>
-        <v>26750922</v>
+        <v>26751838</v>
       </c>
     </row>
     <row r="38" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8675,11 +8677,11 @@
       </c>
       <c r="D38" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,D$36,$D$35)</f>
-        <v>7435.02</v>
+        <v>7401.29</v>
       </c>
       <c r="E38" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,E$36,$D$35)</f>
-        <v>7444.37</v>
+        <v>7430.54</v>
       </c>
       <c r="F38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,F$36,$D$35)</f>
@@ -8695,19 +8697,19 @@
       </c>
       <c r="I38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,I$36,$D$35)</f>
-        <v>29752099.03286355</v>
+        <v>32486225.14378291</v>
       </c>
       <c r="J38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,J$36,$D$35)</f>
-        <v>3973.9061109999998</v>
+        <v>4342.3245720000004</v>
       </c>
       <c r="K38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,K$36,$D$35)</f>
-        <v>2087.112353</v>
+        <v>2287.7689730000002</v>
       </c>
       <c r="L38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,L$36,$D$35)</f>
-        <v>15628598.844702311</v>
+        <v>17117782.581677832</v>
       </c>
       <c r="M38" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,M$36,$D$35)</f>
@@ -8715,11 +8717,11 @@
       </c>
       <c r="N38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,N$36,$D$35)</f>
-        <v>27767</v>
+        <v>30814</v>
       </c>
       <c r="O38" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,O$36,$D$35)</f>
-        <v>43249.784073402778</v>
+        <v>43249.790457673611</v>
       </c>
       <c r="P38" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,P$36,$D$35)</f>
@@ -8727,7 +8729,7 @@
       </c>
       <c r="Q38" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,Q$36,$D$35)</f>
-        <v>46725848</v>
+        <v>46728895</v>
       </c>
     </row>
     <row r="39" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8748,7 +8750,7 @@
       </c>
       <c r="E39" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,E$36,$D$35)</f>
-        <v>8.6300000000000004E-6</v>
+        <v>8.5900000000000008E-6</v>
       </c>
       <c r="F39" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,F$36,$D$35)</f>
@@ -8764,19 +8766,19 @@
       </c>
       <c r="I39" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,I$36,$D$35)</f>
-        <v>903.63612820000003</v>
+        <v>958.56130767000002</v>
       </c>
       <c r="J39" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,J$36,$D$35)</f>
-        <v>104709154</v>
+        <v>111099351</v>
       </c>
       <c r="K39" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,K$36,$D$35)</f>
-        <v>53392516</v>
+        <v>55227194</v>
       </c>
       <c r="L39" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,L$36,$D$35)</f>
-        <v>460.91789722999999</v>
+        <v>476.68662323000001</v>
       </c>
       <c r="M39" s="20" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,M$36,$D$35)</f>
@@ -8784,11 +8786,11 @@
       </c>
       <c r="N39" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,N$36,$D$35)</f>
-        <v>9964</v>
+        <v>10544</v>
       </c>
       <c r="O39" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,O$36,$D$35)</f>
-        <v>43249.784061435188</v>
+        <v>43249.790459687501</v>
       </c>
       <c r="P39" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,P$36,$D$35)</f>
@@ -8796,7 +8798,7 @@
       </c>
       <c r="Q39" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A39,Q$36,$D$35)</f>
-        <v>28850790</v>
+        <v>28851370</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -8899,7 +8901,7 @@
       </c>
       <c r="E43" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,E$42,$D$41)</f>
-        <v>561.5</v>
+        <v>559</v>
       </c>
       <c r="F43" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,F$42,$D$41)</f>
@@ -8915,19 +8917,19 @@
       </c>
       <c r="I43" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,I$42,$D$41)</f>
-        <v>52514496.026789799</v>
+        <v>53285467.580611899</v>
       </c>
       <c r="J43" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,J$42,$D$41)</f>
-        <v>93478.519199999995</v>
+        <v>94855.279790000001</v>
       </c>
       <c r="K43" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,K$42,$D$41)</f>
-        <v>46723.2091</v>
+        <v>47185.969250000002</v>
       </c>
       <c r="L43" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,L$42,$D$41)</f>
-        <v>26240139.5047675</v>
+        <v>26499303.289774001</v>
       </c>
       <c r="M43" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,M$42,$D$41)</f>
@@ -8935,11 +8937,11 @@
       </c>
       <c r="N43" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,N$42,$D$41)</f>
-        <v>63241</v>
+        <v>64157</v>
       </c>
       <c r="O43" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,O$42,$D$41)</f>
-        <v>43249.784061620368</v>
+        <v>43249.790412245369</v>
       </c>
       <c r="P43" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,P$42,$D$41)</f>
@@ -8947,7 +8949,7 @@
       </c>
       <c r="Q43" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A43,Q$42,$D$41)</f>
-        <v>26750922</v>
+        <v>26751838</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -8968,7 +8970,7 @@
       </c>
       <c r="E44" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,E$42,$D$41)</f>
-        <v>7444.37</v>
+        <v>7430.54</v>
       </c>
       <c r="F44" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,F$42,$D$41)</f>
@@ -8984,19 +8986,19 @@
       </c>
       <c r="I44" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,I$42,$D$41)</f>
-        <v>129714114.66223025</v>
+        <v>132448240.77314962</v>
       </c>
       <c r="J44" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,J$42,$D$41)</f>
-        <v>17405.573903</v>
+        <v>17773.992364000002</v>
       </c>
       <c r="K44" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,K$42,$D$41)</f>
-        <v>9354.3132559999995</v>
+        <v>9554.9698759999992</v>
       </c>
       <c r="L44" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,L$42,$D$41)</f>
-        <v>69718853.044642255</v>
+        <v>71208036.781617776</v>
       </c>
       <c r="M44" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,M$42,$D$41)</f>
@@ -9004,11 +9006,11 @@
       </c>
       <c r="N44" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,N$42,$D$41)</f>
-        <v>114326</v>
+        <v>117373</v>
       </c>
       <c r="O44" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,O$42,$D$41)</f>
-        <v>43249.784073402778</v>
+        <v>43249.790457685187</v>
       </c>
       <c r="P44" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,P$42,$D$41)</f>
@@ -9016,7 +9018,7 @@
       </c>
       <c r="Q44" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A44,Q$42,$D$41)</f>
-        <v>46725848</v>
+        <v>46728895</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -9037,7 +9039,7 @@
       </c>
       <c r="E45" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,E$42,$D$41)</f>
-        <v>8.6300000000000004E-6</v>
+        <v>8.5900000000000008E-6</v>
       </c>
       <c r="F45" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,F$42,$D$41)</f>
@@ -9053,19 +9055,19 @@
       </c>
       <c r="I45" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,I$42,$D$41)</f>
-        <v>4559.2420390099996</v>
+        <v>4614.16721848</v>
       </c>
       <c r="J45" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,J$42,$D$41)</f>
-        <v>531640512</v>
+        <v>538030709</v>
       </c>
       <c r="K45" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,K$42,$D$41)</f>
-        <v>245903612</v>
+        <v>247738290</v>
       </c>
       <c r="L45" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,L$42,$D$41)</f>
-        <v>2109.96642647</v>
+        <v>2125.7351524699998</v>
       </c>
       <c r="M45" s="20" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,M$42,$D$41)</f>
@@ -9073,11 +9075,11 @@
       </c>
       <c r="N45" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,N$42,$D$41)</f>
-        <v>43032</v>
+        <v>43612</v>
       </c>
       <c r="O45" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,O$42,$D$41)</f>
-        <v>43249.784061446757</v>
+        <v>43249.790459675925</v>
       </c>
       <c r="P45" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,P$42,$D$41)</f>
@@ -9085,7 +9087,7 @@
       </c>
       <c r="Q45" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A45,Q$42,$D$41)</f>
-        <v>28850790</v>
+        <v>28851370</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -9500,19 +9502,19 @@
       </c>
       <c r="B3" s="2">
         <f>RTD(progId,,GDAX,$A3,B$2)</f>
-        <v>561.85</v>
+        <v>558.51</v>
       </c>
       <c r="C3" s="2">
         <f>RTD(progId,,GDAX,$A3,C$2)</f>
-        <v>561.86</v>
+        <v>558.61</v>
       </c>
       <c r="D3" s="2">
         <f>RTD(progId,,GDAX,$A3,D$2)</f>
-        <v>561.85</v>
+        <v>558.5</v>
       </c>
       <c r="E3" s="2">
         <f>RTD(progId,,GDAX,$A3,E$2)</f>
-        <v>512.05999999999995</v>
+        <v>513.49</v>
       </c>
       <c r="F3" s="2">
         <f>RTD(progId,,GDAX,$A3,F$2)</f>
@@ -9524,7 +9526,7 @@
       </c>
       <c r="H3" s="2">
         <f>RTD(progId,,GDAX,$A3,H$2)</f>
-        <v>141081.61087484</v>
+        <v>141356.15238218001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -9533,19 +9535,19 @@
       </c>
       <c r="B4" s="2">
         <f>RTD(progId,,GDAX,$A4,B$2)</f>
-        <v>7439.41</v>
+        <v>7425.81</v>
       </c>
       <c r="C4" s="2">
         <f>RTD(progId,,GDAX,$A4,C$2)</f>
-        <v>7443.8</v>
+        <v>7425.82</v>
       </c>
       <c r="D4" s="2">
         <f>RTD(progId,,GDAX,$A4,D$2)</f>
-        <v>7439.41</v>
+        <v>7425.82</v>
       </c>
       <c r="E4" s="2">
         <f>RTD(progId,,GDAX,$A4,E$2)</f>
-        <v>7100.01</v>
+        <v>7100</v>
       </c>
       <c r="F4" s="2">
         <f>RTD(progId,,GDAX,$A4,F$2)</f>
@@ -9557,7 +9559,7 @@
       </c>
       <c r="H4" s="2">
         <f>RTD(progId,,GDAX,$A4,H$2)</f>
-        <v>10650.18819447</v>
+        <v>10614.50775662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use _dirtyMap to improve performance
</commit_message>
<xml_diff>
--- a/doc/crypto.xlsx
+++ b/doc/crypto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\Crypto\crypto-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF669BC-B8E3-4A72-8F47-7159D60D8D3C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B019D48-64CB-416D-9724-B751B73A1391}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12225" tabRatio="245" xr2:uid="{FA204BA2-54FD-4EAD-B49B-FB8867D94DC8}"/>
   </bookViews>
@@ -230,7 +230,7 @@
     <t>Drift</t>
   </si>
   <si>
-    <t>This text was added by using code 6/21/2018 6:36:22 PM</t>
+    <t>This text was added by using code 6/24/2018 12:06:07 PM</t>
   </si>
 </sst>
 </file>
@@ -2855,7 +2855,7 @@
   <volType type="realTimeData">
     <main first="crypto">
       <tp>
-        <v>19406</v>
+        <v>26429</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -2863,7 +2863,7 @@
         <tr r="N8" s="1"/>
       </tp>
       <tp>
-        <v>27095</v>
+        <v>42560</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -2871,7 +2871,7 @@
         <tr r="N7" s="1"/>
       </tp>
       <tp>
-        <v>159036</v>
+        <v>225376</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -2879,7 +2879,7 @@
         <tr r="N6" s="1"/>
       </tp>
       <tp>
-        <v>77719</v>
+        <v>113925</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -2887,7 +2887,7 @@
         <tr r="N5" s="1"/>
       </tp>
       <tp>
-        <v>55.041119129999998</v>
+        <v>71.562308580000007</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2896,16 +2896,16 @@
         <tr r="I32" s="1"/>
       </tp>
       <tp>
-        <v>298.56328172000002</v>
+        <v>3.5371970000000003E-2</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>QUOTE_VOL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="I38" s="1"/>
       </tp>
       <tp>
-        <v>5.04</v>
+        <v>2.09</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -2913,7 +2913,7 @@
         <tr r="G9" s="1"/>
       </tp>
       <tp>
-        <v>15745</v>
+        <v>1062151</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -2921,7 +2921,7 @@
         <tr r="K11" s="1"/>
       </tp>
       <tp>
-        <v>0.9</v>
+        <v>4813.5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -2929,7 +2929,7 @@
         <tr r="G8" s="1"/>
       </tp>
       <tp>
-        <v>324853.88</v>
+        <v>416876.88</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -2937,7 +2937,7 @@
         <tr r="L9" s="1"/>
       </tp>
       <tp>
-        <v>501624962</v>
+        <v>539412151</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -2945,7 +2945,7 @@
         <tr r="L11" s="1"/>
       </tp>
       <tp>
-        <v>32839604</v>
+        <v>40848135</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -2953,7 +2953,7 @@
         <tr r="L10" s="1"/>
       </tp>
       <tp>
-        <v>6717.94</v>
+        <v>5819.26</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2962,16 +2962,16 @@
         <tr r="C31" s="1"/>
       </tp>
       <tp>
-        <v>6730</v>
+        <v>5819.26</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>HIGH</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="C37" s="1"/>
       </tp>
       <tp>
-        <v>525.57000000000005</v>
+        <v>426</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2980,16 +2980,16 @@
         <tr r="C30" s="1"/>
       </tp>
       <tp>
-        <v>528.1</v>
+        <v>425.5</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
         <stp>HIGH</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="C36" s="1"/>
       </tp>
       <tp>
-        <v>524.37</v>
+        <v>421.73</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2998,16 +2998,16 @@
         <tr r="B30" s="1"/>
       </tp>
       <tp>
-        <v>524.01</v>
+        <v>425.46</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
         <stp>OPEN</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="B36" s="1"/>
       </tp>
       <tp>
-        <v>6699.32</v>
+        <v>5769.86</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3016,16 +3016,16 @@
         <tr r="B31" s="1"/>
       </tp>
       <tp>
-        <v>6714.52</v>
+        <v>5816.01</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>OPEN</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="B37" s="1"/>
       </tp>
       <tp>
-        <v>3037</v>
+        <v>2527</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3034,16 +3034,16 @@
         <tr r="N31" s="1"/>
       </tp>
       <tp>
-        <v>13368</v>
+        <v>29</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>TRADES</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="N37" s="1"/>
       </tp>
       <tp>
-        <v>1281</v>
+        <v>1628</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3052,16 +3052,16 @@
         <tr r="N30" s="1"/>
       </tp>
       <tp>
-        <v>6415</v>
+        <v>11</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
         <stp>TRADES</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="N36" s="1"/>
       </tp>
       <tp>
-        <v>-1.103E-2</v>
+        <v>-7.8670000000000004E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3069,7 +3069,7 @@
         <tr r="O8" s="1"/>
       </tp>
       <tp>
-        <v>-1.018E-2</v>
+        <v>-0.10082000000000001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3077,7 +3077,7 @@
         <tr r="O7" s="1"/>
       </tp>
       <tp>
-        <v>-1.549E-2</v>
+        <v>-9.6600000000000005E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3085,7 +3085,7 @@
         <tr r="O5" s="1"/>
       </tp>
       <tp>
-        <v>0</v>
+        <v>-4.9759999999999999E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3101,7 +3101,7 @@
         <tr r="D5" s="1"/>
       </tp>
       <tp>
-        <v>15</v>
+        <v>1.0781799999999999</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3109,7 +3109,7 @@
         <tr r="G5" s="1"/>
       </tp>
       <tp>
-        <v>1.8669999999999999E-2</v>
+        <v>0.26954</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3117,7 +3117,7 @@
         <tr r="G7" s="1"/>
       </tp>
       <tp>
-        <v>0.521536</v>
+        <v>5.6798000000000001E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3125,7 +3125,7 @@
         <tr r="G6" s="1"/>
       </tp>
       <tp>
-        <v>1848.5073156999999</v>
+        <v>2224.1238684599998</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3133,7 +3133,7 @@
         <tr r="M9" s="1"/>
       </tp>
       <tp>
-        <v>524.38</v>
+        <v>425.1</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -3141,7 +3141,7 @@
         <tr r="C3" s="2"/>
       </tp>
       <tp>
-        <v>524.37</v>
+        <v>425.09</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -3165,7 +3165,7 @@
         <tr r="D6" s="1"/>
       </tp>
       <tp>
-        <v>6710.69</v>
+        <v>5831.99</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -3173,7 +3173,7 @@
         <tr r="B4" s="2"/>
       </tp>
       <tp>
-        <v>11857</v>
+        <v>1756</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3181,7 +3181,16 @@
         <tr r="K10" s="1"/>
       </tp>
       <tp>
-        <v>43272.75</v>
+        <v>43275.504166666666</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>trxbtc</stp>
+        <stp>OPEN_TIME</stp>
+        <stp>0</stp>
+        <tr r="F38" s="1"/>
+      </tp>
+      <tp>
+        <v>43275.5</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3190,16 +3199,7 @@
         <tr r="F32" s="1"/>
       </tp>
       <tp>
-        <v>43272.666666666664</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>trxbtc</stp>
-        <stp>OPEN_TIME</stp>
-        <stp>7</stp>
-        <tr r="F38" s="1"/>
-      </tp>
-      <tp>
-        <v>6710.7</v>
+        <v>5832</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -3207,7 +3207,7 @@
         <tr r="C4" s="2"/>
       </tp>
       <tp>
-        <v>6682.3</v>
+        <v>5777</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -3215,16 +3215,16 @@
         <tr r="G4" s="2"/>
       </tp>
       <tp>
-        <v>30232542</v>
+        <v>30373882</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>LAST_ID</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="Q38" s="1"/>
       </tp>
       <tp>
-        <v>30232542</v>
+        <v>30373882</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3233,7 +3233,16 @@
         <tr r="Q32" s="1"/>
       </tp>
       <tp>
-        <v>329.83319</v>
+        <v>40.236840000000001</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>ethusdt</stp>
+        <stp>TAKE_BUY_VOL</stp>
+        <stp>0</stp>
+        <tr r="K36" s="1"/>
+      </tp>
+      <tp>
+        <v>1634.19415</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3242,16 +3251,16 @@
         <tr r="K30" s="1"/>
       </tp>
       <tp>
-        <v>1949.8864900000001</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>ethusdt</stp>
+        <v>3.7635740000000002</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>btcusdt</stp>
         <stp>TAKE_BUY_VOL</stp>
-        <stp>7</stp>
-        <tr r="K36" s="1"/>
-      </tp>
-      <tp>
-        <v>255.586726</v>
+        <stp>0</stp>
+        <tr r="K37" s="1"/>
+      </tp>
+      <tp>
+        <v>229.99405400000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3260,16 +3269,16 @@
         <tr r="K31" s="1"/>
       </tp>
       <tp>
-        <v>1358.5464979999999</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>btcusdt</stp>
-        <stp>TAKE_BUY_VOL</stp>
-        <stp>7</stp>
-        <tr r="K37" s="1"/>
-      </tp>
-      <tp>
-        <v>52379441</v>
+        <v>53033953</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>btcusdt</stp>
+        <stp>LAST_ID</stp>
+        <stp>0</stp>
+        <tr r="Q37" s="1"/>
+      </tp>
+      <tp>
+        <v>53033953</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3278,16 +3287,7 @@
         <tr r="Q31" s="1"/>
       </tp>
       <tp>
-        <v>52379441</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>btcusdt</stp>
-        <stp>LAST_ID</stp>
-        <stp>7</stp>
-        <tr r="Q37" s="1"/>
-      </tp>
-      <tp>
-        <v>7.9209999999999995E-5</v>
+        <v>7.674E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3295,7 +3295,7 @@
         <tr r="J10" s="1"/>
       </tp>
       <tp>
-        <v>7.2099999999999996E-6</v>
+        <v>6.5899999999999996E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3303,7 +3303,7 @@
         <tr r="J11" s="1"/>
       </tp>
       <tp>
-        <v>5.5799999999999999E-3</v>
+        <v>5.019E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3311,7 +3311,7 @@
         <tr r="J9" s="1"/>
       </tp>
       <tp>
-        <v>5.5729999999999998E-3</v>
+        <v>5.0140000000000002E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3319,7 +3319,7 @@
         <tr r="H9" s="1"/>
       </tp>
       <tp>
-        <v>7.1999999999999997E-6</v>
+        <v>6.5799999999999997E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3327,7 +3327,7 @@
         <tr r="H11" s="1"/>
       </tp>
       <tp>
-        <v>7.9200000000000001E-5</v>
+        <v>7.6730000000000006E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3335,7 +3335,7 @@
         <tr r="H10" s="1"/>
       </tp>
       <tp>
-        <v>53686</v>
+        <v>1669</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3343,7 +3343,7 @@
         <tr r="G10" s="1"/>
       </tp>
       <tp>
-        <v>521.5</v>
+        <v>421.1</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -3351,16 +3351,7 @@
         <tr r="G3" s="2"/>
       </tp>
       <tp>
-        <v>28994374</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>ethusdt</stp>
-        <stp>LAST_ID</stp>
-        <stp>7</stp>
-        <tr r="Q36" s="1"/>
-      </tp>
-      <tp>
-        <v>28994374</v>
+        <v>29343566</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3369,7 +3360,16 @@
         <tr r="Q30" s="1"/>
       </tp>
       <tp>
-        <v>5.5500000000000002E-3</v>
+        <v>29343566</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>ethusdt</stp>
+        <stp>LAST_ID</stp>
+        <stp>0</stp>
+        <tr r="Q36" s="1"/>
+      </tp>
+      <tp>
+        <v>5.0000000000000001E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3377,7 +3377,7 @@
         <tr r="B9" s="1"/>
       </tp>
       <tp>
-        <v>7.0500000000000003E-6</v>
+        <v>6.4799999999999998E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3385,7 +3385,7 @@
         <tr r="B11" s="1"/>
       </tp>
       <tp>
-        <v>7.9060000000000005E-5</v>
+        <v>7.6260000000000005E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3393,7 +3393,7 @@
         <tr r="B10" s="1"/>
       </tp>
       <tp>
-        <v>1.67</v>
+        <v>0.1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3401,7 +3401,7 @@
         <tr r="K9" s="1"/>
       </tp>
       <tp>
-        <v>229998</v>
+        <v>8917</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3409,7 +3409,7 @@
         <tr r="G11" s="1"/>
       </tp>
       <tp>
-        <v>4136</v>
+        <v>92.7</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3417,7 +3417,7 @@
         <tr r="K8" s="1"/>
       </tp>
       <tp>
-        <v>0.2</v>
+        <v>4.4000000000000002E-4</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3425,7 +3425,7 @@
         <tr r="K7" s="1"/>
       </tp>
       <tp>
-        <v>9.9999999999999995E-7</v>
+        <v>6.4300000000000002E-4</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3433,7 +3433,7 @@
         <tr r="K6" s="1"/>
       </tp>
       <tp>
-        <v>3.0778400000000001</v>
+        <v>0.23496</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3441,7 +3441,7 @@
         <tr r="K5" s="1"/>
       </tp>
       <tp>
-        <v>2625.0613650700002</v>
+        <v>3201.9709302699998</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3449,7 +3449,7 @@
         <tr r="M10" s="1"/>
       </tp>
       <tp>
-        <v>3643.0131911799999</v>
+        <v>3726.3932793899999</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3465,7 +3465,7 @@
         <tr r="D8" s="1"/>
       </tp>
       <tp>
-        <v>1291647</v>
+        <v>1363908</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3473,16 +3473,16 @@
         <tr r="M18" s="1"/>
       </tp>
       <tp>
-        <v>7.17E-6</v>
+        <v>6.5799999999999997E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>OPEN</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="B38" s="1"/>
       </tp>
       <tp>
-        <v>7.1999999999999997E-6</v>
+        <v>6.55E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3491,7 +3491,7 @@
         <tr r="B32" s="1"/>
       </tp>
       <tp>
-        <v>5.4000000000000001E-4</v>
+        <v>7.9000000000000001E-4</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3499,7 +3499,7 @@
         <tr r="I8" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3507,7 +3507,7 @@
         <tr r="K21" s="1"/>
       </tp>
       <tp>
-        <v>0.1</v>
+        <v>0.11</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3515,7 +3515,7 @@
         <tr r="I7" s="1"/>
       </tp>
       <tp>
-        <v>0.54</v>
+        <v>2.74</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3523,7 +3523,7 @@
         <tr r="I6" s="1"/>
       </tp>
       <tp>
-        <v>0.35</v>
+        <v>0.13</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3531,7 +3531,7 @@
         <tr r="I5" s="1"/>
       </tp>
       <tp>
-        <v>4097</v>
+        <v>295</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3539,7 +3539,16 @@
         <tr r="J20" s="1"/>
       </tp>
       <tp>
-        <v>667</v>
+        <v>4</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>trxbtc</stp>
+        <stp>TRADES</stp>
+        <stp>0</stp>
+        <tr r="N38" s="1"/>
+      </tp>
+      <tp>
+        <v>572</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3548,16 +3557,7 @@
         <tr r="N32" s="1"/>
       </tp>
       <tp>
-        <v>4472</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>trxbtc</stp>
-        <stp>TRADES</stp>
-        <stp>7</stp>
-        <tr r="N38" s="1"/>
-      </tp>
-      <tp>
-        <v>14031530</v>
+        <v>14141287</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -3565,7 +3565,7 @@
         <tr r="H19" s="1"/>
       </tp>
       <tp>
-        <v>30232542</v>
+        <v>30373882</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3573,7 +3573,7 @@
         <tr r="M21" s="1"/>
       </tp>
       <tp>
-        <v>52379445</v>
+        <v>53033961</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3581,7 +3581,7 @@
         <tr r="M16" s="1"/>
       </tp>
       <tp>
-        <v>8108510</v>
+        <v>8225958</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3589,7 +3589,7 @@
         <tr r="M17" s="1"/>
       </tp>
       <tp>
-        <v>28994374</v>
+        <v>29343577</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3597,16 +3597,16 @@
         <tr r="M15" s="1"/>
       </tp>
       <tp>
-        <v>7.2400000000000001E-6</v>
+        <v>6.5899999999999996E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>HIGH</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="C38" s="1"/>
       </tp>
       <tp>
-        <v>7.2300000000000002E-6</v>
+        <v>6.6000000000000003E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3623,7 +3623,7 @@
         <tr r="K20" s="1"/>
       </tp>
       <tp>
-        <v>21966660</v>
+        <v>22077467</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3631,7 +3631,7 @@
         <tr r="M20" s="1"/>
       </tp>
       <tp>
-        <v>1783.7</v>
+        <v>76.5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3639,7 +3639,7 @@
         <tr r="J18" s="1"/>
       </tp>
       <tp>
-        <v>1291647</v>
+        <v>1363908</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3655,7 +3655,7 @@
         <tr r="L19" s="1"/>
       </tp>
       <tp>
-        <v>2.2769999999999999E-2</v>
+        <v>4.4999999999999999E-4</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3663,7 +3663,7 @@
         <tr r="J15" s="1"/>
       </tp>
       <tp>
-        <v>2.555E-3</v>
+        <v>1.738E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3671,7 +3671,7 @@
         <tr r="J16" s="1"/>
       </tp>
       <tp>
-        <v>0.95452000000000004</v>
+        <v>0.45900000000000002</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3679,7 +3679,7 @@
         <tr r="J17" s="1"/>
       </tp>
       <tp>
-        <v>0.3</v>
+        <v>0.03</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3688,7 +3688,7 @@
         <tr r="E23" s="1"/>
       </tp>
       <tp>
-        <v>6.9415000000000004E-2</v>
+        <v>0.40464699999999998</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3697,7 +3697,7 @@
         <tr r="E24" s="1"/>
       </tp>
       <tp>
-        <v>0.26966299999999999</v>
+        <v>0.39807700000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3706,7 +3706,7 @@
         <tr r="E19" s="1"/>
       </tp>
       <tp>
-        <v>5.1568399999999999</v>
+        <v>1.4999999999999999E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3715,7 +3715,7 @@
         <tr r="E20" s="1"/>
       </tp>
       <tp>
-        <v>7.8560000000000001E-3</v>
+        <v>0.12544</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3724,7 +3724,7 @@
         <tr r="E21" s="1"/>
       </tp>
       <tp>
-        <v>0.03</v>
+        <v>4.0712999999999999E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3733,7 +3733,7 @@
         <tr r="E22" s="1"/>
       </tp>
       <tp>
-        <v>5.6059999999999999E-3</v>
+        <v>6.4300000000000002E-4</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3742,7 +3742,7 @@
         <tr r="E15" s="1"/>
       </tp>
       <tp>
-        <v>0.58862999999999999</v>
+        <v>1.9255999999999999E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3751,7 +3751,7 @@
         <tr r="E16" s="1"/>
       </tp>
       <tp>
-        <v>0.5</v>
+        <v>2.3529999999999999E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3760,7 +3760,7 @@
         <tr r="E17" s="1"/>
       </tp>
       <tp>
-        <v>0.22800500000000001</v>
+        <v>1.719E-3</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3769,7 +3769,7 @@
         <tr r="E18" s="1"/>
       </tp>
       <tp>
-        <v>197</v>
+        <v>1000</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3777,7 +3777,7 @@
         <tr r="J21" s="1"/>
       </tp>
       <tp>
-        <v>43272.775158055556</v>
+        <v>43275.504237303241</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3785,7 +3785,7 @@
         <tr r="O18" s="1"/>
       </tp>
       <tp>
-        <v>43272.775201192133</v>
+        <v>43275.504220960647</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3793,7 +3793,7 @@
         <tr r="O17" s="1"/>
       </tp>
       <tp>
-        <v>43272.775247094905</v>
+        <v>43275.50424559028</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3801,7 +3801,7 @@
         <tr r="O15" s="1"/>
       </tp>
       <tp>
-        <v>43272.775248356484</v>
+        <v>43275.50424545139</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3809,7 +3809,7 @@
         <tr r="O16" s="1"/>
       </tp>
       <tp>
-        <v>52379445</v>
+        <v>53033961</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3817,7 +3817,7 @@
         <tr r="N16" s="1"/>
       </tp>
       <tp>
-        <v>15867645</v>
+        <v>15993950</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -3825,7 +3825,7 @@
         <tr r="N19" s="1"/>
       </tp>
       <tp>
-        <v>21966660</v>
+        <v>22077467</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3842,7 +3842,7 @@
         <tr r="R4" s="1"/>
       </tp>
       <tp>
-        <v>18182467</v>
+        <v>18281697</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3850,7 +3850,7 @@
         <tr r="H20" s="1"/>
       </tp>
       <tp>
-        <v>30232542</v>
+        <v>30373882</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3858,7 +3858,16 @@
         <tr r="N21" s="1"/>
       </tp>
       <tp>
-        <v>524.75</v>
+        <v>425.23</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>ethusdt</stp>
+        <stp>CLOSE</stp>
+        <stp>0</stp>
+        <tr r="E36" s="1"/>
+      </tp>
+      <tp>
+        <v>425.23</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3866,15 +3875,6 @@
         <stp>5</stp>
         <tr r="E30" s="1"/>
       </tp>
-      <tp>
-        <v>524.75</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>ethusdt</stp>
-        <stp>CLOSE</stp>
-        <stp>7</stp>
-        <tr r="E36" s="1"/>
-      </tp>
       <tp t="b">
         <v>1</v>
         <stp/>
@@ -3884,7 +3884,7 @@
         <tr r="L20" s="1"/>
       </tp>
       <tp>
-        <v>0.68</v>
+        <v>4.83</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -3892,16 +3892,16 @@
         <tr r="J19" s="1"/>
       </tp>
       <tp>
-        <v>6711.48</v>
+        <v>5816</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>CLOSE</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="E37" s="1"/>
       </tp>
       <tp>
-        <v>6711.48</v>
+        <v>5816</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3918,13 +3918,13 @@
         <tr r="K19" s="1"/>
       </tp>
       <tp>
-        <v>43272.775239756942</v>
+        <v>43275.50423042824</v>
         <stp/>
         <stp>CLOCK</stp>
         <tr r="N1" s="1"/>
       </tp>
       <tp>
-        <v>28994374</v>
+        <v>29343577</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3932,16 +3932,7 @@
         <tr r="N15" s="1"/>
       </tp>
       <tp>
-        <v>23202516</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>trxbtc</stp>
-        <stp>TAKE_BUY_VOL</stp>
-        <stp>7</stp>
-        <tr r="K38" s="1"/>
-      </tp>
-      <tp>
-        <v>4363991</v>
+        <v>9096658</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3950,7 +3941,16 @@
         <tr r="K32" s="1"/>
       </tp>
       <tp>
-        <v>6.3270000000000007E-2</v>
+        <v>5358</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>trxbtc</stp>
+        <stp>TAKE_BUY_VOL</stp>
+        <stp>0</stp>
+        <tr r="K38" s="1"/>
+      </tp>
+      <tp>
+        <v>13</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3959,7 +3959,7 @@
         <tr r="A23" s="1"/>
       </tp>
       <tp>
-        <v>0.2</v>
+        <v>0.20258200000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3968,7 +3968,7 @@
         <tr r="A24" s="1"/>
       </tp>
       <tp>
-        <v>0.6</v>
+        <v>0.49871599999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3977,7 +3977,7 @@
         <tr r="A19" s="1"/>
       </tp>
       <tp>
-        <v>1</v>
+        <v>5.982418</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3986,7 +3986,7 @@
         <tr r="A20" s="1"/>
       </tp>
       <tp>
-        <v>0.31148599999999999</v>
+        <v>1.002596</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3995,7 +3995,7 @@
         <tr r="A21" s="1"/>
       </tp>
       <tp>
-        <v>4.9556999999999997E-2</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -4004,7 +4004,7 @@
         <tr r="A22" s="1"/>
       </tp>
       <tp>
-        <v>0.521536</v>
+        <v>5.6798000000000001E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -4013,7 +4013,7 @@
         <tr r="A15" s="1"/>
       </tp>
       <tp>
-        <v>1.5252950000000001</v>
+        <v>0.25776500000000002</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -4022,7 +4022,7 @@
         <tr r="A16" s="1"/>
       </tp>
       <tp>
-        <v>5.0729249999999997</v>
+        <v>0.89890599999999998</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -4031,7 +4031,7 @@
         <tr r="A17" s="1"/>
       </tp>
       <tp>
-        <v>2.9E-5</v>
+        <v>0.49645899999999998</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -4040,7 +4040,7 @@
         <tr r="A18" s="1"/>
       </tp>
       <tp>
-        <v>4390.8098624599997</v>
+        <v>9930.5915274500003</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4048,7 +4048,7 @@
         <tr r="H4" s="2"/>
       </tp>
       <tp>
-        <v>53323.979076390002</v>
+        <v>112160.9920632</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4061,7 +4061,7 @@
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>FINAL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="H37" s="1"/>
       </tp>
       <tp t="b">
@@ -4074,7 +4074,7 @@
         <tr r="H31" s="1"/>
       </tp>
       <tp>
-        <v>1183574</v>
+        <v>1250089</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4090,7 +4090,7 @@
         <tr r="L21" s="1"/>
       </tp>
       <tp>
-        <v>46048483</v>
+        <v>46656230</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4098,7 +4098,7 @@
         <tr r="H16" s="1"/>
       </tp>
       <tp>
-        <v>7162878</v>
+        <v>7271417</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4106,7 +4106,7 @@
         <tr r="H17" s="1"/>
       </tp>
       <tp>
-        <v>25807361</v>
+        <v>26132724</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4114,7 +4114,7 @@
         <tr r="H15" s="1"/>
       </tp>
       <tp>
-        <v>18803800</v>
+        <v>18898921</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4127,20 +4127,20 @@
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
         <stp>FINAL</stp>
+        <stp>0</stp>
+        <tr r="H36" s="1"/>
+      </tp>
+      <tp t="b">
+        <v>0</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>ethusdt</stp>
+        <stp>FINAL</stp>
         <stp>5</stp>
         <tr r="H30" s="1"/>
       </tp>
-      <tp t="b">
-        <v>0</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>ethusdt</stp>
-        <stp>FINAL</stp>
-        <stp>7</stp>
-        <tr r="H36" s="1"/>
-      </tp>
-      <tp>
-        <v>8108510</v>
+      <tp>
+        <v>8225958</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4148,7 +4148,7 @@
         <tr r="N17" s="1"/>
       </tp>
       <tp>
-        <v>15867644</v>
+        <v>15993950</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4156,7 +4156,7 @@
         <tr r="M19" s="1"/>
       </tp>
       <tp>
-        <v>31580</v>
+        <v>39937</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4164,7 +4164,7 @@
         <tr r="N10" s="1"/>
       </tp>
       <tp>
-        <v>521.11</v>
+        <v>419.53</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4172,7 +4172,7 @@
         <tr r="B5" s="1"/>
       </tp>
       <tp>
-        <v>-5.9300000000000004E-3</v>
+        <v>-3.8030000000000001E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4180,7 +4180,7 @@
         <tr r="P8" s="1"/>
       </tp>
       <tp>
-        <v>-1.9699999999999999E-4</v>
+        <v>-4.0499999999999998E-4</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -4188,16 +4188,16 @@
         <tr r="P9" s="1"/>
       </tp>
       <tp>
-        <v>4679.08205</v>
+        <v>40.533670000000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
         <stp>VOL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="J36" s="1"/>
       </tp>
       <tp>
-        <v>561.30701999999997</v>
+        <v>2806.54324</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4206,7 +4206,7 @@
         <tr r="J30" s="1"/>
       </tp>
       <tp>
-        <v>-8.25</v>
+        <v>-45.5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4214,7 +4214,7 @@
         <tr r="P5" s="1"/>
       </tp>
       <tp>
-        <v>-0.99</v>
+        <v>-8.32</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4222,7 +4222,7 @@
         <tr r="P7" s="1"/>
       </tp>
       <tp>
-        <v>-0.03</v>
+        <v>-304.39</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4230,7 +4230,7 @@
         <tr r="P6" s="1"/>
       </tp>
       <tp>
-        <v>96.3</v>
+        <v>74.2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4238,7 +4238,7 @@
         <tr r="J7" s="1"/>
       </tp>
       <tp>
-        <v>6672.57</v>
+        <v>5750</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4246,7 +4246,7 @@
         <tr r="B6" s="1"/>
       </tp>
       <tp>
-        <v>96.2</v>
+        <v>74.09</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4254,7 +4254,7 @@
         <tr r="H7" s="1"/>
       </tp>
       <tp>
-        <v>30331461.5</v>
+        <v>37511258.960000001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4262,7 +4262,7 @@
         <tr r="L8" s="1"/>
       </tp>
       <tp>
-        <v>-9.2499999999999995E-3</v>
+        <v>-3.0079999999999999E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4270,7 +4270,7 @@
         <tr r="O10" s="1"/>
       </tp>
       <tp>
-        <v>0.53173999999999999</v>
+        <v>0.44619999999999999</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4278,7 +4278,7 @@
         <tr r="I18" s="1"/>
       </tp>
       <tp>
-        <v>0.54900000000000004</v>
+        <v>0.51</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4286,16 +4286,16 @@
         <tr r="C8" s="1"/>
       </tp>
       <tp>
-        <v>43272.77524722222</v>
+        <v>43275.504224583332</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>Event_Time</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="O37" s="1"/>
       </tp>
       <tp>
-        <v>43272.775247256941</v>
+        <v>43275.504224571756</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4304,16 +4304,16 @@
         <tr r="O31" s="1"/>
       </tp>
       <tp>
-        <v>43272.775247141202</v>
+        <v>43275.504226874997</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
         <stp>Event_Time</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="O36" s="1"/>
       </tp>
       <tp>
-        <v>43272.775247141202</v>
+        <v>43275.504226874997</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4322,7 +4322,7 @@
         <tr r="O30" s="1"/>
       </tp>
       <tp>
-        <v>54195</v>
+        <v>50410</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4330,7 +4330,7 @@
         <tr r="N11" s="1"/>
       </tp>
       <tp>
-        <v>96</v>
+        <v>73.22</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4338,7 +4338,7 @@
         <tr r="B7" s="1"/>
       </tp>
       <tp>
-        <v>468.25885399999999</v>
+        <v>429.42262799999997</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4347,16 +4347,16 @@
         <tr r="J31" s="1"/>
       </tp>
       <tp>
-        <v>2333.8420609999998</v>
+        <v>12.166264999999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>VOL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="J37" s="1"/>
       </tp>
       <tp>
-        <v>6710.94</v>
+        <v>5813.26</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4364,7 +4364,7 @@
         <tr r="H6" s="1"/>
       </tp>
       <tp>
-        <v>5.8669999999999998E-3</v>
+        <v>5.5659999999999998E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -4372,16 +4372,7 @@
         <tr r="C9" s="1"/>
       </tp>
       <tp>
-        <v>41483246</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>trxbtc</stp>
-        <stp>VOL</stp>
-        <stp>7</stp>
-        <tr r="J38" s="1"/>
-      </tp>
-      <tp>
-        <v>7639550</v>
+        <v>10901760</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4390,7 +4381,16 @@
         <tr r="J32" s="1"/>
       </tp>
       <tp>
-        <v>6711.48</v>
+        <v>5372</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>trxbtc</stp>
+        <stp>VOL</stp>
+        <stp>0</stp>
+        <tr r="J38" s="1"/>
+      </tp>
+      <tp>
+        <v>5816</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4398,7 +4398,7 @@
         <tr r="J6" s="1"/>
       </tp>
       <tp>
-        <v>524.75</v>
+        <v>425.62</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4406,7 +4406,7 @@
         <tr r="J5" s="1"/>
       </tp>
       <tp>
-        <v>6795</v>
+        <v>6260</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4414,7 +4414,7 @@
         <tr r="C6" s="1"/>
       </tp>
       <tp>
-        <v>99.3</v>
+        <v>84.67</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4422,7 +4422,7 @@
         <tr r="C7" s="1"/>
       </tp>
       <tp>
-        <v>544.98</v>
+        <v>481</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4439,12 +4439,12 @@
         <tr r="M31" s="1"/>
       </tp>
       <tp t="s">
-        <v>FourHour</v>
+        <v>OneMinute</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>INTERVAL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="M37" s="1"/>
       </tp>
       <tp t="s">
@@ -4457,16 +4457,16 @@
         <tr r="M30" s="1"/>
       </tp>
       <tp t="s">
-        <v>FourHour</v>
+        <v>OneMinute</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
         <stp>INTERVAL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="M36" s="1"/>
       </tp>
       <tp>
-        <v>-1.37E-2</v>
+        <v>-7.5840000000000005E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4474,7 +4474,7 @@
         <tr r="O11" s="1"/>
       </tp>
       <tp>
-        <v>524.4</v>
+        <v>425.49</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4482,16 +4482,16 @@
         <tr r="H5" s="1"/>
       </tp>
       <tp>
-        <v>52366074</v>
+        <v>53033925</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>FIRST_ID</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="P37" s="1"/>
       </tp>
       <tp>
-        <v>52376405</v>
+        <v>53031427</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4500,16 +4500,16 @@
         <tr r="P31" s="1"/>
       </tp>
       <tp>
-        <v>28987960</v>
+        <v>29343556</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
         <stp>FIRST_ID</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="P36" s="1"/>
       </tp>
       <tp>
-        <v>28993094</v>
+        <v>29341939</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4518,7 +4518,7 @@
         <tr r="P30" s="1"/>
       </tp>
       <tp>
-        <v>0.53227000000000002</v>
+        <v>0.44619999999999999</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4526,16 +4526,7 @@
         <tr r="J8" s="1"/>
       </tp>
       <tp>
-        <v>43272.83333332176</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>ethusdt</stp>
-        <stp>CLOSE_TIME</stp>
-        <stp>7</stp>
-        <tr r="G36" s="1"/>
-      </tp>
-      <tp>
-        <v>43272.791666655095</v>
+        <v>43275.541666655095</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4544,16 +4535,16 @@
         <tr r="G30" s="1"/>
       </tp>
       <tp>
-        <v>43272.83333332176</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>btcusdt</stp>
+        <v>43275.504861099536</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>ethusdt</stp>
         <stp>CLOSE_TIME</stp>
-        <stp>7</stp>
-        <tr r="G37" s="1"/>
-      </tp>
-      <tp>
-        <v>43272.791666655095</v>
+        <stp>0</stp>
+        <tr r="G36" s="1"/>
+      </tp>
+      <tp>
+        <v>43275.541666655095</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4562,7 +4553,16 @@
         <tr r="G31" s="1"/>
       </tp>
       <tp>
-        <v>7.4800000000000004E-6</v>
+        <v>43275.504861099536</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>btcusdt</stp>
+        <stp>CLOSE_TIME</stp>
+        <stp>0</stp>
+        <tr r="G37" s="1"/>
+      </tp>
+      <tp>
+        <v>7.2400000000000001E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4570,7 +4570,7 @@
         <tr r="C11" s="1"/>
       </tp>
       <tp>
-        <v>136926.61968999999</v>
+        <v>201061.72119000001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4578,7 +4578,7 @@
         <tr r="L7" s="1"/>
       </tp>
       <tp>
-        <v>0.53173000000000004</v>
+        <v>0.44540999999999997</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4586,7 +4586,7 @@
         <tr r="H8" s="1"/>
       </tp>
       <tp>
-        <v>7.1799999999999999E-6</v>
+        <v>6.5400000000000001E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4595,12 +4595,12 @@
         <tr r="D32" s="1"/>
       </tp>
       <tp>
-        <v>7.1199999999999996E-6</v>
+        <v>6.5799999999999997E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>LOW</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="D38" s="1"/>
       </tp>
       <tp t="b">
@@ -4609,7 +4609,7 @@
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>FINAL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="H38" s="1"/>
       </tp>
       <tp t="b">
@@ -4622,16 +4622,7 @@
         <tr r="H32" s="1"/>
       </tp>
       <tp>
-        <v>6695.31</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>btcusdt</stp>
-        <stp>LOW</stp>
-        <stp>7</stp>
-        <tr r="D37" s="1"/>
-      </tp>
-      <tp>
-        <v>6695.31</v>
+        <v>5750</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4640,7 +4631,16 @@
         <tr r="D31" s="1"/>
       </tp>
       <tp>
-        <v>-7.4000000000000001E-7</v>
+        <v>5812</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>btcusdt</stp>
+        <stp>LOW</stp>
+        <stp>0</stp>
+        <tr r="D37" s="1"/>
+      </tp>
+      <tp>
+        <v>-2.3800000000000001E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4648,7 +4648,7 @@
         <tr r="P10" s="1"/>
       </tp>
       <tp>
-        <v>6711.58</v>
+        <v>5819.24</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4656,7 +4656,7 @@
         <tr r="I16" s="1"/>
       </tp>
       <tp>
-        <v>96.3</v>
+        <v>74.2</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4664,7 +4664,7 @@
         <tr r="I17" s="1"/>
       </tp>
       <tp>
-        <v>-3.4110000000000001E-2</v>
+        <v>-7.4740000000000001E-2</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -4672,7 +4672,7 @@
         <tr r="O9" s="1"/>
       </tp>
       <tp>
-        <v>-9.9999999999999995E-8</v>
+        <v>-5.4000000000000002E-7</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4680,7 +4680,16 @@
         <tr r="P11" s="1"/>
       </tp>
       <tp>
-        <v>524.02</v>
+        <v>425.23</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>ethusdt</stp>
+        <stp>LOW</stp>
+        <stp>0</stp>
+        <tr r="D36" s="1"/>
+      </tp>
+      <tp>
+        <v>420.52</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4689,16 +4698,7 @@
         <tr r="D30" s="1"/>
       </tp>
       <tp>
-        <v>523.20000000000005</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>ethusdt</stp>
-        <stp>LOW</stp>
-        <stp>7</stp>
-        <tr r="D36" s="1"/>
-      </tp>
-      <tp>
-        <v>81627.515069999994</v>
+        <v>145641.74358000001</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4706,7 +4706,7 @@
         <tr r="L5" s="1"/>
       </tp>
       <tp>
-        <v>25581.509341000001</v>
+        <v>38566.177426000002</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4714,7 +4714,7 @@
         <tr r="L6" s="1"/>
       </tp>
       <tp>
-        <v>0.52898999999999996</v>
+        <v>0.43724000000000002</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4722,7 +4722,7 @@
         <tr r="B8" s="1"/>
       </tp>
       <tp>
-        <v>8.0909999999999996E-5</v>
+        <v>8.0129999999999993E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4730,16 +4730,16 @@
         <tr r="C10" s="1"/>
       </tp>
       <tp>
-        <v>7.1999999999999997E-6</v>
+        <v>6.5899999999999996E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>CLOSE</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="E38" s="1"/>
       </tp>
       <tp>
-        <v>7.1999999999999997E-6</v>
+        <v>6.5899999999999996E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4748,7 +4748,16 @@
         <tr r="E32" s="1"/>
       </tp>
       <tp>
-        <v>1714131.17581939</v>
+        <v>21885.311260030001</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>btcusdt</stp>
+        <stp>TAKE_BUY_QUOTE_VOL</stp>
+        <stp>0</stp>
+        <tr r="L37" s="1"/>
+      </tp>
+      <tp>
+        <v>1331989.6847904101</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4757,16 +4766,16 @@
         <tr r="L31" s="1"/>
       </tp>
       <tp>
-        <v>9121321.0814994201</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>btcusdt</stp>
+        <v>17119.1973579</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>ethusdt</stp>
         <stp>TAKE_BUY_QUOTE_VOL</stp>
-        <stp>7</stp>
-        <tr r="L37" s="1"/>
-      </tp>
-      <tp>
-        <v>173148.7662027</v>
+        <stp>0</stp>
+        <tr r="L36" s="1"/>
+      </tp>
+      <tp>
+        <v>693184.39220050001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4775,16 +4784,7 @@
         <tr r="L30" s="1"/>
       </tp>
       <tp>
-        <v>1024821.046414</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>ethusdt</stp>
-        <stp>TAKE_BUY_QUOTE_VOL</stp>
-        <stp>7</stp>
-        <tr r="L36" s="1"/>
-      </tp>
-      <tp>
-        <v>37124</v>
+        <v>46916</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -4792,7 +4792,7 @@
         <tr r="N9" s="1"/>
       </tp>
       <tp>
-        <v>524.75</v>
+        <v>425.5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4800,16 +4800,16 @@
         <tr r="I15" s="1"/>
       </tp>
       <tp>
-        <v>43272.666666666664</v>
+        <v>43275.504166666666</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
         <stp>OPEN_TIME</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="F36" s="1"/>
       </tp>
       <tp>
-        <v>43272.75</v>
+        <v>43275.5</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4826,7 +4826,7 @@
         <tr r="I10" s="1"/>
       </tp>
       <tp>
-        <v>97.3</v>
+        <v>82.09</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4834,7 +4834,7 @@
         <tr r="E7" s="1"/>
       </tp>
       <tp>
-        <v>6716.88</v>
+        <v>6106.92</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4842,7 +4842,7 @@
         <tr r="E6" s="1"/>
       </tp>
       <tp>
-        <v>43272.775196666669</v>
+        <v>43275.504218483795</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4850,7 +4850,7 @@
         <tr r="O19" s="1"/>
       </tp>
       <tp>
-        <v>5.7759999999999999E-3</v>
+        <v>5.4019999999999997E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4858,7 +4858,7 @@
         <tr r="F9" s="1"/>
       </tp>
       <tp>
-        <v>533</v>
+        <v>468.4</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4866,7 +4866,7 @@
         <tr r="F5" s="1"/>
       </tp>
       <tp>
-        <v>6716.89</v>
+        <v>6106.91</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4874,7 +4874,7 @@
         <tr r="F6" s="1"/>
       </tp>
       <tp>
-        <v>97.34</v>
+        <v>82.1</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4906,7 +4906,7 @@
         <tr r="K15" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4914,7 +4914,7 @@
         <tr r="K18" s="1"/>
       </tp>
       <tp>
-        <v>544.23</v>
+        <v>481.74</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4922,7 +4922,7 @@
         <tr r="F3" s="2"/>
       </tp>
       <tp>
-        <v>6787</v>
+        <v>6250</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4930,7 +4930,7 @@
         <tr r="F4" s="2"/>
       </tp>
       <tp>
-        <v>0.53739999999999999</v>
+        <v>0.48248999999999997</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4938,7 +4938,16 @@
         <tr r="F8" s="1"/>
       </tp>
       <tp>
-        <v>43272.75</v>
+        <v>43275.504166666666</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>btcusdt</stp>
+        <stp>OPEN_TIME</stp>
+        <stp>0</stp>
+        <tr r="F37" s="1"/>
+      </tp>
+      <tp>
+        <v>43275.5</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4947,16 +4956,7 @@
         <tr r="F31" s="1"/>
       </tp>
       <tp>
-        <v>43272.666666666664</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>btcusdt</stp>
-        <stp>OPEN_TIME</stp>
-        <stp>7</stp>
-        <tr r="F37" s="1"/>
-      </tp>
-      <tp>
-        <v>533</v>
+        <v>468.03</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4972,7 +4972,7 @@
         <tr r="I11" s="1"/>
       </tp>
       <tp>
-        <v>5.77E-3</v>
+        <v>5.4019999999999997E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4980,12 +4980,12 @@
         <tr r="E9" s="1"/>
       </tp>
       <tp t="s">
-        <v>FourHour</v>
+        <v>OneMinute</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>INTERVAL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="M38" s="1"/>
       </tp>
       <tp t="s">
@@ -4998,7 +4998,7 @@
         <tr r="M32" s="1"/>
       </tp>
       <tp>
-        <v>3139880.2264629598</v>
+        <v>2484420.3918971098</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -5007,25 +5007,16 @@
         <tr r="I31" s="1"/>
       </tp>
       <tp>
-        <v>15666748.907512249</v>
+        <v>70730.094461560002</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
         <stp>QUOTE_VOL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="I37" s="1"/>
       </tp>
       <tp>
-        <v>2459763.8007513001</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>ethusdt</stp>
-        <stp>QUOTE_VOL</stp>
-        <stp>7</stp>
-        <tr r="I36" s="1"/>
-      </tp>
-      <tp>
-        <v>294590.46438630001</v>
+        <v>1190024.8954306</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -5034,7 +5025,16 @@
         <tr r="I30" s="1"/>
       </tp>
       <tp>
-        <v>524.37</v>
+        <v>17245.418378800001</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>ethusdt</stp>
+        <stp>QUOTE_VOL</stp>
+        <stp>0</stp>
+        <tr r="I36" s="1"/>
+      </tp>
+      <tp>
+        <v>425</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -5042,7 +5042,7 @@
         <tr r="D3" s="2"/>
       </tp>
       <tp>
-        <v>6710.7</v>
+        <v>5832</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -5050,7 +5050,7 @@
         <tr r="D4" s="2"/>
       </tp>
       <tp>
-        <v>5.5789999999999998E-3</v>
+        <v>5.0140000000000002E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -5058,16 +5058,7 @@
         <tr r="I19" s="1"/>
       </tp>
       <tp>
-        <v>43272.774856863427</v>
-        <stp/>
-        <stp>BINANCE_CANDLE</stp>
-        <stp>trxbtc</stp>
-        <stp>Event_Time</stp>
-        <stp>7</stp>
-        <tr r="O38" s="1"/>
-      </tp>
-      <tp>
-        <v>43272.774856863427</v>
+        <v>43275.504239236114</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5076,7 +5067,16 @@
         <tr r="O32" s="1"/>
       </tp>
       <tp>
-        <v>16326777.37042</v>
+        <v>43275.504239236114</v>
+        <stp/>
+        <stp>BINANCE_CANDLE</stp>
+        <stp>trxbtc</stp>
+        <stp>Event_Time</stp>
+        <stp>0</stp>
+        <tr r="O38" s="1"/>
+      </tp>
+      <tp>
+        <v>17468589.970353</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -5100,7 +5100,7 @@
         <tr r="D11" s="1"/>
       </tp>
       <tp>
-        <v>0.53766000000000003</v>
+        <v>0.4829</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -5108,16 +5108,16 @@
         <tr r="E8" s="1"/>
       </tp>
       <tp>
-        <v>43272.83333332176</v>
+        <v>43275.504861099536</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>CLOSE_TIME</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="G38" s="1"/>
       </tp>
       <tp>
-        <v>43272.791666655095</v>
+        <v>43275.541666655095</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5126,7 +5126,7 @@
         <tr r="G32" s="1"/>
       </tp>
       <tp>
-        <v>30231876</v>
+        <v>30373311</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5135,16 +5135,16 @@
         <tr r="P32" s="1"/>
       </tp>
       <tp>
-        <v>30228071</v>
+        <v>30373879</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>FIRST_ID</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="P38" s="1"/>
       </tp>
       <tp>
-        <v>8.0030000000000005E-5</v>
+        <v>7.9040000000000002E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -5152,7 +5152,7 @@
         <tr r="F10" s="1"/>
       </tp>
       <tp>
-        <v>43272.774856863427</v>
+        <v>43275.504239259259</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -5160,7 +5160,7 @@
         <tr r="O21" s="1"/>
       </tp>
       <tp>
-        <v>43546324.6828418</v>
+        <v>65249326.970757201</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -5176,7 +5176,7 @@
         <tr r="D9" s="1"/>
       </tp>
       <tp>
-        <v>31.460917139999999</v>
+        <v>59.702030530000002</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5185,16 +5185,16 @@
         <tr r="L32" s="1"/>
       </tp>
       <tp>
-        <v>167.13227093</v>
+        <v>3.5279850000000001E-2</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
         <stp>TAKE_BUY_QUOTE_VOL</stp>
-        <stp>7</stp>
+        <stp>0</stp>
         <tr r="L38" s="1"/>
       </tp>
       <tp>
-        <v>7.1999999999999997E-6</v>
+        <v>6.5899999999999996E-6</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -5202,7 +5202,7 @@
         <tr r="I21" s="1"/>
       </tp>
       <tp>
-        <v>7.9220000000000004E-5</v>
+        <v>7.6730000000000006E-5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -5210,7 +5210,7 @@
         <tr r="I20" s="1"/>
       </tp>
       <tp>
-        <v>7.3100000000000003E-6</v>
+        <v>7.0999999999999998E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -5218,7 +5218,7 @@
         <tr r="F11" s="1"/>
       </tp>
       <tp>
-        <v>172194484.02763015</v>
+        <v>229696728.22816449</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -5226,7 +5226,7 @@
         <tr r="M6" s="1"/>
       </tp>
       <tp>
-        <v>13304802.9063682</v>
+        <v>15833956.9253697</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -5234,7 +5234,7 @@
         <tr r="M7" s="1"/>
       </tp>
       <tp>
-        <v>7.3000000000000004E-6</v>
+        <v>7.0899999999999999E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -5242,7 +5242,7 @@
         <tr r="E11" s="1"/>
       </tp>
       <tp>
-        <v>8.0030000000000005E-5</v>
+        <v>7.9019999999999999E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -5250,7 +5250,7 @@
         <tr r="E10" s="1"/>
       </tp>
       <tp>
-        <v>6708.66</v>
+        <v>5812.93</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5259,7 +5259,7 @@
         <tr r="B19" s="1"/>
       </tp>
       <tp>
-        <v>6707.92</v>
+        <v>5812</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5268,7 +5268,7 @@
         <tr r="B20" s="1"/>
       </tp>
       <tp>
-        <v>6707.83</v>
+        <v>5810</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5277,7 +5277,7 @@
         <tr r="B21" s="1"/>
       </tp>
       <tp>
-        <v>6707.79</v>
+        <v>5809.59</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5286,7 +5286,7 @@
         <tr r="B22" s="1"/>
       </tp>
       <tp>
-        <v>6710.94</v>
+        <v>5813.26</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5295,7 +5295,7 @@
         <tr r="B15" s="1"/>
       </tp>
       <tp>
-        <v>6709.83</v>
+        <v>5813.24</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5304,7 +5304,7 @@
         <tr r="B16" s="1"/>
       </tp>
       <tp>
-        <v>6709.82</v>
+        <v>5813.18</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5313,7 +5313,7 @@
         <tr r="B17" s="1"/>
       </tp>
       <tp>
-        <v>6708.69</v>
+        <v>5813.17</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5322,7 +5322,7 @@
         <tr r="B18" s="1"/>
       </tp>
       <tp>
-        <v>6706.96</v>
+        <v>5809.5</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5331,7 +5331,7 @@
         <tr r="B23" s="1"/>
       </tp>
       <tp>
-        <v>6706.52</v>
+        <v>5808.47</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5340,7 +5340,7 @@
         <tr r="B24" s="1"/>
       </tp>
       <tp>
-        <v>532.67999999999995</v>
+        <v>472.93</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -5348,7 +5348,7 @@
         <tr r="E3" s="2"/>
       </tp>
       <tp>
-        <v>6711.55</v>
+        <v>6134</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -5356,7 +5356,7 @@
         <tr r="E4" s="2"/>
       </tp>
       <tp>
-        <v>43272.775216319445</v>
+        <v>43275.504244618052</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -5372,7 +5372,7 @@
         <tr r="L18" s="1"/>
       </tp>
       <tp>
-        <v>6717.83</v>
+        <v>5822.66</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5381,7 +5381,7 @@
         <tr r="D24" s="1"/>
       </tp>
       <tp>
-        <v>6717.55</v>
+        <v>5822.64</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5390,7 +5390,7 @@
         <tr r="D23" s="1"/>
       </tp>
       <tp>
-        <v>6711.69</v>
+        <v>5819.74</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5399,7 +5399,7 @@
         <tr r="D18" s="1"/>
       </tp>
       <tp>
-        <v>6711.64</v>
+        <v>5819.26</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5408,7 +5408,7 @@
         <tr r="D17" s="1"/>
       </tp>
       <tp>
-        <v>6711.58</v>
+        <v>5819.25</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5417,7 +5417,7 @@
         <tr r="D16" s="1"/>
       </tp>
       <tp>
-        <v>6711.48</v>
+        <v>5816</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5426,7 +5426,7 @@
         <tr r="D15" s="1"/>
       </tp>
       <tp>
-        <v>6717.54</v>
+        <v>5821.22</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5435,7 +5435,7 @@
         <tr r="D22" s="1"/>
       </tp>
       <tp>
-        <v>6716.09</v>
+        <v>5820.91</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5444,7 +5444,7 @@
         <tr r="D21" s="1"/>
       </tp>
       <tp>
-        <v>6713.37</v>
+        <v>5820.73</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5453,7 +5453,7 @@
         <tr r="D20" s="1"/>
       </tp>
       <tp>
-        <v>6712.97</v>
+        <v>5820</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5486,7 +5486,7 @@
         <tr r="L15" s="1"/>
       </tp>
       <tp>
-        <v>6.9999999999999999E-6</v>
+        <v>5.0000000000000004E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -6056,8 +6056,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6101,7 +6101,7 @@
       </c>
       <c r="N1" s="38">
         <f>RTD(progId,,"CLOCK")</f>
-        <v>43272.775239756942</v>
+        <v>43275.50423042824</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -6192,11 +6192,11 @@
       </c>
       <c r="B5" s="2">
         <f>RTD(progId,,BINANCE,$A5,B$4)</f>
-        <v>521.11</v>
+        <v>419.53</v>
       </c>
       <c r="C5" s="2">
         <f>RTD(progId,,BINANCE,$A5,C$4)</f>
-        <v>544.98</v>
+        <v>481</v>
       </c>
       <c r="D5" s="2" t="str">
         <f>RTD(progId,,BINANCE,$A5,D$4)</f>
@@ -6204,51 +6204,51 @@
       </c>
       <c r="E5" s="2">
         <f>RTD(progId,,BINANCE_24H,$A5,E$4)</f>
-        <v>533</v>
+        <v>468.03</v>
       </c>
       <c r="F5" s="2">
         <f>RTD(progId,,BINANCE_24H,$A5,F$4)</f>
-        <v>533</v>
+        <v>468.4</v>
       </c>
       <c r="G5" s="2">
         <f>RTD(progId,,BINANCE,$A5,G$4)</f>
-        <v>15</v>
+        <v>1.0781799999999999</v>
       </c>
       <c r="H5" s="2">
         <f>RTD(progId,,BINANCE,$A5,H$4)</f>
-        <v>524.4</v>
+        <v>425.49</v>
       </c>
       <c r="I5" s="2">
         <f>RTD(progId,,BINANCE,$A5,I$4)</f>
-        <v>0.35</v>
+        <v>0.13</v>
       </c>
       <c r="J5" s="2">
         <f>RTD(progId,,BINANCE,$A5,J$4)</f>
-        <v>524.75</v>
+        <v>425.62</v>
       </c>
       <c r="K5" s="2">
         <f>RTD(progId,,BINANCE,$A5,K$4)</f>
-        <v>3.0778400000000001</v>
+        <v>0.23496</v>
       </c>
       <c r="L5" s="9">
         <f>RTD(progId,,BINANCE,$A5,L$4)</f>
-        <v>81627.515069999994</v>
+        <v>145641.74358000001</v>
       </c>
       <c r="M5" s="39">
         <f>RTD(progId,,BINANCE,$A5,M$4)</f>
-        <v>43546324.6828418</v>
+        <v>65249326.970757201</v>
       </c>
       <c r="N5" s="9">
         <f>RTD(progId,,BINANCE,$A5,N$4)</f>
-        <v>77719</v>
+        <v>113925</v>
       </c>
       <c r="O5" s="10">
         <f>RTD(progId,,BINANCE,$A5,O$4)</f>
-        <v>-1.549E-2</v>
+        <v>-9.6600000000000005E-2</v>
       </c>
       <c r="P5" s="2">
         <f>RTD(progId,,BINANCE,$A5,P$4)</f>
-        <v>-8.25</v>
+        <v>-45.5</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -6257,11 +6257,11 @@
       </c>
       <c r="B6" s="2">
         <f>RTD(progId,,BINANCE,$A6,B$4)</f>
-        <v>6672.57</v>
+        <v>5750</v>
       </c>
       <c r="C6" s="2">
         <f>RTD(progId,,BINANCE,$A6,C$4)</f>
-        <v>6795</v>
+        <v>6260</v>
       </c>
       <c r="D6" s="2" t="str">
         <f>RTD(progId,,BINANCE,$A6,D$4)</f>
@@ -6269,51 +6269,51 @@
       </c>
       <c r="E6" s="2">
         <f>RTD(progId,,BINANCE_24H,$A6,E$4)</f>
-        <v>6716.88</v>
+        <v>6106.92</v>
       </c>
       <c r="F6" s="2">
         <f>RTD(progId,,BINANCE_24H,$A6,F$4)</f>
-        <v>6716.89</v>
+        <v>6106.91</v>
       </c>
       <c r="G6" s="2">
         <f>RTD(progId,,BINANCE,$A6,G$4)</f>
-        <v>0.521536</v>
+        <v>5.6798000000000001E-2</v>
       </c>
       <c r="H6" s="2">
         <f>RTD(progId,,BINANCE,$A6,H$4)</f>
-        <v>6710.94</v>
+        <v>5813.26</v>
       </c>
       <c r="I6" s="2">
         <f>RTD(progId,,BINANCE,$A6,I$4)</f>
-        <v>0.54</v>
+        <v>2.74</v>
       </c>
       <c r="J6" s="2">
         <f>RTD(progId,,BINANCE,$A6,J$4)</f>
-        <v>6711.48</v>
+        <v>5816</v>
       </c>
       <c r="K6" s="2">
         <f>RTD(progId,,BINANCE,$A6,K$4)</f>
-        <v>9.9999999999999995E-7</v>
+        <v>6.4300000000000002E-4</v>
       </c>
       <c r="L6" s="9">
         <f>RTD(progId,,BINANCE,$A6,L$4)</f>
-        <v>25581.509341000001</v>
+        <v>38566.177426000002</v>
       </c>
       <c r="M6" s="39">
         <f>RTD(progId,,BINANCE,$A6,M$4)</f>
-        <v>172194484.02763015</v>
+        <v>229696728.22816449</v>
       </c>
       <c r="N6" s="9">
         <f>RTD(progId,,BINANCE,$A6,N$4)</f>
-        <v>159036</v>
+        <v>225376</v>
       </c>
       <c r="O6" s="10">
         <f>RTD(progId,,BINANCE,$A6,O$4)</f>
-        <v>0</v>
+        <v>-4.9759999999999999E-2</v>
       </c>
       <c r="P6" s="2">
         <f>RTD(progId,,BINANCE,$A6,P$4)</f>
-        <v>-0.03</v>
+        <v>-304.39</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -6322,11 +6322,11 @@
       </c>
       <c r="B7" s="2">
         <f>RTD(progId,,BINANCE,$A7,B$4)</f>
-        <v>96</v>
+        <v>73.22</v>
       </c>
       <c r="C7" s="2">
         <f>RTD(progId,,BINANCE,$A7,C$4)</f>
-        <v>99.3</v>
+        <v>84.67</v>
       </c>
       <c r="D7" s="2" t="str">
         <f>RTD(progId,,BINANCE,$A7,D$4)</f>
@@ -6334,51 +6334,51 @@
       </c>
       <c r="E7" s="2">
         <f>RTD(progId,,BINANCE_24H,$A7,E$4)</f>
-        <v>97.3</v>
+        <v>82.09</v>
       </c>
       <c r="F7" s="2">
         <f>RTD(progId,,BINANCE_24H,$A7,F$4)</f>
-        <v>97.34</v>
+        <v>82.1</v>
       </c>
       <c r="G7" s="2">
         <f>RTD(progId,,BINANCE,$A7,G$4)</f>
-        <v>1.8669999999999999E-2</v>
+        <v>0.26954</v>
       </c>
       <c r="H7" s="2">
         <f>RTD(progId,,BINANCE,$A7,H$4)</f>
-        <v>96.2</v>
+        <v>74.09</v>
       </c>
       <c r="I7" s="2">
         <f>RTD(progId,,BINANCE,$A7,I$4)</f>
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="J7" s="2">
         <f>RTD(progId,,BINANCE,$A7,J$4)</f>
-        <v>96.3</v>
+        <v>74.2</v>
       </c>
       <c r="K7" s="2">
         <f>RTD(progId,,BINANCE,$A7,K$4)</f>
-        <v>0.2</v>
+        <v>4.4000000000000002E-4</v>
       </c>
       <c r="L7" s="9">
         <f>RTD(progId,,BINANCE,$A7,L$4)</f>
-        <v>136926.61968999999</v>
+        <v>201061.72119000001</v>
       </c>
       <c r="M7" s="39">
         <f>RTD(progId,,BINANCE,$A7,M$4)</f>
-        <v>13304802.9063682</v>
+        <v>15833956.9253697</v>
       </c>
       <c r="N7" s="9">
         <f>RTD(progId,,BINANCE,$A7,N$4)</f>
-        <v>27095</v>
+        <v>42560</v>
       </c>
       <c r="O7" s="10">
         <f>RTD(progId,,BINANCE,$A7,O$4)</f>
-        <v>-1.018E-2</v>
+        <v>-0.10082000000000001</v>
       </c>
       <c r="P7" s="2">
         <f>RTD(progId,,BINANCE,$A7,P$4)</f>
-        <v>-0.99</v>
+        <v>-8.32</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -6387,11 +6387,11 @@
       </c>
       <c r="B8" s="2">
         <f>RTD(progId,,BINANCE,$A8,B$4)</f>
-        <v>0.52898999999999996</v>
+        <v>0.43724000000000002</v>
       </c>
       <c r="C8" s="2">
         <f>RTD(progId,,BINANCE,$A8,C$4)</f>
-        <v>0.54900000000000004</v>
+        <v>0.51</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>RTD(progId,,BINANCE,$A8,D$4)</f>
@@ -6399,51 +6399,51 @@
       </c>
       <c r="E8" s="2">
         <f>RTD(progId,,BINANCE_24H,$A8,E$4)</f>
-        <v>0.53766000000000003</v>
+        <v>0.4829</v>
       </c>
       <c r="F8" s="2">
         <f>RTD(progId,,BINANCE_24H,$A8,F$4)</f>
-        <v>0.53739999999999999</v>
+        <v>0.48248999999999997</v>
       </c>
       <c r="G8" s="9">
         <f>RTD(progId,,BINANCE,$A8,G$4)</f>
-        <v>0.9</v>
+        <v>4813.5</v>
       </c>
       <c r="H8" s="2">
         <f>RTD(progId,,BINANCE,$A8,H$4)</f>
-        <v>0.53173000000000004</v>
+        <v>0.44540999999999997</v>
       </c>
       <c r="I8" s="2">
         <f>RTD(progId,,BINANCE,$A8,I$4)</f>
-        <v>5.4000000000000001E-4</v>
+        <v>7.9000000000000001E-4</v>
       </c>
       <c r="J8" s="2">
         <f>RTD(progId,,BINANCE,$A8,J$4)</f>
-        <v>0.53227000000000002</v>
+        <v>0.44619999999999999</v>
       </c>
       <c r="K8" s="2">
         <f>RTD(progId,,BINANCE,$A8,K$4)</f>
-        <v>4136</v>
+        <v>92.7</v>
       </c>
       <c r="L8" s="9">
         <f>RTD(progId,,BINANCE,$A8,L$4)</f>
-        <v>30331461.5</v>
+        <v>37511258.960000001</v>
       </c>
       <c r="M8" s="39">
         <f>RTD(progId,,BINANCE,$A8,M$4)</f>
-        <v>16326777.37042</v>
+        <v>17468589.970353</v>
       </c>
       <c r="N8" s="9">
         <f>RTD(progId,,BINANCE,$A8,N$4)</f>
-        <v>19406</v>
+        <v>26429</v>
       </c>
       <c r="O8" s="10">
         <f>RTD(progId,,BINANCE,$A8,O$4)</f>
-        <v>-1.103E-2</v>
+        <v>-7.8670000000000004E-2</v>
       </c>
       <c r="P8" s="2">
         <f>RTD(progId,,BINANCE,$A8,P$4)</f>
-        <v>-5.9300000000000004E-3</v>
+        <v>-3.8030000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -6452,11 +6452,11 @@
       </c>
       <c r="B9" s="2">
         <f>RTD(progId,,BINANCE,$A9,B$4)</f>
-        <v>5.5500000000000002E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C9" s="2">
         <f>RTD(progId,,BINANCE,$A9,C$4)</f>
-        <v>5.8669999999999998E-3</v>
+        <v>5.5659999999999998E-3</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>RTD(progId,,BINANCE,$A9,D$4)</f>
@@ -6464,51 +6464,51 @@
       </c>
       <c r="E9" s="2">
         <f>RTD(progId,,BINANCE_24H,$A9,E$4)</f>
-        <v>5.77E-3</v>
+        <v>5.4019999999999997E-3</v>
       </c>
       <c r="F9" s="2">
         <f>RTD(progId,,BINANCE_24H,$A9,F$4)</f>
-        <v>5.7759999999999999E-3</v>
+        <v>5.4019999999999997E-3</v>
       </c>
       <c r="G9" s="9">
         <f>RTD(progId,,BINANCE,$A9,G$4)</f>
-        <v>5.04</v>
+        <v>2.09</v>
       </c>
       <c r="H9" s="2">
         <f>RTD(progId,,BINANCE,$A9,H$4)</f>
-        <v>5.5729999999999998E-3</v>
+        <v>5.0140000000000002E-3</v>
       </c>
       <c r="I9" s="2">
         <f>RTD(progId,,BINANCE,$A9,I$4)</f>
-        <v>6.9999999999999999E-6</v>
+        <v>5.0000000000000004E-6</v>
       </c>
       <c r="J9" s="2">
         <f>RTD(progId,,BINANCE,$A9,J$4)</f>
-        <v>5.5799999999999999E-3</v>
+        <v>5.019E-3</v>
       </c>
       <c r="K9" s="2">
         <f>RTD(progId,,BINANCE,$A9,K$4)</f>
-        <v>1.67</v>
+        <v>0.1</v>
       </c>
       <c r="L9" s="9">
         <f>RTD(progId,,BINANCE,$A9,L$4)</f>
-        <v>324853.88</v>
+        <v>416876.88</v>
       </c>
       <c r="M9" s="39">
         <f>RTD(progId,,BINANCE,$A9,M$4)</f>
-        <v>1848.5073156999999</v>
+        <v>2224.1238684599998</v>
       </c>
       <c r="N9" s="9">
         <f>RTD(progId,,BINANCE,$A9,N$4)</f>
-        <v>37124</v>
+        <v>46916</v>
       </c>
       <c r="O9" s="10">
         <f>RTD(progId,,BINANCE,$A9,O$4)</f>
-        <v>-3.4110000000000001E-2</v>
+        <v>-7.4740000000000001E-2</v>
       </c>
       <c r="P9" s="2">
         <f>RTD(progId,,BINANCE,$A9,P$4)</f>
-        <v>-1.9699999999999999E-4</v>
+        <v>-4.0499999999999998E-4</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -6522,11 +6522,11 @@
       </c>
       <c r="B10" s="2">
         <f>RTD(progId,,BINANCE,$A10,B$4)</f>
-        <v>7.9060000000000005E-5</v>
+        <v>7.6260000000000005E-5</v>
       </c>
       <c r="C10" s="2">
         <f>RTD(progId,,BINANCE,$A10,C$4)</f>
-        <v>8.0909999999999996E-5</v>
+        <v>8.0129999999999993E-5</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>RTD(progId,,BINANCE,$A10,D$4)</f>
@@ -6534,19 +6534,19 @@
       </c>
       <c r="E10" s="2">
         <f>RTD(progId,,BINANCE_24H,$A10,E$4)</f>
-        <v>8.0030000000000005E-5</v>
+        <v>7.9019999999999999E-5</v>
       </c>
       <c r="F10" s="2">
         <f>RTD(progId,,BINANCE_24H,$A10,F$4)</f>
-        <v>8.0030000000000005E-5</v>
+        <v>7.9040000000000002E-5</v>
       </c>
       <c r="G10" s="9">
         <f>RTD(progId,,BINANCE,$A10,G$4)</f>
-        <v>53686</v>
+        <v>1669</v>
       </c>
       <c r="H10" s="2">
         <f>RTD(progId,,BINANCE,$A10,H$4)</f>
-        <v>7.9200000000000001E-5</v>
+        <v>7.6730000000000006E-5</v>
       </c>
       <c r="I10" s="2">
         <f>RTD(progId,,BINANCE,$A10,I$4)</f>
@@ -6554,31 +6554,31 @@
       </c>
       <c r="J10" s="2">
         <f>RTD(progId,,BINANCE,$A10,J$4)</f>
-        <v>7.9209999999999995E-5</v>
+        <v>7.674E-5</v>
       </c>
       <c r="K10" s="2">
         <f>RTD(progId,,BINANCE,$A10,K$4)</f>
-        <v>11857</v>
+        <v>1756</v>
       </c>
       <c r="L10" s="9">
         <f>RTD(progId,,BINANCE,$A10,L$4)</f>
-        <v>32839604</v>
+        <v>40848135</v>
       </c>
       <c r="M10" s="39">
         <f>RTD(progId,,BINANCE,$A10,M$4)</f>
-        <v>2625.0613650700002</v>
+        <v>3201.9709302699998</v>
       </c>
       <c r="N10" s="9">
         <f>RTD(progId,,BINANCE,$A10,N$4)</f>
-        <v>31580</v>
+        <v>39937</v>
       </c>
       <c r="O10" s="10">
         <f>RTD(progId,,BINANCE,$A10,O$4)</f>
-        <v>-9.2499999999999995E-3</v>
+        <v>-3.0079999999999999E-2</v>
       </c>
       <c r="P10" s="2">
         <f>RTD(progId,,BINANCE,$A10,P$4)</f>
-        <v>-7.4000000000000001E-7</v>
+        <v>-2.3800000000000001E-6</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6587,11 +6587,11 @@
       </c>
       <c r="B11" s="2">
         <f>RTD(progId,,BINANCE,$A11,B$4)</f>
-        <v>7.0500000000000003E-6</v>
+        <v>6.4799999999999998E-6</v>
       </c>
       <c r="C11" s="2">
         <f>RTD(progId,,BINANCE,$A11,C$4)</f>
-        <v>7.4800000000000004E-6</v>
+        <v>7.2400000000000001E-6</v>
       </c>
       <c r="D11" s="2" t="str">
         <f>RTD(progId,,BINANCE,$A11,D$4)</f>
@@ -6599,19 +6599,19 @@
       </c>
       <c r="E11" s="2">
         <f>RTD(progId,,BINANCE_24H,$A11,E$4)</f>
-        <v>7.3000000000000004E-6</v>
+        <v>7.0899999999999999E-6</v>
       </c>
       <c r="F11" s="2">
         <f>RTD(progId,,BINANCE_24H,$A11,F$4)</f>
-        <v>7.3100000000000003E-6</v>
+        <v>7.0999999999999998E-6</v>
       </c>
       <c r="G11" s="9">
         <f>RTD(progId,,BINANCE,$A11,G$4)</f>
-        <v>229998</v>
+        <v>8917</v>
       </c>
       <c r="H11" s="2">
         <f>RTD(progId,,BINANCE,$A11,H$4)</f>
-        <v>7.1999999999999997E-6</v>
+        <v>6.5799999999999997E-6</v>
       </c>
       <c r="I11" s="2">
         <f>RTD(progId,,BINANCE,$A11,I$4)</f>
@@ -6619,31 +6619,31 @@
       </c>
       <c r="J11" s="2">
         <f>RTD(progId,,BINANCE,$A11,J$4)</f>
-        <v>7.2099999999999996E-6</v>
+        <v>6.5899999999999996E-6</v>
       </c>
       <c r="K11" s="2">
         <f>RTD(progId,,BINANCE,$A11,K$4)</f>
-        <v>15745</v>
+        <v>1062151</v>
       </c>
       <c r="L11" s="9">
         <f>RTD(progId,,BINANCE,$A11,L$4)</f>
-        <v>501624962</v>
+        <v>539412151</v>
       </c>
       <c r="M11" s="39">
         <f>RTD(progId,,BINANCE,$A11,M$4)</f>
-        <v>3643.0131911799999</v>
+        <v>3726.3932793899999</v>
       </c>
       <c r="N11" s="9">
         <f>RTD(progId,,BINANCE,$A11,N$4)</f>
-        <v>54195</v>
+        <v>50410</v>
       </c>
       <c r="O11" s="10">
         <f>RTD(progId,,BINANCE,$A11,O$4)</f>
-        <v>-1.37E-2</v>
+        <v>-7.5840000000000005E-2</v>
       </c>
       <c r="P11" s="2">
         <f>RTD(progId,,BINANCE,$A11,P$4)</f>
-        <v>-9.9999999999999995E-8</v>
+        <v>-5.4000000000000002E-7</v>
       </c>
     </row>
     <row r="12" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6730,22 +6730,22 @@
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C15)</f>
-        <v>0.521536</v>
+        <v>5.6798000000000001E-2</v>
       </c>
       <c r="B15" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C15)</f>
-        <v>6710.94</v>
+        <v>5813.26</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
       </c>
       <c r="D15" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C15)</f>
-        <v>6711.48</v>
+        <v>5816</v>
       </c>
       <c r="E15" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C15)</f>
-        <v>5.6059999999999999E-3</v>
+        <v>6.4300000000000002E-4</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -6753,15 +6753,15 @@
       </c>
       <c r="H15" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G15,H$14)</f>
-        <v>25807361</v>
+        <v>26132724</v>
       </c>
       <c r="I15" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G15,I$14)</f>
-        <v>524.75</v>
+        <v>425.5</v>
       </c>
       <c r="J15" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G15,J$14)</f>
-        <v>2.2769999999999999E-2</v>
+        <v>4.4999999999999999E-4</v>
       </c>
       <c r="K15" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G15,K$14)</f>
@@ -6773,15 +6773,15 @@
       </c>
       <c r="M15" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G15,M$14)</f>
-        <v>28994374</v>
+        <v>29343577</v>
       </c>
       <c r="N15" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G15,N$14)</f>
-        <v>28994374</v>
+        <v>29343577</v>
       </c>
       <c r="O15" s="30">
         <f>RTD(progId,,BINACE_TRADE,$G15,O$14)</f>
-        <v>43272.775247094905</v>
+        <v>43275.50424559028</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -6792,11 +6792,11 @@
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C16)</f>
-        <v>1.5252950000000001</v>
+        <v>0.25776500000000002</v>
       </c>
       <c r="B16" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C16)</f>
-        <v>6709.83</v>
+        <v>5813.24</v>
       </c>
       <c r="C16" s="8">
         <f>C15+1</f>
@@ -6804,11 +6804,11 @@
       </c>
       <c r="D16" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C16)</f>
-        <v>6711.58</v>
+        <v>5819.25</v>
       </c>
       <c r="E16" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C16)</f>
-        <v>0.58862999999999999</v>
+        <v>1.9255999999999999E-2</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
@@ -6816,15 +6816,15 @@
       </c>
       <c r="H16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,H$14)</f>
-        <v>46048483</v>
+        <v>46656230</v>
       </c>
       <c r="I16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,I$14)</f>
-        <v>6711.58</v>
+        <v>5819.24</v>
       </c>
       <c r="J16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,J$14)</f>
-        <v>2.555E-3</v>
+        <v>1.738E-3</v>
       </c>
       <c r="K16" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G16,K$14)</f>
@@ -6836,15 +6836,15 @@
       </c>
       <c r="M16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,M$14)</f>
-        <v>52379445</v>
+        <v>53033961</v>
       </c>
       <c r="N16" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G16,N$14)</f>
-        <v>52379445</v>
+        <v>53033961</v>
       </c>
       <c r="O16" s="30">
         <f>RTD(progId,,BINACE_TRADE,$G16,O$14)</f>
-        <v>43272.775248356484</v>
+        <v>43275.50424545139</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -6855,11 +6855,11 @@
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C17)</f>
-        <v>5.0729249999999997</v>
+        <v>0.89890599999999998</v>
       </c>
       <c r="B17" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C17)</f>
-        <v>6709.82</v>
+        <v>5813.18</v>
       </c>
       <c r="C17" s="8">
         <f t="shared" ref="C17:C24" si="0">C16+1</f>
@@ -6867,11 +6867,11 @@
       </c>
       <c r="D17" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C17)</f>
-        <v>6711.64</v>
+        <v>5819.26</v>
       </c>
       <c r="E17" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C17)</f>
-        <v>0.5</v>
+        <v>2.3529999999999999E-2</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -6879,15 +6879,15 @@
       </c>
       <c r="H17" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G17,H$14)</f>
-        <v>7162878</v>
+        <v>7271417</v>
       </c>
       <c r="I17" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G17,I$14)</f>
-        <v>96.3</v>
+        <v>74.2</v>
       </c>
       <c r="J17" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G17,J$14)</f>
-        <v>0.95452000000000004</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="K17" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G17,K$14)</f>
@@ -6899,15 +6899,15 @@
       </c>
       <c r="M17" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G17,M$14)</f>
-        <v>8108510</v>
+        <v>8225958</v>
       </c>
       <c r="N17" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G17,N$14)</f>
-        <v>8108510</v>
+        <v>8225958</v>
       </c>
       <c r="O17" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G17,O$14)</f>
-        <v>43272.775201192133</v>
+        <v>43275.504220960647</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -6918,11 +6918,11 @@
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C18)</f>
-        <v>2.9E-5</v>
+        <v>0.49645899999999998</v>
       </c>
       <c r="B18" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C18)</f>
-        <v>6708.69</v>
+        <v>5813.17</v>
       </c>
       <c r="C18" s="8">
         <f t="shared" si="0"/>
@@ -6930,11 +6930,11 @@
       </c>
       <c r="D18" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C18)</f>
-        <v>6711.69</v>
+        <v>5819.74</v>
       </c>
       <c r="E18" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C18)</f>
-        <v>0.22800500000000001</v>
+        <v>1.719E-3</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
@@ -6942,19 +6942,19 @@
       </c>
       <c r="H18" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G18,H$14)</f>
-        <v>1183574</v>
+        <v>1250089</v>
       </c>
       <c r="I18" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G18,I$14)</f>
-        <v>0.53173999999999999</v>
+        <v>0.44619999999999999</v>
       </c>
       <c r="J18" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G18,J$14)</f>
-        <v>1783.7</v>
+        <v>76.5</v>
       </c>
       <c r="K18" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G18,K$14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G18,L$14)</f>
@@ -6962,25 +6962,25 @@
       </c>
       <c r="M18" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G18,M$14)</f>
-        <v>1291647</v>
+        <v>1363908</v>
       </c>
       <c r="N18" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G18,N$14)</f>
-        <v>1291647</v>
+        <v>1363908</v>
       </c>
       <c r="O18" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G18,O$14)</f>
-        <v>43272.775158055556</v>
+        <v>43275.504237303241</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C19)</f>
-        <v>0.6</v>
+        <v>0.49871599999999999</v>
       </c>
       <c r="B19" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C19)</f>
-        <v>6708.66</v>
+        <v>5812.93</v>
       </c>
       <c r="C19" s="8">
         <f t="shared" si="0"/>
@@ -6988,11 +6988,11 @@
       </c>
       <c r="D19" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C19)</f>
-        <v>6712.97</v>
+        <v>5820</v>
       </c>
       <c r="E19" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C19)</f>
-        <v>0.26966299999999999</v>
+        <v>0.39807700000000001</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
@@ -7000,15 +7000,15 @@
       </c>
       <c r="H19" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G19,H$14)</f>
-        <v>14031530</v>
+        <v>14141287</v>
       </c>
       <c r="I19" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G19,I$14)</f>
-        <v>5.5789999999999998E-3</v>
+        <v>5.0140000000000002E-3</v>
       </c>
       <c r="J19" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G19,J$14)</f>
-        <v>0.68</v>
+        <v>4.83</v>
       </c>
       <c r="K19" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G19,K$14)</f>
@@ -7020,25 +7020,25 @@
       </c>
       <c r="M19" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G19,M$14)</f>
-        <v>15867644</v>
+        <v>15993950</v>
       </c>
       <c r="N19" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G19,N$14)</f>
-        <v>15867645</v>
+        <v>15993950</v>
       </c>
       <c r="O19" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G19,O$14)</f>
-        <v>43272.775196666669</v>
+        <v>43275.504218483795</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C20)</f>
-        <v>1</v>
+        <v>5.982418</v>
       </c>
       <c r="B20" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C20)</f>
-        <v>6707.92</v>
+        <v>5812</v>
       </c>
       <c r="C20" s="8">
         <f t="shared" si="0"/>
@@ -7046,11 +7046,11 @@
       </c>
       <c r="D20" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C20)</f>
-        <v>6713.37</v>
+        <v>5820.73</v>
       </c>
       <c r="E20" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C20)</f>
-        <v>5.1568399999999999</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
@@ -7058,15 +7058,15 @@
       </c>
       <c r="H20" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G20,H$14)</f>
-        <v>18182467</v>
+        <v>18281697</v>
       </c>
       <c r="I20" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G20,I$14)</f>
-        <v>7.9220000000000004E-5</v>
+        <v>7.6730000000000006E-5</v>
       </c>
       <c r="J20" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G20,J$14)</f>
-        <v>4097</v>
+        <v>295</v>
       </c>
       <c r="K20" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G20,K$14)</f>
@@ -7078,25 +7078,25 @@
       </c>
       <c r="M20" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G20,M$14)</f>
-        <v>21966660</v>
+        <v>22077467</v>
       </c>
       <c r="N20" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G20,N$14)</f>
-        <v>21966660</v>
+        <v>22077467</v>
       </c>
       <c r="O20" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G20,O$14)</f>
-        <v>43272.775216319445</v>
+        <v>43275.504244618052</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C21)</f>
-        <v>0.31148599999999999</v>
+        <v>1.002596</v>
       </c>
       <c r="B21" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C21)</f>
-        <v>6707.83</v>
+        <v>5810</v>
       </c>
       <c r="C21" s="8">
         <f t="shared" si="0"/>
@@ -7104,11 +7104,11 @@
       </c>
       <c r="D21" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C21)</f>
-        <v>6716.09</v>
+        <v>5820.91</v>
       </c>
       <c r="E21" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C21)</f>
-        <v>7.8560000000000001E-3</v>
+        <v>0.12544</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
@@ -7116,19 +7116,19 @@
       </c>
       <c r="H21" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G21,H$14)</f>
-        <v>18803800</v>
+        <v>18898921</v>
       </c>
       <c r="I21" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G21,I$14)</f>
-        <v>7.1999999999999997E-6</v>
+        <v>6.5899999999999996E-6</v>
       </c>
       <c r="J21" s="14">
         <f>RTD(progId,,BINACE_TRADE,$G21,J$14)</f>
-        <v>197</v>
+        <v>1000</v>
       </c>
       <c r="K21" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G21,K$14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="14" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G21,L$14)</f>
@@ -7136,25 +7136,25 @@
       </c>
       <c r="M21" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G21,M$14)</f>
-        <v>30232542</v>
+        <v>30373882</v>
       </c>
       <c r="N21" s="20">
         <f>RTD(progId,,BINACE_TRADE,$G21,N$14)</f>
-        <v>30232542</v>
+        <v>30373882</v>
       </c>
       <c r="O21" s="31">
         <f>RTD(progId,,BINACE_TRADE,$G21,O$14)</f>
-        <v>43272.774856863427</v>
+        <v>43275.504239259259</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C22)</f>
-        <v>4.9556999999999997E-2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C22)</f>
-        <v>6707.79</v>
+        <v>5809.59</v>
       </c>
       <c r="C22" s="8">
         <f t="shared" si="0"/>
@@ -7162,21 +7162,21 @@
       </c>
       <c r="D22" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C22)</f>
-        <v>6717.54</v>
+        <v>5821.22</v>
       </c>
       <c r="E22" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C22)</f>
-        <v>0.03</v>
+        <v>4.0712999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C23)</f>
-        <v>6.3270000000000007E-2</v>
+        <v>13</v>
       </c>
       <c r="B23" s="17">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C23)</f>
-        <v>6706.96</v>
+        <v>5809.5</v>
       </c>
       <c r="C23" s="8">
         <f t="shared" si="0"/>
@@ -7184,21 +7184,21 @@
       </c>
       <c r="D23" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C23)</f>
-        <v>6717.55</v>
+        <v>5822.64</v>
       </c>
       <c r="E23" s="18">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C23)</f>
-        <v>0.3</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C24)</f>
-        <v>0.2</v>
+        <v>0.20258200000000001</v>
       </c>
       <c r="B24" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C24)</f>
-        <v>6706.52</v>
+        <v>5808.47</v>
       </c>
       <c r="C24" s="34">
         <f t="shared" si="0"/>
@@ -7206,33 +7206,33 @@
       </c>
       <c r="D24" s="35">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C24)</f>
-        <v>6717.83</v>
+        <v>5822.66</v>
       </c>
       <c r="E24" s="35">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C24)</f>
-        <v>6.9415000000000004E-2</v>
+        <v>0.40464699999999998</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <f>SUM(Table3[BID_DEPTH_SIZE])</f>
-        <v>9.3440979999999971</v>
+        <v>23.396239999999999</v>
       </c>
       <c r="B25" s="15">
         <f>SUMPRODUCT(Table3[BID_DEPTH_SIZE],Table3[BID_DEPTH])</f>
-        <v>62693.657572809985</v>
+        <v>135943.81313960999</v>
       </c>
       <c r="C25" s="16">
         <f>D25-B25</f>
-        <v>-14653.391249679982</v>
+        <v>-129778.99218146999</v>
       </c>
       <c r="D25" s="15">
         <f>SUMPRODUCT(Table3[ASK_DEPTH_SIZE],Table3[ASK_DEPTH])</f>
-        <v>48040.266323130003</v>
+        <v>6164.8209581400006</v>
       </c>
       <c r="E25" s="13">
         <f>SUM(Table3[ASK_DEPTH_SIZE])</f>
-        <v>7.1560150000000009</v>
+        <v>1.0590250000000001</v>
       </c>
       <c r="F25" s="9"/>
       <c r="H25" s="1"/>
@@ -7243,14 +7243,14 @@
     <row r="26" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="32">
         <f>B15-B24</f>
-        <v>4.4199999999991633</v>
+        <v>4.7899999999999636</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="32">
         <f>D15-D24</f>
-        <v>-6.3500000000003638</v>
+        <v>-6.6599999999998545</v>
       </c>
       <c r="F26" s="9"/>
       <c r="I26" s="4"/>
@@ -7336,27 +7336,27 @@
       </c>
       <c r="B30" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,B$29,$D$28)</f>
-        <v>524.37</v>
+        <v>421.73</v>
       </c>
       <c r="C30" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,C$29,$D$28)</f>
-        <v>525.57000000000005</v>
+        <v>426</v>
       </c>
       <c r="D30" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,D$29,$D$28)</f>
-        <v>524.02</v>
+        <v>420.52</v>
       </c>
       <c r="E30" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,E$29,$D$28)</f>
-        <v>524.75</v>
+        <v>425.23</v>
       </c>
       <c r="F30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,F$29,$D$28)</f>
-        <v>43272.75</v>
+        <v>43275.5</v>
       </c>
       <c r="G30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,G$29,$D$28)</f>
-        <v>43272.791666655095</v>
+        <v>43275.541666655095</v>
       </c>
       <c r="H30" s="14" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,H$29,$D$28)</f>
@@ -7364,19 +7364,19 @@
       </c>
       <c r="I30" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,I$29,$D$28)</f>
-        <v>294590.46438630001</v>
+        <v>1190024.8954306</v>
       </c>
       <c r="J30" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,J$29,$D$28)</f>
-        <v>561.30701999999997</v>
+        <v>2806.54324</v>
       </c>
       <c r="K30" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,K$29,$D$28)</f>
-        <v>329.83319</v>
+        <v>1634.19415</v>
       </c>
       <c r="L30" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,L$29,$D$28)</f>
-        <v>173148.7662027</v>
+        <v>693184.39220050001</v>
       </c>
       <c r="M30" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,M$29,$D$28)</f>
@@ -7384,19 +7384,19 @@
       </c>
       <c r="N30" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,N$29,$D$28)</f>
-        <v>1281</v>
+        <v>1628</v>
       </c>
       <c r="O30" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,O$29,$D$28)</f>
-        <v>43272.775247141202</v>
+        <v>43275.504226874997</v>
       </c>
       <c r="P30" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,P$29,$D$28)</f>
-        <v>28993094</v>
+        <v>29341939</v>
       </c>
       <c r="Q30" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,Q$29,$D$28)</f>
-        <v>28994374</v>
+        <v>29343566</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -7405,27 +7405,27 @@
       </c>
       <c r="B31" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,B$29,$D$28)</f>
-        <v>6699.32</v>
+        <v>5769.86</v>
       </c>
       <c r="C31" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,C$29,$D$28)</f>
-        <v>6717.94</v>
+        <v>5819.26</v>
       </c>
       <c r="D31" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,D$29,$D$28)</f>
-        <v>6695.31</v>
+        <v>5750</v>
       </c>
       <c r="E31" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,E$29,$D$28)</f>
-        <v>6711.48</v>
+        <v>5816</v>
       </c>
       <c r="F31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,F$29,$D$28)</f>
-        <v>43272.75</v>
+        <v>43275.5</v>
       </c>
       <c r="G31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,G$29,$D$28)</f>
-        <v>43272.791666655095</v>
+        <v>43275.541666655095</v>
       </c>
       <c r="H31" s="14" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,H$29,$D$28)</f>
@@ -7433,19 +7433,19 @@
       </c>
       <c r="I31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,I$29,$D$28)</f>
-        <v>3139880.2264629598</v>
+        <v>2484420.3918971098</v>
       </c>
       <c r="J31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,J$29,$D$28)</f>
-        <v>468.25885399999999</v>
+        <v>429.42262799999997</v>
       </c>
       <c r="K31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,K$29,$D$28)</f>
-        <v>255.586726</v>
+        <v>229.99405400000001</v>
       </c>
       <c r="L31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,L$29,$D$28)</f>
-        <v>1714131.17581939</v>
+        <v>1331989.6847904101</v>
       </c>
       <c r="M31" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,M$29,$D$28)</f>
@@ -7453,19 +7453,19 @@
       </c>
       <c r="N31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,N$29,$D$28)</f>
-        <v>3037</v>
+        <v>2527</v>
       </c>
       <c r="O31" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,O$29,$D$28)</f>
-        <v>43272.775247256941</v>
+        <v>43275.504224571756</v>
       </c>
       <c r="P31" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,P$29,$D$28)</f>
-        <v>52376405</v>
+        <v>53031427</v>
       </c>
       <c r="Q31" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,Q$29,$D$28)</f>
-        <v>52379441</v>
+        <v>53033953</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -7474,27 +7474,27 @@
       </c>
       <c r="B32" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,B$29,$D$28)</f>
-        <v>7.1999999999999997E-6</v>
+        <v>6.55E-6</v>
       </c>
       <c r="C32" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,C$29,$D$28)</f>
-        <v>7.2300000000000002E-6</v>
+        <v>6.6000000000000003E-6</v>
       </c>
       <c r="D32" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,D$29,$D$28)</f>
-        <v>7.1799999999999999E-6</v>
+        <v>6.5400000000000001E-6</v>
       </c>
       <c r="E32" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,E$29,$D$28)</f>
-        <v>7.1999999999999997E-6</v>
+        <v>6.5899999999999996E-6</v>
       </c>
       <c r="F32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,F$29,$D$28)</f>
-        <v>43272.75</v>
+        <v>43275.5</v>
       </c>
       <c r="G32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,G$29,$D$28)</f>
-        <v>43272.791666655095</v>
+        <v>43275.541666655095</v>
       </c>
       <c r="H32" s="20" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,H$29,$D$28)</f>
@@ -7502,19 +7502,19 @@
       </c>
       <c r="I32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,I$29,$D$28)</f>
-        <v>55.041119129999998</v>
+        <v>71.562308580000007</v>
       </c>
       <c r="J32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,J$29,$D$28)</f>
-        <v>7639550</v>
+        <v>10901760</v>
       </c>
       <c r="K32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,K$29,$D$28)</f>
-        <v>4363991</v>
+        <v>9096658</v>
       </c>
       <c r="L32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,L$29,$D$28)</f>
-        <v>31.460917139999999</v>
+        <v>59.702030530000002</v>
       </c>
       <c r="M32" s="20" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,M$29,$D$28)</f>
@@ -7522,19 +7522,19 @@
       </c>
       <c r="N32" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,N$29,$D$28)</f>
-        <v>667</v>
+        <v>572</v>
       </c>
       <c r="O32" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,O$29,$D$28)</f>
-        <v>43272.774856863427</v>
+        <v>43275.504239236114</v>
       </c>
       <c r="P32" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,P$29,$D$28)</f>
-        <v>30231876</v>
+        <v>30373311</v>
       </c>
       <c r="Q32" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,Q$29,$D$28)</f>
-        <v>30232542</v>
+        <v>30373882</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -7551,7 +7551,7 @@
         <v>60</v>
       </c>
       <c r="D34" s="29">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7613,27 +7613,27 @@
       </c>
       <c r="B36" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,B$35,$D$34)</f>
-        <v>524.01</v>
+        <v>425.46</v>
       </c>
       <c r="C36" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,C$35,$D$34)</f>
-        <v>528.1</v>
+        <v>425.5</v>
       </c>
       <c r="D36" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,D$35,$D$34)</f>
-        <v>523.20000000000005</v>
+        <v>425.23</v>
       </c>
       <c r="E36" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,E$35,$D$34)</f>
-        <v>524.75</v>
+        <v>425.23</v>
       </c>
       <c r="F36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,F$35,$D$34)</f>
-        <v>43272.666666666664</v>
+        <v>43275.504166666666</v>
       </c>
       <c r="G36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,G$35,$D$34)</f>
-        <v>43272.83333332176</v>
+        <v>43275.504861099536</v>
       </c>
       <c r="H36" s="14" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,H$35,$D$34)</f>
@@ -7641,39 +7641,39 @@
       </c>
       <c r="I36" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,I$35,$D$34)</f>
-        <v>2459763.8007513001</v>
+        <v>17245.418378800001</v>
       </c>
       <c r="J36" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,J$35,$D$34)</f>
-        <v>4679.08205</v>
+        <v>40.533670000000001</v>
       </c>
       <c r="K36" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,K$35,$D$34)</f>
-        <v>1949.8864900000001</v>
+        <v>40.236840000000001</v>
       </c>
       <c r="L36" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,L$35,$D$34)</f>
-        <v>1024821.046414</v>
+        <v>17119.1973579</v>
       </c>
       <c r="M36" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,M$35,$D$34)</f>
-        <v>FourHour</v>
+        <v>OneMinute</v>
       </c>
       <c r="N36" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,N$35,$D$34)</f>
-        <v>6415</v>
+        <v>11</v>
       </c>
       <c r="O36" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,O$35,$D$34)</f>
-        <v>43272.775247141202</v>
+        <v>43275.504226874997</v>
       </c>
       <c r="P36" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,P$35,$D$34)</f>
-        <v>28987960</v>
+        <v>29343556</v>
       </c>
       <c r="Q36" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,Q$35,$D$34)</f>
-        <v>28994374</v>
+        <v>29343566</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7682,27 +7682,27 @@
       </c>
       <c r="B37" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,B$35,$D$34)</f>
-        <v>6714.52</v>
+        <v>5816.01</v>
       </c>
       <c r="C37" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,C$35,$D$34)</f>
-        <v>6730</v>
+        <v>5819.26</v>
       </c>
       <c r="D37" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,D$35,$D$34)</f>
-        <v>6695.31</v>
+        <v>5812</v>
       </c>
       <c r="E37" s="14">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,E$35,$D$34)</f>
-        <v>6711.48</v>
+        <v>5816</v>
       </c>
       <c r="F37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,F$35,$D$34)</f>
-        <v>43272.666666666664</v>
+        <v>43275.504166666666</v>
       </c>
       <c r="G37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,G$35,$D$34)</f>
-        <v>43272.83333332176</v>
+        <v>43275.504861099536</v>
       </c>
       <c r="H37" s="14" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,H$35,$D$34)</f>
@@ -7710,39 +7710,39 @@
       </c>
       <c r="I37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,I$35,$D$34)</f>
-        <v>15666748.907512249</v>
+        <v>70730.094461560002</v>
       </c>
       <c r="J37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,J$35,$D$34)</f>
-        <v>2333.8420609999998</v>
+        <v>12.166264999999999</v>
       </c>
       <c r="K37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,K$35,$D$34)</f>
-        <v>1358.5464979999999</v>
+        <v>3.7635740000000002</v>
       </c>
       <c r="L37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,L$35,$D$34)</f>
-        <v>9121321.0814994201</v>
+        <v>21885.311260030001</v>
       </c>
       <c r="M37" s="14" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,M$35,$D$34)</f>
-        <v>FourHour</v>
+        <v>OneMinute</v>
       </c>
       <c r="N37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,N$35,$D$34)</f>
-        <v>13368</v>
+        <v>29</v>
       </c>
       <c r="O37" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,O$35,$D$34)</f>
-        <v>43272.77524722222</v>
+        <v>43275.504224583332</v>
       </c>
       <c r="P37" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,P$35,$D$34)</f>
-        <v>52366074</v>
+        <v>53033925</v>
       </c>
       <c r="Q37" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,Q$35,$D$34)</f>
-        <v>52379441</v>
+        <v>53033953</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7751,27 +7751,27 @@
       </c>
       <c r="B38" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,B$35,$D$34)</f>
-        <v>7.17E-6</v>
+        <v>6.5799999999999997E-6</v>
       </c>
       <c r="C38" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,C$35,$D$34)</f>
-        <v>7.2400000000000001E-6</v>
+        <v>6.5899999999999996E-6</v>
       </c>
       <c r="D38" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,D$35,$D$34)</f>
-        <v>7.1199999999999996E-6</v>
+        <v>6.5799999999999997E-6</v>
       </c>
       <c r="E38" s="20">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,E$35,$D$34)</f>
-        <v>7.1999999999999997E-6</v>
+        <v>6.5899999999999996E-6</v>
       </c>
       <c r="F38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,F$35,$D$34)</f>
-        <v>43272.666666666664</v>
+        <v>43275.504166666666</v>
       </c>
       <c r="G38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,G$35,$D$34)</f>
-        <v>43272.83333332176</v>
+        <v>43275.504861099536</v>
       </c>
       <c r="H38" s="20" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,H$35,$D$34)</f>
@@ -7779,39 +7779,39 @@
       </c>
       <c r="I38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,I$35,$D$34)</f>
-        <v>298.56328172000002</v>
+        <v>3.5371970000000003E-2</v>
       </c>
       <c r="J38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,J$35,$D$34)</f>
-        <v>41483246</v>
+        <v>5372</v>
       </c>
       <c r="K38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,K$35,$D$34)</f>
-        <v>23202516</v>
+        <v>5358</v>
       </c>
       <c r="L38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,L$35,$D$34)</f>
-        <v>167.13227093</v>
+        <v>3.5279850000000001E-2</v>
       </c>
       <c r="M38" s="20" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,M$35,$D$34)</f>
-        <v>FourHour</v>
+        <v>OneMinute</v>
       </c>
       <c r="N38" s="27">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,N$35,$D$34)</f>
-        <v>4472</v>
+        <v>4</v>
       </c>
       <c r="O38" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,O$35,$D$34)</f>
-        <v>43272.774856863427</v>
+        <v>43275.504239236114</v>
       </c>
       <c r="P38" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,P$35,$D$34)</f>
-        <v>30228071</v>
+        <v>30373879</v>
       </c>
       <c r="Q38" s="28">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,Q$35,$D$34)</f>
-        <v>30232542</v>
+        <v>30373882</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -8231,31 +8231,31 @@
       </c>
       <c r="B3" s="2">
         <f>RTD(progId,,GDAX,$A3,B$2)</f>
-        <v>524.37</v>
+        <v>425.09</v>
       </c>
       <c r="C3" s="2">
         <f>RTD(progId,,GDAX,$A3,C$2)</f>
-        <v>524.38</v>
+        <v>425.1</v>
       </c>
       <c r="D3" s="2">
         <f>RTD(progId,,GDAX,$A3,D$2)</f>
-        <v>524.37</v>
+        <v>425</v>
       </c>
       <c r="E3" s="2">
         <f>RTD(progId,,GDAX,$A3,E$2)</f>
-        <v>532.67999999999995</v>
+        <v>472.93</v>
       </c>
       <c r="F3" s="2">
         <f>RTD(progId,,GDAX,$A3,F$2)</f>
-        <v>544.23</v>
+        <v>481.74</v>
       </c>
       <c r="G3" s="2">
         <f>RTD(progId,,GDAX,$A3,G$2)</f>
-        <v>521.5</v>
+        <v>421.1</v>
       </c>
       <c r="H3" s="2">
         <f>RTD(progId,,GDAX,$A3,H$2)</f>
-        <v>53323.979076390002</v>
+        <v>112160.9920632</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8264,31 +8264,31 @@
       </c>
       <c r="B4" s="2">
         <f>RTD(progId,,GDAX,$A4,B$2)</f>
-        <v>6710.69</v>
+        <v>5831.99</v>
       </c>
       <c r="C4" s="2">
         <f>RTD(progId,,GDAX,$A4,C$2)</f>
-        <v>6710.7</v>
+        <v>5832</v>
       </c>
       <c r="D4" s="2">
         <f>RTD(progId,,GDAX,$A4,D$2)</f>
-        <v>6710.7</v>
+        <v>5832</v>
       </c>
       <c r="E4" s="2">
         <f>RTD(progId,,GDAX,$A4,E$2)</f>
-        <v>6711.55</v>
+        <v>6134</v>
       </c>
       <c r="F4" s="2">
         <f>RTD(progId,,GDAX,$A4,F$2)</f>
-        <v>6787</v>
+        <v>6250</v>
       </c>
       <c r="G4" s="2">
         <f>RTD(progId,,GDAX,$A4,G$2)</f>
-        <v>6682.3</v>
+        <v>5777</v>
       </c>
       <c r="H4" s="2">
         <f>RTD(progId,,GDAX,$A4,H$2)</f>
-        <v>4390.8098624599997</v>
+        <v>9930.5915274500003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lock Binance updates so they are in-sync, the RTD values are consistent  in Excel.
</commit_message>
<xml_diff>
--- a/doc/crypto.xlsx
+++ b/doc/crypto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\Crypto\crypto-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C3895F-DBAD-48D2-8E7B-E4F324294BFC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7412A5CE-1688-4062-A988-8CEDCF4ED0BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12225" tabRatio="245" xr2:uid="{FA204BA2-54FD-4EAD-B49B-FB8867D94DC8}"/>
   </bookViews>
@@ -274,7 +274,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -539,7 +540,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -596,6 +597,7 @@
     </xf>
     <xf numFmtId="43" fontId="1" fillId="9" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="8" xfId="7" applyFill="1"/>
+    <xf numFmtId="41" fontId="1" fillId="9" borderId="0" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20% - Accent1" xfId="8" builtinId="30"/>
@@ -2398,7 +2400,7 @@
   <volType type="realTimeData">
     <main first="crypto">
       <tp>
-        <v>31617</v>
+        <v>42575</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -2406,7 +2408,7 @@
         <tr r="O11" s="1"/>
       </tp>
       <tp>
-        <v>10.75266519</v>
+        <v>58.244677230000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2415,7 +2417,7 @@
         <tr r="I32" s="1"/>
       </tp>
       <tp>
-        <v>2.5591176099999999</v>
+        <v>1.352538E-2</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2432,7 +2434,7 @@
         <tr r="N19" s="1"/>
       </tp>
       <tp>
-        <v>6124.22</v>
+        <v>6622</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2441,7 +2443,7 @@
         <tr r="C31" s="1"/>
       </tp>
       <tp>
-        <v>6124.22</v>
+        <v>6597.99</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2450,7 +2452,7 @@
         <tr r="C37" s="1"/>
       </tp>
       <tp>
-        <v>437.69</v>
+        <v>471.31</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2459,7 +2461,7 @@
         <tr r="C30" s="1"/>
       </tp>
       <tp>
-        <v>437.5</v>
+        <v>468.98</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2468,7 +2470,7 @@
         <tr r="C36" s="1"/>
       </tp>
       <tp>
-        <v>436.19</v>
+        <v>470.45</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2477,7 +2479,7 @@
         <tr r="B30" s="1"/>
       </tp>
       <tp>
-        <v>437.5</v>
+        <v>468.92</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2486,7 +2488,7 @@
         <tr r="B36" s="1"/>
       </tp>
       <tp>
-        <v>6112</v>
+        <v>6612.96</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2495,7 +2497,7 @@
         <tr r="B31" s="1"/>
       </tp>
       <tp>
-        <v>6121.85</v>
+        <v>6596</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2504,7 +2506,7 @@
         <tr r="B37" s="1"/>
       </tp>
       <tp>
-        <v>669</v>
+        <v>2737</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2513,7 +2515,7 @@
         <tr r="N31" s="1"/>
       </tp>
       <tp>
-        <v>40</v>
+        <v>7</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2522,7 +2524,7 @@
         <tr r="N37" s="1"/>
       </tp>
       <tp>
-        <v>522</v>
+        <v>1228</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2531,7 +2533,7 @@
         <tr r="N30" s="1"/>
       </tp>
       <tp>
-        <v>39</v>
+        <v>62</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2539,10 +2541,8 @@
         <stp>0</stp>
         <tr r="N36" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>1.7659999999999999E-2</v>
+      <tp>
+        <v>-1.4930000000000001E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -2550,7 +2550,7 @@
         <tr r="P11" s="1"/>
       </tp>
       <tp>
-        <v>26312</v>
+        <v>53832</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -2558,7 +2558,7 @@
         <tr r="O10" s="1"/>
       </tp>
       <tp>
-        <v>437.35</v>
+        <v>468.01</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -2573,10 +2573,8 @@
         <stp>ICEBERG_ALLOWED</stp>
         <tr r="P18" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>437.34</v>
+      <tp>
+        <v>468</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -2584,7 +2582,7 @@
         <tr r="B3" s="2"/>
       </tp>
       <tp>
-        <v>6121.59</v>
+        <v>6596.21</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -2592,7 +2590,7 @@
         <tr r="B4" s="2"/>
       </tp>
       <tp>
-        <v>43278.964583333334</v>
+        <v>43284.722222222219</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2601,7 +2599,7 @@
         <tr r="F38" s="1"/>
       </tp>
       <tp>
-        <v>43278.958333333336</v>
+        <v>43284.708333333336</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2610,7 +2608,7 @@
         <tr r="F32" s="1"/>
       </tp>
       <tp>
-        <v>1.83E-2</v>
+        <v>8.2199999999999999E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -2618,7 +2616,7 @@
         <tr r="P10" s="1"/>
       </tp>
       <tp>
-        <v>6121.6</v>
+        <v>6596.5</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -2650,7 +2648,7 @@
         <tr r="T16" s="1"/>
       </tp>
       <tp>
-        <v>1.2449999999999999E-2</v>
+        <v>2.0889999999999999E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -2674,7 +2672,7 @@
         <tr r="P16" s="1"/>
       </tp>
       <tp>
-        <v>5983.56</v>
+        <v>6535</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -2682,7 +2680,7 @@
         <tr r="G4" s="2"/>
       </tp>
       <tp>
-        <v>30503305</v>
+        <v>30862956</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2691,7 +2689,7 @@
         <tr r="Q38" s="1"/>
       </tp>
       <tp>
-        <v>30503305</v>
+        <v>30862956</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2700,7 +2698,7 @@
         <tr r="Q32" s="1"/>
       </tp>
       <tp>
-        <v>7.6538199999999996</v>
+        <v>48.726190000000003</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2709,7 +2707,7 @@
         <tr r="K36" s="1"/>
       </tp>
       <tp>
-        <v>337.96368999999999</v>
+        <v>791.60347999999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2718,7 +2716,7 @@
         <tr r="K30" s="1"/>
       </tp>
       <tp>
-        <v>1.3622460000000001</v>
+        <v>0.22354499999999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2727,7 +2725,7 @@
         <tr r="K37" s="1"/>
       </tp>
       <tp>
-        <v>66.647732000000005</v>
+        <v>186.756066</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2736,7 +2734,7 @@
         <tr r="K31" s="1"/>
       </tp>
       <tp>
-        <v>53577027</v>
+        <v>54784346</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2745,7 +2743,7 @@
         <tr r="Q37" s="1"/>
       </tp>
       <tp>
-        <v>53577027</v>
+        <v>54784340</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2786,7 +2784,7 @@
         <tr r="N21" s="1"/>
       </tp>
       <tp>
-        <v>31665</v>
+        <v>68913</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -2802,7 +2800,7 @@
         <tr r="P15" s="1"/>
       </tp>
       <tp>
-        <v>420.12</v>
+        <v>461.69</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -2810,7 +2808,7 @@
         <tr r="G3" s="2"/>
       </tp>
       <tp>
-        <v>29661422</v>
+        <v>30325160</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2819,7 +2817,7 @@
         <tr r="Q30" s="1"/>
       </tp>
       <tp>
-        <v>29661422</v>
+        <v>30325160</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2828,7 +2826,7 @@
         <tr r="Q36" s="1"/>
       </tp>
       <tp>
-        <v>4.8419999999999999E-3</v>
+        <v>5.4000000000000003E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -2836,7 +2834,7 @@
         <tr r="B9" s="1"/>
       </tp>
       <tp>
-        <v>6.1199999999999999E-6</v>
+        <v>5.8300000000000001E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -2844,7 +2842,7 @@
         <tr r="B11" s="1"/>
       </tp>
       <tp>
-        <v>7.483E-5</v>
+        <v>7.3609999999999995E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -2875,8 +2873,6 @@
         <stp>ORDER_TYPES</stp>
         <tr r="U20" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
         <v>XRP</v>
         <stp/>
@@ -2901,10 +2897,8 @@
         <stp>QUOTE_ASSET_PRECISION</stp>
         <tr r="S18" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>6.3099999999999997E-6</v>
+      <tp>
+        <v>5.9399999999999999E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2913,7 +2907,7 @@
         <tr r="B38" s="1"/>
       </tp>
       <tp>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2922,7 +2916,7 @@
         <tr r="B32" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -2930,7 +2924,7 @@
         <tr r="K21" s="1"/>
       </tp>
       <tp>
-        <v>2E-8</v>
+        <v>1E-8</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -2938,7 +2932,7 @@
         <tr r="J11" s="1"/>
       </tp>
       <tp>
-        <v>125</v>
+        <v>24</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -2946,7 +2940,7 @@
         <tr r="J20" s="1"/>
       </tp>
       <tp>
-        <v>27</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2955,7 +2949,7 @@
         <tr r="N38" s="1"/>
       </tp>
       <tp>
-        <v>148</v>
+        <v>543</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2964,27 +2958,23 @@
         <tr r="N32" s="1"/>
       </tp>
       <tp>
-        <v>14265123</v>
+        <v>14520756</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
         <stp>TRADE_ID</stp>
         <tr r="H19" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>617</v>
+      <tp>
+        <v>356</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
         <stp>BID_SIZE</stp>
         <tr r="H10" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>13262478.120725</v>
+      <tp>
+        <v>21439989.816296</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -2992,7 +2982,7 @@
         <tr r="N8" s="1"/>
       </tp>
       <tp>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3001,7 +2991,7 @@
         <tr r="C38" s="1"/>
       </tp>
       <tp>
-        <v>6.3400000000000003E-6</v>
+        <v>5.9699999999999996E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3010,7 +3000,7 @@
         <tr r="C32" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3018,7 +3008,7 @@
         <tr r="K20" s="1"/>
       </tp>
       <tp>
-        <v>277254</v>
+        <v>325948</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3026,7 +3016,7 @@
         <tr r="H11" s="1"/>
       </tp>
       <tp>
-        <v>3.87</v>
+        <v>98.8</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3034,7 +3024,7 @@
         <tr r="L9" s="1"/>
       </tp>
       <tp>
-        <v>4.9999999999999998E-8</v>
+        <v>8.9999999999999999E-8</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3042,7 +3032,7 @@
         <tr r="J10" s="1"/>
       </tp>
       <tp>
-        <v>0.18398</v>
+        <v>1.24308</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -3050,7 +3040,7 @@
         <tr r="L5" s="1"/>
       </tp>
       <tp>
-        <v>13.523709999999999</v>
+        <v>5.5398800000000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -3058,17 +3048,15 @@
         <tr r="L7" s="1"/>
       </tp>
       <tp>
-        <v>13.766325</v>
+        <v>1.3532390000000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
         <stp>ASK_SIZE</stp>
         <tr r="L6" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>3073</v>
+      <tp>
+        <v>2466</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3076,7 +3064,7 @@
         <tr r="J18" s="1"/>
       </tp>
       <tp>
-        <v>1987.3001538000001</v>
+        <v>3426.7021633099998</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3084,17 +3072,15 @@
         <tr r="N11" s="1"/>
       </tp>
       <tp>
-        <v>2413.62485118</v>
+        <v>3901.26588558</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
         <stp>QUOTE_VOL</stp>
         <tr r="N10" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>0.40221000000000001</v>
+      <tp>
+        <v>1.403</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3102,7 +3088,7 @@
         <tr r="J15" s="1"/>
       </tp>
       <tp>
-        <v>9.9999999999999995E-7</v>
+        <v>1.707E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3110,7 +3096,7 @@
         <tr r="J16" s="1"/>
       </tp>
       <tp>
-        <v>10.11631</v>
+        <v>2.7E-4</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3118,7 +3104,7 @@
         <tr r="J17" s="1"/>
       </tp>
       <tp>
-        <v>0.186</v>
+        <v>7.5883999999999993E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3127,7 +3113,7 @@
         <tr r="E23" s="1"/>
       </tp>
       <tp>
-        <v>1.7555999999999999E-2</v>
+        <v>4.7562E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3136,7 +3122,7 @@
         <tr r="E24" s="1"/>
       </tp>
       <tp>
-        <v>0.02</v>
+        <v>0.03</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3145,7 +3131,7 @@
         <tr r="E19" s="1"/>
       </tp>
       <tp>
-        <v>6.1490999999999997E-2</v>
+        <v>0.56970900000000002</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3154,7 +3140,7 @@
         <tr r="E20" s="1"/>
       </tp>
       <tp>
-        <v>2.3491000000000001E-2</v>
+        <v>1.0923020000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3163,7 +3149,7 @@
         <tr r="E21" s="1"/>
       </tp>
       <tp>
-        <v>5.0000000000000001E-3</v>
+        <v>0.79949999999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3172,7 +3158,7 @@
         <tr r="E22" s="1"/>
       </tp>
       <tp>
-        <v>2.0010000000000002E-3</v>
+        <v>6.4515000000000003E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3181,7 +3167,7 @@
         <tr r="E15" s="1"/>
       </tp>
       <tp>
-        <v>2</v>
+        <v>1.707E-3</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3190,7 +3176,7 @@
         <tr r="E16" s="1"/>
       </tp>
       <tp>
-        <v>0.117368</v>
+        <v>0.91054900000000005</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3199,7 +3185,7 @@
         <tr r="E17" s="1"/>
       </tp>
       <tp>
-        <v>9.7145999999999996E-2</v>
+        <v>0.111301</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3207,10 +3193,8 @@
         <stp>3</stp>
         <tr r="E18" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>16708</v>
+      <tp>
+        <v>2277</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3218,7 +3202,7 @@
         <tr r="J21" s="1"/>
       </tp>
       <tp>
-        <v>2175</v>
+        <v>1663</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -3226,7 +3210,7 @@
         <tr r="L8" s="1"/>
       </tp>
       <tp>
-        <v>43278.964962256941</v>
+        <v>43284.722218692128</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3234,7 +3218,7 @@
         <tr r="L18" s="1"/>
       </tp>
       <tp>
-        <v>43278.964950520836</v>
+        <v>43284.72225363426</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3242,7 +3226,7 @@
         <tr r="L17" s="1"/>
       </tp>
       <tp>
-        <v>43278.964961307873</v>
+        <v>43284.722217199072</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3250,17 +3234,15 @@
         <tr r="L15" s="1"/>
       </tp>
       <tp>
-        <v>43278.964959756944</v>
+        <v>43284.722259803239</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
         <stp>TRADE_TIME</stp>
         <tr r="L16" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
-        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",29655415,441.03000000,0.04725000,"2018-06-27T21:01:30.14-04:00",true,true],["ETHUSDT",29655416,441.15000000,0.03880000,"2018-06-27T21:01:32.892-04:00",true,false],["ETHUSDT",29655417,441.05000000,0.10000000,"2018-06-27T21:01:36.76-04:00",true,true],["ETHUSDT",29655418,441.07000000,0.10000000,"2018-06-27T21:01:50.891-04:00",true,true],["ETHUSDT",29655419,441.07000000,0.99988000,"2018-06-27T21:01:52.801-04:00",true,true],["ETHUSDT",29655420,441.07000000,3.43110000,"2018-06-27T21:01:52.815-04:00",true,true],["ETHUSDT",29655421,441.08000000,0.18116000,"2018-06-27T21:01:53.605-04:00",true,false],["ETHUSDT",29655422,441.08000000,0.51401000,"2018-06-27T21:01:57.015-04:00",true,false],["ETHUSDT",29655423,441.08000000,0.23800000,"2018-06-27T21:01:57.154-04:00",true,false],["ETHUSDT",29655424,441.07000000,0.00005000,"2018-06-27T21:02:00.108-04:00",true,true]]</v>
+        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",30325041,468.88000000,0.15959000,"2018-07-03T17:17:31.738-04:00",true,true],["ETHUSDT",30325042,468.88000000,0.00041000,"2018-07-03T17:17:37.266-04:00",true,true],["ETHUSDT",30325043,468.86000000,2.08320000,"2018-07-03T17:17:39.711-04:00",true,false],["ETHUSDT",30325044,468.75000000,0.03180000,"2018-07-03T17:17:41.766-04:00",true,true],["ETHUSDT",30325045,468.75000000,0.16820000,"2018-07-03T17:17:41.766-04:00",true,true],["ETHUSDT",30325046,468.75000000,0.15428000,"2018-07-03T17:17:43.196-04:00",true,true],["ETHUSDT",30325047,468.86000000,4.75865000,"2018-07-03T17:17:47.152-04:00",true,false],["ETHUSDT",30325048,468.97000000,4.17426000,"2018-07-03T17:17:47.17-04:00",true,false],["ETHUSDT",30325049,468.77000000,0.09950000,"2018-07-03T17:17:48.792-04:00",true,true],["ETHUSDT",30325050,468.95000000,0.02592000,"2018-07-03T17:17:52.165-04:00",true,false]]</v>
         <stp/>
         <stp>BINANCE_HISTORY</stp>
         <stp>ETHUSDT</stp>
@@ -3269,7 +3251,7 @@
         <tr r="G24" s="1"/>
       </tp>
       <tp>
-        <v>18374353</v>
+        <v>18577123</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3277,7 +3259,7 @@
         <tr r="H20" s="1"/>
       </tp>
       <tp>
-        <v>437.21</v>
+        <v>468.93</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3286,7 +3268,7 @@
         <tr r="E36" s="1"/>
       </tp>
       <tp>
-        <v>437.21</v>
+        <v>468.93</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3311,7 +3293,7 @@
         <tr r="S16" s="1"/>
       </tp>
       <tp>
-        <v>38856</v>
+        <v>62318</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3319,7 +3301,7 @@
         <tr r="L11" s="1"/>
       </tp>
       <tp>
-        <v>263.92592999999999</v>
+        <v>0.40920000000000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -3327,7 +3309,7 @@
         <tr r="H7" s="1"/>
       </tp>
       <tp>
-        <v>1.9999990000000001</v>
+        <v>0.52357699999999996</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -3335,7 +3317,7 @@
         <tr r="H6" s="1"/>
       </tp>
       <tp>
-        <v>0.4022</v>
+        <v>1.7000000000000001E-4</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -3343,7 +3325,7 @@
         <tr r="H5" s="1"/>
       </tp>
       <tp>
-        <v>81.09</v>
+        <v>2.48</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3351,7 +3333,7 @@
         <tr r="H9" s="1"/>
       </tp>
       <tp>
-        <v>110039912.12355807</v>
+        <v>224411913.22751993</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -3359,17 +3341,15 @@
         <tr r="N6" s="1"/>
       </tp>
       <tp>
-        <v>10792524.8653311</v>
+        <v>15882625.5011223</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
         <stp>QUOTE_VOL</stp>
         <tr r="N7" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>1545</v>
+      <tp>
+        <v>353.5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -3377,7 +3357,7 @@
         <tr r="H8" s="1"/>
       </tp>
       <tp>
-        <v>1.94</v>
+        <v>1.5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -3385,7 +3365,7 @@
         <tr r="J19" s="1"/>
       </tp>
       <tp>
-        <v>6120.31</v>
+        <v>6593.27</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3394,7 +3374,7 @@
         <tr r="E37" s="1"/>
       </tp>
       <tp>
-        <v>6120.31</v>
+        <v>6596</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3411,13 +3391,13 @@
         <tr r="K19" s="1"/>
       </tp>
       <tp>
-        <v>43278.964926203706</v>
+        <v>43284.72226396991</v>
         <stp/>
         <stp>CLOCK</stp>
         <tr r="T4" s="1"/>
       </tp>
       <tp>
-        <v>6.9999999999999999E-6</v>
+        <v>1.1E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3425,7 +3405,7 @@
         <tr r="J9" s="1"/>
       </tp>
       <tp>
-        <v>402711</v>
+        <v>5257284</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3434,7 +3414,7 @@
         <tr r="K32" s="1"/>
       </tp>
       <tp>
-        <v>19421</v>
+        <v>2277</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3443,7 +3423,7 @@
         <tr r="K38" s="1"/>
       </tp>
       <tp>
-        <v>9.4579999999999994E-3</v>
+        <v>11.064577</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3461,7 +3441,7 @@
         <tr r="A24" s="1"/>
       </tp>
       <tp>
-        <v>0.13</v>
+        <v>0.62049699999999997</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3470,7 +3450,7 @@
         <tr r="A19" s="1"/>
       </tp>
       <tp>
-        <v>1.2006349999999999</v>
+        <v>1.9989999999999999E-3</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3479,7 +3459,7 @@
         <tr r="A20" s="1"/>
       </tp>
       <tp>
-        <v>1.402452</v>
+        <v>0.48682999999999998</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3488,7 +3468,7 @@
         <tr r="A21" s="1"/>
       </tp>
       <tp>
-        <v>2.14E-3</v>
+        <v>0.1</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3497,7 +3477,7 @@
         <tr r="A22" s="1"/>
       </tp>
       <tp>
-        <v>0.45286999999999999</v>
+        <v>0.756328</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3506,7 +3486,7 @@
         <tr r="A15" s="1"/>
       </tp>
       <tp>
-        <v>0.98260999999999998</v>
+        <v>1.6233999999999998E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3515,7 +3495,7 @@
         <tr r="A16" s="1"/>
       </tp>
       <tp>
-        <v>0.131438</v>
+        <v>5.6000000000000001E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3524,7 +3504,7 @@
         <tr r="A17" s="1"/>
       </tp>
       <tp>
-        <v>0.28172999999999998</v>
+        <v>1.7946E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3533,7 +3513,7 @@
         <tr r="A18" s="1"/>
       </tp>
       <tp>
-        <v>6586.7504915700001</v>
+        <v>6147.1162924800001</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -3541,7 +3521,7 @@
         <tr r="H4" s="2"/>
       </tp>
       <tp>
-        <v>64914.849068449999</v>
+        <v>68576.476604249998</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -3556,8 +3536,6 @@
         <stp>QUOTE_ASSET_PRECISION</stp>
         <tr r="S15" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="b">
         <v>0</v>
         <stp/>
@@ -3577,7 +3555,7 @@
         <tr r="H31" s="1"/>
       </tp>
       <tp>
-        <v>1309729</v>
+        <v>1428847</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3585,14 +3563,14 @@
         <tr r="H18" s="1"/>
       </tp>
       <tp>
-        <v>-753</v>
+        <v>-935</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>DRIFT</stp>
         <tr r="T5" s="1"/>
       </tp>
       <tp>
-        <v>47162353</v>
+        <v>48261642</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3600,7 +3578,7 @@
         <tr r="H16" s="1"/>
       </tp>
       <tp>
-        <v>7365223</v>
+        <v>7519854</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3608,7 +3586,7 @@
         <tr r="H17" s="1"/>
       </tp>
       <tp>
-        <v>26430861</v>
+        <v>27042665</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3616,7 +3594,7 @@
         <tr r="H15" s="1"/>
       </tp>
       <tp>
-        <v>1455.25969192</v>
+        <v>3367.3331261399999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3624,7 +3602,7 @@
         <tr r="N9" s="1"/>
       </tp>
       <tp>
-        <v>18989603</v>
+        <v>19221669</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3650,7 +3628,7 @@
         <tr r="H30" s="1"/>
       </tp>
       <tp>
-        <v>40889650.717068903</v>
+        <v>81175585.563029304</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -3658,7 +3636,7 @@
         <tr r="N5" s="1"/>
       </tp>
       <tp>
-        <v>1857</v>
+        <v>780</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3666,7 +3644,7 @@
         <tr r="L10" s="1"/>
       </tp>
       <tp>
-        <v>43278.874161562497</v>
+        <v>43284.720387337962</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>EXCHANGE_TIME</stp>
@@ -3697,15 +3675,13 @@
         <tr r="Q19" s="1"/>
       </tp>
       <tp>
-        <v>420.19</v>
+        <v>462.5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
         <stp>LOW</stp>
         <tr r="B5" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
         <v>USDT</v>
         <stp/>
@@ -3715,7 +3691,7 @@
         <tr r="R17" s="1"/>
       </tp>
       <tp>
-        <v>11.668279999999999</v>
+        <v>134.20161999999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3724,7 +3700,7 @@
         <tr r="J36" s="1"/>
       </tp>
       <tp>
-        <v>471.63035000000002</v>
+        <v>1437.56467</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3741,7 +3717,7 @@
         <tr r="O21" s="1"/>
       </tp>
       <tp>
-        <v>6.3300000000000004E-6</v>
+        <v>5.93E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3749,7 +3725,7 @@
         <tr r="I11" s="1"/>
       </tp>
       <tp>
-        <v>7.6719999999999997E-5</v>
+        <v>7.483E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3757,7 +3733,7 @@
         <tr r="I10" s="1"/>
       </tp>
       <tp>
-        <v>4.9579999999999997E-3</v>
+        <v>5.6169999999999996E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3789,7 +3765,7 @@
         <tr r="Q17" s="1"/>
       </tp>
       <tp>
-        <v>5971</v>
+        <v>6519.99</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3797,7 +3773,7 @@
         <tr r="B6" s="1"/>
       </tp>
       <tp>
-        <v>4.9649999999999998E-3</v>
+        <v>5.6259999999999999E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3805,7 +3781,7 @@
         <tr r="K9" s="1"/>
       </tp>
       <tp>
-        <v>7.682E-5</v>
+        <v>7.4870000000000007E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3813,7 +3789,7 @@
         <tr r="K10" s="1"/>
       </tp>
       <tp>
-        <v>6.3500000000000002E-6</v>
+        <v>5.9399999999999999E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3837,17 +3813,15 @@
         <tr r="S19" s="1"/>
       </tp>
       <tp>
-        <v>0.46751999999999999</v>
+        <v>0.49326999999999999</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
         <stp>PRICE</stp>
         <tr r="I18" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>0.47517999999999999</v>
+      <tp>
+        <v>0.52</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3855,7 +3829,7 @@
         <tr r="C8" s="1"/>
       </tp>
       <tp>
-        <v>43278.96493736111</v>
+        <v>43284.722259895832</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3864,7 +3838,7 @@
         <tr r="O37" s="1"/>
       </tp>
       <tp>
-        <v>43278.96493736111</v>
+        <v>43284.722245023149</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3873,7 +3847,7 @@
         <tr r="O31" s="1"/>
       </tp>
       <tp>
-        <v>43278.96496135417</v>
+        <v>43284.722217222225</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3882,7 +3856,7 @@
         <tr r="O36" s="1"/>
       </tp>
       <tp>
-        <v>43278.96496135417</v>
+        <v>43284.722217222225</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3891,7 +3865,7 @@
         <tr r="O30" s="1"/>
       </tp>
       <tp>
-        <v>74.91</v>
+        <v>84.75</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3899,7 +3873,7 @@
         <tr r="B7" s="1"/>
       </tp>
       <tp>
-        <v>107.72978999999999</v>
+        <v>362.47585800000002</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3908,7 +3882,7 @@
         <tr r="J31" s="1"/>
       </tp>
       <tp>
-        <v>1.9042159999999999</v>
+        <v>0.27246199999999998</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3917,7 +3891,7 @@
         <tr r="J37" s="1"/>
       </tp>
       <tp>
-        <v>4.9890000000000004E-3</v>
+        <v>5.8349999999999999E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3933,7 +3907,7 @@
         <tr r="U17" s="1"/>
       </tp>
       <tp>
-        <v>1703752</v>
+        <v>9791683</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3942,7 +3916,7 @@
         <tr r="J32" s="1"/>
       </tp>
       <tp>
-        <v>405317</v>
+        <v>2277</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3958,8 +3932,6 @@
         <stp>QUOTE_ASSET</stp>
         <tr r="R15" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
         <v>USDT</v>
         <stp/>
@@ -3968,8 +3940,6 @@
         <stp>QUOTE_ASSET</stp>
         <tr r="R16" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="b">
         <v>0</v>
         <stp/>
@@ -3995,7 +3965,7 @@
         <tr r="P19" s="1"/>
       </tp>
       <tp>
-        <v>6190.43</v>
+        <v>6679.35</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -4003,7 +3973,7 @@
         <tr r="C6" s="1"/>
       </tp>
       <tp>
-        <v>81.75</v>
+        <v>90</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -4011,15 +3981,13 @@
         <tr r="C7" s="1"/>
       </tp>
       <tp>
-        <v>445.95</v>
+        <v>486.98</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
         <stp>HIGH</stp>
         <tr r="C5" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
         <v>OneHour</v>
         <stp/>
@@ -4056,8 +4024,6 @@
         <stp>0</stp>
         <tr r="M36" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp>
         <v>1</v>
         <stp/>
@@ -4099,7 +4065,7 @@
         <tr r="T20" s="1"/>
       </tp>
       <tp>
-        <v>53576988</v>
+        <v>54784340</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4108,7 +4074,7 @@
         <tr r="P37" s="1"/>
       </tp>
       <tp>
-        <v>53576359</v>
+        <v>54781604</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4117,7 +4083,7 @@
         <tr r="P31" s="1"/>
       </tp>
       <tp>
-        <v>29661384</v>
+        <v>30325099</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4126,7 +4092,7 @@
         <tr r="P36" s="1"/>
       </tp>
       <tp>
-        <v>29660901</v>
+        <v>30323933</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4135,7 +4101,7 @@
         <tr r="P30" s="1"/>
       </tp>
       <tp>
-        <v>315445343</v>
+        <v>572222720</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -4143,7 +4109,7 @@
         <tr r="M11" s="1"/>
       </tp>
       <tp>
-        <v>31805978</v>
+        <v>51677984</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -4151,17 +4117,15 @@
         <tr r="M10" s="1"/>
       </tp>
       <tp>
-        <v>296294.64</v>
+        <v>598657.79</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
         <stp>VOL</stp>
         <tr r="M9" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>43278.999999988424</v>
+      <tp>
+        <v>43284.749999988424</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4170,7 +4134,7 @@
         <tr r="G30" s="1"/>
       </tp>
       <tp>
-        <v>43278.965277766205</v>
+        <v>43284.72222221065</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4179,7 +4143,7 @@
         <tr r="G36" s="1"/>
       </tp>
       <tp>
-        <v>43278.999999988424</v>
+        <v>43284.749999988424</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4188,7 +4152,7 @@
         <tr r="G31" s="1"/>
       </tp>
       <tp>
-        <v>43278.965277766205</v>
+        <v>43284.72291665509</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4197,7 +4161,7 @@
         <tr r="G37" s="1"/>
       </tp>
       <tp>
-        <v>6.4799999999999998E-6</v>
+        <v>6.1399999999999997E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4205,7 +4169,7 @@
         <tr r="C11" s="1"/>
       </tp>
       <tp>
-        <v>6.2999999999999998E-6</v>
+        <v>5.9200000000000001E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4214,7 +4178,7 @@
         <tr r="D32" s="1"/>
       </tp>
       <tp>
-        <v>6.2999999999999998E-6</v>
+        <v>5.9399999999999999E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4241,7 +4205,7 @@
         <tr r="H32" s="1"/>
       </tp>
       <tp>
-        <v>24087</v>
+        <v>32593</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4249,7 +4213,7 @@
         <tr r="O7" s="1"/>
       </tp>
       <tp>
-        <v>92806</v>
+        <v>217438</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4257,7 +4221,7 @@
         <tr r="O6" s="1"/>
       </tp>
       <tp>
-        <v>70110</v>
+        <v>128396</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4265,7 +4229,7 @@
         <tr r="O5" s="1"/>
       </tp>
       <tp>
-        <v>16853</v>
+        <v>27840</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4273,7 +4237,7 @@
         <tr r="O8" s="1"/>
       </tp>
       <tp>
-        <v>6112</v>
+        <v>6586.03</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4282,7 +4246,7 @@
         <tr r="D31" s="1"/>
       </tp>
       <tp>
-        <v>6120.31</v>
+        <v>6593.27</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4290,10 +4254,8 @@
         <stp>0</stp>
         <tr r="D37" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>6.4149999999999999E-2</v>
+      <tp>
+        <v>1.3860000000000001E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4301,7 +4263,7 @@
         <tr r="P7" s="1"/>
       </tp>
       <tp>
-        <v>1.7299999999999999E-2</v>
+        <v>-1.423E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4309,7 +4271,7 @@
         <tr r="P5" s="1"/>
       </tp>
       <tp>
-        <v>8.6800000000000002E-3</v>
+        <v>-6.3299999999999997E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4317,17 +4279,15 @@
         <tr r="P6" s="1"/>
       </tp>
       <tp>
-        <v>2.6110000000000001E-2</v>
+        <v>3.2100000000000002E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
         <stp>PRICE%</stp>
         <tr r="P8" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>6120.31</v>
+      <tp>
+        <v>6593.27</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4335,15 +4295,13 @@
         <tr r="I16" s="1"/>
       </tp>
       <tp>
-        <v>80.52</v>
+        <v>87.17</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
         <stp>PRICE</stp>
         <tr r="I17" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
         <v>XRPBTC</v>
         <stp/>
@@ -4352,8 +4310,6 @@
         <stp>NAME</stp>
         <tr r="Q20" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
         <v>USDT</v>
         <stp/>
@@ -4363,7 +4319,7 @@
         <tr r="R18" s="1"/>
       </tp>
       <tp>
-        <v>437</v>
+        <v>467.93</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4372,7 +4328,7 @@
         <tr r="D36" s="1"/>
       </tp>
       <tp>
-        <v>436.18</v>
+        <v>467.93</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4388,8 +4344,6 @@
         <stp>STATUS</stp>
         <tr r="T21" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
         <v>8</v>
         <stp/>
@@ -4406,8 +4360,6 @@
         <stp>BASE_ASSET_PRECISION</stp>
         <tr r="O19" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
         <v>TRXBTC</v>
         <stp/>
@@ -4416,18 +4368,14 @@
         <stp>NAME</stp>
         <tr r="Q21" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>0.45134000000000002</v>
+      <tp>
+        <v>0.48514000000000002</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
         <stp>LOW</stp>
         <tr r="B8" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
       <tp t="s">
         <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
         <stp/>
@@ -4436,10 +4384,8 @@
         <stp>ORDER_TYPES</stp>
         <tr r="U18" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>7.695E-5</v>
+      <tp>
+        <v>7.8139999999999994E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4479,7 +4425,7 @@
         <tr r="N17" s="1"/>
       </tp>
       <tp>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4488,7 +4434,7 @@
         <tr r="E38" s="1"/>
       </tp>
       <tp>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4497,7 +4443,7 @@
         <tr r="E32" s="1"/>
       </tp>
       <tp>
-        <v>8341.6207168599994</v>
+        <v>1474.9476208200001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4506,7 +4452,7 @@
         <tr r="L37" s="1"/>
       </tp>
       <tp>
-        <v>407601.03467939998</v>
+        <v>1232565.7239691401</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4515,7 +4461,7 @@
         <tr r="L31" s="1"/>
       </tp>
       <tp>
-        <v>3347.0526055</v>
+        <v>22830.8364043</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4524,7 +4470,7 @@
         <tr r="L36" s="1"/>
       </tp>
       <tp>
-        <v>147569.46521630001</v>
+        <v>371589.88051839999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4557,7 +4503,7 @@
         <tr r="O15" s="1"/>
       </tp>
       <tp>
-        <v>437.27</v>
+        <v>468.93</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4565,7 +4511,7 @@
         <tr r="I15" s="1"/>
       </tp>
       <tp>
-        <v>137168.66536000001</v>
+        <v>182963.56307</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4573,7 +4519,7 @@
         <tr r="M7" s="1"/>
       </tp>
       <tp>
-        <v>0.47122999999999998</v>
+        <v>0.49278</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4581,7 +4527,7 @@
         <tr r="I8" s="1"/>
       </tp>
       <tp>
-        <v>43278.964583333334</v>
+        <v>43284.72152777778</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4590,7 +4536,7 @@
         <tr r="F36" s="1"/>
       </tp>
       <tp>
-        <v>43278.958333333336</v>
+        <v>43284.708333333336</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4599,7 +4545,7 @@
         <tr r="F30" s="1"/>
       </tp>
       <tp>
-        <v>76.45</v>
+        <v>85.9</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4607,7 +4553,7 @@
         <tr r="D7" s="1"/>
       </tp>
       <tp>
-        <v>6083</v>
+        <v>6636.01</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4615,7 +4561,7 @@
         <tr r="D6" s="1"/>
       </tp>
       <tp>
-        <v>43278.964934884258</v>
+        <v>43284.722140613427</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4623,7 +4569,7 @@
         <tr r="L19" s="1"/>
       </tp>
       <tp>
-        <v>4.8859999999999997E-3</v>
+        <v>5.5030000000000001E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4631,7 +4577,7 @@
         <tr r="G9" s="1"/>
       </tp>
       <tp>
-        <v>433.59</v>
+        <v>475.71</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4639,7 +4585,7 @@
         <tr r="G5" s="1"/>
       </tp>
       <tp>
-        <v>0.47217999999999999</v>
+        <v>0.49362</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4647,7 +4593,7 @@
         <tr r="K8" s="1"/>
       </tp>
       <tp>
-        <v>6084.03</v>
+        <v>6636.01</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4655,7 +4601,7 @@
         <tr r="G6" s="1"/>
       </tp>
       <tp>
-        <v>76.58</v>
+        <v>85.84</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4663,7 +4609,7 @@
         <tr r="G7" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4687,17 +4633,15 @@
         <tr r="K15" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
         <stp>BUYER_IS_MAKER</stp>
         <tr r="K18" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>446.21</v>
+      <tp>
+        <v>486.76</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4705,7 +4649,7 @@
         <tr r="F3" s="2"/>
       </tp>
       <tp>
-        <v>6175.43</v>
+        <v>6673.99</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4713,7 +4657,7 @@
         <tr r="F4" s="2"/>
       </tp>
       <tp>
-        <v>0.46</v>
+        <v>0.49210999999999999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4721,7 +4665,7 @@
         <tr r="G8" s="1"/>
       </tp>
       <tp>
-        <v>43278.964583333334</v>
+        <v>43284.722222222219</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4730,7 +4674,7 @@
         <tr r="F37" s="1"/>
       </tp>
       <tp>
-        <v>43278.958333333336</v>
+        <v>43284.708333333336</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4739,7 +4683,7 @@
         <tr r="F31" s="1"/>
       </tp>
       <tp>
-        <v>1.4100000000000001E-6</v>
+        <v>7.0999999999999998E-7</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -4747,7 +4691,7 @@
         <tr r="Q10" s="1"/>
       </tp>
       <tp>
-        <v>433.68</v>
+        <v>475.7</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4755,7 +4699,7 @@
         <tr r="D5" s="1"/>
       </tp>
       <tp>
-        <v>94297.359890000007</v>
+        <v>171552.397</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4763,7 +4707,7 @@
         <tr r="M5" s="1"/>
       </tp>
       <tp>
-        <v>4.8979999999999996E-3</v>
+        <v>5.5030000000000001E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4789,7 +4733,7 @@
         <tr r="M32" s="1"/>
       </tp>
       <tp>
-        <v>1.1000000000000001E-7</v>
+        <v>-8.9999999999999999E-8</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -4797,7 +4741,7 @@
         <tr r="Q11" s="1"/>
       </tp>
       <tp>
-        <v>658826.19390307995</v>
+        <v>2392227.0247127102</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4806,7 +4750,7 @@
         <tr r="I31" s="1"/>
       </tp>
       <tp>
-        <v>11659.568683519999</v>
+        <v>1797.6540783099999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4814,10 +4758,8 @@
         <stp>0</stp>
         <tr r="I37" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>205944.56736799999</v>
+      <tp>
+        <v>674654.7416978</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4826,7 +4768,7 @@
         <tr r="I30" s="1"/>
       </tp>
       <tp>
-        <v>5102.0120073999997</v>
+        <v>62870.438001199997</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4835,7 +4777,7 @@
         <tr r="I36" s="1"/>
       </tp>
       <tp>
-        <v>437.35</v>
+        <v>468.01</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4843,7 +4785,7 @@
         <tr r="D3" s="2"/>
       </tp>
       <tp>
-        <v>6121.6</v>
+        <v>6596.5</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4851,7 +4793,7 @@
         <tr r="D4" s="2"/>
       </tp>
       <tp>
-        <v>4.9329999999999999E-3</v>
+        <v>5.5999999999999999E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4859,7 +4801,7 @@
         <tr r="I19" s="1"/>
       </tp>
       <tp>
-        <v>43278.964896134261</v>
+        <v>43284.722241145835</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4868,7 +4810,7 @@
         <tr r="O32" s="1"/>
       </tp>
       <tp>
-        <v>43278.964896134261</v>
+        <v>43284.722241145835</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4876,10 +4818,8 @@
         <stp>0</stp>
         <tr r="O38" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>18052.040830000002</v>
+      <tp>
+        <v>33994.790332999997</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4894,7 +4834,7 @@
         <tr r="T7" s="1"/>
       </tp>
       <tp>
-        <v>4.91</v>
+        <v>1.37</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4902,7 +4842,7 @@
         <tr r="Q7" s="1"/>
       </tp>
       <tp>
-        <v>52.83</v>
+        <v>-42.03</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4910,7 +4850,7 @@
         <tr r="Q6" s="1"/>
       </tp>
       <tp>
-        <v>6.0999999999999999E-5</v>
+        <v>1.16E-4</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4918,7 +4858,7 @@
         <tr r="Q9" s="1"/>
       </tp>
       <tp>
-        <v>7.5</v>
+        <v>-6.77</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4926,27 +4866,23 @@
         <tr r="Q5" s="1"/>
       </tp>
       <tp>
-        <v>0.45843</v>
+        <v>0.49210999999999999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
         <stp>CLOSE</stp>
         <tr r="D8" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>0.11</v>
+      <tp>
+        <v>0.19</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
         <stp>Spread</stp>
         <tr r="J7" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>2.84</v>
+      <tp>
+        <v>1.27</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4954,7 +4890,7 @@
         <tr r="J6" s="1"/>
       </tp>
       <tp>
-        <v>7.0000000000000007E-2</v>
+        <v>0.14000000000000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4962,17 +4898,15 @@
         <tr r="J5" s="1"/>
       </tp>
       <tp>
-        <v>4.2999999999999999E-4</v>
+        <v>8.3000000000000001E-4</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
         <stp>Spread</stp>
         <tr r="J8" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>43278.965277766205</v>
+      <tp>
+        <v>43284.72291665509</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4981,7 +4915,7 @@
         <tr r="G38" s="1"/>
       </tp>
       <tp>
-        <v>43278.999999988424</v>
+        <v>43284.749999988424</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4990,7 +4924,7 @@
         <tr r="G32" s="1"/>
       </tp>
       <tp>
-        <v>30503158</v>
+        <v>30862414</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4999,7 +4933,7 @@
         <tr r="P32" s="1"/>
       </tp>
       <tp>
-        <v>30503279</v>
+        <v>30862956</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5008,7 +4942,7 @@
         <tr r="P38" s="1"/>
       </tp>
       <tp>
-        <v>81.290000000000006</v>
+        <v>87.03</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -5016,7 +4950,7 @@
         <tr r="I7" s="1"/>
       </tp>
       <tp>
-        <v>28599972.699999999</v>
+        <v>43030472.700000003</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -5024,7 +4958,7 @@
         <tr r="M8" s="1"/>
       </tp>
       <tp>
-        <v>7.5480000000000002E-5</v>
+        <v>7.4120000000000002E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -5032,7 +4966,7 @@
         <tr r="G10" s="1"/>
       </tp>
       <tp>
-        <v>43278.964896064812</v>
+        <v>43284.722241087962</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -5040,7 +4974,7 @@
         <tr r="L21" s="1"/>
       </tp>
       <tp>
-        <v>1.1990000000000001E-2</v>
+        <v>1.5100000000000001E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -5048,7 +4982,7 @@
         <tr r="Q8" s="1"/>
       </tp>
       <tp>
-        <v>81.400000000000006</v>
+        <v>87.22</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -5056,17 +4990,15 @@
         <tr r="K7" s="1"/>
       </tp>
       <tp t="s">
-        <v>ETHBTC|LTCBTC|BNBBTC|NEOBTC|QTUMETH|EOSETH|SNTETH|BNTETH|BCCBTC|GASBTC|BNBETH|BTCUSDT|ETHUSDT|HSRBTC|OAXETH|DNTETH|MCOETH|ICNETH|MCOBTC|WTCBTC|WTCETH|LRCBTC|LRCETH|QTUMBTC|YOYOBTC|OMGBTC|OMGETH|ZRXBTC|ZRXETH|STRATBTC|STRATETH|SNGLSBTC|SNGLSETH|BQXBTC|BQXETH|KNCBTC|KNCETH|FUNBTC|FUNETH|SNMBTC|SNMETH|NEOETH|IOTABTC|IOTAETH|LINKBTC|LINKETH|XVGBTC|XVGETH|SALTBTC|SALTETH|MDABTC|MDAETH|MTLBTC|MTLETH|SUBBTC|SUBETH|EOSBTC|SNTBTC|ETCETH|ETCBTC|MTHBTC|MTHETH|ENGBTC|ENGETH|DNTBTC|ZECBTC|ZECETH|BNTBTC|ASTBTC|ASTETH|DASHBTC|DASHETH|OAXBTC|ICNBTC|BTGBTC|BTGETH|EVXBTC|EVXETH|REQBTC|REQETH|VIBBTC|VIBETH|HSRETH|TRXBTC|TRXETH|POWRBTC|POWRETH|ARKBTC|ARKETH|YOYOETH|XRPBTC|XRPETH|MODBTC|MODETH|ENJBTC|ENJETH|STORJBTC|STORJETH|BNBUSDT|VENBNB|YOYOBNB|POWRBNB|VENBTC|VENETH|KMDBTC|KMDETH|NULSBNB|RCNBTC|RCNETH|RCNBNB|NULSBTC|NULSETH|RDNBTC|RDNETH|RDNBNB|XMRBTC|XMRETH|DLTBNB|WTCBNB|DLTBTC|DLTETH|AMBBTC|AMBETH|AMBBNB|BCCETH|BCCUSDT|BCCBNB|BATBTC|BATETH|BATBNB|BCPTBTC|BCPTETH|BCPTBNB|ARNBTC|ARNETH|GVTBTC|GVTETH|CDTBTC|CDTETH|GXSBTC|GXSETH|NEOUSDT|NEOBNB|POEBTC|POEETH|QSPBTC|QSPETH|QSPBNB|BTSBTC|BTSETH|BTSBNB|XZCBTC|XZCETH|XZCBNB|LSKBTC|LSKETH|LSKBNB|TNTBTC|TNTETH|FUELBTC|FUELETH|MANABTC|MANAETH|BCDBTC|BCDETH|DGDBTC|DGDETH|IOTABNB|ADXBTC|ADXETH|ADXBNB|ADABTC|ADAETH|PPTBTC|PPTETH|CMTBTC|CMTETH|CMTBNB|XLMBTC|XLMETH|XLMBNB|CNDBTC|CNDETH|CNDBNB|LENDBTC|LENDETH|WABIBTC|WABIETH|WABIBNB|LTCETH|LTCUSDT|LTCBNB|TNBBTC|TNBETH|WAVESBTC|WAVESETH|WAVESBNB|GTOBTC|GTOETH|GTOBNB|ICXBTC|ICXETH|ICXBNB|OSTBTC|OSTETH|OSTBNB|ELFBTC|ELFETH|AIONBTC|AIONETH|AIONBNB|NEBLBTC|NEBLETH|NEBLBNB|BRDBTC|BRDETH|BRDBNB|MCOBNB|EDOBTC|EDOETH|WINGSBTC|WINGSETH|NAVBTC|NAVETH|NAVBNB|LUNBTC|LUNETH|TRIGBTC|TRIGETH|TRIGBNB|APPCBTC|APPCETH|APPCBNB|VIBEBTC|VIBEETH|RLCBTC|RLCETH|RLCBNB|INSBTC|INSETH|PIVXBTC|PIVXETH|PIVXBNB|IOSTBTC|IOSTETH|CHATBTC|CHATETH|STEEMBTC|STEEMETH|STEEMBNB|NANOBTC|NANOETH|NANOBNB|VIABTC|VIAETH|VIABNB|BLZBTC|BLZETH|BLZBNB|AEBTC|AEETH|AEBNB|RPXBTC|RPXETH|RPXBNB|NCASHBTC|NCASHETH|NCASHBNB|POABTC|POAETH|POABNB|ZILBTC|ZILETH|ZILBNB|ONTBTC|ONTETH|ONTBNB|STORMBTC|STORMETH|STORMBNB|QTUMBNB|QTUMUSDT|XEMBTC|XEMETH|XEMBNB|WANBTC|WANETH|WANBNB|WPRBTC|WPRETH|QLCBTC|QLCETH|SYSBTC|SYSETH|SYSBNB|QLCBNB|GRSBTC|GRSETH|ADAUSDT|ADABNB|CLOAKBTC|CLOAKETH|GNTBTC|GNTETH|GNTBNB|LOOMBTC|LOOMETH|LOOMBNB|XRPUSDT|BCNBTC|BCNETH|BCNBNB|REPBTC|REPETH|REPBNB|TUSDBTC|TUSDETH|TUSDBNB|ZENBTC|ZENETH|ZENBNB|SKYBTC|SKYETH|SKYBNB|EOSUSDT|EOSBNB|CVCBTC|CVCETH|CVCBNB|THETABTC|THETAETH|THETABNB|XRPBNB|TUSDUSDT|IOTAUSDT|XLMUSDT|IOTXBTC|IOTXETH|QKCBTC|QKCETH|AGIBTC|AGIETH|AGIBNB|NXSBTC|NXSETH|NXSBNB|ENJBNB|DATABTC|DATAETH|ONTUSDT|TRXUSDT|ETCUSDT|ETCBNB|ICXUSDT|SCBTC|SCETH|SCBNB|NPXSBTC|NPXSETH|VENUSDT|KEYBTC|KEYETH|</v>
+        <v>ETHBTC|LTCBTC|BNBBTC|NEOBTC|QTUMETH|EOSETH|SNTETH|BNTETH|BCCBTC|GASBTC|BNBETH|BTCUSDT|ETHUSDT|HSRBTC|OAXETH|DNTETH|MCOETH|ICNETH|MCOBTC|WTCBTC|WTCETH|LRCBTC|LRCETH|QTUMBTC|YOYOBTC|OMGBTC|OMGETH|ZRXBTC|ZRXETH|STRATBTC|STRATETH|SNGLSBTC|SNGLSETH|BQXBTC|BQXETH|KNCBTC|KNCETH|FUNBTC|FUNETH|SNMBTC|SNMETH|NEOETH|IOTABTC|IOTAETH|LINKBTC|LINKETH|XVGBTC|XVGETH|SALTBTC|SALTETH|MDABTC|MDAETH|MTLBTC|MTLETH|SUBBTC|SUBETH|EOSBTC|SNTBTC|ETCETH|ETCBTC|MTHBTC|MTHETH|ENGBTC|ENGETH|DNTBTC|ZECBTC|ZECETH|BNTBTC|ASTBTC|ASTETH|DASHBTC|DASHETH|OAXBTC|ICNBTC|BTGBTC|BTGETH|EVXBTC|EVXETH|REQBTC|REQETH|VIBBTC|VIBETH|HSRETH|TRXBTC|TRXETH|POWRBTC|POWRETH|ARKBTC|ARKETH|YOYOETH|XRPBTC|XRPETH|MODBTC|MODETH|ENJBTC|ENJETH|STORJBTC|STORJETH|BNBUSDT|VENBNB|YOYOBNB|POWRBNB|VENBTC|VENETH|KMDBTC|KMDETH|NULSBNB|RCNBTC|RCNETH|RCNBNB|NULSBTC|NULSETH|RDNBTC|RDNETH|RDNBNB|XMRBTC|XMRETH|DLTBNB|WTCBNB|DLTBTC|DLTETH|AMBBTC|AMBETH|AMBBNB|BCCETH|BCCUSDT|BCCBNB|BATBTC|BATETH|BATBNB|BCPTBTC|BCPTETH|BCPTBNB|ARNBTC|ARNETH|GVTBTC|GVTETH|CDTBTC|CDTETH|GXSBTC|GXSETH|NEOUSDT|NEOBNB|POEBTC|POEETH|QSPBTC|QSPETH|QSPBNB|BTSBTC|BTSETH|BTSBNB|XZCBTC|XZCETH|XZCBNB|LSKBTC|LSKETH|LSKBNB|TNTBTC|TNTETH|FUELBTC|FUELETH|MANABTC|MANAETH|BCDBTC|BCDETH|DGDBTC|DGDETH|IOTABNB|ADXBTC|ADXETH|ADXBNB|ADABTC|ADAETH|PPTBTC|PPTETH|CMTBTC|CMTETH|CMTBNB|XLMBTC|XLMETH|XLMBNB|CNDBTC|CNDETH|CNDBNB|LENDBTC|LENDETH|WABIBTC|WABIETH|WABIBNB|LTCETH|LTCUSDT|LTCBNB|TNBBTC|TNBETH|WAVESBTC|WAVESETH|WAVESBNB|GTOBTC|GTOETH|GTOBNB|ICXBTC|ICXETH|ICXBNB|OSTBTC|OSTETH|OSTBNB|ELFBTC|ELFETH|AIONBTC|AIONETH|AIONBNB|NEBLBTC|NEBLETH|NEBLBNB|BRDBTC|BRDETH|BRDBNB|MCOBNB|EDOBTC|EDOETH|WINGSBTC|WINGSETH|NAVBTC|NAVETH|NAVBNB|LUNBTC|LUNETH|TRIGBTC|TRIGETH|TRIGBNB|APPCBTC|APPCETH|APPCBNB|VIBEBTC|VIBEETH|RLCBTC|RLCETH|RLCBNB|INSBTC|INSETH|PIVXBTC|PIVXETH|PIVXBNB|IOSTBTC|IOSTETH|CHATBTC|CHATETH|STEEMBTC|STEEMETH|STEEMBNB|NANOBTC|NANOETH|NANOBNB|VIABTC|VIAETH|VIABNB|BLZBTC|BLZETH|BLZBNB|AEBTC|AEETH|AEBNB|RPXBTC|RPXETH|RPXBNB|NCASHBTC|NCASHETH|NCASHBNB|POABTC|POAETH|POABNB|ZILBTC|ZILETH|ZILBNB|ONTBTC|ONTETH|ONTBNB|STORMBTC|STORMETH|STORMBNB|QTUMBNB|QTUMUSDT|XEMBTC|XEMETH|XEMBNB|WANBTC|WANETH|WANBNB|WPRBTC|WPRETH|QLCBTC|QLCETH|SYSBTC|SYSETH|SYSBNB|QLCBNB|GRSBTC|GRSETH|ADAUSDT|ADABNB|CLOAKBTC|CLOAKETH|GNTBTC|GNTETH|GNTBNB|LOOMBTC|LOOMETH|LOOMBNB|XRPUSDT|BCNBTC|BCNETH|BCNBNB|REPBTC|REPETH|REPBNB|TUSDBTC|TUSDETH|TUSDBNB|ZENBTC|ZENETH|ZENBNB|SKYBTC|SKYETH|SKYBNB|EOSUSDT|EOSBNB|CVCBTC|CVCETH|CVCBNB|THETABTC|THETAETH|THETABNB|XRPBNB|TUSDUSDT|IOTAUSDT|XLMUSDT|IOTXBTC|IOTXETH|QKCBTC|QKCETH|AGIBTC|AGIETH|AGIBNB|NXSBTC|NXSETH|NXSBNB|ENJBNB|DATABTC|DATAETH|ONTUSDT|TRXUSDT|ETCUSDT|ETCBNB|ICXUSDT|SCBTC|SCETH|SCBNB|NPXSBTC|NPXSETH|VENUSDT|KEYBTC|KEYETH|NASBTC|NASETH|NASBNB|</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp/>
         <stp>EXCHANGE_SYMBOLS</stp>
         <tr r="T8" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>2.54358087</v>
+      <tp>
+        <v>31.2854311</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5075,7 +5007,7 @@
         <tr r="L32" s="1"/>
       </tp>
       <tp>
-        <v>0.12261337999999999</v>
+        <v>1.352538E-2</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5084,7 +5016,7 @@
         <tr r="L38" s="1"/>
       </tp>
       <tp>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -5092,7 +5024,7 @@
         <tr r="I21" s="1"/>
       </tp>
       <tp>
-        <v>7.6279999999999995E-5</v>
+        <v>7.4930000000000003E-5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -5100,7 +5032,7 @@
         <tr r="I20" s="1"/>
       </tp>
       <tp>
-        <v>6136.86</v>
+        <v>6595.24</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -5108,7 +5040,7 @@
         <tr r="K6" s="1"/>
       </tp>
       <tp>
-        <v>6.2500000000000003E-6</v>
+        <v>6.0299999999999999E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -5116,7 +5048,7 @@
         <tr r="G11" s="1"/>
       </tp>
       <tp>
-        <v>6134.02</v>
+        <v>6593.97</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -5124,7 +5056,7 @@
         <tr r="I6" s="1"/>
       </tp>
       <tp>
-        <v>6.2199999999999997E-6</v>
+        <v>6.0299999999999999E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -5132,7 +5064,7 @@
         <tr r="D11" s="1"/>
       </tp>
       <tp>
-        <v>7.5389999999999995E-5</v>
+        <v>7.4129999999999997E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -5140,7 +5072,7 @@
         <tr r="D10" s="1"/>
       </tp>
       <tp>
-        <v>6117.21</v>
+        <v>6593.03</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5149,7 +5081,7 @@
         <tr r="B19" s="1"/>
       </tp>
       <tp>
-        <v>6116.54</v>
+        <v>6591.89</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5158,7 +5090,7 @@
         <tr r="B20" s="1"/>
       </tp>
       <tp>
-        <v>6116.44</v>
+        <v>6591.4</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5167,7 +5099,7 @@
         <tr r="B21" s="1"/>
       </tp>
       <tp>
-        <v>6115.77</v>
+        <v>6590.01</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5176,7 +5108,7 @@
         <tr r="B22" s="1"/>
       </tp>
       <tp>
-        <v>6120.31</v>
+        <v>6593.27</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5185,7 +5117,7 @@
         <tr r="B15" s="1"/>
       </tp>
       <tp>
-        <v>6120.3</v>
+        <v>6593.26</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5194,7 +5126,7 @@
         <tr r="B16" s="1"/>
       </tp>
       <tp>
-        <v>6118.72</v>
+        <v>6593.18</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5203,7 +5135,7 @@
         <tr r="B17" s="1"/>
       </tp>
       <tp>
-        <v>6117.53</v>
+        <v>6593.14</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5212,7 +5144,7 @@
         <tr r="B18" s="1"/>
       </tp>
       <tp>
-        <v>6114.46</v>
+        <v>6590</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5221,7 +5153,7 @@
         <tr r="B23" s="1"/>
       </tp>
       <tp>
-        <v>6113.33</v>
+        <v>6588.64</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5230,7 +5162,7 @@
         <tr r="B24" s="1"/>
       </tp>
       <tp>
-        <v>431.23</v>
+        <v>475.27</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -5238,7 +5170,7 @@
         <tr r="E3" s="2"/>
       </tp>
       <tp>
-        <v>441</v>
+        <v>468.76</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -5246,7 +5178,7 @@
         <tr r="I5" s="1"/>
       </tp>
       <tp>
-        <v>6079.99</v>
+        <v>6626.31</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -5254,7 +5186,7 @@
         <tr r="E4" s="2"/>
       </tp>
       <tp>
-        <v>43278.964883043984</v>
+        <v>43284.722096273152</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -5262,7 +5194,7 @@
         <tr r="L20" s="1"/>
       </tp>
       <tp>
-        <v>6129.2</v>
+        <v>6603.78</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5271,7 +5203,7 @@
         <tr r="D24" s="1"/>
       </tp>
       <tp>
-        <v>6128.68</v>
+        <v>6603</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5280,7 +5212,7 @@
         <tr r="D23" s="1"/>
       </tp>
       <tp>
-        <v>6124.26</v>
+        <v>6599.61</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5289,7 +5221,7 @@
         <tr r="D18" s="1"/>
       </tp>
       <tp>
-        <v>6124.22</v>
+        <v>6597.99</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5298,7 +5230,7 @@
         <tr r="D17" s="1"/>
       </tp>
       <tp>
-        <v>6123.82</v>
+        <v>6597.98</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5307,7 +5239,7 @@
         <tr r="D16" s="1"/>
       </tp>
       <tp>
-        <v>6120.32</v>
+        <v>6597.97</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5316,7 +5248,7 @@
         <tr r="D15" s="1"/>
       </tp>
       <tp>
-        <v>6128</v>
+        <v>6601.54</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5325,7 +5257,7 @@
         <tr r="D22" s="1"/>
       </tp>
       <tp>
-        <v>6126.03</v>
+        <v>6600</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5334,7 +5266,7 @@
         <tr r="D21" s="1"/>
       </tp>
       <tp>
-        <v>6125</v>
+        <v>6599.99</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5343,7 +5275,7 @@
         <tr r="D20" s="1"/>
       </tp>
       <tp>
-        <v>6124.39</v>
+        <v>6599.98</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5351,10 +5283,8 @@
         <stp>4</stp>
         <tr r="D19" s="1"/>
       </tp>
-    </main>
-    <main first="crypto">
-      <tp>
-        <v>441.07</v>
+      <tp>
+        <v>468.91</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -5880,7 +5810,7 @@
   <dimension ref="A1:U108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5898,12 +5828,12 @@
     <col min="11" max="11" width="15.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" customWidth="1"/>
     <col min="17" max="17" width="20.42578125" customWidth="1"/>
     <col min="18" max="18" width="13.140625" customWidth="1"/>
     <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
     <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.28515625" customWidth="1"/>
     <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -5993,7 +5923,7 @@
       </c>
       <c r="T4" s="37">
         <f>RTD(progId,,"CLOCK")</f>
-        <v>43278.964926203706</v>
+        <v>43284.72226396991</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -6002,66 +5932,66 @@
       </c>
       <c r="B5" s="2">
         <f>RTD(progId,,BINANCE,$A5,B$4)</f>
-        <v>420.19</v>
+        <v>462.5</v>
       </c>
       <c r="C5" s="2">
         <f>RTD(progId,,BINANCE,$A5,C$4)</f>
-        <v>445.95</v>
+        <v>486.98</v>
       </c>
       <c r="D5" s="2">
         <f>RTD(progId,,BINANCE_24H,$A5,D$4)</f>
-        <v>433.68</v>
+        <v>475.7</v>
       </c>
       <c r="G5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,G$4)</f>
-        <v>433.59</v>
+        <v>475.71</v>
       </c>
       <c r="H5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,H$4)</f>
-        <v>0.4022</v>
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="I5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,I$4)</f>
-        <v>441</v>
+        <v>468.76</v>
       </c>
       <c r="J5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,J$4)</f>
-        <v>7.0000000000000007E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,K$4)</f>
-        <v>441.07</v>
+        <v>468.91</v>
       </c>
       <c r="L5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,L$4)</f>
-        <v>0.18398</v>
+        <v>1.24308</v>
       </c>
       <c r="M5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,M$4)</f>
-        <v>94297.359890000007</v>
-      </c>
-      <c r="N5" s="40">
+        <v>171552.397</v>
+      </c>
+      <c r="N5" s="42">
         <f>RTD(progId,,BINANCE_24H,$A5,N$4)</f>
-        <v>40889650.717068903</v>
+        <v>81175585.563029304</v>
       </c>
       <c r="O5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,O$4)</f>
-        <v>70110</v>
+        <v>128396</v>
       </c>
       <c r="P5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,P$4)</f>
-        <v>1.7299999999999999E-2</v>
+        <v>-1.423E-2</v>
       </c>
       <c r="Q5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,Q$4)</f>
-        <v>7.5</v>
+        <v>-6.77</v>
       </c>
       <c r="S5" s="38" t="s">
         <v>61</v>
       </c>
       <c r="T5" s="36">
         <f>RTD(progId,,BINANCE,S5)</f>
-        <v>-753</v>
+        <v>-935</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -6070,66 +6000,66 @@
       </c>
       <c r="B6" s="2">
         <f>RTD(progId,,BINANCE,$A6,B$4)</f>
-        <v>5971</v>
+        <v>6519.99</v>
       </c>
       <c r="C6" s="2">
         <f>RTD(progId,,BINANCE,$A6,C$4)</f>
-        <v>6190.43</v>
+        <v>6679.35</v>
       </c>
       <c r="D6" s="2">
         <f>RTD(progId,,BINANCE_24H,$A6,D$4)</f>
-        <v>6083</v>
+        <v>6636.01</v>
       </c>
       <c r="G6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,G$4)</f>
-        <v>6084.03</v>
+        <v>6636.01</v>
       </c>
       <c r="H6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,H$4)</f>
-        <v>1.9999990000000001</v>
+        <v>0.52357699999999996</v>
       </c>
       <c r="I6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,I$4)</f>
-        <v>6134.02</v>
+        <v>6593.97</v>
       </c>
       <c r="J6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,J$4)</f>
-        <v>2.84</v>
+        <v>1.27</v>
       </c>
       <c r="K6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,K$4)</f>
-        <v>6136.86</v>
+        <v>6595.24</v>
       </c>
       <c r="L6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,L$4)</f>
-        <v>13.766325</v>
+        <v>1.3532390000000001</v>
       </c>
       <c r="M6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,M$4)</f>
-        <v>18052.040830000002</v>
-      </c>
-      <c r="N6" s="40">
+        <v>33994.790332999997</v>
+      </c>
+      <c r="N6" s="42">
         <f>RTD(progId,,BINANCE_24H,$A6,N$4)</f>
-        <v>110039912.12355807</v>
+        <v>224411913.22751993</v>
       </c>
       <c r="O6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,O$4)</f>
-        <v>92806</v>
+        <v>217438</v>
       </c>
       <c r="P6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,P$4)</f>
-        <v>8.6800000000000002E-3</v>
+        <v>-6.3299999999999997E-3</v>
       </c>
       <c r="Q6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,Q$4)</f>
-        <v>52.83</v>
+        <v>-42.03</v>
       </c>
       <c r="S6" s="38" t="s">
         <v>62</v>
       </c>
       <c r="T6" s="37">
         <f>RTD(progId,,BINANCE,S6)</f>
-        <v>43278.874161562497</v>
+        <v>43284.720387337962</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -6138,59 +6068,59 @@
       </c>
       <c r="B7" s="2">
         <f>RTD(progId,,BINANCE,$A7,B$4)</f>
-        <v>74.91</v>
+        <v>84.75</v>
       </c>
       <c r="C7" s="2">
         <f>RTD(progId,,BINANCE,$A7,C$4)</f>
-        <v>81.75</v>
+        <v>90</v>
       </c>
       <c r="D7" s="2">
         <f>RTD(progId,,BINANCE_24H,$A7,D$4)</f>
-        <v>76.45</v>
+        <v>85.9</v>
       </c>
       <c r="G7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,G$4)</f>
-        <v>76.58</v>
+        <v>85.84</v>
       </c>
       <c r="H7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,H$4)</f>
-        <v>263.92592999999999</v>
+        <v>0.40920000000000001</v>
       </c>
       <c r="I7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,I$4)</f>
-        <v>81.290000000000006</v>
+        <v>87.03</v>
       </c>
       <c r="J7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,J$4)</f>
-        <v>0.11</v>
+        <v>0.19</v>
       </c>
       <c r="K7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,K$4)</f>
-        <v>81.400000000000006</v>
+        <v>87.22</v>
       </c>
       <c r="L7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,L$4)</f>
-        <v>13.523709999999999</v>
+        <v>5.5398800000000001</v>
       </c>
       <c r="M7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,M$4)</f>
-        <v>137168.66536000001</v>
-      </c>
-      <c r="N7" s="40">
+        <v>182963.56307</v>
+      </c>
+      <c r="N7" s="42">
         <f>RTD(progId,,BINANCE_24H,$A7,N$4)</f>
-        <v>10792524.8653311</v>
+        <v>15882625.5011223</v>
       </c>
       <c r="O7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,O$4)</f>
-        <v>24087</v>
+        <v>32593</v>
       </c>
       <c r="P7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,P$4)</f>
-        <v>6.4149999999999999E-2</v>
+        <v>1.3860000000000001E-2</v>
       </c>
       <c r="Q7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,Q$4)</f>
-        <v>4.91</v>
+        <v>1.37</v>
       </c>
       <c r="S7" s="38" t="s">
         <v>63</v>
@@ -6206,66 +6136,66 @@
       </c>
       <c r="B8" s="2">
         <f>RTD(progId,,BINANCE,$A8,B$4)</f>
-        <v>0.45134000000000002</v>
+        <v>0.48514000000000002</v>
       </c>
       <c r="C8" s="2">
         <f>RTD(progId,,BINANCE,$A8,C$4)</f>
-        <v>0.47517999999999999</v>
+        <v>0.52</v>
       </c>
       <c r="D8" s="2">
         <f>RTD(progId,,BINANCE_24H,$A8,D$4)</f>
-        <v>0.45843</v>
+        <v>0.49210999999999999</v>
       </c>
       <c r="G8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,G$4)</f>
-        <v>0.46</v>
+        <v>0.49210999999999999</v>
       </c>
       <c r="H8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,H$4)</f>
-        <v>1545</v>
+        <v>353.5</v>
       </c>
       <c r="I8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,I$4)</f>
-        <v>0.47122999999999998</v>
+        <v>0.49278</v>
       </c>
       <c r="J8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,J$4)</f>
-        <v>4.2999999999999999E-4</v>
+        <v>8.3000000000000001E-4</v>
       </c>
       <c r="K8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,K$4)</f>
-        <v>0.47217999999999999</v>
+        <v>0.49362</v>
       </c>
       <c r="L8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,L$4)</f>
-        <v>2175</v>
+        <v>1663</v>
       </c>
       <c r="M8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,M$4)</f>
-        <v>28599972.699999999</v>
-      </c>
-      <c r="N8" s="40">
+        <v>43030472.700000003</v>
+      </c>
+      <c r="N8" s="42">
         <f>RTD(progId,,BINANCE_24H,$A8,N$4)</f>
-        <v>13262478.120725</v>
+        <v>21439989.816296</v>
       </c>
       <c r="O8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,O$4)</f>
-        <v>16853</v>
+        <v>27840</v>
       </c>
       <c r="P8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,P$4)</f>
-        <v>2.6110000000000001E-2</v>
+        <v>3.2100000000000002E-3</v>
       </c>
       <c r="Q8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,Q$4)</f>
-        <v>1.1990000000000001E-2</v>
+        <v>1.5100000000000001E-3</v>
       </c>
       <c r="S8" s="38" t="s">
         <v>64</v>
       </c>
       <c r="T8" s="36" t="str">
         <f>RTD(progId,,BINANCE,,S8)</f>
-        <v>ETHBTC|LTCBTC|BNBBTC|NEOBTC|QTUMETH|EOSETH|SNTETH|BNTETH|BCCBTC|GASBTC|BNBETH|BTCUSDT|ETHUSDT|HSRBTC|OAXETH|DNTETH|MCOETH|ICNETH|MCOBTC|WTCBTC|WTCETH|LRCBTC|LRCETH|QTUMBTC|YOYOBTC|OMGBTC|OMGETH|ZRXBTC|ZRXETH|STRATBTC|STRATETH|SNGLSBTC|SNGLSETH|BQXBTC|BQXETH|KNCBTC|KNCETH|FUNBTC|FUNETH|SNMBTC|SNMETH|NEOETH|IOTABTC|IOTAETH|LINKBTC|LINKETH|XVGBTC|XVGETH|SALTBTC|SALTETH|MDABTC|MDAETH|MTLBTC|MTLETH|SUBBTC|SUBETH|EOSBTC|SNTBTC|ETCETH|ETCBTC|MTHBTC|MTHETH|ENGBTC|ENGETH|DNTBTC|ZECBTC|ZECETH|BNTBTC|ASTBTC|ASTETH|DASHBTC|DASHETH|OAXBTC|ICNBTC|BTGBTC|BTGETH|EVXBTC|EVXETH|REQBTC|REQETH|VIBBTC|VIBETH|HSRETH|TRXBTC|TRXETH|POWRBTC|POWRETH|ARKBTC|ARKETH|YOYOETH|XRPBTC|XRPETH|MODBTC|MODETH|ENJBTC|ENJETH|STORJBTC|STORJETH|BNBUSDT|VENBNB|YOYOBNB|POWRBNB|VENBTC|VENETH|KMDBTC|KMDETH|NULSBNB|RCNBTC|RCNETH|RCNBNB|NULSBTC|NULSETH|RDNBTC|RDNETH|RDNBNB|XMRBTC|XMRETH|DLTBNB|WTCBNB|DLTBTC|DLTETH|AMBBTC|AMBETH|AMBBNB|BCCETH|BCCUSDT|BCCBNB|BATBTC|BATETH|BATBNB|BCPTBTC|BCPTETH|BCPTBNB|ARNBTC|ARNETH|GVTBTC|GVTETH|CDTBTC|CDTETH|GXSBTC|GXSETH|NEOUSDT|NEOBNB|POEBTC|POEETH|QSPBTC|QSPETH|QSPBNB|BTSBTC|BTSETH|BTSBNB|XZCBTC|XZCETH|XZCBNB|LSKBTC|LSKETH|LSKBNB|TNTBTC|TNTETH|FUELBTC|FUELETH|MANABTC|MANAETH|BCDBTC|BCDETH|DGDBTC|DGDETH|IOTABNB|ADXBTC|ADXETH|ADXBNB|ADABTC|ADAETH|PPTBTC|PPTETH|CMTBTC|CMTETH|CMTBNB|XLMBTC|XLMETH|XLMBNB|CNDBTC|CNDETH|CNDBNB|LENDBTC|LENDETH|WABIBTC|WABIETH|WABIBNB|LTCETH|LTCUSDT|LTCBNB|TNBBTC|TNBETH|WAVESBTC|WAVESETH|WAVESBNB|GTOBTC|GTOETH|GTOBNB|ICXBTC|ICXETH|ICXBNB|OSTBTC|OSTETH|OSTBNB|ELFBTC|ELFETH|AIONBTC|AIONETH|AIONBNB|NEBLBTC|NEBLETH|NEBLBNB|BRDBTC|BRDETH|BRDBNB|MCOBNB|EDOBTC|EDOETH|WINGSBTC|WINGSETH|NAVBTC|NAVETH|NAVBNB|LUNBTC|LUNETH|TRIGBTC|TRIGETH|TRIGBNB|APPCBTC|APPCETH|APPCBNB|VIBEBTC|VIBEETH|RLCBTC|RLCETH|RLCBNB|INSBTC|INSETH|PIVXBTC|PIVXETH|PIVXBNB|IOSTBTC|IOSTETH|CHATBTC|CHATETH|STEEMBTC|STEEMETH|STEEMBNB|NANOBTC|NANOETH|NANOBNB|VIABTC|VIAETH|VIABNB|BLZBTC|BLZETH|BLZBNB|AEBTC|AEETH|AEBNB|RPXBTC|RPXETH|RPXBNB|NCASHBTC|NCASHETH|NCASHBNB|POABTC|POAETH|POABNB|ZILBTC|ZILETH|ZILBNB|ONTBTC|ONTETH|ONTBNB|STORMBTC|STORMETH|STORMBNB|QTUMBNB|QTUMUSDT|XEMBTC|XEMETH|XEMBNB|WANBTC|WANETH|WANBNB|WPRBTC|WPRETH|QLCBTC|QLCETH|SYSBTC|SYSETH|SYSBNB|QLCBNB|GRSBTC|GRSETH|ADAUSDT|ADABNB|CLOAKBTC|CLOAKETH|GNTBTC|GNTETH|GNTBNB|LOOMBTC|LOOMETH|LOOMBNB|XRPUSDT|BCNBTC|BCNETH|BCNBNB|REPBTC|REPETH|REPBNB|TUSDBTC|TUSDETH|TUSDBNB|ZENBTC|ZENETH|ZENBNB|SKYBTC|SKYETH|SKYBNB|EOSUSDT|EOSBNB|CVCBTC|CVCETH|CVCBNB|THETABTC|THETAETH|THETABNB|XRPBNB|TUSDUSDT|IOTAUSDT|XLMUSDT|IOTXBTC|IOTXETH|QKCBTC|QKCETH|AGIBTC|AGIETH|AGIBNB|NXSBTC|NXSETH|NXSBNB|ENJBNB|DATABTC|DATAETH|ONTUSDT|TRXUSDT|ETCUSDT|ETCBNB|ICXUSDT|SCBTC|SCETH|SCBNB|NPXSBTC|NPXSETH|VENUSDT|KEYBTC|KEYETH|</v>
+        <v>ETHBTC|LTCBTC|BNBBTC|NEOBTC|QTUMETH|EOSETH|SNTETH|BNTETH|BCCBTC|GASBTC|BNBETH|BTCUSDT|ETHUSDT|HSRBTC|OAXETH|DNTETH|MCOETH|ICNETH|MCOBTC|WTCBTC|WTCETH|LRCBTC|LRCETH|QTUMBTC|YOYOBTC|OMGBTC|OMGETH|ZRXBTC|ZRXETH|STRATBTC|STRATETH|SNGLSBTC|SNGLSETH|BQXBTC|BQXETH|KNCBTC|KNCETH|FUNBTC|FUNETH|SNMBTC|SNMETH|NEOETH|IOTABTC|IOTAETH|LINKBTC|LINKETH|XVGBTC|XVGETH|SALTBTC|SALTETH|MDABTC|MDAETH|MTLBTC|MTLETH|SUBBTC|SUBETH|EOSBTC|SNTBTC|ETCETH|ETCBTC|MTHBTC|MTHETH|ENGBTC|ENGETH|DNTBTC|ZECBTC|ZECETH|BNTBTC|ASTBTC|ASTETH|DASHBTC|DASHETH|OAXBTC|ICNBTC|BTGBTC|BTGETH|EVXBTC|EVXETH|REQBTC|REQETH|VIBBTC|VIBETH|HSRETH|TRXBTC|TRXETH|POWRBTC|POWRETH|ARKBTC|ARKETH|YOYOETH|XRPBTC|XRPETH|MODBTC|MODETH|ENJBTC|ENJETH|STORJBTC|STORJETH|BNBUSDT|VENBNB|YOYOBNB|POWRBNB|VENBTC|VENETH|KMDBTC|KMDETH|NULSBNB|RCNBTC|RCNETH|RCNBNB|NULSBTC|NULSETH|RDNBTC|RDNETH|RDNBNB|XMRBTC|XMRETH|DLTBNB|WTCBNB|DLTBTC|DLTETH|AMBBTC|AMBETH|AMBBNB|BCCETH|BCCUSDT|BCCBNB|BATBTC|BATETH|BATBNB|BCPTBTC|BCPTETH|BCPTBNB|ARNBTC|ARNETH|GVTBTC|GVTETH|CDTBTC|CDTETH|GXSBTC|GXSETH|NEOUSDT|NEOBNB|POEBTC|POEETH|QSPBTC|QSPETH|QSPBNB|BTSBTC|BTSETH|BTSBNB|XZCBTC|XZCETH|XZCBNB|LSKBTC|LSKETH|LSKBNB|TNTBTC|TNTETH|FUELBTC|FUELETH|MANABTC|MANAETH|BCDBTC|BCDETH|DGDBTC|DGDETH|IOTABNB|ADXBTC|ADXETH|ADXBNB|ADABTC|ADAETH|PPTBTC|PPTETH|CMTBTC|CMTETH|CMTBNB|XLMBTC|XLMETH|XLMBNB|CNDBTC|CNDETH|CNDBNB|LENDBTC|LENDETH|WABIBTC|WABIETH|WABIBNB|LTCETH|LTCUSDT|LTCBNB|TNBBTC|TNBETH|WAVESBTC|WAVESETH|WAVESBNB|GTOBTC|GTOETH|GTOBNB|ICXBTC|ICXETH|ICXBNB|OSTBTC|OSTETH|OSTBNB|ELFBTC|ELFETH|AIONBTC|AIONETH|AIONBNB|NEBLBTC|NEBLETH|NEBLBNB|BRDBTC|BRDETH|BRDBNB|MCOBNB|EDOBTC|EDOETH|WINGSBTC|WINGSETH|NAVBTC|NAVETH|NAVBNB|LUNBTC|LUNETH|TRIGBTC|TRIGETH|TRIGBNB|APPCBTC|APPCETH|APPCBNB|VIBEBTC|VIBEETH|RLCBTC|RLCETH|RLCBNB|INSBTC|INSETH|PIVXBTC|PIVXETH|PIVXBNB|IOSTBTC|IOSTETH|CHATBTC|CHATETH|STEEMBTC|STEEMETH|STEEMBNB|NANOBTC|NANOETH|NANOBNB|VIABTC|VIAETH|VIABNB|BLZBTC|BLZETH|BLZBNB|AEBTC|AEETH|AEBNB|RPXBTC|RPXETH|RPXBNB|NCASHBTC|NCASHETH|NCASHBNB|POABTC|POAETH|POABNB|ZILBTC|ZILETH|ZILBNB|ONTBTC|ONTETH|ONTBNB|STORMBTC|STORMETH|STORMBNB|QTUMBNB|QTUMUSDT|XEMBTC|XEMETH|XEMBNB|WANBTC|WANETH|WANBNB|WPRBTC|WPRETH|QLCBTC|QLCETH|SYSBTC|SYSETH|SYSBNB|QLCBNB|GRSBTC|GRSETH|ADAUSDT|ADABNB|CLOAKBTC|CLOAKETH|GNTBTC|GNTETH|GNTBNB|LOOMBTC|LOOMETH|LOOMBNB|XRPUSDT|BCNBTC|BCNETH|BCNBNB|REPBTC|REPETH|REPBNB|TUSDBTC|TUSDETH|TUSDBNB|ZENBTC|ZENETH|ZENBNB|SKYBTC|SKYETH|SKYBNB|EOSUSDT|EOSBNB|CVCBTC|CVCETH|CVCBNB|THETABTC|THETAETH|THETABNB|XRPBNB|TUSDUSDT|IOTAUSDT|XLMUSDT|IOTXBTC|IOTXETH|QKCBTC|QKCETH|AGIBTC|AGIETH|AGIBNB|NXSBTC|NXSETH|NXSBNB|ENJBNB|DATABTC|DATAETH|ONTUSDT|TRXUSDT|ETCUSDT|ETCBNB|ICXUSDT|SCBTC|SCETH|SCBNB|NPXSBTC|NPXSETH|VENUSDT|KEYBTC|KEYETH|NASBTC|NASETH|NASBNB|</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -6274,59 +6204,59 @@
       </c>
       <c r="B9" s="2">
         <f>RTD(progId,,BINANCE,$A9,B$4)</f>
-        <v>4.8419999999999999E-3</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="C9" s="2">
         <f>RTD(progId,,BINANCE,$A9,C$4)</f>
-        <v>4.9890000000000004E-3</v>
+        <v>5.8349999999999999E-3</v>
       </c>
       <c r="D9" s="2">
         <f>RTD(progId,,BINANCE_24H,$A9,D$4)</f>
-        <v>4.8979999999999996E-3</v>
+        <v>5.5030000000000001E-3</v>
       </c>
       <c r="G9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,G$4)</f>
-        <v>4.8859999999999997E-3</v>
+        <v>5.5030000000000001E-3</v>
       </c>
       <c r="H9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,H$4)</f>
-        <v>81.09</v>
+        <v>2.48</v>
       </c>
       <c r="I9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,I$4)</f>
-        <v>4.9579999999999997E-3</v>
+        <v>5.6169999999999996E-3</v>
       </c>
       <c r="J9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,J$4)</f>
-        <v>6.9999999999999999E-6</v>
+        <v>1.1E-5</v>
       </c>
       <c r="K9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,K$4)</f>
-        <v>4.9649999999999998E-3</v>
+        <v>5.6259999999999999E-3</v>
       </c>
       <c r="L9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,L$4)</f>
-        <v>3.87</v>
+        <v>98.8</v>
       </c>
       <c r="M9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,M$4)</f>
-        <v>296294.64</v>
-      </c>
-      <c r="N9" s="40">
+        <v>598657.79</v>
+      </c>
+      <c r="N9" s="42">
         <f>RTD(progId,,BINANCE_24H,$A9,N$4)</f>
-        <v>1455.25969192</v>
+        <v>3367.3331261399999</v>
       </c>
       <c r="O9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,O$4)</f>
-        <v>31665</v>
+        <v>68913</v>
       </c>
       <c r="P9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,P$4)</f>
-        <v>1.2449999999999999E-2</v>
+        <v>2.0889999999999999E-2</v>
       </c>
       <c r="Q9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,Q$4)</f>
-        <v>6.0999999999999999E-5</v>
+        <v>1.16E-4</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6335,59 +6265,59 @@
       </c>
       <c r="B10" s="2">
         <f>RTD(progId,,BINANCE,$A10,B$4)</f>
-        <v>7.483E-5</v>
+        <v>7.3609999999999995E-5</v>
       </c>
       <c r="C10" s="2">
         <f>RTD(progId,,BINANCE,$A10,C$4)</f>
-        <v>7.695E-5</v>
+        <v>7.8139999999999994E-5</v>
       </c>
       <c r="D10" s="2">
         <f>RTD(progId,,BINANCE_24H,$A10,D$4)</f>
-        <v>7.5389999999999995E-5</v>
+        <v>7.4129999999999997E-5</v>
       </c>
       <c r="G10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,G$4)</f>
-        <v>7.5480000000000002E-5</v>
+        <v>7.4120000000000002E-5</v>
       </c>
       <c r="H10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,H$4)</f>
-        <v>617</v>
+        <v>356</v>
       </c>
       <c r="I10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,I$4)</f>
-        <v>7.6719999999999997E-5</v>
+        <v>7.483E-5</v>
       </c>
       <c r="J10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,J$4)</f>
-        <v>4.9999999999999998E-8</v>
+        <v>8.9999999999999999E-8</v>
       </c>
       <c r="K10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,K$4)</f>
-        <v>7.682E-5</v>
+        <v>7.4870000000000007E-5</v>
       </c>
       <c r="L10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,L$4)</f>
-        <v>1857</v>
+        <v>780</v>
       </c>
       <c r="M10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,M$4)</f>
-        <v>31805978</v>
-      </c>
-      <c r="N10" s="40">
+        <v>51677984</v>
+      </c>
+      <c r="N10" s="42">
         <f>RTD(progId,,BINANCE_24H,$A10,N$4)</f>
-        <v>2413.62485118</v>
+        <v>3901.26588558</v>
       </c>
       <c r="O10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,O$4)</f>
-        <v>26312</v>
+        <v>53832</v>
       </c>
       <c r="P10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,P$4)</f>
-        <v>1.83E-2</v>
+        <v>8.2199999999999999E-3</v>
       </c>
       <c r="Q10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,Q$4)</f>
-        <v>1.4100000000000001E-6</v>
+        <v>7.0999999999999998E-7</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6396,59 +6326,59 @@
       </c>
       <c r="B11" s="2">
         <f>RTD(progId,,BINANCE,$A11,B$4)</f>
-        <v>6.1199999999999999E-6</v>
+        <v>5.8300000000000001E-6</v>
       </c>
       <c r="C11" s="2">
         <f>RTD(progId,,BINANCE,$A11,C$4)</f>
-        <v>6.4799999999999998E-6</v>
+        <v>6.1399999999999997E-6</v>
       </c>
       <c r="D11" s="2">
         <f>RTD(progId,,BINANCE_24H,$A11,D$4)</f>
-        <v>6.2199999999999997E-6</v>
+        <v>6.0299999999999999E-6</v>
       </c>
       <c r="G11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,G$4)</f>
-        <v>6.2500000000000003E-6</v>
+        <v>6.0299999999999999E-6</v>
       </c>
       <c r="H11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,H$4)</f>
-        <v>277254</v>
+        <v>325948</v>
       </c>
       <c r="I11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,I$4)</f>
-        <v>6.3300000000000004E-6</v>
+        <v>5.93E-6</v>
       </c>
       <c r="J11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,J$4)</f>
-        <v>2E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="K11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,K$4)</f>
-        <v>6.3500000000000002E-6</v>
+        <v>5.9399999999999999E-6</v>
       </c>
       <c r="L11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,L$4)</f>
-        <v>38856</v>
+        <v>62318</v>
       </c>
       <c r="M11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,M$4)</f>
-        <v>315445343</v>
-      </c>
-      <c r="N11" s="40">
+        <v>572222720</v>
+      </c>
+      <c r="N11" s="42">
         <f>RTD(progId,,BINANCE_24H,$A11,N$4)</f>
-        <v>1987.3001538000001</v>
+        <v>3426.7021633099998</v>
       </c>
       <c r="O11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,O$4)</f>
-        <v>31617</v>
+        <v>42575</v>
       </c>
       <c r="P11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,P$4)</f>
-        <v>1.7659999999999999E-2</v>
+        <v>-1.4930000000000001E-2</v>
       </c>
       <c r="Q11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,Q$4)</f>
-        <v>1.1000000000000001E-7</v>
+        <v>-8.9999999999999999E-8</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6536,22 +6466,22 @@
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C15)</f>
-        <v>0.45286999999999999</v>
+        <v>0.756328</v>
       </c>
       <c r="B15" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C15)</f>
-        <v>6120.31</v>
+        <v>6593.27</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
       </c>
       <c r="D15" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C15)</f>
-        <v>6120.32</v>
+        <v>6597.97</v>
       </c>
       <c r="E15" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C15)</f>
-        <v>2.0010000000000002E-3</v>
+        <v>6.4515000000000003E-2</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -6559,15 +6489,15 @@
       </c>
       <c r="H15" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G15,H$14)</f>
-        <v>26430861</v>
+        <v>27042665</v>
       </c>
       <c r="I15" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G15,I$14)</f>
-        <v>437.27</v>
+        <v>468.93</v>
       </c>
       <c r="J15" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G15,J$14)</f>
-        <v>0.40221000000000001</v>
+        <v>1.403</v>
       </c>
       <c r="K15" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G15,K$14)</f>
@@ -6575,7 +6505,7 @@
       </c>
       <c r="L15" s="28">
         <f>RTD(progId,,BINACE_TRADE,$G15,L$14)</f>
-        <v>43278.964961307873</v>
+        <v>43284.722217199072</v>
       </c>
       <c r="N15" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G15,N$14)</f>
@@ -6613,11 +6543,11 @@
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C16)</f>
-        <v>0.98260999999999998</v>
+        <v>1.6233999999999998E-2</v>
       </c>
       <c r="B16" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C16)</f>
-        <v>6120.3</v>
+        <v>6593.26</v>
       </c>
       <c r="C16" s="8">
         <f>C15+1</f>
@@ -6625,11 +6555,11 @@
       </c>
       <c r="D16" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C16)</f>
-        <v>6123.82</v>
+        <v>6597.98</v>
       </c>
       <c r="E16" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C16)</f>
-        <v>2</v>
+        <v>1.707E-3</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
@@ -6637,15 +6567,15 @@
       </c>
       <c r="H16" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G16,H$14)</f>
-        <v>47162353</v>
+        <v>48261642</v>
       </c>
       <c r="I16" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G16,I$14)</f>
-        <v>6120.31</v>
+        <v>6593.27</v>
       </c>
       <c r="J16" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G16,J$14)</f>
-        <v>9.9999999999999995E-7</v>
+        <v>1.707E-3</v>
       </c>
       <c r="K16" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G16,K$14)</f>
@@ -6653,7 +6583,7 @@
       </c>
       <c r="L16" s="28">
         <f>RTD(progId,,BINACE_TRADE,$G16,L$14)</f>
-        <v>43278.964959756944</v>
+        <v>43284.722259803239</v>
       </c>
       <c r="N16" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G16,N$14)</f>
@@ -6691,11 +6621,11 @@
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C17)</f>
-        <v>0.131438</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="B17" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C17)</f>
-        <v>6118.72</v>
+        <v>6593.18</v>
       </c>
       <c r="C17" s="8">
         <f t="shared" ref="C17:C24" si="0">C16+1</f>
@@ -6703,11 +6633,11 @@
       </c>
       <c r="D17" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C17)</f>
-        <v>6124.22</v>
+        <v>6597.99</v>
       </c>
       <c r="E17" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C17)</f>
-        <v>0.117368</v>
+        <v>0.91054900000000005</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -6715,23 +6645,23 @@
       </c>
       <c r="H17" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G17,H$14)</f>
-        <v>7365223</v>
+        <v>7519854</v>
       </c>
       <c r="I17" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G17,I$14)</f>
-        <v>80.52</v>
+        <v>87.17</v>
       </c>
       <c r="J17" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G17,J$14)</f>
-        <v>10.11631</v>
+        <v>2.7E-4</v>
       </c>
       <c r="K17" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G17,K$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G17,L$14)</f>
-        <v>43278.964950520836</v>
+        <v>43284.72225363426</v>
       </c>
       <c r="N17" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G17,N$14)</f>
@@ -6769,11 +6699,11 @@
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C18)</f>
-        <v>0.28172999999999998</v>
+        <v>1.7946E-2</v>
       </c>
       <c r="B18" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C18)</f>
-        <v>6117.53</v>
+        <v>6593.14</v>
       </c>
       <c r="C18" s="8">
         <f t="shared" si="0"/>
@@ -6781,11 +6711,11 @@
       </c>
       <c r="D18" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C18)</f>
-        <v>6124.26</v>
+        <v>6599.61</v>
       </c>
       <c r="E18" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C18)</f>
-        <v>9.7145999999999996E-2</v>
+        <v>0.111301</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
@@ -6793,23 +6723,23 @@
       </c>
       <c r="H18" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G18,H$14)</f>
-        <v>1309729</v>
+        <v>1428847</v>
       </c>
       <c r="I18" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G18,I$14)</f>
-        <v>0.46751999999999999</v>
+        <v>0.49326999999999999</v>
       </c>
       <c r="J18" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G18,J$14)</f>
-        <v>3073</v>
+        <v>2466</v>
       </c>
       <c r="K18" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G18,K$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G18,L$14)</f>
-        <v>43278.964962256941</v>
+        <v>43284.722218692128</v>
       </c>
       <c r="N18" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G18,N$14)</f>
@@ -6847,11 +6777,11 @@
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C19)</f>
-        <v>0.13</v>
+        <v>0.62049699999999997</v>
       </c>
       <c r="B19" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C19)</f>
-        <v>6117.21</v>
+        <v>6593.03</v>
       </c>
       <c r="C19" s="8">
         <f t="shared" si="0"/>
@@ -6859,11 +6789,11 @@
       </c>
       <c r="D19" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C19)</f>
-        <v>6124.39</v>
+        <v>6599.98</v>
       </c>
       <c r="E19" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C19)</f>
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
@@ -6871,15 +6801,15 @@
       </c>
       <c r="H19" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G19,H$14)</f>
-        <v>14265123</v>
+        <v>14520756</v>
       </c>
       <c r="I19" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G19,I$14)</f>
-        <v>4.9329999999999999E-3</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="J19" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G19,J$14)</f>
-        <v>1.94</v>
+        <v>1.5</v>
       </c>
       <c r="K19" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G19,K$14)</f>
@@ -6887,7 +6817,7 @@
       </c>
       <c r="L19" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G19,L$14)</f>
-        <v>43278.964934884258</v>
+        <v>43284.722140613427</v>
       </c>
       <c r="N19" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G19,N$14)</f>
@@ -6925,11 +6855,11 @@
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C20)</f>
-        <v>1.2006349999999999</v>
+        <v>1.9989999999999999E-3</v>
       </c>
       <c r="B20" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C20)</f>
-        <v>6116.54</v>
+        <v>6591.89</v>
       </c>
       <c r="C20" s="8">
         <f t="shared" si="0"/>
@@ -6937,11 +6867,11 @@
       </c>
       <c r="D20" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C20)</f>
-        <v>6125</v>
+        <v>6599.99</v>
       </c>
       <c r="E20" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C20)</f>
-        <v>6.1490999999999997E-2</v>
+        <v>0.56970900000000002</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
@@ -6949,23 +6879,23 @@
       </c>
       <c r="H20" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G20,H$14)</f>
-        <v>18374353</v>
+        <v>18577123</v>
       </c>
       <c r="I20" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G20,I$14)</f>
-        <v>7.6279999999999995E-5</v>
+        <v>7.4930000000000003E-5</v>
       </c>
       <c r="J20" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G20,J$14)</f>
-        <v>125</v>
+        <v>24</v>
       </c>
       <c r="K20" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G20,K$14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G20,L$14)</f>
-        <v>43278.964883043984</v>
+        <v>43284.722096273152</v>
       </c>
       <c r="N20" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G20,N$14)</f>
@@ -7003,11 +6933,11 @@
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C21)</f>
-        <v>1.402452</v>
+        <v>0.48682999999999998</v>
       </c>
       <c r="B21" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C21)</f>
-        <v>6116.44</v>
+        <v>6591.4</v>
       </c>
       <c r="C21" s="8">
         <f t="shared" si="0"/>
@@ -7015,11 +6945,11 @@
       </c>
       <c r="D21" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C21)</f>
-        <v>6126.03</v>
+        <v>6600</v>
       </c>
       <c r="E21" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C21)</f>
-        <v>2.3491000000000001E-2</v>
+        <v>1.0923020000000001</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
@@ -7027,23 +6957,23 @@
       </c>
       <c r="H21" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G21,H$14)</f>
-        <v>18989603</v>
+        <v>19221669</v>
       </c>
       <c r="I21" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G21,I$14)</f>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
       </c>
       <c r="J21" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G21,J$14)</f>
-        <v>16708</v>
+        <v>2277</v>
       </c>
       <c r="K21" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G21,K$14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G21,L$14)</f>
-        <v>43278.964896064812</v>
+        <v>43284.722241087962</v>
       </c>
       <c r="N21" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G21,N$14)</f>
@@ -7081,11 +7011,11 @@
     <row r="22" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C22)</f>
-        <v>2.14E-3</v>
+        <v>0.1</v>
       </c>
       <c r="B22" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C22)</f>
-        <v>6115.77</v>
+        <v>6590.01</v>
       </c>
       <c r="C22" s="8">
         <f t="shared" si="0"/>
@@ -7093,21 +7023,21 @@
       </c>
       <c r="D22" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C22)</f>
-        <v>6128</v>
+        <v>6601.54</v>
       </c>
       <c r="E22" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C22)</f>
-        <v>5.0000000000000001E-3</v>
+        <v>0.79949999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C23)</f>
-        <v>9.4579999999999994E-3</v>
+        <v>11.064577</v>
       </c>
       <c r="B23" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C23)</f>
-        <v>6114.46</v>
+        <v>6590</v>
       </c>
       <c r="C23" s="8">
         <f t="shared" si="0"/>
@@ -7115,11 +7045,11 @@
       </c>
       <c r="D23" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C23)</f>
-        <v>6128.68</v>
+        <v>6603</v>
       </c>
       <c r="E23" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C23)</f>
-        <v>0.186</v>
+        <v>7.5883999999999993E-2</v>
       </c>
       <c r="G23" s="34" t="s">
         <v>55</v>
@@ -7139,7 +7069,7 @@
       </c>
       <c r="B24" s="31">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C24)</f>
-        <v>6113.33</v>
+        <v>6588.64</v>
       </c>
       <c r="C24" s="32">
         <f t="shared" si="0"/>
@@ -7147,38 +7077,38 @@
       </c>
       <c r="D24" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C24)</f>
-        <v>6129.2</v>
+        <v>6603.78</v>
       </c>
       <c r="E24" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C24)</f>
-        <v>1.7555999999999999E-2</v>
+        <v>4.7562E-2</v>
       </c>
       <c r="G24" s="35" t="str">
         <f>RTD(progId,,BINANCE_HISTORY,J23,"a,b,c",10)</f>
-        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",29655415,441.03000000,0.04725000,"2018-06-27T21:01:30.14-04:00",true,true],["ETHUSDT",29655416,441.15000000,0.03880000,"2018-06-27T21:01:32.892-04:00",true,false],["ETHUSDT",29655417,441.05000000,0.10000000,"2018-06-27T21:01:36.76-04:00",true,true],["ETHUSDT",29655418,441.07000000,0.10000000,"2018-06-27T21:01:50.891-04:00",true,true],["ETHUSDT",29655419,441.07000000,0.99988000,"2018-06-27T21:01:52.801-04:00",true,true],["ETHUSDT",29655420,441.07000000,3.43110000,"2018-06-27T21:01:52.815-04:00",true,true],["ETHUSDT",29655421,441.08000000,0.18116000,"2018-06-27T21:01:53.605-04:00",true,false],["ETHUSDT",29655422,441.08000000,0.51401000,"2018-06-27T21:01:57.015-04:00",true,false],["ETHUSDT",29655423,441.08000000,0.23800000,"2018-06-27T21:01:57.154-04:00",true,false],["ETHUSDT",29655424,441.07000000,0.00005000,"2018-06-27T21:02:00.108-04:00",true,true]]</v>
+        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",30325041,468.88000000,0.15959000,"2018-07-03T17:17:31.738-04:00",true,true],["ETHUSDT",30325042,468.88000000,0.00041000,"2018-07-03T17:17:37.266-04:00",true,true],["ETHUSDT",30325043,468.86000000,2.08320000,"2018-07-03T17:17:39.711-04:00",true,false],["ETHUSDT",30325044,468.75000000,0.03180000,"2018-07-03T17:17:41.766-04:00",true,true],["ETHUSDT",30325045,468.75000000,0.16820000,"2018-07-03T17:17:41.766-04:00",true,true],["ETHUSDT",30325046,468.75000000,0.15428000,"2018-07-03T17:17:43.196-04:00",true,true],["ETHUSDT",30325047,468.86000000,4.75865000,"2018-07-03T17:17:47.152-04:00",true,false],["ETHUSDT",30325048,468.97000000,4.17426000,"2018-07-03T17:17:47.17-04:00",true,false],["ETHUSDT",30325049,468.77000000,0.09950000,"2018-07-03T17:17:48.792-04:00",true,true],["ETHUSDT",30325050,468.95000000,0.02592000,"2018-07-03T17:17:52.165-04:00",true,false]]</v>
       </c>
       <c r="H24"/>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <f>SUM(Table3[BID_DEPTH_SIZE])</f>
-        <v>5.5933330000000003</v>
+        <v>14.120411000000001</v>
       </c>
       <c r="B25" s="14">
         <f>SUMPRODUCT(Table3[BID_DEPTH_SIZE],Table3[BID_DEPTH])</f>
-        <v>34214.527943219997</v>
+        <v>93057.475481860005</v>
       </c>
       <c r="C25" s="39">
         <f>B25-D25</f>
-        <v>18719.700907049999</v>
+        <v>68617.859737060004</v>
       </c>
       <c r="D25" s="14">
         <f>SUMPRODUCT(Table3[ASK_DEPTH_SIZE],Table3[ASK_DEPTH])</f>
-        <v>15494.827036169998</v>
+        <v>24439.615744800001</v>
       </c>
       <c r="E25" s="12">
         <f>SUM(Table3[ASK_DEPTH_SIZE])</f>
-        <v>2.5300529999999997</v>
+        <v>3.7030290000000003</v>
       </c>
       <c r="F25" s="9"/>
       <c r="H25" s="1"/>
@@ -7189,14 +7119,14 @@
     <row r="26" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="30">
         <f>B15-B24</f>
-        <v>6.9800000000004729</v>
+        <v>4.6300000000001091</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D26" s="30">
         <f>D15-D24</f>
-        <v>-8.8800000000001091</v>
+        <v>-5.8099999999994907</v>
       </c>
       <c r="F26" s="9"/>
       <c r="I26" s="4"/>
@@ -7282,27 +7212,27 @@
       </c>
       <c r="B30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,B$29,$D$28)</f>
-        <v>436.19</v>
+        <v>470.45</v>
       </c>
       <c r="C30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,C$29,$D$28)</f>
-        <v>437.69</v>
+        <v>471.31</v>
       </c>
       <c r="D30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,D$29,$D$28)</f>
-        <v>436.18</v>
+        <v>467.93</v>
       </c>
       <c r="E30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,E$29,$D$28)</f>
-        <v>437.21</v>
+        <v>468.93</v>
       </c>
       <c r="F30" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,F$29,$D$28)</f>
-        <v>43278.958333333336</v>
+        <v>43284.708333333336</v>
       </c>
       <c r="G30" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,G$29,$D$28)</f>
-        <v>43278.999999988424</v>
+        <v>43284.749999988424</v>
       </c>
       <c r="H30" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,H$29,$D$28)</f>
@@ -7310,19 +7240,19 @@
       </c>
       <c r="I30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,I$29,$D$28)</f>
-        <v>205944.56736799999</v>
+        <v>674654.7416978</v>
       </c>
       <c r="J30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,J$29,$D$28)</f>
-        <v>471.63035000000002</v>
+        <v>1437.56467</v>
       </c>
       <c r="K30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,K$29,$D$28)</f>
-        <v>337.96368999999999</v>
+        <v>791.60347999999999</v>
       </c>
       <c r="L30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,L$29,$D$28)</f>
-        <v>147569.46521630001</v>
+        <v>371589.88051839999</v>
       </c>
       <c r="M30" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,M$29,$D$28)</f>
@@ -7330,19 +7260,19 @@
       </c>
       <c r="N30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,N$29,$D$28)</f>
-        <v>522</v>
+        <v>1228</v>
       </c>
       <c r="O30" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,O$29,$D$28)</f>
-        <v>43278.96496135417</v>
+        <v>43284.722217222225</v>
       </c>
       <c r="P30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,P$29,$D$28)</f>
-        <v>29660901</v>
+        <v>30323933</v>
       </c>
       <c r="Q30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,Q$29,$D$28)</f>
-        <v>29661422</v>
+        <v>30325160</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -7351,27 +7281,27 @@
       </c>
       <c r="B31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,B$29,$D$28)</f>
-        <v>6112</v>
+        <v>6612.96</v>
       </c>
       <c r="C31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,C$29,$D$28)</f>
-        <v>6124.22</v>
+        <v>6622</v>
       </c>
       <c r="D31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,D$29,$D$28)</f>
-        <v>6112</v>
+        <v>6586.03</v>
       </c>
       <c r="E31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,E$29,$D$28)</f>
-        <v>6120.31</v>
+        <v>6596</v>
       </c>
       <c r="F31" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,F$29,$D$28)</f>
-        <v>43278.958333333336</v>
+        <v>43284.708333333336</v>
       </c>
       <c r="G31" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,G$29,$D$28)</f>
-        <v>43278.999999988424</v>
+        <v>43284.749999988424</v>
       </c>
       <c r="H31" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,H$29,$D$28)</f>
@@ -7379,19 +7309,19 @@
       </c>
       <c r="I31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,I$29,$D$28)</f>
-        <v>658826.19390307995</v>
+        <v>2392227.0247127102</v>
       </c>
       <c r="J31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,J$29,$D$28)</f>
-        <v>107.72978999999999</v>
+        <v>362.47585800000002</v>
       </c>
       <c r="K31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,K$29,$D$28)</f>
-        <v>66.647732000000005</v>
+        <v>186.756066</v>
       </c>
       <c r="L31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,L$29,$D$28)</f>
-        <v>407601.03467939998</v>
+        <v>1232565.7239691401</v>
       </c>
       <c r="M31" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,M$29,$D$28)</f>
@@ -7399,19 +7329,19 @@
       </c>
       <c r="N31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,N$29,$D$28)</f>
-        <v>669</v>
+        <v>2737</v>
       </c>
       <c r="O31" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,O$29,$D$28)</f>
-        <v>43278.96493736111</v>
+        <v>43284.722245023149</v>
       </c>
       <c r="P31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,P$29,$D$28)</f>
-        <v>53576359</v>
+        <v>54781604</v>
       </c>
       <c r="Q31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,Q$29,$D$28)</f>
-        <v>53577027</v>
+        <v>54784340</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -7420,27 +7350,27 @@
       </c>
       <c r="B32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,B$29,$D$28)</f>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
       </c>
       <c r="C32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,C$29,$D$28)</f>
-        <v>6.3400000000000003E-6</v>
+        <v>5.9699999999999996E-6</v>
       </c>
       <c r="D32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,D$29,$D$28)</f>
-        <v>6.2999999999999998E-6</v>
+        <v>5.9200000000000001E-6</v>
       </c>
       <c r="E32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,E$29,$D$28)</f>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
       </c>
       <c r="F32" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,F$29,$D$28)</f>
-        <v>43278.958333333336</v>
+        <v>43284.708333333336</v>
       </c>
       <c r="G32" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,G$29,$D$28)</f>
-        <v>43278.999999988424</v>
+        <v>43284.749999988424</v>
       </c>
       <c r="H32" s="18" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,H$29,$D$28)</f>
@@ -7448,19 +7378,19 @@
       </c>
       <c r="I32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,I$29,$D$28)</f>
-        <v>10.75266519</v>
+        <v>58.244677230000001</v>
       </c>
       <c r="J32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,J$29,$D$28)</f>
-        <v>1703752</v>
+        <v>9791683</v>
       </c>
       <c r="K32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,K$29,$D$28)</f>
-        <v>402711</v>
+        <v>5257284</v>
       </c>
       <c r="L32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,L$29,$D$28)</f>
-        <v>2.54358087</v>
+        <v>31.2854311</v>
       </c>
       <c r="M32" s="18" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,M$29,$D$28)</f>
@@ -7468,19 +7398,19 @@
       </c>
       <c r="N32" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,N$29,$D$28)</f>
-        <v>148</v>
+        <v>543</v>
       </c>
       <c r="O32" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,O$29,$D$28)</f>
-        <v>43278.964896134261</v>
+        <v>43284.722241145835</v>
       </c>
       <c r="P32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,P$29,$D$28)</f>
-        <v>30503158</v>
+        <v>30862414</v>
       </c>
       <c r="Q32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,Q$29,$D$28)</f>
-        <v>30503305</v>
+        <v>30862956</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -7559,27 +7489,27 @@
       </c>
       <c r="B36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,B$35,$D$34)</f>
-        <v>437.5</v>
+        <v>468.92</v>
       </c>
       <c r="C36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,C$35,$D$34)</f>
-        <v>437.5</v>
+        <v>468.98</v>
       </c>
       <c r="D36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,D$35,$D$34)</f>
-        <v>437</v>
+        <v>467.93</v>
       </c>
       <c r="E36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,E$35,$D$34)</f>
-        <v>437.21</v>
+        <v>468.93</v>
       </c>
       <c r="F36" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,F$35,$D$34)</f>
-        <v>43278.964583333334</v>
+        <v>43284.72152777778</v>
       </c>
       <c r="G36" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,G$35,$D$34)</f>
-        <v>43278.965277766205</v>
+        <v>43284.72222221065</v>
       </c>
       <c r="H36" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,H$35,$D$34)</f>
@@ -7587,19 +7517,19 @@
       </c>
       <c r="I36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,I$35,$D$34)</f>
-        <v>5102.0120073999997</v>
+        <v>62870.438001199997</v>
       </c>
       <c r="J36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,J$35,$D$34)</f>
-        <v>11.668279999999999</v>
+        <v>134.20161999999999</v>
       </c>
       <c r="K36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,K$35,$D$34)</f>
-        <v>7.6538199999999996</v>
+        <v>48.726190000000003</v>
       </c>
       <c r="L36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,L$35,$D$34)</f>
-        <v>3347.0526055</v>
+        <v>22830.8364043</v>
       </c>
       <c r="M36" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,M$35,$D$34)</f>
@@ -7607,19 +7537,19 @@
       </c>
       <c r="N36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,N$35,$D$34)</f>
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="O36" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,O$35,$D$34)</f>
-        <v>43278.96496135417</v>
+        <v>43284.722217222225</v>
       </c>
       <c r="P36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,P$35,$D$34)</f>
-        <v>29661384</v>
+        <v>30325099</v>
       </c>
       <c r="Q36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,Q$35,$D$34)</f>
-        <v>29661422</v>
+        <v>30325160</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7628,27 +7558,27 @@
       </c>
       <c r="B37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,B$35,$D$34)</f>
-        <v>6121.85</v>
+        <v>6596</v>
       </c>
       <c r="C37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,C$35,$D$34)</f>
-        <v>6124.22</v>
+        <v>6597.99</v>
       </c>
       <c r="D37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,D$35,$D$34)</f>
-        <v>6120.31</v>
+        <v>6593.27</v>
       </c>
       <c r="E37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,E$35,$D$34)</f>
-        <v>6120.31</v>
+        <v>6593.27</v>
       </c>
       <c r="F37" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,F$35,$D$34)</f>
-        <v>43278.964583333334</v>
+        <v>43284.722222222219</v>
       </c>
       <c r="G37" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,G$35,$D$34)</f>
-        <v>43278.965277766205</v>
+        <v>43284.72291665509</v>
       </c>
       <c r="H37" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,H$35,$D$34)</f>
@@ -7656,19 +7586,19 @@
       </c>
       <c r="I37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,I$35,$D$34)</f>
-        <v>11659.568683519999</v>
+        <v>1797.6540783099999</v>
       </c>
       <c r="J37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,J$35,$D$34)</f>
-        <v>1.9042159999999999</v>
+        <v>0.27246199999999998</v>
       </c>
       <c r="K37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,K$35,$D$34)</f>
-        <v>1.3622460000000001</v>
+        <v>0.22354499999999999</v>
       </c>
       <c r="L37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,L$35,$D$34)</f>
-        <v>8341.6207168599994</v>
+        <v>1474.9476208200001</v>
       </c>
       <c r="M37" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,M$35,$D$34)</f>
@@ -7676,19 +7606,19 @@
       </c>
       <c r="N37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,N$35,$D$34)</f>
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="O37" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,O$35,$D$34)</f>
-        <v>43278.96493736111</v>
+        <v>43284.722259895832</v>
       </c>
       <c r="P37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,P$35,$D$34)</f>
-        <v>53576988</v>
+        <v>54784340</v>
       </c>
       <c r="Q37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,Q$35,$D$34)</f>
-        <v>53577027</v>
+        <v>54784346</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7697,27 +7627,27 @@
       </c>
       <c r="B38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,B$35,$D$34)</f>
-        <v>6.3099999999999997E-6</v>
+        <v>5.9399999999999999E-6</v>
       </c>
       <c r="C38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,C$35,$D$34)</f>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
       </c>
       <c r="D38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,D$35,$D$34)</f>
-        <v>6.2999999999999998E-6</v>
+        <v>5.9399999999999999E-6</v>
       </c>
       <c r="E38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,E$35,$D$34)</f>
-        <v>6.3199999999999996E-6</v>
+        <v>5.9399999999999999E-6</v>
       </c>
       <c r="F38" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,F$35,$D$34)</f>
-        <v>43278.964583333334</v>
+        <v>43284.722222222219</v>
       </c>
       <c r="G38" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,G$35,$D$34)</f>
-        <v>43278.965277766205</v>
+        <v>43284.72291665509</v>
       </c>
       <c r="H38" s="18" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,H$35,$D$34)</f>
@@ -7725,19 +7655,19 @@
       </c>
       <c r="I38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,I$35,$D$34)</f>
-        <v>2.5591176099999999</v>
+        <v>1.352538E-2</v>
       </c>
       <c r="J38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,J$35,$D$34)</f>
-        <v>405317</v>
+        <v>2277</v>
       </c>
       <c r="K38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,K$35,$D$34)</f>
-        <v>19421</v>
+        <v>2277</v>
       </c>
       <c r="L38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,L$35,$D$34)</f>
-        <v>0.12261337999999999</v>
+        <v>1.352538E-2</v>
       </c>
       <c r="M38" s="18" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,M$35,$D$34)</f>
@@ -7745,19 +7675,19 @@
       </c>
       <c r="N38" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,N$35,$D$34)</f>
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="O38" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,O$35,$D$34)</f>
-        <v>43278.964896134261</v>
+        <v>43284.722241145835</v>
       </c>
       <c r="P38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,P$35,$D$34)</f>
-        <v>30503279</v>
+        <v>30862956</v>
       </c>
       <c r="Q38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,Q$35,$D$34)</f>
-        <v>30503305</v>
+        <v>30862956</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -8150,31 +8080,31 @@
       </c>
       <c r="B3" s="2">
         <f>RTD(progId,,GDAX,$A3,B$2)</f>
-        <v>437.34</v>
+        <v>468</v>
       </c>
       <c r="C3" s="2">
         <f>RTD(progId,,GDAX,$A3,C$2)</f>
-        <v>437.35</v>
+        <v>468.01</v>
       </c>
       <c r="D3" s="2">
         <f>RTD(progId,,GDAX,$A3,D$2)</f>
-        <v>437.35</v>
+        <v>468.01</v>
       </c>
       <c r="E3" s="2">
         <f>RTD(progId,,GDAX,$A3,E$2)</f>
-        <v>431.23</v>
+        <v>475.27</v>
       </c>
       <c r="F3" s="2">
         <f>RTD(progId,,GDAX,$A3,F$2)</f>
-        <v>446.21</v>
+        <v>486.76</v>
       </c>
       <c r="G3" s="2">
         <f>RTD(progId,,GDAX,$A3,G$2)</f>
-        <v>420.12</v>
+        <v>461.69</v>
       </c>
       <c r="H3" s="2">
         <f>RTD(progId,,GDAX,$A3,H$2)</f>
-        <v>64914.849068449999</v>
+        <v>68576.476604249998</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8183,31 +8113,31 @@
       </c>
       <c r="B4" s="2">
         <f>RTD(progId,,GDAX,$A4,B$2)</f>
-        <v>6121.59</v>
+        <v>6596.21</v>
       </c>
       <c r="C4" s="2">
         <f>RTD(progId,,GDAX,$A4,C$2)</f>
-        <v>6121.6</v>
+        <v>6596.5</v>
       </c>
       <c r="D4" s="2">
         <f>RTD(progId,,GDAX,$A4,D$2)</f>
-        <v>6121.6</v>
+        <v>6596.5</v>
       </c>
       <c r="E4" s="2">
         <f>RTD(progId,,GDAX,$A4,E$2)</f>
-        <v>6079.99</v>
+        <v>6626.31</v>
       </c>
       <c r="F4" s="2">
         <f>RTD(progId,,GDAX,$A4,F$2)</f>
-        <v>6175.43</v>
+        <v>6673.99</v>
       </c>
       <c r="G4" s="2">
         <f>RTD(progId,,GDAX,$A4,G$2)</f>
-        <v>5983.56</v>
+        <v>6535</v>
       </c>
       <c r="H4" s="2">
         <f>RTD(progId,,GDAX,$A4,H$2)</f>
-        <v>6586.7504915700001</v>
+        <v>6147.1162924800001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
return EXCHANGE_SYMBOLS as Json Array
</commit_message>
<xml_diff>
--- a/doc/crypto.xlsx
+++ b/doc/crypto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\Crypto\crypto-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7412A5CE-1688-4062-A988-8CEDCF4ED0BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6FE897-269A-4AAF-9B6C-4DEE6E248649}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12225" tabRatio="245" xr2:uid="{FA204BA2-54FD-4EAD-B49B-FB8867D94DC8}"/>
   </bookViews>
@@ -2400,7 +2400,7 @@
   <volType type="realTimeData">
     <main first="crypto">
       <tp>
-        <v>42575</v>
+        <v>30240</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -2408,7 +2408,7 @@
         <tr r="O11" s="1"/>
       </tp>
       <tp>
-        <v>58.244677230000001</v>
+        <v>35.743519800000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2417,7 +2417,7 @@
         <tr r="I32" s="1"/>
       </tp>
       <tp>
-        <v>1.352538E-2</v>
+        <v>0.18112928</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2434,7 +2434,7 @@
         <tr r="N19" s="1"/>
       </tp>
       <tp>
-        <v>6622</v>
+        <v>6691.01</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2443,7 +2443,7 @@
         <tr r="C31" s="1"/>
       </tp>
       <tp>
-        <v>6597.99</v>
+        <v>6671.01</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2452,7 +2452,7 @@
         <tr r="C37" s="1"/>
       </tp>
       <tp>
-        <v>471.31</v>
+        <v>474.62</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2461,7 +2461,7 @@
         <tr r="C30" s="1"/>
       </tp>
       <tp>
-        <v>468.98</v>
+        <v>472.62</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2470,7 +2470,7 @@
         <tr r="C36" s="1"/>
       </tp>
       <tp>
-        <v>470.45</v>
+        <v>473.21</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2479,7 +2479,7 @@
         <tr r="B30" s="1"/>
       </tp>
       <tp>
-        <v>468.92</v>
+        <v>472.61</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2488,7 +2488,7 @@
         <tr r="B36" s="1"/>
       </tp>
       <tp>
-        <v>6612.96</v>
+        <v>6683.77</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2497,7 +2497,7 @@
         <tr r="B31" s="1"/>
       </tp>
       <tp>
-        <v>6596</v>
+        <v>6670.01</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2506,7 +2506,7 @@
         <tr r="B37" s="1"/>
       </tp>
       <tp>
-        <v>2737</v>
+        <v>4014</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2515,7 +2515,7 @@
         <tr r="N31" s="1"/>
       </tp>
       <tp>
-        <v>7</v>
+        <v>64</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2524,7 +2524,7 @@
         <tr r="N37" s="1"/>
       </tp>
       <tp>
-        <v>1228</v>
+        <v>2114</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2533,7 +2533,7 @@
         <tr r="N30" s="1"/>
       </tp>
       <tp>
-        <v>62</v>
+        <v>26</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2542,7 +2542,7 @@
         <tr r="N36" s="1"/>
       </tp>
       <tp>
-        <v>-1.4930000000000001E-2</v>
+        <v>-1.6900000000000001E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -2550,7 +2550,7 @@
         <tr r="P11" s="1"/>
       </tp>
       <tp>
-        <v>53832</v>
+        <v>30879</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -2558,7 +2558,7 @@
         <tr r="O10" s="1"/>
       </tp>
       <tp>
-        <v>468.01</v>
+        <v>471.77</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -2574,7 +2574,7 @@
         <tr r="P18" s="1"/>
       </tp>
       <tp>
-        <v>468</v>
+        <v>471.76</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -2582,7 +2582,7 @@
         <tr r="B3" s="2"/>
       </tp>
       <tp>
-        <v>6596.21</v>
+        <v>6663.66</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -2590,7 +2590,7 @@
         <tr r="B4" s="2"/>
       </tp>
       <tp>
-        <v>43284.722222222219</v>
+        <v>43285.51666666667</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2599,7 +2599,7 @@
         <tr r="F38" s="1"/>
       </tp>
       <tp>
-        <v>43284.708333333336</v>
+        <v>43285.5</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2608,7 +2608,7 @@
         <tr r="F32" s="1"/>
       </tp>
       <tp>
-        <v>8.2199999999999999E-3</v>
+        <v>-2.121E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -2616,7 +2616,7 @@
         <tr r="P10" s="1"/>
       </tp>
       <tp>
-        <v>6596.5</v>
+        <v>6663.67</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -2648,7 +2648,7 @@
         <tr r="T16" s="1"/>
       </tp>
       <tp>
-        <v>2.0889999999999999E-2</v>
+        <v>4.7629999999999999E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -2672,7 +2672,7 @@
         <tr r="P16" s="1"/>
       </tp>
       <tp>
-        <v>6535</v>
+        <v>6411.51</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -2680,7 +2680,7 @@
         <tr r="G4" s="2"/>
       </tp>
       <tp>
-        <v>30862956</v>
+        <v>30882892</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2689,7 +2689,7 @@
         <tr r="Q38" s="1"/>
       </tp>
       <tp>
-        <v>30862956</v>
+        <v>30882892</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2698,7 +2698,7 @@
         <tr r="Q32" s="1"/>
       </tp>
       <tp>
-        <v>48.726190000000003</v>
+        <v>6.88591</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2707,7 +2707,7 @@
         <tr r="K36" s="1"/>
       </tp>
       <tp>
-        <v>791.60347999999999</v>
+        <v>1193.0365300000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2716,7 +2716,7 @@
         <tr r="K30" s="1"/>
       </tp>
       <tp>
-        <v>0.22354499999999999</v>
+        <v>2.0317949999999998</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2725,7 +2725,7 @@
         <tr r="K37" s="1"/>
       </tp>
       <tp>
-        <v>186.756066</v>
+        <v>366.14173099999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2734,7 +2734,7 @@
         <tr r="K31" s="1"/>
       </tp>
       <tp>
-        <v>54784346</v>
+        <v>54910928</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2743,7 +2743,7 @@
         <tr r="Q37" s="1"/>
       </tp>
       <tp>
-        <v>54784340</v>
+        <v>54910928</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2784,7 +2784,7 @@
         <tr r="N21" s="1"/>
       </tp>
       <tp>
-        <v>68913</v>
+        <v>51127</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -2800,7 +2800,7 @@
         <tr r="P15" s="1"/>
       </tp>
       <tp>
-        <v>461.69</v>
+        <v>451.35</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -2808,7 +2808,7 @@
         <tr r="G3" s="2"/>
       </tp>
       <tp>
-        <v>30325160</v>
+        <v>30393432</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2817,7 +2817,7 @@
         <tr r="Q30" s="1"/>
       </tp>
       <tp>
-        <v>30325160</v>
+        <v>30393432</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2826,7 +2826,7 @@
         <tr r="Q36" s="1"/>
       </tp>
       <tp>
-        <v>5.4000000000000003E-3</v>
+        <v>5.4349999999999997E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -2834,7 +2834,7 @@
         <tr r="B9" s="1"/>
       </tp>
       <tp>
-        <v>5.8300000000000001E-6</v>
+        <v>5.7699999999999998E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -2842,7 +2842,7 @@
         <tr r="B11" s="1"/>
       </tp>
       <tp>
-        <v>7.3609999999999995E-5</v>
+        <v>7.3490000000000003E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -2898,7 +2898,7 @@
         <tr r="S18" s="1"/>
       </tp>
       <tp>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2907,7 +2907,7 @@
         <tr r="B38" s="1"/>
       </tp>
       <tp>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2932,7 +2932,7 @@
         <tr r="J11" s="1"/>
       </tp>
       <tp>
-        <v>24</v>
+        <v>377</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -2940,7 +2940,7 @@
         <tr r="J20" s="1"/>
       </tp>
       <tp>
-        <v>1</v>
+        <v>5</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2949,7 +2949,7 @@
         <tr r="N38" s="1"/>
       </tp>
       <tp>
-        <v>543</v>
+        <v>500</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2958,7 +2958,7 @@
         <tr r="N32" s="1"/>
       </tp>
       <tp>
-        <v>14520756</v>
+        <v>14554128</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -2966,7 +2966,7 @@
         <tr r="H19" s="1"/>
       </tp>
       <tp>
-        <v>356</v>
+        <v>3086</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -2974,7 +2974,7 @@
         <tr r="H10" s="1"/>
       </tp>
       <tp>
-        <v>21439989.816296</v>
+        <v>14130749.716714</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -2982,7 +2982,7 @@
         <tr r="N8" s="1"/>
       </tp>
       <tp>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2991,7 +2991,7 @@
         <tr r="C38" s="1"/>
       </tp>
       <tp>
-        <v>5.9699999999999996E-6</v>
+        <v>5.9100000000000002E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3008,7 +3008,7 @@
         <tr r="K20" s="1"/>
       </tp>
       <tp>
-        <v>325948</v>
+        <v>1035439</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3016,7 +3016,7 @@
         <tr r="H11" s="1"/>
       </tp>
       <tp>
-        <v>98.8</v>
+        <v>6.58</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3024,7 +3024,7 @@
         <tr r="L9" s="1"/>
       </tp>
       <tp>
-        <v>8.9999999999999999E-8</v>
+        <v>7.0000000000000005E-8</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3032,7 +3032,7 @@
         <tr r="J10" s="1"/>
       </tp>
       <tp>
-        <v>1.24308</v>
+        <v>2.6858599999999999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -3040,7 +3040,7 @@
         <tr r="L5" s="1"/>
       </tp>
       <tp>
-        <v>5.5398800000000001</v>
+        <v>0.56000000000000005</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -3048,15 +3048,15 @@
         <tr r="L7" s="1"/>
       </tp>
       <tp>
-        <v>1.3532390000000001</v>
+        <v>0.26262600000000003</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
         <stp>ASK_SIZE</stp>
         <tr r="L6" s="1"/>
       </tp>
-      <tp>
-        <v>2466</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3064,7 +3064,7 @@
         <tr r="J18" s="1"/>
       </tp>
       <tp>
-        <v>3426.7021633099998</v>
+        <v>2358.1084988900002</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3072,7 +3072,7 @@
         <tr r="N11" s="1"/>
       </tp>
       <tp>
-        <v>3901.26588558</v>
+        <v>2711.1513072399998</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3080,7 +3080,7 @@
         <tr r="N10" s="1"/>
       </tp>
       <tp>
-        <v>1.403</v>
+        <v>0.91744999999999999</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3088,7 +3088,7 @@
         <tr r="J15" s="1"/>
       </tp>
       <tp>
-        <v>1.707E-3</v>
+        <v>0.109002</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3096,7 +3096,7 @@
         <tr r="J16" s="1"/>
       </tp>
       <tp>
-        <v>2.7E-4</v>
+        <v>2.5009299999999999</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3104,7 +3104,7 @@
         <tr r="J17" s="1"/>
       </tp>
       <tp>
-        <v>7.5883999999999993E-2</v>
+        <v>0.57014500000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3113,7 +3113,7 @@
         <tr r="E23" s="1"/>
       </tp>
       <tp>
-        <v>4.7562E-2</v>
+        <v>0.01</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3122,7 +3122,7 @@
         <tr r="E24" s="1"/>
       </tp>
       <tp>
-        <v>0.03</v>
+        <v>0.49435000000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3131,7 +3131,7 @@
         <tr r="E19" s="1"/>
       </tp>
       <tp>
-        <v>0.56970900000000002</v>
+        <v>9.4730999999999996E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3140,7 +3140,7 @@
         <tr r="E20" s="1"/>
       </tp>
       <tp>
-        <v>1.0923020000000001</v>
+        <v>7.5079999999999999E-3</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3149,7 +3149,7 @@
         <tr r="E21" s="1"/>
       </tp>
       <tp>
-        <v>0.79949999999999999</v>
+        <v>0.66981900000000005</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3158,7 +3158,7 @@
         <tr r="E22" s="1"/>
       </tp>
       <tp>
-        <v>6.4515000000000003E-2</v>
+        <v>2.0254000000000001E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3167,7 +3167,7 @@
         <tr r="E15" s="1"/>
       </tp>
       <tp>
-        <v>1.707E-3</v>
+        <v>0.35168100000000002</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3176,7 +3176,7 @@
         <tr r="E16" s="1"/>
       </tp>
       <tp>
-        <v>0.91054900000000005</v>
+        <v>4.7935999999999999E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3185,7 +3185,7 @@
         <tr r="E17" s="1"/>
       </tp>
       <tp>
-        <v>0.111301</v>
+        <v>5.6000000000000001E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3194,7 +3194,7 @@
         <tr r="E18" s="1"/>
       </tp>
       <tp>
-        <v>2277</v>
+        <v>500</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3202,15 +3202,15 @@
         <tr r="J21" s="1"/>
       </tp>
       <tp>
-        <v>1663</v>
+        <v>3292</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
         <stp>ASK_SIZE</stp>
         <tr r="L8" s="1"/>
       </tp>
-      <tp>
-        <v>43284.722218692128</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3218,7 +3218,7 @@
         <tr r="L18" s="1"/>
       </tp>
       <tp>
-        <v>43284.72225363426</v>
+        <v>43285.516921724535</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3226,7 +3226,7 @@
         <tr r="L17" s="1"/>
       </tp>
       <tp>
-        <v>43284.722217199072</v>
+        <v>43285.517101666665</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3234,7 +3234,7 @@
         <tr r="L15" s="1"/>
       </tp>
       <tp>
-        <v>43284.722259803239</v>
+        <v>43285.517102048609</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3242,7 +3242,7 @@
         <tr r="L16" s="1"/>
       </tp>
       <tp t="s">
-        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",30325041,468.88000000,0.15959000,"2018-07-03T17:17:31.738-04:00",true,true],["ETHUSDT",30325042,468.88000000,0.00041000,"2018-07-03T17:17:37.266-04:00",true,true],["ETHUSDT",30325043,468.86000000,2.08320000,"2018-07-03T17:17:39.711-04:00",true,false],["ETHUSDT",30325044,468.75000000,0.03180000,"2018-07-03T17:17:41.766-04:00",true,true],["ETHUSDT",30325045,468.75000000,0.16820000,"2018-07-03T17:17:41.766-04:00",true,true],["ETHUSDT",30325046,468.75000000,0.15428000,"2018-07-03T17:17:43.196-04:00",true,true],["ETHUSDT",30325047,468.86000000,4.75865000,"2018-07-03T17:17:47.152-04:00",true,false],["ETHUSDT",30325048,468.97000000,4.17426000,"2018-07-03T17:17:47.17-04:00",true,false],["ETHUSDT",30325049,468.77000000,0.09950000,"2018-07-03T17:17:48.792-04:00",true,true],["ETHUSDT",30325050,468.95000000,0.02592000,"2018-07-03T17:17:52.165-04:00",true,false]]</v>
+        <v>Server error: {"code":-2015,"msg":"Invalid API-key, IP, or permissions for action."}</v>
         <stp/>
         <stp>BINANCE_HISTORY</stp>
         <stp>ETHUSDT</stp>
@@ -3251,7 +3251,7 @@
         <tr r="G24" s="1"/>
       </tp>
       <tp>
-        <v>18577123</v>
+        <v>18596602</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3259,7 +3259,7 @@
         <tr r="H20" s="1"/>
       </tp>
       <tp>
-        <v>468.93</v>
+        <v>471.3</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3268,7 +3268,7 @@
         <tr r="E36" s="1"/>
       </tp>
       <tp>
-        <v>468.93</v>
+        <v>471.3</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3293,7 +3293,7 @@
         <tr r="S16" s="1"/>
       </tp>
       <tp>
-        <v>62318</v>
+        <v>73326</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3301,7 +3301,7 @@
         <tr r="L11" s="1"/>
       </tp>
       <tp>
-        <v>0.40920000000000001</v>
+        <v>1.537E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -3309,7 +3309,7 @@
         <tr r="H7" s="1"/>
       </tp>
       <tp>
-        <v>0.52357699999999996</v>
+        <v>6.7424999999999999E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -3317,7 +3317,7 @@
         <tr r="H6" s="1"/>
       </tp>
       <tp>
-        <v>1.7000000000000001E-4</v>
+        <v>2.4573100000000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -3325,7 +3325,7 @@
         <tr r="H5" s="1"/>
       </tp>
       <tp>
-        <v>2.48</v>
+        <v>0.03</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3333,7 +3333,7 @@
         <tr r="H9" s="1"/>
       </tp>
       <tp>
-        <v>224411913.22751993</v>
+        <v>191494800.14948204</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -3341,7 +3341,7 @@
         <tr r="N6" s="1"/>
       </tp>
       <tp>
-        <v>15882625.5011223</v>
+        <v>11444940.7380598</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -3349,7 +3349,7 @@
         <tr r="N7" s="1"/>
       </tp>
       <tp>
-        <v>353.5</v>
+        <v>6902.4</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -3357,7 +3357,7 @@
         <tr r="H8" s="1"/>
       </tp>
       <tp>
-        <v>1.5</v>
+        <v>15.4</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -3365,7 +3365,7 @@
         <tr r="J19" s="1"/>
       </tp>
       <tp>
-        <v>6593.27</v>
+        <v>6664.13</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3374,7 +3374,7 @@
         <tr r="E37" s="1"/>
       </tp>
       <tp>
-        <v>6596</v>
+        <v>6664.13</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3391,13 +3391,13 @@
         <tr r="K19" s="1"/>
       </tp>
       <tp>
-        <v>43284.72226396991</v>
+        <v>43285.517097245371</v>
         <stp/>
         <stp>CLOCK</stp>
         <tr r="T4" s="1"/>
       </tp>
       <tp>
-        <v>1.1E-5</v>
+        <v>9.9999999999999995E-7</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3405,7 +3405,7 @@
         <tr r="J9" s="1"/>
       </tp>
       <tp>
-        <v>5257284</v>
+        <v>2043046</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3414,7 +3414,7 @@
         <tr r="K32" s="1"/>
       </tp>
       <tp>
-        <v>2277</v>
+        <v>30752</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3423,7 +3423,7 @@
         <tr r="K38" s="1"/>
       </tp>
       <tp>
-        <v>11.064577</v>
+        <v>3.8E-3</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3432,7 +3432,7 @@
         <tr r="A23" s="1"/>
       </tp>
       <tp>
-        <v>1</v>
+        <v>0.97992699999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3441,7 +3441,7 @@
         <tr r="A24" s="1"/>
       </tp>
       <tp>
-        <v>0.62049699999999997</v>
+        <v>9.0060000000000001E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3450,7 +3450,7 @@
         <tr r="A19" s="1"/>
       </tp>
       <tp>
-        <v>1.9989999999999999E-3</v>
+        <v>4.0910000000000002</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3459,7 +3459,7 @@
         <tr r="A20" s="1"/>
       </tp>
       <tp>
-        <v>0.48682999999999998</v>
+        <v>0.109</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3468,7 +3468,7 @@
         <tr r="A21" s="1"/>
       </tp>
       <tp>
-        <v>0.1</v>
+        <v>4.413157</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3477,7 +3477,7 @@
         <tr r="A22" s="1"/>
       </tp>
       <tp>
-        <v>0.756328</v>
+        <v>1.992E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3486,7 +3486,7 @@
         <tr r="A15" s="1"/>
       </tp>
       <tp>
-        <v>1.6233999999999998E-2</v>
+        <v>0.98658500000000005</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3495,7 +3495,7 @@
         <tr r="A16" s="1"/>
       </tp>
       <tp>
-        <v>5.6000000000000001E-2</v>
+        <v>2.9922629999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3504,7 +3504,7 @@
         <tr r="A17" s="1"/>
       </tp>
       <tp>
-        <v>1.7946E-2</v>
+        <v>5.6000000000000001E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3513,7 +3513,7 @@
         <tr r="A18" s="1"/>
       </tp>
       <tp>
-        <v>6147.1162924800001</v>
+        <v>7532.5732854899998</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -3521,7 +3521,7 @@
         <tr r="H4" s="2"/>
       </tp>
       <tp>
-        <v>68576.476604249998</v>
+        <v>64263.177474869997</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -3554,8 +3554,8 @@
         <stp>5</stp>
         <tr r="H31" s="1"/>
       </tp>
-      <tp>
-        <v>1428847</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3563,14 +3563,14 @@
         <tr r="H18" s="1"/>
       </tp>
       <tp>
-        <v>-935</v>
+        <v>-443</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>DRIFT</stp>
         <tr r="T5" s="1"/>
       </tp>
       <tp>
-        <v>48261642</v>
+        <v>48377931</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3578,7 +3578,7 @@
         <tr r="H16" s="1"/>
       </tp>
       <tp>
-        <v>7519854</v>
+        <v>7533270</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3586,7 +3586,7 @@
         <tr r="H17" s="1"/>
       </tp>
       <tp>
-        <v>27042665</v>
+        <v>27105497</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3594,7 +3594,7 @@
         <tr r="H15" s="1"/>
       </tp>
       <tp>
-        <v>3367.3331261399999</v>
+        <v>2938.16672982</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3602,7 +3602,7 @@
         <tr r="N9" s="1"/>
       </tp>
       <tp>
-        <v>19221669</v>
+        <v>19233907</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3628,7 +3628,7 @@
         <tr r="H30" s="1"/>
       </tp>
       <tp>
-        <v>81175585.563029304</v>
+        <v>56432388.176379703</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -3636,7 +3636,7 @@
         <tr r="N5" s="1"/>
       </tp>
       <tp>
-        <v>780</v>
+        <v>2199</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3644,7 +3644,7 @@
         <tr r="L10" s="1"/>
       </tp>
       <tp>
-        <v>43284.720387337962</v>
+        <v>43285.516620439812</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>EXCHANGE_TIME</stp>
@@ -3675,7 +3675,7 @@
         <tr r="Q19" s="1"/>
       </tp>
       <tp>
-        <v>462.5</v>
+        <v>457</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3691,7 +3691,7 @@
         <tr r="R17" s="1"/>
       </tp>
       <tp>
-        <v>134.20161999999999</v>
+        <v>26.591799999999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3700,7 +3700,7 @@
         <tr r="J36" s="1"/>
       </tp>
       <tp>
-        <v>1437.56467</v>
+        <v>2463.4826800000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3717,7 +3717,7 @@
         <tr r="O21" s="1"/>
       </tp>
       <tp>
-        <v>5.93E-6</v>
+        <v>5.8799999999999996E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3725,7 +3725,7 @@
         <tr r="I11" s="1"/>
       </tp>
       <tp>
-        <v>7.483E-5</v>
+        <v>7.4190000000000006E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3733,7 +3733,7 @@
         <tr r="I10" s="1"/>
       </tp>
       <tp>
-        <v>5.6169999999999996E-3</v>
+        <v>5.8050000000000003E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3765,7 +3765,7 @@
         <tr r="Q17" s="1"/>
       </tp>
       <tp>
-        <v>6519.99</v>
+        <v>6441.11</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3773,7 +3773,7 @@
         <tr r="B6" s="1"/>
       </tp>
       <tp>
-        <v>5.6259999999999999E-3</v>
+        <v>5.8069999999999997E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3781,7 +3781,7 @@
         <tr r="K9" s="1"/>
       </tp>
       <tp>
-        <v>7.4870000000000007E-5</v>
+        <v>7.428E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3789,7 +3789,7 @@
         <tr r="K10" s="1"/>
       </tp>
       <tp>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3812,8 +3812,8 @@
         <stp>QUOTE_ASSET_PRECISION</stp>
         <tr r="S19" s="1"/>
       </tp>
-      <tp>
-        <v>0.49326999999999999</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3821,7 +3821,7 @@
         <tr r="I18" s="1"/>
       </tp>
       <tp>
-        <v>0.52</v>
+        <v>0.50654999999999994</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3829,7 +3829,7 @@
         <tr r="C8" s="1"/>
       </tp>
       <tp>
-        <v>43284.722259895832</v>
+        <v>43285.517102071761</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3838,7 +3838,7 @@
         <tr r="O37" s="1"/>
       </tp>
       <tp>
-        <v>43284.722245023149</v>
+        <v>43285.517102083337</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3847,7 +3847,7 @@
         <tr r="O31" s="1"/>
       </tp>
       <tp>
-        <v>43284.722217222225</v>
+        <v>43285.517101504629</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3856,7 +3856,7 @@
         <tr r="O36" s="1"/>
       </tp>
       <tp>
-        <v>43284.722217222225</v>
+        <v>43285.517101504629</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3865,7 +3865,7 @@
         <tr r="O30" s="1"/>
       </tp>
       <tp>
-        <v>84.75</v>
+        <v>83.64</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3873,7 +3873,7 @@
         <tr r="B7" s="1"/>
       </tp>
       <tp>
-        <v>362.47585800000002</v>
+        <v>717.961096</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3882,7 +3882,7 @@
         <tr r="J31" s="1"/>
       </tp>
       <tp>
-        <v>0.27246199999999998</v>
+        <v>10.200435000000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3891,7 +3891,7 @@
         <tr r="J37" s="1"/>
       </tp>
       <tp>
-        <v>5.8349999999999999E-3</v>
+        <v>6.1910000000000003E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3907,7 +3907,7 @@
         <tr r="U17" s="1"/>
       </tp>
       <tp>
-        <v>9791683</v>
+        <v>6062958</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3916,7 +3916,7 @@
         <tr r="J32" s="1"/>
       </tp>
       <tp>
-        <v>2277</v>
+        <v>30752</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3965,7 +3965,7 @@
         <tr r="P19" s="1"/>
       </tp>
       <tp>
-        <v>6679.35</v>
+        <v>6784.92</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3973,7 +3973,7 @@
         <tr r="C6" s="1"/>
       </tp>
       <tp>
-        <v>90</v>
+        <v>89.01</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3981,7 +3981,7 @@
         <tr r="C7" s="1"/>
       </tp>
       <tp>
-        <v>486.98</v>
+        <v>482.7</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4065,7 +4065,7 @@
         <tr r="T20" s="1"/>
       </tp>
       <tp>
-        <v>54784340</v>
+        <v>54910865</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4074,7 +4074,7 @@
         <tr r="P37" s="1"/>
       </tp>
       <tp>
-        <v>54781604</v>
+        <v>54906915</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4083,7 +4083,7 @@
         <tr r="P31" s="1"/>
       </tp>
       <tp>
-        <v>30325099</v>
+        <v>30393407</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4092,7 +4092,7 @@
         <tr r="P36" s="1"/>
       </tp>
       <tp>
-        <v>30323933</v>
+        <v>30391319</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4101,7 +4101,7 @@
         <tr r="P30" s="1"/>
       </tp>
       <tp>
-        <v>572222720</v>
+        <v>399604654</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -4109,7 +4109,7 @@
         <tr r="M11" s="1"/>
       </tp>
       <tp>
-        <v>51677984</v>
+        <v>36351363</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -4117,7 +4117,7 @@
         <tr r="M10" s="1"/>
       </tp>
       <tp>
-        <v>598657.79</v>
+        <v>506889</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4125,7 +4125,7 @@
         <tr r="M9" s="1"/>
       </tp>
       <tp>
-        <v>43284.749999988424</v>
+        <v>43285.541666655095</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4134,7 +4134,7 @@
         <tr r="G30" s="1"/>
       </tp>
       <tp>
-        <v>43284.72222221065</v>
+        <v>43285.517361099533</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4143,7 +4143,7 @@
         <tr r="G36" s="1"/>
       </tp>
       <tp>
-        <v>43284.749999988424</v>
+        <v>43285.541666655095</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4152,7 +4152,7 @@
         <tr r="G31" s="1"/>
       </tp>
       <tp>
-        <v>43284.72291665509</v>
+        <v>43285.517361099533</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4161,7 +4161,7 @@
         <tr r="G37" s="1"/>
       </tp>
       <tp>
-        <v>6.1399999999999997E-6</v>
+        <v>5.9900000000000002E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4169,7 +4169,7 @@
         <tr r="C11" s="1"/>
       </tp>
       <tp>
-        <v>5.9200000000000001E-6</v>
+        <v>5.8799999999999996E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4178,7 +4178,7 @@
         <tr r="D32" s="1"/>
       </tp>
       <tp>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4205,7 +4205,7 @@
         <tr r="H32" s="1"/>
       </tp>
       <tp>
-        <v>32593</v>
+        <v>20628</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4213,7 +4213,7 @@
         <tr r="O7" s="1"/>
       </tp>
       <tp>
-        <v>217438</v>
+        <v>168939</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4221,7 +4221,7 @@
         <tr r="O6" s="1"/>
       </tp>
       <tp>
-        <v>128396</v>
+        <v>92427</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4229,7 +4229,7 @@
         <tr r="O5" s="1"/>
       </tp>
       <tp>
-        <v>27840</v>
+        <v>17606</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4237,7 +4237,7 @@
         <tr r="O8" s="1"/>
       </tp>
       <tp>
-        <v>6586.03</v>
+        <v>6650.93</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4246,7 +4246,7 @@
         <tr r="D31" s="1"/>
       </tp>
       <tp>
-        <v>6593.27</v>
+        <v>6662.15</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4255,7 +4255,7 @@
         <tr r="D37" s="1"/>
       </tp>
       <tp>
-        <v>1.3860000000000001E-2</v>
+        <v>5.3299999999999997E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4263,7 +4263,7 @@
         <tr r="P7" s="1"/>
       </tp>
       <tp>
-        <v>-1.423E-2</v>
+        <v>6.2899999999999996E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4271,7 +4271,7 @@
         <tr r="P5" s="1"/>
       </tp>
       <tp>
-        <v>-6.3299999999999997E-3</v>
+        <v>1.191E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4279,7 +4279,7 @@
         <tr r="P6" s="1"/>
       </tp>
       <tp>
-        <v>3.2100000000000002E-3</v>
+        <v>-9.2899999999999996E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4287,7 +4287,7 @@
         <tr r="P8" s="1"/>
       </tp>
       <tp>
-        <v>6593.27</v>
+        <v>6664.13</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4295,7 +4295,7 @@
         <tr r="I16" s="1"/>
       </tp>
       <tp>
-        <v>87.17</v>
+        <v>86.86</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4319,7 +4319,7 @@
         <tr r="R18" s="1"/>
       </tp>
       <tp>
-        <v>467.93</v>
+        <v>471.3</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4328,7 +4328,7 @@
         <tr r="D36" s="1"/>
       </tp>
       <tp>
-        <v>467.93</v>
+        <v>471.03</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4369,7 +4369,7 @@
         <tr r="Q21" s="1"/>
       </tp>
       <tp>
-        <v>0.48514000000000002</v>
+        <v>0.47800999999999999</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4385,7 +4385,7 @@
         <tr r="U18" s="1"/>
       </tp>
       <tp>
-        <v>7.8139999999999994E-5</v>
+        <v>7.6240000000000002E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4425,7 +4425,7 @@
         <tr r="N17" s="1"/>
       </tp>
       <tp>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4434,7 +4434,7 @@
         <tr r="E38" s="1"/>
       </tp>
       <tp>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4443,7 +4443,7 @@
         <tr r="E32" s="1"/>
       </tp>
       <tp>
-        <v>1474.9476208200001</v>
+        <v>13547.573522049999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4452,7 +4452,7 @@
         <tr r="L37" s="1"/>
       </tp>
       <tp>
-        <v>1232565.7239691401</v>
+        <v>2447502.1504584299</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4461,7 +4461,7 @@
         <tr r="L31" s="1"/>
       </tp>
       <tp>
-        <v>22830.8364043</v>
+        <v>3252.4823544999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4470,7 +4470,7 @@
         <tr r="L36" s="1"/>
       </tp>
       <tp>
-        <v>371589.88051839999</v>
+        <v>564552.89316370001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4503,7 +4503,7 @@
         <tr r="O15" s="1"/>
       </tp>
       <tp>
-        <v>468.93</v>
+        <v>471.3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4511,7 +4511,7 @@
         <tr r="I15" s="1"/>
       </tp>
       <tp>
-        <v>182963.56307</v>
+        <v>132521.51637999999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4519,7 +4519,7 @@
         <tr r="M7" s="1"/>
       </tp>
       <tp>
-        <v>0.49278</v>
+        <v>0.49421999999999999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4527,7 +4527,7 @@
         <tr r="I8" s="1"/>
       </tp>
       <tp>
-        <v>43284.72152777778</v>
+        <v>43285.51666666667</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4536,7 +4536,7 @@
         <tr r="F36" s="1"/>
       </tp>
       <tp>
-        <v>43284.708333333336</v>
+        <v>43285.5</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4545,7 +4545,7 @@
         <tr r="F30" s="1"/>
       </tp>
       <tp>
-        <v>85.9</v>
+        <v>86.41</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4553,7 +4553,7 @@
         <tr r="D7" s="1"/>
       </tp>
       <tp>
-        <v>6636.01</v>
+        <v>6591.31</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4561,7 +4561,7 @@
         <tr r="D6" s="1"/>
       </tp>
       <tp>
-        <v>43284.722140613427</v>
+        <v>43285.517102199075</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4569,7 +4569,7 @@
         <tr r="L19" s="1"/>
       </tp>
       <tp>
-        <v>5.5030000000000001E-3</v>
+        <v>5.5440000000000003E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4577,7 +4577,7 @@
         <tr r="G9" s="1"/>
       </tp>
       <tp>
-        <v>475.71</v>
+        <v>469.52</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4585,7 +4585,7 @@
         <tr r="G5" s="1"/>
       </tp>
       <tp>
-        <v>0.49362</v>
+        <v>0.49541000000000002</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4593,7 +4593,7 @@
         <tr r="K8" s="1"/>
       </tp>
       <tp>
-        <v>6636.01</v>
+        <v>6589.41</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4601,7 +4601,7 @@
         <tr r="G6" s="1"/>
       </tp>
       <tp>
-        <v>85.84</v>
+        <v>86.38</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4609,7 +4609,7 @@
         <tr r="G7" s="1"/>
       </tp>
       <tp t="b">
-        <v>1</v>
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4625,15 +4625,15 @@
         <tr r="K16" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
         <stp>BUYER_IS_MAKER</stp>
         <tr r="K15" s="1"/>
       </tp>
-      <tp t="b">
-        <v>1</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4641,7 +4641,7 @@
         <tr r="K18" s="1"/>
       </tp>
       <tp>
-        <v>486.76</v>
+        <v>482.01</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4649,7 +4649,7 @@
         <tr r="F3" s="2"/>
       </tp>
       <tp>
-        <v>6673.99</v>
+        <v>6796.62</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4657,7 +4657,7 @@
         <tr r="F4" s="2"/>
       </tp>
       <tp>
-        <v>0.49210999999999999</v>
+        <v>0.49940000000000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4665,7 +4665,7 @@
         <tr r="G8" s="1"/>
       </tp>
       <tp>
-        <v>43284.722222222219</v>
+        <v>43285.51666666667</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4674,7 +4674,7 @@
         <tr r="F37" s="1"/>
       </tp>
       <tp>
-        <v>43284.708333333336</v>
+        <v>43285.5</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4683,7 +4683,7 @@
         <tr r="F31" s="1"/>
       </tp>
       <tp>
-        <v>7.0999999999999998E-7</v>
+        <v>-1.66E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -4691,7 +4691,7 @@
         <tr r="Q10" s="1"/>
       </tp>
       <tp>
-        <v>475.7</v>
+        <v>469.12</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4699,7 +4699,7 @@
         <tr r="D5" s="1"/>
       </tp>
       <tp>
-        <v>171552.397</v>
+        <v>120420.34009</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4707,7 +4707,7 @@
         <tr r="M5" s="1"/>
       </tp>
       <tp>
-        <v>5.5030000000000001E-3</v>
+        <v>5.5380000000000004E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4733,7 +4733,7 @@
         <tr r="M32" s="1"/>
       </tp>
       <tp>
-        <v>-8.9999999999999999E-8</v>
+        <v>-1E-8</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -4741,7 +4741,7 @@
         <tr r="Q11" s="1"/>
       </tp>
       <tp>
-        <v>2392227.0247127102</v>
+        <v>4797712.7030429197</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4750,7 +4750,7 @@
         <tr r="I31" s="1"/>
       </tp>
       <tp>
-        <v>1797.6540783099999</v>
+        <v>67997.397360820003</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4759,7 +4759,7 @@
         <tr r="I37" s="1"/>
       </tp>
       <tp>
-        <v>674654.7416978</v>
+        <v>1165600.1691212</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4768,7 +4768,7 @@
         <tr r="I30" s="1"/>
       </tp>
       <tp>
-        <v>62870.438001199997</v>
+        <v>12544.048344999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4777,7 +4777,7 @@
         <tr r="I36" s="1"/>
       </tp>
       <tp>
-        <v>468.01</v>
+        <v>471.77</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4785,7 +4785,7 @@
         <tr r="D3" s="2"/>
       </tp>
       <tp>
-        <v>6596.5</v>
+        <v>6663.67</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4793,7 +4793,7 @@
         <tr r="D4" s="2"/>
       </tp>
       <tp>
-        <v>5.5999999999999999E-3</v>
+        <v>5.7980000000000002E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4801,7 +4801,7 @@
         <tr r="I19" s="1"/>
       </tp>
       <tp>
-        <v>43284.722241145835</v>
+        <v>43285.516921388888</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4810,7 +4810,7 @@
         <tr r="O32" s="1"/>
       </tp>
       <tp>
-        <v>43284.722241145835</v>
+        <v>43285.516921388888</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4819,7 +4819,7 @@
         <tr r="O38" s="1"/>
       </tp>
       <tp>
-        <v>33994.790332999997</v>
+        <v>29075.271000000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4834,7 +4834,7 @@
         <tr r="T7" s="1"/>
       </tp>
       <tp>
-        <v>1.37</v>
+        <v>0.46</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4842,7 +4842,7 @@
         <tr r="Q7" s="1"/>
       </tp>
       <tp>
-        <v>-42.03</v>
+        <v>72.8</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4850,7 +4850,7 @@
         <tr r="Q6" s="1"/>
       </tp>
       <tp>
-        <v>1.16E-4</v>
+        <v>2.63E-4</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4858,7 +4858,7 @@
         <tr r="Q9" s="1"/>
       </tp>
       <tp>
-        <v>-6.77</v>
+        <v>2.91</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4866,7 +4866,7 @@
         <tr r="Q5" s="1"/>
       </tp>
       <tp>
-        <v>0.49210999999999999</v>
+        <v>0.49924000000000002</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4874,7 +4874,7 @@
         <tr r="D8" s="1"/>
       </tp>
       <tp>
-        <v>0.19</v>
+        <v>0.15</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4882,7 +4882,7 @@
         <tr r="J7" s="1"/>
       </tp>
       <tp>
-        <v>1.27</v>
+        <v>5.72</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4890,7 +4890,7 @@
         <tr r="J6" s="1"/>
       </tp>
       <tp>
-        <v>0.14000000000000001</v>
+        <v>0.51</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4898,7 +4898,7 @@
         <tr r="J5" s="1"/>
       </tp>
       <tp>
-        <v>8.3000000000000001E-4</v>
+        <v>1.1800000000000001E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4906,7 +4906,7 @@
         <tr r="J8" s="1"/>
       </tp>
       <tp>
-        <v>43284.72291665509</v>
+        <v>43285.517361099533</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4915,7 +4915,7 @@
         <tr r="G38" s="1"/>
       </tp>
       <tp>
-        <v>43284.749999988424</v>
+        <v>43285.541666655095</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4924,7 +4924,7 @@
         <tr r="G32" s="1"/>
       </tp>
       <tp>
-        <v>30862414</v>
+        <v>30882393</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4933,7 +4933,7 @@
         <tr r="P32" s="1"/>
       </tp>
       <tp>
-        <v>30862956</v>
+        <v>30882888</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4942,7 +4942,7 @@
         <tr r="P38" s="1"/>
       </tp>
       <tp>
-        <v>87.03</v>
+        <v>86.7</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4950,7 +4950,7 @@
         <tr r="I7" s="1"/>
       </tp>
       <tp>
-        <v>43030472.700000003</v>
+        <v>28720303.899999999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4958,7 +4958,7 @@
         <tr r="M8" s="1"/>
       </tp>
       <tp>
-        <v>7.4120000000000002E-5</v>
+        <v>7.5850000000000001E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -4966,7 +4966,7 @@
         <tr r="G10" s="1"/>
       </tp>
       <tp>
-        <v>43284.722241087962</v>
+        <v>43285.516921377312</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4974,7 +4974,7 @@
         <tr r="L21" s="1"/>
       </tp>
       <tp>
-        <v>1.5100000000000001E-3</v>
+        <v>-4.64E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4982,7 +4982,7 @@
         <tr r="Q8" s="1"/>
       </tp>
       <tp>
-        <v>87.22</v>
+        <v>86.85</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4990,7 +4990,7 @@
         <tr r="K7" s="1"/>
       </tp>
       <tp t="s">
-        <v>ETHBTC|LTCBTC|BNBBTC|NEOBTC|QTUMETH|EOSETH|SNTETH|BNTETH|BCCBTC|GASBTC|BNBETH|BTCUSDT|ETHUSDT|HSRBTC|OAXETH|DNTETH|MCOETH|ICNETH|MCOBTC|WTCBTC|WTCETH|LRCBTC|LRCETH|QTUMBTC|YOYOBTC|OMGBTC|OMGETH|ZRXBTC|ZRXETH|STRATBTC|STRATETH|SNGLSBTC|SNGLSETH|BQXBTC|BQXETH|KNCBTC|KNCETH|FUNBTC|FUNETH|SNMBTC|SNMETH|NEOETH|IOTABTC|IOTAETH|LINKBTC|LINKETH|XVGBTC|XVGETH|SALTBTC|SALTETH|MDABTC|MDAETH|MTLBTC|MTLETH|SUBBTC|SUBETH|EOSBTC|SNTBTC|ETCETH|ETCBTC|MTHBTC|MTHETH|ENGBTC|ENGETH|DNTBTC|ZECBTC|ZECETH|BNTBTC|ASTBTC|ASTETH|DASHBTC|DASHETH|OAXBTC|ICNBTC|BTGBTC|BTGETH|EVXBTC|EVXETH|REQBTC|REQETH|VIBBTC|VIBETH|HSRETH|TRXBTC|TRXETH|POWRBTC|POWRETH|ARKBTC|ARKETH|YOYOETH|XRPBTC|XRPETH|MODBTC|MODETH|ENJBTC|ENJETH|STORJBTC|STORJETH|BNBUSDT|VENBNB|YOYOBNB|POWRBNB|VENBTC|VENETH|KMDBTC|KMDETH|NULSBNB|RCNBTC|RCNETH|RCNBNB|NULSBTC|NULSETH|RDNBTC|RDNETH|RDNBNB|XMRBTC|XMRETH|DLTBNB|WTCBNB|DLTBTC|DLTETH|AMBBTC|AMBETH|AMBBNB|BCCETH|BCCUSDT|BCCBNB|BATBTC|BATETH|BATBNB|BCPTBTC|BCPTETH|BCPTBNB|ARNBTC|ARNETH|GVTBTC|GVTETH|CDTBTC|CDTETH|GXSBTC|GXSETH|NEOUSDT|NEOBNB|POEBTC|POEETH|QSPBTC|QSPETH|QSPBNB|BTSBTC|BTSETH|BTSBNB|XZCBTC|XZCETH|XZCBNB|LSKBTC|LSKETH|LSKBNB|TNTBTC|TNTETH|FUELBTC|FUELETH|MANABTC|MANAETH|BCDBTC|BCDETH|DGDBTC|DGDETH|IOTABNB|ADXBTC|ADXETH|ADXBNB|ADABTC|ADAETH|PPTBTC|PPTETH|CMTBTC|CMTETH|CMTBNB|XLMBTC|XLMETH|XLMBNB|CNDBTC|CNDETH|CNDBNB|LENDBTC|LENDETH|WABIBTC|WABIETH|WABIBNB|LTCETH|LTCUSDT|LTCBNB|TNBBTC|TNBETH|WAVESBTC|WAVESETH|WAVESBNB|GTOBTC|GTOETH|GTOBNB|ICXBTC|ICXETH|ICXBNB|OSTBTC|OSTETH|OSTBNB|ELFBTC|ELFETH|AIONBTC|AIONETH|AIONBNB|NEBLBTC|NEBLETH|NEBLBNB|BRDBTC|BRDETH|BRDBNB|MCOBNB|EDOBTC|EDOETH|WINGSBTC|WINGSETH|NAVBTC|NAVETH|NAVBNB|LUNBTC|LUNETH|TRIGBTC|TRIGETH|TRIGBNB|APPCBTC|APPCETH|APPCBNB|VIBEBTC|VIBEETH|RLCBTC|RLCETH|RLCBNB|INSBTC|INSETH|PIVXBTC|PIVXETH|PIVXBNB|IOSTBTC|IOSTETH|CHATBTC|CHATETH|STEEMBTC|STEEMETH|STEEMBNB|NANOBTC|NANOETH|NANOBNB|VIABTC|VIAETH|VIABNB|BLZBTC|BLZETH|BLZBNB|AEBTC|AEETH|AEBNB|RPXBTC|RPXETH|RPXBNB|NCASHBTC|NCASHETH|NCASHBNB|POABTC|POAETH|POABNB|ZILBTC|ZILETH|ZILBNB|ONTBTC|ONTETH|ONTBNB|STORMBTC|STORMETH|STORMBNB|QTUMBNB|QTUMUSDT|XEMBTC|XEMETH|XEMBNB|WANBTC|WANETH|WANBNB|WPRBTC|WPRETH|QLCBTC|QLCETH|SYSBTC|SYSETH|SYSBNB|QLCBNB|GRSBTC|GRSETH|ADAUSDT|ADABNB|CLOAKBTC|CLOAKETH|GNTBTC|GNTETH|GNTBNB|LOOMBTC|LOOMETH|LOOMBNB|XRPUSDT|BCNBTC|BCNETH|BCNBNB|REPBTC|REPETH|REPBNB|TUSDBTC|TUSDETH|TUSDBNB|ZENBTC|ZENETH|ZENBNB|SKYBTC|SKYETH|SKYBNB|EOSUSDT|EOSBNB|CVCBTC|CVCETH|CVCBNB|THETABTC|THETAETH|THETABNB|XRPBNB|TUSDUSDT|IOTAUSDT|XLMUSDT|IOTXBTC|IOTXETH|QKCBTC|QKCETH|AGIBTC|AGIETH|AGIBNB|NXSBTC|NXSETH|NXSBNB|ENJBNB|DATABTC|DATAETH|ONTUSDT|TRXUSDT|ETCUSDT|ETCBNB|ICXUSDT|SCBTC|SCETH|SCBNB|NPXSBTC|NPXSETH|VENUSDT|KEYBTC|KEYETH|NASBTC|NASETH|NASBNB|</v>
+        <v>["ETHBTC","LTCBTC","BNBBTC","NEOBTC","QTUMETH","EOSETH","SNTETH","BNTETH","BCCBTC","GASBTC","BNBETH","BTCUSDT","ETHUSDT","HSRBTC","OAXETH","DNTETH","MCOETH","ICNETH","MCOBTC","WTCBTC","WTCETH","LRCBTC","LRCETH","QTUMBTC","YOYOBTC","OMGBTC","OMGETH","ZRXBTC","ZRXETH","STRATBTC","STRATETH","SNGLSBTC","SNGLSETH","BQXBTC","BQXETH","KNCBTC","KNCETH","FUNBTC","FUNETH","SNMBTC","SNMETH","NEOETH","IOTABTC","IOTAETH","LINKBTC","LINKETH","XVGBTC","XVGETH","SALTBTC","SALTETH","MDABTC","MDAETH","MTLBTC","MTLETH","SUBBTC","SUBETH","EOSBTC","SNTBTC","ETCETH","ETCBTC","MTHBTC","MTHETH","ENGBTC","ENGETH","DNTBTC","ZECBTC","ZECETH","BNTBTC","ASTBTC","ASTETH","DASHBTC","DASHETH","OAXBTC","ICNBTC","BTGBTC","BTGETH","EVXBTC","EVXETH","REQBTC","REQETH","VIBBTC","VIBETH","HSRETH","TRXBTC","TRXETH","POWRBTC","POWRETH","ARKBTC","ARKETH","YOYOETH","XRPBTC","XRPETH","MODBTC","MODETH","ENJBTC","ENJETH","STORJBTC","STORJETH","BNBUSDT","VENBNB","YOYOBNB","POWRBNB","VENBTC","VENETH","KMDBTC","KMDETH","NULSBNB","RCNBTC","RCNETH","RCNBNB","NULSBTC","NULSETH","RDNBTC","RDNETH","RDNBNB","XMRBTC","XMRETH","DLTBNB","WTCBNB","DLTBTC","DLTETH","AMBBTC","AMBETH","AMBBNB","BCCETH","BCCUSDT","BCCBNB","BATBTC","BATETH","BATBNB","BCPTBTC","BCPTETH","BCPTBNB","ARNBTC","ARNETH","GVTBTC","GVTETH","CDTBTC","CDTETH","GXSBTC","GXSETH","NEOUSDT","NEOBNB","POEBTC","POEETH","QSPBTC","QSPETH","QSPBNB","BTSBTC","BTSETH","BTSBNB","XZCBTC","XZCETH","XZCBNB","LSKBTC","LSKETH","LSKBNB","TNTBTC","TNTETH","FUELBTC","FUELETH","MANABTC","MANAETH","BCDBTC","BCDETH","DGDBTC","DGDETH","IOTABNB","ADXBTC","ADXETH","ADXBNB","ADABTC","ADAETH","PPTBTC","PPTETH","CMTBTC","CMTETH","CMTBNB","XLMBTC","XLMETH","XLMBNB","CNDBTC","CNDETH","CNDBNB","LENDBTC","LENDETH","WABIBTC","WABIETH","WABIBNB","LTCETH","LTCUSDT","LTCBNB","TNBBTC","TNBETH","WAVESBTC","WAVESETH","WAVESBNB","GTOBTC","GTOETH","GTOBNB","ICXBTC","ICXETH","ICXBNB","OSTBTC","OSTETH","OSTBNB","ELFBTC","ELFETH","AIONBTC","AIONETH","AIONBNB","NEBLBTC","NEBLETH","NEBLBNB","BRDBTC","BRDETH","BRDBNB","MCOBNB","EDOBTC","EDOETH","WINGSBTC","WINGSETH","NAVBTC","NAVETH","NAVBNB","LUNBTC","LUNETH","TRIGBTC","TRIGETH","TRIGBNB","APPCBTC","APPCETH","APPCBNB","VIBEBTC","VIBEETH","RLCBTC","RLCETH","RLCBNB","INSBTC","INSETH","PIVXBTC","PIVXETH","PIVXBNB","IOSTBTC","IOSTETH","CHATBTC","CHATETH","STEEMBTC","STEEMETH","STEEMBNB","NANOBTC","NANOETH","NANOBNB","VIABTC","VIAETH","VIABNB","BLZBTC","BLZETH","BLZBNB","AEBTC","AEETH","AEBNB","RPXBTC","RPXETH","RPXBNB","NCASHBTC","NCASHETH","NCASHBNB","POABTC","POAETH","POABNB","ZILBTC","ZILETH","ZILBNB","ONTBTC","ONTETH","ONTBNB","STORMBTC","STORMETH","STORMBNB","QTUMBNB","QTUMUSDT","XEMBTC","XEMETH","XEMBNB","WANBTC","WANETH","WANBNB","WPRBTC","WPRETH","QLCBTC","QLCETH","SYSBTC","SYSETH","SYSBNB","QLCBNB","GRSBTC","GRSETH","ADAUSDT","ADABNB","CLOAKBTC","CLOAKETH","GNTBTC","GNTETH","GNTBNB","LOOMBTC","LOOMETH","LOOMBNB","XRPUSDT","BCNBTC","BCNETH","BCNBNB","REPBTC","REPETH","REPBNB","TUSDBTC","TUSDETH","TUSDBNB","ZENBTC","ZENETH","ZENBNB","SKYBTC","SKYETH","SKYBNB","EOSUSDT","EOSBNB","CVCBTC","CVCETH","CVCBNB","THETABTC","THETAETH","THETABNB","XRPBNB","TUSDUSDT","IOTAUSDT","XLMUSDT","IOTXBTC","IOTXETH","QKCBTC","QKCETH","AGIBTC","AGIETH","AGIBNB","NXSBTC","NXSETH","NXSBNB","ENJBNB","DATABTC","DATAETH","ONTUSDT","TRXUSDT","ETCUSDT","ETCBNB","ICXUSDT","SCBTC","SCETH","SCBNB","NPXSBTC","NPXSETH","VENUSDT","KEYBTC","KEYETH","NASBTC","NASETH","NASBNB"]</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp/>
@@ -4998,7 +4998,7 @@
         <tr r="T8" s="1"/>
       </tp>
       <tp>
-        <v>31.2854311</v>
+        <v>12.049877589999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5007,7 +5007,7 @@
         <tr r="L32" s="1"/>
       </tp>
       <tp>
-        <v>1.352538E-2</v>
+        <v>0.18112928</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5016,7 +5016,7 @@
         <tr r="L38" s="1"/>
       </tp>
       <tp>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -5024,7 +5024,7 @@
         <tr r="I21" s="1"/>
       </tp>
       <tp>
-        <v>7.4930000000000003E-5</v>
+        <v>7.4259999999999997E-5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -5032,7 +5032,7 @@
         <tr r="I20" s="1"/>
       </tp>
       <tp>
-        <v>6595.24</v>
+        <v>6669.86</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -5040,7 +5040,7 @@
         <tr r="K6" s="1"/>
       </tp>
       <tp>
-        <v>6.0299999999999999E-6</v>
+        <v>5.9000000000000003E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -5048,7 +5048,7 @@
         <tr r="G11" s="1"/>
       </tp>
       <tp>
-        <v>6593.97</v>
+        <v>6664.1</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -5056,7 +5056,7 @@
         <tr r="I6" s="1"/>
       </tp>
       <tp>
-        <v>6.0299999999999999E-6</v>
+        <v>5.9000000000000003E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -5064,7 +5064,7 @@
         <tr r="D11" s="1"/>
       </tp>
       <tp>
-        <v>7.4129999999999997E-5</v>
+        <v>7.5820000000000003E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -5072,7 +5072,7 @@
         <tr r="D10" s="1"/>
       </tp>
       <tp>
-        <v>6593.03</v>
+        <v>6662.15</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5081,7 +5081,7 @@
         <tr r="B19" s="1"/>
       </tp>
       <tp>
-        <v>6591.89</v>
+        <v>6661.45</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5090,7 +5090,7 @@
         <tr r="B20" s="1"/>
       </tp>
       <tp>
-        <v>6591.4</v>
+        <v>6661.02</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5099,7 +5099,7 @@
         <tr r="B21" s="1"/>
       </tp>
       <tp>
-        <v>6590.01</v>
+        <v>6660.61</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5108,7 +5108,7 @@
         <tr r="B22" s="1"/>
       </tp>
       <tp>
-        <v>6593.27</v>
+        <v>6665</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5117,7 +5117,7 @@
         <tr r="B15" s="1"/>
       </tp>
       <tp>
-        <v>6593.26</v>
+        <v>6664.77</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5126,7 +5126,7 @@
         <tr r="B16" s="1"/>
       </tp>
       <tp>
-        <v>6593.18</v>
+        <v>6664.13</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5135,7 +5135,7 @@
         <tr r="B17" s="1"/>
       </tp>
       <tp>
-        <v>6593.14</v>
+        <v>6663.73</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5144,7 +5144,7 @@
         <tr r="B18" s="1"/>
       </tp>
       <tp>
-        <v>6590</v>
+        <v>6660.53</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5153,7 +5153,7 @@
         <tr r="B23" s="1"/>
       </tp>
       <tp>
-        <v>6588.64</v>
+        <v>6660</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5162,7 +5162,7 @@
         <tr r="B24" s="1"/>
       </tp>
       <tp>
-        <v>475.27</v>
+        <v>468.56</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -5170,7 +5170,7 @@
         <tr r="E3" s="2"/>
       </tp>
       <tp>
-        <v>468.76</v>
+        <v>471.53</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -5178,7 +5178,7 @@
         <tr r="I5" s="1"/>
       </tp>
       <tp>
-        <v>6626.31</v>
+        <v>6589.99</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -5186,7 +5186,7 @@
         <tr r="E4" s="2"/>
       </tp>
       <tp>
-        <v>43284.722096273152</v>
+        <v>43285.517003391207</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -5194,7 +5194,7 @@
         <tr r="L20" s="1"/>
       </tp>
       <tp>
-        <v>6603.78</v>
+        <v>6669.87</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5203,7 +5203,7 @@
         <tr r="D24" s="1"/>
       </tp>
       <tp>
-        <v>6603</v>
+        <v>6669.86</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5212,7 +5212,7 @@
         <tr r="D23" s="1"/>
       </tp>
       <tp>
-        <v>6599.61</v>
+        <v>6668.74</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5221,7 +5221,7 @@
         <tr r="D18" s="1"/>
       </tp>
       <tp>
-        <v>6597.99</v>
+        <v>6668</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5230,7 +5230,7 @@
         <tr r="D17" s="1"/>
       </tp>
       <tp>
-        <v>6597.98</v>
+        <v>6667.97</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5239,7 +5239,7 @@
         <tr r="D16" s="1"/>
       </tp>
       <tp>
-        <v>6597.97</v>
+        <v>6667.96</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5248,7 +5248,7 @@
         <tr r="D15" s="1"/>
       </tp>
       <tp>
-        <v>6601.54</v>
+        <v>6669.51</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5257,7 +5257,7 @@
         <tr r="D22" s="1"/>
       </tp>
       <tp>
-        <v>6600</v>
+        <v>6669</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5266,7 +5266,7 @@
         <tr r="D21" s="1"/>
       </tp>
       <tp>
-        <v>6599.99</v>
+        <v>6668.91</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5275,7 +5275,7 @@
         <tr r="D20" s="1"/>
       </tp>
       <tp>
-        <v>6599.98</v>
+        <v>6668.78</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5284,7 +5284,7 @@
         <tr r="D19" s="1"/>
       </tp>
       <tp>
-        <v>468.91</v>
+        <v>472.03</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -5810,7 +5810,7 @@
   <dimension ref="A1:U108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5923,7 +5923,7 @@
       </c>
       <c r="T4" s="37">
         <f>RTD(progId,,"CLOCK")</f>
-        <v>43284.72226396991</v>
+        <v>43285.517097245371</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5932,66 +5932,66 @@
       </c>
       <c r="B5" s="2">
         <f>RTD(progId,,BINANCE,$A5,B$4)</f>
-        <v>462.5</v>
+        <v>457</v>
       </c>
       <c r="C5" s="2">
         <f>RTD(progId,,BINANCE,$A5,C$4)</f>
-        <v>486.98</v>
+        <v>482.7</v>
       </c>
       <c r="D5" s="2">
         <f>RTD(progId,,BINANCE_24H,$A5,D$4)</f>
-        <v>475.7</v>
+        <v>469.12</v>
       </c>
       <c r="G5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,G$4)</f>
-        <v>475.71</v>
+        <v>469.52</v>
       </c>
       <c r="H5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,H$4)</f>
-        <v>1.7000000000000001E-4</v>
+        <v>2.4573100000000001</v>
       </c>
       <c r="I5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,I$4)</f>
-        <v>468.76</v>
+        <v>471.53</v>
       </c>
       <c r="J5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,J$4)</f>
-        <v>0.14000000000000001</v>
+        <v>0.51</v>
       </c>
       <c r="K5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,K$4)</f>
-        <v>468.91</v>
+        <v>472.03</v>
       </c>
       <c r="L5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,L$4)</f>
-        <v>1.24308</v>
+        <v>2.6858599999999999</v>
       </c>
       <c r="M5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,M$4)</f>
-        <v>171552.397</v>
+        <v>120420.34009</v>
       </c>
       <c r="N5" s="42">
         <f>RTD(progId,,BINANCE_24H,$A5,N$4)</f>
-        <v>81175585.563029304</v>
+        <v>56432388.176379703</v>
       </c>
       <c r="O5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,O$4)</f>
-        <v>128396</v>
+        <v>92427</v>
       </c>
       <c r="P5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,P$4)</f>
-        <v>-1.423E-2</v>
+        <v>6.2899999999999996E-3</v>
       </c>
       <c r="Q5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,Q$4)</f>
-        <v>-6.77</v>
+        <v>2.91</v>
       </c>
       <c r="S5" s="38" t="s">
         <v>61</v>
       </c>
       <c r="T5" s="36">
         <f>RTD(progId,,BINANCE,S5)</f>
-        <v>-935</v>
+        <v>-443</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -6000,66 +6000,66 @@
       </c>
       <c r="B6" s="2">
         <f>RTD(progId,,BINANCE,$A6,B$4)</f>
-        <v>6519.99</v>
+        <v>6441.11</v>
       </c>
       <c r="C6" s="2">
         <f>RTD(progId,,BINANCE,$A6,C$4)</f>
-        <v>6679.35</v>
+        <v>6784.92</v>
       </c>
       <c r="D6" s="2">
         <f>RTD(progId,,BINANCE_24H,$A6,D$4)</f>
-        <v>6636.01</v>
+        <v>6591.31</v>
       </c>
       <c r="G6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,G$4)</f>
-        <v>6636.01</v>
+        <v>6589.41</v>
       </c>
       <c r="H6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,H$4)</f>
-        <v>0.52357699999999996</v>
+        <v>6.7424999999999999E-2</v>
       </c>
       <c r="I6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,I$4)</f>
-        <v>6593.97</v>
+        <v>6664.1</v>
       </c>
       <c r="J6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,J$4)</f>
-        <v>1.27</v>
+        <v>5.72</v>
       </c>
       <c r="K6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,K$4)</f>
-        <v>6595.24</v>
+        <v>6669.86</v>
       </c>
       <c r="L6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,L$4)</f>
-        <v>1.3532390000000001</v>
+        <v>0.26262600000000003</v>
       </c>
       <c r="M6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,M$4)</f>
-        <v>33994.790332999997</v>
+        <v>29075.271000000001</v>
       </c>
       <c r="N6" s="42">
         <f>RTD(progId,,BINANCE_24H,$A6,N$4)</f>
-        <v>224411913.22751993</v>
+        <v>191494800.14948204</v>
       </c>
       <c r="O6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,O$4)</f>
-        <v>217438</v>
+        <v>168939</v>
       </c>
       <c r="P6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,P$4)</f>
-        <v>-6.3299999999999997E-3</v>
+        <v>1.191E-2</v>
       </c>
       <c r="Q6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,Q$4)</f>
-        <v>-42.03</v>
+        <v>72.8</v>
       </c>
       <c r="S6" s="38" t="s">
         <v>62</v>
       </c>
       <c r="T6" s="37">
         <f>RTD(progId,,BINANCE,S6)</f>
-        <v>43284.720387337962</v>
+        <v>43285.516620439812</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -6068,59 +6068,59 @@
       </c>
       <c r="B7" s="2">
         <f>RTD(progId,,BINANCE,$A7,B$4)</f>
-        <v>84.75</v>
+        <v>83.64</v>
       </c>
       <c r="C7" s="2">
         <f>RTD(progId,,BINANCE,$A7,C$4)</f>
-        <v>90</v>
+        <v>89.01</v>
       </c>
       <c r="D7" s="2">
         <f>RTD(progId,,BINANCE_24H,$A7,D$4)</f>
-        <v>85.9</v>
+        <v>86.41</v>
       </c>
       <c r="G7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,G$4)</f>
-        <v>85.84</v>
+        <v>86.38</v>
       </c>
       <c r="H7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,H$4)</f>
-        <v>0.40920000000000001</v>
+        <v>1.537E-2</v>
       </c>
       <c r="I7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,I$4)</f>
-        <v>87.03</v>
+        <v>86.7</v>
       </c>
       <c r="J7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,J$4)</f>
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="K7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,K$4)</f>
-        <v>87.22</v>
+        <v>86.85</v>
       </c>
       <c r="L7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,L$4)</f>
-        <v>5.5398800000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="M7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,M$4)</f>
-        <v>182963.56307</v>
+        <v>132521.51637999999</v>
       </c>
       <c r="N7" s="42">
         <f>RTD(progId,,BINANCE_24H,$A7,N$4)</f>
-        <v>15882625.5011223</v>
+        <v>11444940.7380598</v>
       </c>
       <c r="O7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,O$4)</f>
-        <v>32593</v>
+        <v>20628</v>
       </c>
       <c r="P7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,P$4)</f>
-        <v>1.3860000000000001E-2</v>
+        <v>5.3299999999999997E-3</v>
       </c>
       <c r="Q7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,Q$4)</f>
-        <v>1.37</v>
+        <v>0.46</v>
       </c>
       <c r="S7" s="38" t="s">
         <v>63</v>
@@ -6136,66 +6136,66 @@
       </c>
       <c r="B8" s="2">
         <f>RTD(progId,,BINANCE,$A8,B$4)</f>
-        <v>0.48514000000000002</v>
+        <v>0.47800999999999999</v>
       </c>
       <c r="C8" s="2">
         <f>RTD(progId,,BINANCE,$A8,C$4)</f>
-        <v>0.52</v>
+        <v>0.50654999999999994</v>
       </c>
       <c r="D8" s="2">
         <f>RTD(progId,,BINANCE_24H,$A8,D$4)</f>
-        <v>0.49210999999999999</v>
+        <v>0.49924000000000002</v>
       </c>
       <c r="G8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,G$4)</f>
-        <v>0.49210999999999999</v>
+        <v>0.49940000000000001</v>
       </c>
       <c r="H8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,H$4)</f>
-        <v>353.5</v>
+        <v>6902.4</v>
       </c>
       <c r="I8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,I$4)</f>
-        <v>0.49278</v>
+        <v>0.49421999999999999</v>
       </c>
       <c r="J8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,J$4)</f>
-        <v>8.3000000000000001E-4</v>
+        <v>1.1800000000000001E-3</v>
       </c>
       <c r="K8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,K$4)</f>
-        <v>0.49362</v>
+        <v>0.49541000000000002</v>
       </c>
       <c r="L8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,L$4)</f>
-        <v>1663</v>
+        <v>3292</v>
       </c>
       <c r="M8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,M$4)</f>
-        <v>43030472.700000003</v>
+        <v>28720303.899999999</v>
       </c>
       <c r="N8" s="42">
         <f>RTD(progId,,BINANCE_24H,$A8,N$4)</f>
-        <v>21439989.816296</v>
+        <v>14130749.716714</v>
       </c>
       <c r="O8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,O$4)</f>
-        <v>27840</v>
+        <v>17606</v>
       </c>
       <c r="P8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,P$4)</f>
-        <v>3.2100000000000002E-3</v>
+        <v>-9.2899999999999996E-3</v>
       </c>
       <c r="Q8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,Q$4)</f>
-        <v>1.5100000000000001E-3</v>
+        <v>-4.64E-3</v>
       </c>
       <c r="S8" s="38" t="s">
         <v>64</v>
       </c>
       <c r="T8" s="36" t="str">
         <f>RTD(progId,,BINANCE,,S8)</f>
-        <v>ETHBTC|LTCBTC|BNBBTC|NEOBTC|QTUMETH|EOSETH|SNTETH|BNTETH|BCCBTC|GASBTC|BNBETH|BTCUSDT|ETHUSDT|HSRBTC|OAXETH|DNTETH|MCOETH|ICNETH|MCOBTC|WTCBTC|WTCETH|LRCBTC|LRCETH|QTUMBTC|YOYOBTC|OMGBTC|OMGETH|ZRXBTC|ZRXETH|STRATBTC|STRATETH|SNGLSBTC|SNGLSETH|BQXBTC|BQXETH|KNCBTC|KNCETH|FUNBTC|FUNETH|SNMBTC|SNMETH|NEOETH|IOTABTC|IOTAETH|LINKBTC|LINKETH|XVGBTC|XVGETH|SALTBTC|SALTETH|MDABTC|MDAETH|MTLBTC|MTLETH|SUBBTC|SUBETH|EOSBTC|SNTBTC|ETCETH|ETCBTC|MTHBTC|MTHETH|ENGBTC|ENGETH|DNTBTC|ZECBTC|ZECETH|BNTBTC|ASTBTC|ASTETH|DASHBTC|DASHETH|OAXBTC|ICNBTC|BTGBTC|BTGETH|EVXBTC|EVXETH|REQBTC|REQETH|VIBBTC|VIBETH|HSRETH|TRXBTC|TRXETH|POWRBTC|POWRETH|ARKBTC|ARKETH|YOYOETH|XRPBTC|XRPETH|MODBTC|MODETH|ENJBTC|ENJETH|STORJBTC|STORJETH|BNBUSDT|VENBNB|YOYOBNB|POWRBNB|VENBTC|VENETH|KMDBTC|KMDETH|NULSBNB|RCNBTC|RCNETH|RCNBNB|NULSBTC|NULSETH|RDNBTC|RDNETH|RDNBNB|XMRBTC|XMRETH|DLTBNB|WTCBNB|DLTBTC|DLTETH|AMBBTC|AMBETH|AMBBNB|BCCETH|BCCUSDT|BCCBNB|BATBTC|BATETH|BATBNB|BCPTBTC|BCPTETH|BCPTBNB|ARNBTC|ARNETH|GVTBTC|GVTETH|CDTBTC|CDTETH|GXSBTC|GXSETH|NEOUSDT|NEOBNB|POEBTC|POEETH|QSPBTC|QSPETH|QSPBNB|BTSBTC|BTSETH|BTSBNB|XZCBTC|XZCETH|XZCBNB|LSKBTC|LSKETH|LSKBNB|TNTBTC|TNTETH|FUELBTC|FUELETH|MANABTC|MANAETH|BCDBTC|BCDETH|DGDBTC|DGDETH|IOTABNB|ADXBTC|ADXETH|ADXBNB|ADABTC|ADAETH|PPTBTC|PPTETH|CMTBTC|CMTETH|CMTBNB|XLMBTC|XLMETH|XLMBNB|CNDBTC|CNDETH|CNDBNB|LENDBTC|LENDETH|WABIBTC|WABIETH|WABIBNB|LTCETH|LTCUSDT|LTCBNB|TNBBTC|TNBETH|WAVESBTC|WAVESETH|WAVESBNB|GTOBTC|GTOETH|GTOBNB|ICXBTC|ICXETH|ICXBNB|OSTBTC|OSTETH|OSTBNB|ELFBTC|ELFETH|AIONBTC|AIONETH|AIONBNB|NEBLBTC|NEBLETH|NEBLBNB|BRDBTC|BRDETH|BRDBNB|MCOBNB|EDOBTC|EDOETH|WINGSBTC|WINGSETH|NAVBTC|NAVETH|NAVBNB|LUNBTC|LUNETH|TRIGBTC|TRIGETH|TRIGBNB|APPCBTC|APPCETH|APPCBNB|VIBEBTC|VIBEETH|RLCBTC|RLCETH|RLCBNB|INSBTC|INSETH|PIVXBTC|PIVXETH|PIVXBNB|IOSTBTC|IOSTETH|CHATBTC|CHATETH|STEEMBTC|STEEMETH|STEEMBNB|NANOBTC|NANOETH|NANOBNB|VIABTC|VIAETH|VIABNB|BLZBTC|BLZETH|BLZBNB|AEBTC|AEETH|AEBNB|RPXBTC|RPXETH|RPXBNB|NCASHBTC|NCASHETH|NCASHBNB|POABTC|POAETH|POABNB|ZILBTC|ZILETH|ZILBNB|ONTBTC|ONTETH|ONTBNB|STORMBTC|STORMETH|STORMBNB|QTUMBNB|QTUMUSDT|XEMBTC|XEMETH|XEMBNB|WANBTC|WANETH|WANBNB|WPRBTC|WPRETH|QLCBTC|QLCETH|SYSBTC|SYSETH|SYSBNB|QLCBNB|GRSBTC|GRSETH|ADAUSDT|ADABNB|CLOAKBTC|CLOAKETH|GNTBTC|GNTETH|GNTBNB|LOOMBTC|LOOMETH|LOOMBNB|XRPUSDT|BCNBTC|BCNETH|BCNBNB|REPBTC|REPETH|REPBNB|TUSDBTC|TUSDETH|TUSDBNB|ZENBTC|ZENETH|ZENBNB|SKYBTC|SKYETH|SKYBNB|EOSUSDT|EOSBNB|CVCBTC|CVCETH|CVCBNB|THETABTC|THETAETH|THETABNB|XRPBNB|TUSDUSDT|IOTAUSDT|XLMUSDT|IOTXBTC|IOTXETH|QKCBTC|QKCETH|AGIBTC|AGIETH|AGIBNB|NXSBTC|NXSETH|NXSBNB|ENJBNB|DATABTC|DATAETH|ONTUSDT|TRXUSDT|ETCUSDT|ETCBNB|ICXUSDT|SCBTC|SCETH|SCBNB|NPXSBTC|NPXSETH|VENUSDT|KEYBTC|KEYETH|NASBTC|NASETH|NASBNB|</v>
+        <v>["ETHBTC","LTCBTC","BNBBTC","NEOBTC","QTUMETH","EOSETH","SNTETH","BNTETH","BCCBTC","GASBTC","BNBETH","BTCUSDT","ETHUSDT","HSRBTC","OAXETH","DNTETH","MCOETH","ICNETH","MCOBTC","WTCBTC","WTCETH","LRCBTC","LRCETH","QTUMBTC","YOYOBTC","OMGBTC","OMGETH","ZRXBTC","ZRXETH","STRATBTC","STRATETH","SNGLSBTC","SNGLSETH","BQXBTC","BQXETH","KNCBTC","KNCETH","FUNBTC","FUNETH","SNMBTC","SNMETH","NEOETH","IOTABTC","IOTAETH","LINKBTC","LINKETH","XVGBTC","XVGETH","SALTBTC","SALTETH","MDABTC","MDAETH","MTLBTC","MTLETH","SUBBTC","SUBETH","EOSBTC","SNTBTC","ETCETH","ETCBTC","MTHBTC","MTHETH","ENGBTC","ENGETH","DNTBTC","ZECBTC","ZECETH","BNTBTC","ASTBTC","ASTETH","DASHBTC","DASHETH","OAXBTC","ICNBTC","BTGBTC","BTGETH","EVXBTC","EVXETH","REQBTC","REQETH","VIBBTC","VIBETH","HSRETH","TRXBTC","TRXETH","POWRBTC","POWRETH","ARKBTC","ARKETH","YOYOETH","XRPBTC","XRPETH","MODBTC","MODETH","ENJBTC","ENJETH","STORJBTC","STORJETH","BNBUSDT","VENBNB","YOYOBNB","POWRBNB","VENBTC","VENETH","KMDBTC","KMDETH","NULSBNB","RCNBTC","RCNETH","RCNBNB","NULSBTC","NULSETH","RDNBTC","RDNETH","RDNBNB","XMRBTC","XMRETH","DLTBNB","WTCBNB","DLTBTC","DLTETH","AMBBTC","AMBETH","AMBBNB","BCCETH","BCCUSDT","BCCBNB","BATBTC","BATETH","BATBNB","BCPTBTC","BCPTETH","BCPTBNB","ARNBTC","ARNETH","GVTBTC","GVTETH","CDTBTC","CDTETH","GXSBTC","GXSETH","NEOUSDT","NEOBNB","POEBTC","POEETH","QSPBTC","QSPETH","QSPBNB","BTSBTC","BTSETH","BTSBNB","XZCBTC","XZCETH","XZCBNB","LSKBTC","LSKETH","LSKBNB","TNTBTC","TNTETH","FUELBTC","FUELETH","MANABTC","MANAETH","BCDBTC","BCDETH","DGDBTC","DGDETH","IOTABNB","ADXBTC","ADXETH","ADXBNB","ADABTC","ADAETH","PPTBTC","PPTETH","CMTBTC","CMTETH","CMTBNB","XLMBTC","XLMETH","XLMBNB","CNDBTC","CNDETH","CNDBNB","LENDBTC","LENDETH","WABIBTC","WABIETH","WABIBNB","LTCETH","LTCUSDT","LTCBNB","TNBBTC","TNBETH","WAVESBTC","WAVESETH","WAVESBNB","GTOBTC","GTOETH","GTOBNB","ICXBTC","ICXETH","ICXBNB","OSTBTC","OSTETH","OSTBNB","ELFBTC","ELFETH","AIONBTC","AIONETH","AIONBNB","NEBLBTC","NEBLETH","NEBLBNB","BRDBTC","BRDETH","BRDBNB","MCOBNB","EDOBTC","EDOETH","WINGSBTC","WINGSETH","NAVBTC","NAVETH","NAVBNB","LUNBTC","LUNETH","TRIGBTC","TRIGETH","TRIGBNB","APPCBTC","APPCETH","APPCBNB","VIBEBTC","VIBEETH","RLCBTC","RLCETH","RLCBNB","INSBTC","INSETH","PIVXBTC","PIVXETH","PIVXBNB","IOSTBTC","IOSTETH","CHATBTC","CHATETH","STEEMBTC","STEEMETH","STEEMBNB","NANOBTC","NANOETH","NANOBNB","VIABTC","VIAETH","VIABNB","BLZBTC","BLZETH","BLZBNB","AEBTC","AEETH","AEBNB","RPXBTC","RPXETH","RPXBNB","NCASHBTC","NCASHETH","NCASHBNB","POABTC","POAETH","POABNB","ZILBTC","ZILETH","ZILBNB","ONTBTC","ONTETH","ONTBNB","STORMBTC","STORMETH","STORMBNB","QTUMBNB","QTUMUSDT","XEMBTC","XEMETH","XEMBNB","WANBTC","WANETH","WANBNB","WPRBTC","WPRETH","QLCBTC","QLCETH","SYSBTC","SYSETH","SYSBNB","QLCBNB","GRSBTC","GRSETH","ADAUSDT","ADABNB","CLOAKBTC","CLOAKETH","GNTBTC","GNTETH","GNTBNB","LOOMBTC","LOOMETH","LOOMBNB","XRPUSDT","BCNBTC","BCNETH","BCNBNB","REPBTC","REPETH","REPBNB","TUSDBTC","TUSDETH","TUSDBNB","ZENBTC","ZENETH","ZENBNB","SKYBTC","SKYETH","SKYBNB","EOSUSDT","EOSBNB","CVCBTC","CVCETH","CVCBNB","THETABTC","THETAETH","THETABNB","XRPBNB","TUSDUSDT","IOTAUSDT","XLMUSDT","IOTXBTC","IOTXETH","QKCBTC","QKCETH","AGIBTC","AGIETH","AGIBNB","NXSBTC","NXSETH","NXSBNB","ENJBNB","DATABTC","DATAETH","ONTUSDT","TRXUSDT","ETCUSDT","ETCBNB","ICXUSDT","SCBTC","SCETH","SCBNB","NPXSBTC","NPXSETH","VENUSDT","KEYBTC","KEYETH","NASBTC","NASETH","NASBNB"]</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -6204,59 +6204,59 @@
       </c>
       <c r="B9" s="2">
         <f>RTD(progId,,BINANCE,$A9,B$4)</f>
-        <v>5.4000000000000003E-3</v>
+        <v>5.4349999999999997E-3</v>
       </c>
       <c r="C9" s="2">
         <f>RTD(progId,,BINANCE,$A9,C$4)</f>
-        <v>5.8349999999999999E-3</v>
+        <v>6.1910000000000003E-3</v>
       </c>
       <c r="D9" s="2">
         <f>RTD(progId,,BINANCE_24H,$A9,D$4)</f>
-        <v>5.5030000000000001E-3</v>
+        <v>5.5380000000000004E-3</v>
       </c>
       <c r="G9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,G$4)</f>
-        <v>5.5030000000000001E-3</v>
+        <v>5.5440000000000003E-3</v>
       </c>
       <c r="H9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,H$4)</f>
-        <v>2.48</v>
+        <v>0.03</v>
       </c>
       <c r="I9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,I$4)</f>
-        <v>5.6169999999999996E-3</v>
+        <v>5.8050000000000003E-3</v>
       </c>
       <c r="J9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,J$4)</f>
-        <v>1.1E-5</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="K9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,K$4)</f>
-        <v>5.6259999999999999E-3</v>
+        <v>5.8069999999999997E-3</v>
       </c>
       <c r="L9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,L$4)</f>
-        <v>98.8</v>
+        <v>6.58</v>
       </c>
       <c r="M9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,M$4)</f>
-        <v>598657.79</v>
+        <v>506889</v>
       </c>
       <c r="N9" s="42">
         <f>RTD(progId,,BINANCE_24H,$A9,N$4)</f>
-        <v>3367.3331261399999</v>
+        <v>2938.16672982</v>
       </c>
       <c r="O9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,O$4)</f>
-        <v>68913</v>
+        <v>51127</v>
       </c>
       <c r="P9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,P$4)</f>
-        <v>2.0889999999999999E-2</v>
+        <v>4.7629999999999999E-2</v>
       </c>
       <c r="Q9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,Q$4)</f>
-        <v>1.16E-4</v>
+        <v>2.63E-4</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6265,59 +6265,59 @@
       </c>
       <c r="B10" s="2">
         <f>RTD(progId,,BINANCE,$A10,B$4)</f>
-        <v>7.3609999999999995E-5</v>
+        <v>7.3490000000000003E-5</v>
       </c>
       <c r="C10" s="2">
         <f>RTD(progId,,BINANCE,$A10,C$4)</f>
-        <v>7.8139999999999994E-5</v>
+        <v>7.6240000000000002E-5</v>
       </c>
       <c r="D10" s="2">
         <f>RTD(progId,,BINANCE_24H,$A10,D$4)</f>
-        <v>7.4129999999999997E-5</v>
+        <v>7.5820000000000003E-5</v>
       </c>
       <c r="G10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,G$4)</f>
-        <v>7.4120000000000002E-5</v>
+        <v>7.5850000000000001E-5</v>
       </c>
       <c r="H10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,H$4)</f>
-        <v>356</v>
+        <v>3086</v>
       </c>
       <c r="I10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,I$4)</f>
-        <v>7.483E-5</v>
+        <v>7.4190000000000006E-5</v>
       </c>
       <c r="J10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,J$4)</f>
-        <v>8.9999999999999999E-8</v>
+        <v>7.0000000000000005E-8</v>
       </c>
       <c r="K10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,K$4)</f>
-        <v>7.4870000000000007E-5</v>
+        <v>7.428E-5</v>
       </c>
       <c r="L10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,L$4)</f>
-        <v>780</v>
+        <v>2199</v>
       </c>
       <c r="M10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,M$4)</f>
-        <v>51677984</v>
+        <v>36351363</v>
       </c>
       <c r="N10" s="42">
         <f>RTD(progId,,BINANCE_24H,$A10,N$4)</f>
-        <v>3901.26588558</v>
+        <v>2711.1513072399998</v>
       </c>
       <c r="O10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,O$4)</f>
-        <v>53832</v>
+        <v>30879</v>
       </c>
       <c r="P10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,P$4)</f>
-        <v>8.2199999999999999E-3</v>
+        <v>-2.121E-2</v>
       </c>
       <c r="Q10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,Q$4)</f>
-        <v>7.0999999999999998E-7</v>
+        <v>-1.66E-6</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6326,27 +6326,27 @@
       </c>
       <c r="B11" s="2">
         <f>RTD(progId,,BINANCE,$A11,B$4)</f>
-        <v>5.8300000000000001E-6</v>
+        <v>5.7699999999999998E-6</v>
       </c>
       <c r="C11" s="2">
         <f>RTD(progId,,BINANCE,$A11,C$4)</f>
-        <v>6.1399999999999997E-6</v>
+        <v>5.9900000000000002E-6</v>
       </c>
       <c r="D11" s="2">
         <f>RTD(progId,,BINANCE_24H,$A11,D$4)</f>
-        <v>6.0299999999999999E-6</v>
+        <v>5.9000000000000003E-6</v>
       </c>
       <c r="G11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,G$4)</f>
-        <v>6.0299999999999999E-6</v>
+        <v>5.9000000000000003E-6</v>
       </c>
       <c r="H11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,H$4)</f>
-        <v>325948</v>
+        <v>1035439</v>
       </c>
       <c r="I11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,I$4)</f>
-        <v>5.93E-6</v>
+        <v>5.8799999999999996E-6</v>
       </c>
       <c r="J11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,J$4)</f>
@@ -6354,31 +6354,31 @@
       </c>
       <c r="K11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,K$4)</f>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
       </c>
       <c r="L11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,L$4)</f>
-        <v>62318</v>
+        <v>73326</v>
       </c>
       <c r="M11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,M$4)</f>
-        <v>572222720</v>
+        <v>399604654</v>
       </c>
       <c r="N11" s="42">
         <f>RTD(progId,,BINANCE_24H,$A11,N$4)</f>
-        <v>3426.7021633099998</v>
+        <v>2358.1084988900002</v>
       </c>
       <c r="O11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,O$4)</f>
-        <v>42575</v>
+        <v>30240</v>
       </c>
       <c r="P11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,P$4)</f>
-        <v>-1.4930000000000001E-2</v>
+        <v>-1.6900000000000001E-3</v>
       </c>
       <c r="Q11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,Q$4)</f>
-        <v>-8.9999999999999999E-8</v>
+        <v>-1E-8</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6466,22 +6466,22 @@
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C15)</f>
-        <v>0.756328</v>
+        <v>1.992E-2</v>
       </c>
       <c r="B15" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C15)</f>
-        <v>6593.27</v>
+        <v>6665</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
       </c>
       <c r="D15" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C15)</f>
-        <v>6597.97</v>
+        <v>6667.96</v>
       </c>
       <c r="E15" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C15)</f>
-        <v>6.4515000000000003E-2</v>
+        <v>2.0254000000000001E-2</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -6489,23 +6489,23 @@
       </c>
       <c r="H15" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G15,H$14)</f>
-        <v>27042665</v>
+        <v>27105497</v>
       </c>
       <c r="I15" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G15,I$14)</f>
-        <v>468.93</v>
+        <v>471.3</v>
       </c>
       <c r="J15" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G15,J$14)</f>
-        <v>1.403</v>
+        <v>0.91744999999999999</v>
       </c>
       <c r="K15" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G15,K$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="28">
         <f>RTD(progId,,BINACE_TRADE,$G15,L$14)</f>
-        <v>43284.722217199072</v>
+        <v>43285.517101666665</v>
       </c>
       <c r="N15" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G15,N$14)</f>
@@ -6543,11 +6543,11 @@
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C16)</f>
-        <v>1.6233999999999998E-2</v>
+        <v>0.98658500000000005</v>
       </c>
       <c r="B16" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C16)</f>
-        <v>6593.26</v>
+        <v>6664.77</v>
       </c>
       <c r="C16" s="8">
         <f>C15+1</f>
@@ -6555,11 +6555,11 @@
       </c>
       <c r="D16" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C16)</f>
-        <v>6597.98</v>
+        <v>6667.97</v>
       </c>
       <c r="E16" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C16)</f>
-        <v>1.707E-3</v>
+        <v>0.35168100000000002</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
@@ -6567,15 +6567,15 @@
       </c>
       <c r="H16" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G16,H$14)</f>
-        <v>48261642</v>
+        <v>48377931</v>
       </c>
       <c r="I16" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G16,I$14)</f>
-        <v>6593.27</v>
+        <v>6664.13</v>
       </c>
       <c r="J16" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G16,J$14)</f>
-        <v>1.707E-3</v>
+        <v>0.109002</v>
       </c>
       <c r="K16" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G16,K$14)</f>
@@ -6583,7 +6583,7 @@
       </c>
       <c r="L16" s="28">
         <f>RTD(progId,,BINACE_TRADE,$G16,L$14)</f>
-        <v>43284.722259803239</v>
+        <v>43285.517102048609</v>
       </c>
       <c r="N16" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G16,N$14)</f>
@@ -6621,11 +6621,11 @@
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C17)</f>
-        <v>5.6000000000000001E-2</v>
+        <v>2.9922629999999999</v>
       </c>
       <c r="B17" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C17)</f>
-        <v>6593.18</v>
+        <v>6664.13</v>
       </c>
       <c r="C17" s="8">
         <f t="shared" ref="C17:C24" si="0">C16+1</f>
@@ -6633,11 +6633,11 @@
       </c>
       <c r="D17" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C17)</f>
-        <v>6597.99</v>
+        <v>6668</v>
       </c>
       <c r="E17" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C17)</f>
-        <v>0.91054900000000005</v>
+        <v>4.7935999999999999E-2</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -6645,23 +6645,23 @@
       </c>
       <c r="H17" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G17,H$14)</f>
-        <v>7519854</v>
+        <v>7533270</v>
       </c>
       <c r="I17" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G17,I$14)</f>
-        <v>87.17</v>
+        <v>86.86</v>
       </c>
       <c r="J17" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G17,J$14)</f>
-        <v>2.7E-4</v>
+        <v>2.5009299999999999</v>
       </c>
       <c r="K17" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G17,K$14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G17,L$14)</f>
-        <v>43284.72225363426</v>
+        <v>43285.516921724535</v>
       </c>
       <c r="N17" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G17,N$14)</f>
@@ -6699,11 +6699,11 @@
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C18)</f>
-        <v>1.7946E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="B18" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C18)</f>
-        <v>6593.14</v>
+        <v>6663.73</v>
       </c>
       <c r="C18" s="8">
         <f t="shared" si="0"/>
@@ -6711,35 +6711,35 @@
       </c>
       <c r="D18" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C18)</f>
-        <v>6599.61</v>
+        <v>6668.74</v>
       </c>
       <c r="E18" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C18)</f>
-        <v>0.111301</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="13" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G18,H$14)</f>
-        <v>1428847</v>
-      </c>
-      <c r="I18" s="13">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="I18" s="13" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G18,I$14)</f>
-        <v>0.49326999999999999</v>
-      </c>
-      <c r="J18" s="13">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="J18" s="13" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G18,J$14)</f>
-        <v>2466</v>
-      </c>
-      <c r="K18" s="13" t="b">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="K18" s="13" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G18,K$14)</f>
-        <v>1</v>
-      </c>
-      <c r="L18" s="29">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="L18" s="29" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G18,L$14)</f>
-        <v>43284.722218692128</v>
+        <v>&lt;?&gt;</v>
       </c>
       <c r="N18" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G18,N$14)</f>
@@ -6777,11 +6777,11 @@
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C19)</f>
-        <v>0.62049699999999997</v>
+        <v>9.0060000000000001E-2</v>
       </c>
       <c r="B19" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C19)</f>
-        <v>6593.03</v>
+        <v>6662.15</v>
       </c>
       <c r="C19" s="8">
         <f t="shared" si="0"/>
@@ -6789,11 +6789,11 @@
       </c>
       <c r="D19" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C19)</f>
-        <v>6599.98</v>
+        <v>6668.78</v>
       </c>
       <c r="E19" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C19)</f>
-        <v>0.03</v>
+        <v>0.49435000000000001</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
@@ -6801,15 +6801,15 @@
       </c>
       <c r="H19" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G19,H$14)</f>
-        <v>14520756</v>
+        <v>14554128</v>
       </c>
       <c r="I19" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G19,I$14)</f>
-        <v>5.5999999999999999E-3</v>
+        <v>5.7980000000000002E-3</v>
       </c>
       <c r="J19" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G19,J$14)</f>
-        <v>1.5</v>
+        <v>15.4</v>
       </c>
       <c r="K19" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G19,K$14)</f>
@@ -6817,7 +6817,7 @@
       </c>
       <c r="L19" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G19,L$14)</f>
-        <v>43284.722140613427</v>
+        <v>43285.517102199075</v>
       </c>
       <c r="N19" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G19,N$14)</f>
@@ -6855,11 +6855,11 @@
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C20)</f>
-        <v>1.9989999999999999E-3</v>
+        <v>4.0910000000000002</v>
       </c>
       <c r="B20" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C20)</f>
-        <v>6591.89</v>
+        <v>6661.45</v>
       </c>
       <c r="C20" s="8">
         <f t="shared" si="0"/>
@@ -6867,11 +6867,11 @@
       </c>
       <c r="D20" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C20)</f>
-        <v>6599.99</v>
+        <v>6668.91</v>
       </c>
       <c r="E20" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C20)</f>
-        <v>0.56970900000000002</v>
+        <v>9.4730999999999996E-2</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
@@ -6879,15 +6879,15 @@
       </c>
       <c r="H20" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G20,H$14)</f>
-        <v>18577123</v>
+        <v>18596602</v>
       </c>
       <c r="I20" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G20,I$14)</f>
-        <v>7.4930000000000003E-5</v>
+        <v>7.4259999999999997E-5</v>
       </c>
       <c r="J20" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G20,J$14)</f>
-        <v>24</v>
+        <v>377</v>
       </c>
       <c r="K20" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G20,K$14)</f>
@@ -6895,7 +6895,7 @@
       </c>
       <c r="L20" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G20,L$14)</f>
-        <v>43284.722096273152</v>
+        <v>43285.517003391207</v>
       </c>
       <c r="N20" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G20,N$14)</f>
@@ -6933,11 +6933,11 @@
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C21)</f>
-        <v>0.48682999999999998</v>
+        <v>0.109</v>
       </c>
       <c r="B21" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C21)</f>
-        <v>6591.4</v>
+        <v>6661.02</v>
       </c>
       <c r="C21" s="8">
         <f t="shared" si="0"/>
@@ -6945,11 +6945,11 @@
       </c>
       <c r="D21" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C21)</f>
-        <v>6600</v>
+        <v>6669</v>
       </c>
       <c r="E21" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C21)</f>
-        <v>1.0923020000000001</v>
+        <v>7.5079999999999999E-3</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
@@ -6957,15 +6957,15 @@
       </c>
       <c r="H21" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G21,H$14)</f>
-        <v>19221669</v>
+        <v>19233907</v>
       </c>
       <c r="I21" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G21,I$14)</f>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
       </c>
       <c r="J21" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G21,J$14)</f>
-        <v>2277</v>
+        <v>500</v>
       </c>
       <c r="K21" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G21,K$14)</f>
@@ -6973,7 +6973,7 @@
       </c>
       <c r="L21" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G21,L$14)</f>
-        <v>43284.722241087962</v>
+        <v>43285.516921377312</v>
       </c>
       <c r="N21" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G21,N$14)</f>
@@ -7011,11 +7011,11 @@
     <row r="22" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C22)</f>
-        <v>0.1</v>
+        <v>4.413157</v>
       </c>
       <c r="B22" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C22)</f>
-        <v>6590.01</v>
+        <v>6660.61</v>
       </c>
       <c r="C22" s="8">
         <f t="shared" si="0"/>
@@ -7023,21 +7023,21 @@
       </c>
       <c r="D22" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C22)</f>
-        <v>6601.54</v>
+        <v>6669.51</v>
       </c>
       <c r="E22" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C22)</f>
-        <v>0.79949999999999999</v>
+        <v>0.66981900000000005</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C23)</f>
-        <v>11.064577</v>
+        <v>3.8E-3</v>
       </c>
       <c r="B23" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C23)</f>
-        <v>6590</v>
+        <v>6660.53</v>
       </c>
       <c r="C23" s="8">
         <f t="shared" si="0"/>
@@ -7045,11 +7045,11 @@
       </c>
       <c r="D23" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C23)</f>
-        <v>6603</v>
+        <v>6669.86</v>
       </c>
       <c r="E23" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C23)</f>
-        <v>7.5883999999999993E-2</v>
+        <v>0.57014500000000001</v>
       </c>
       <c r="G23" s="34" t="s">
         <v>55</v>
@@ -7065,11 +7065,11 @@
     <row r="24" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="31">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C24)</f>
-        <v>1</v>
+        <v>0.97992699999999999</v>
       </c>
       <c r="B24" s="31">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C24)</f>
-        <v>6588.64</v>
+        <v>6660</v>
       </c>
       <c r="C24" s="32">
         <f t="shared" si="0"/>
@@ -7077,38 +7077,38 @@
       </c>
       <c r="D24" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C24)</f>
-        <v>6603.78</v>
+        <v>6669.87</v>
       </c>
       <c r="E24" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C24)</f>
-        <v>4.7562E-2</v>
+        <v>0.01</v>
       </c>
       <c r="G24" s="35" t="str">
         <f>RTD(progId,,BINANCE_HISTORY,J23,"a,b,c",10)</f>
-        <v>[["SYMBOL","TRADE_ID","PRICE","QUANTITY","TRADE_TIME","IS_BEST_MATCH","BUYER_IS_MAKER"],["ETHUSDT",30325041,468.88000000,0.15959000,"2018-07-03T17:17:31.738-04:00",true,true],["ETHUSDT",30325042,468.88000000,0.00041000,"2018-07-03T17:17:37.266-04:00",true,true],["ETHUSDT",30325043,468.86000000,2.08320000,"2018-07-03T17:17:39.711-04:00",true,false],["ETHUSDT",30325044,468.75000000,0.03180000,"2018-07-03T17:17:41.766-04:00",true,true],["ETHUSDT",30325045,468.75000000,0.16820000,"2018-07-03T17:17:41.766-04:00",true,true],["ETHUSDT",30325046,468.75000000,0.15428000,"2018-07-03T17:17:43.196-04:00",true,true],["ETHUSDT",30325047,468.86000000,4.75865000,"2018-07-03T17:17:47.152-04:00",true,false],["ETHUSDT",30325048,468.97000000,4.17426000,"2018-07-03T17:17:47.17-04:00",true,false],["ETHUSDT",30325049,468.77000000,0.09950000,"2018-07-03T17:17:48.792-04:00",true,true],["ETHUSDT",30325050,468.95000000,0.02592000,"2018-07-03T17:17:52.165-04:00",true,false]]</v>
+        <v>Server error: {"code":-2015,"msg":"Invalid API-key, IP, or permissions for action."}</v>
       </c>
       <c r="H24"/>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <f>SUM(Table3[BID_DEPTH_SIZE])</f>
-        <v>14.120411000000001</v>
+        <v>13.741712000000001</v>
       </c>
       <c r="B25" s="14">
         <f>SUMPRODUCT(Table3[BID_DEPTH_SIZE],Table3[BID_DEPTH])</f>
-        <v>93057.475481860005</v>
+        <v>91546.105255410002</v>
       </c>
       <c r="C25" s="39">
         <f>B25-D25</f>
-        <v>68617.859737060004</v>
+        <v>76057.582041400005</v>
       </c>
       <c r="D25" s="14">
         <f>SUMPRODUCT(Table3[ASK_DEPTH_SIZE],Table3[ASK_DEPTH])</f>
-        <v>24439.615744800001</v>
+        <v>15488.523214010002</v>
       </c>
       <c r="E25" s="12">
         <f>SUM(Table3[ASK_DEPTH_SIZE])</f>
-        <v>3.7030290000000003</v>
+        <v>2.3224239999999998</v>
       </c>
       <c r="F25" s="9"/>
       <c r="H25" s="1"/>
@@ -7119,14 +7119,14 @@
     <row r="26" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="30">
         <f>B15-B24</f>
-        <v>4.6300000000001091</v>
+        <v>5</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D26" s="30">
         <f>D15-D24</f>
-        <v>-5.8099999999994907</v>
+        <v>-1.9099999999998545</v>
       </c>
       <c r="F26" s="9"/>
       <c r="I26" s="4"/>
@@ -7212,27 +7212,27 @@
       </c>
       <c r="B30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,B$29,$D$28)</f>
-        <v>470.45</v>
+        <v>473.21</v>
       </c>
       <c r="C30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,C$29,$D$28)</f>
-        <v>471.31</v>
+        <v>474.62</v>
       </c>
       <c r="D30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,D$29,$D$28)</f>
-        <v>467.93</v>
+        <v>471.03</v>
       </c>
       <c r="E30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,E$29,$D$28)</f>
-        <v>468.93</v>
+        <v>471.3</v>
       </c>
       <c r="F30" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,F$29,$D$28)</f>
-        <v>43284.708333333336</v>
+        <v>43285.5</v>
       </c>
       <c r="G30" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,G$29,$D$28)</f>
-        <v>43284.749999988424</v>
+        <v>43285.541666655095</v>
       </c>
       <c r="H30" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,H$29,$D$28)</f>
@@ -7240,19 +7240,19 @@
       </c>
       <c r="I30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,I$29,$D$28)</f>
-        <v>674654.7416978</v>
+        <v>1165600.1691212</v>
       </c>
       <c r="J30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,J$29,$D$28)</f>
-        <v>1437.56467</v>
+        <v>2463.4826800000001</v>
       </c>
       <c r="K30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,K$29,$D$28)</f>
-        <v>791.60347999999999</v>
+        <v>1193.0365300000001</v>
       </c>
       <c r="L30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,L$29,$D$28)</f>
-        <v>371589.88051839999</v>
+        <v>564552.89316370001</v>
       </c>
       <c r="M30" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,M$29,$D$28)</f>
@@ -7260,19 +7260,19 @@
       </c>
       <c r="N30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,N$29,$D$28)</f>
-        <v>1228</v>
+        <v>2114</v>
       </c>
       <c r="O30" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,O$29,$D$28)</f>
-        <v>43284.722217222225</v>
+        <v>43285.517101504629</v>
       </c>
       <c r="P30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,P$29,$D$28)</f>
-        <v>30323933</v>
+        <v>30391319</v>
       </c>
       <c r="Q30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,Q$29,$D$28)</f>
-        <v>30325160</v>
+        <v>30393432</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -7281,27 +7281,27 @@
       </c>
       <c r="B31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,B$29,$D$28)</f>
-        <v>6612.96</v>
+        <v>6683.77</v>
       </c>
       <c r="C31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,C$29,$D$28)</f>
-        <v>6622</v>
+        <v>6691.01</v>
       </c>
       <c r="D31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,D$29,$D$28)</f>
-        <v>6586.03</v>
+        <v>6650.93</v>
       </c>
       <c r="E31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,E$29,$D$28)</f>
-        <v>6596</v>
+        <v>6664.13</v>
       </c>
       <c r="F31" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,F$29,$D$28)</f>
-        <v>43284.708333333336</v>
+        <v>43285.5</v>
       </c>
       <c r="G31" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,G$29,$D$28)</f>
-        <v>43284.749999988424</v>
+        <v>43285.541666655095</v>
       </c>
       <c r="H31" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,H$29,$D$28)</f>
@@ -7309,19 +7309,19 @@
       </c>
       <c r="I31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,I$29,$D$28)</f>
-        <v>2392227.0247127102</v>
+        <v>4797712.7030429197</v>
       </c>
       <c r="J31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,J$29,$D$28)</f>
-        <v>362.47585800000002</v>
+        <v>717.961096</v>
       </c>
       <c r="K31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,K$29,$D$28)</f>
-        <v>186.756066</v>
+        <v>366.14173099999999</v>
       </c>
       <c r="L31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,L$29,$D$28)</f>
-        <v>1232565.7239691401</v>
+        <v>2447502.1504584299</v>
       </c>
       <c r="M31" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,M$29,$D$28)</f>
@@ -7329,19 +7329,19 @@
       </c>
       <c r="N31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,N$29,$D$28)</f>
-        <v>2737</v>
+        <v>4014</v>
       </c>
       <c r="O31" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,O$29,$D$28)</f>
-        <v>43284.722245023149</v>
+        <v>43285.517102083337</v>
       </c>
       <c r="P31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,P$29,$D$28)</f>
-        <v>54781604</v>
+        <v>54906915</v>
       </c>
       <c r="Q31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,Q$29,$D$28)</f>
-        <v>54784340</v>
+        <v>54910928</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -7350,27 +7350,27 @@
       </c>
       <c r="B32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,B$29,$D$28)</f>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
       </c>
       <c r="C32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,C$29,$D$28)</f>
-        <v>5.9699999999999996E-6</v>
+        <v>5.9100000000000002E-6</v>
       </c>
       <c r="D32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,D$29,$D$28)</f>
-        <v>5.9200000000000001E-6</v>
+        <v>5.8799999999999996E-6</v>
       </c>
       <c r="E32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,E$29,$D$28)</f>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
       </c>
       <c r="F32" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,F$29,$D$28)</f>
-        <v>43284.708333333336</v>
+        <v>43285.5</v>
       </c>
       <c r="G32" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,G$29,$D$28)</f>
-        <v>43284.749999988424</v>
+        <v>43285.541666655095</v>
       </c>
       <c r="H32" s="18" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,H$29,$D$28)</f>
@@ -7378,19 +7378,19 @@
       </c>
       <c r="I32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,I$29,$D$28)</f>
-        <v>58.244677230000001</v>
+        <v>35.743519800000001</v>
       </c>
       <c r="J32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,J$29,$D$28)</f>
-        <v>9791683</v>
+        <v>6062958</v>
       </c>
       <c r="K32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,K$29,$D$28)</f>
-        <v>5257284</v>
+        <v>2043046</v>
       </c>
       <c r="L32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,L$29,$D$28)</f>
-        <v>31.2854311</v>
+        <v>12.049877589999999</v>
       </c>
       <c r="M32" s="18" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,M$29,$D$28)</f>
@@ -7398,19 +7398,19 @@
       </c>
       <c r="N32" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,N$29,$D$28)</f>
-        <v>543</v>
+        <v>500</v>
       </c>
       <c r="O32" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,O$29,$D$28)</f>
-        <v>43284.722241145835</v>
+        <v>43285.516921388888</v>
       </c>
       <c r="P32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,P$29,$D$28)</f>
-        <v>30862414</v>
+        <v>30882393</v>
       </c>
       <c r="Q32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,Q$29,$D$28)</f>
-        <v>30862956</v>
+        <v>30882892</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -7489,27 +7489,27 @@
       </c>
       <c r="B36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,B$35,$D$34)</f>
-        <v>468.92</v>
+        <v>472.61</v>
       </c>
       <c r="C36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,C$35,$D$34)</f>
-        <v>468.98</v>
+        <v>472.62</v>
       </c>
       <c r="D36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,D$35,$D$34)</f>
-        <v>467.93</v>
+        <v>471.3</v>
       </c>
       <c r="E36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,E$35,$D$34)</f>
-        <v>468.93</v>
+        <v>471.3</v>
       </c>
       <c r="F36" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,F$35,$D$34)</f>
-        <v>43284.72152777778</v>
+        <v>43285.51666666667</v>
       </c>
       <c r="G36" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,G$35,$D$34)</f>
-        <v>43284.72222221065</v>
+        <v>43285.517361099533</v>
       </c>
       <c r="H36" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,H$35,$D$34)</f>
@@ -7517,19 +7517,19 @@
       </c>
       <c r="I36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,I$35,$D$34)</f>
-        <v>62870.438001199997</v>
+        <v>12544.048344999999</v>
       </c>
       <c r="J36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,J$35,$D$34)</f>
-        <v>134.20161999999999</v>
+        <v>26.591799999999999</v>
       </c>
       <c r="K36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,K$35,$D$34)</f>
-        <v>48.726190000000003</v>
+        <v>6.88591</v>
       </c>
       <c r="L36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,L$35,$D$34)</f>
-        <v>22830.8364043</v>
+        <v>3252.4823544999999</v>
       </c>
       <c r="M36" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,M$35,$D$34)</f>
@@ -7537,19 +7537,19 @@
       </c>
       <c r="N36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,N$35,$D$34)</f>
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="O36" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,O$35,$D$34)</f>
-        <v>43284.722217222225</v>
+        <v>43285.517101504629</v>
       </c>
       <c r="P36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,P$35,$D$34)</f>
-        <v>30325099</v>
+        <v>30393407</v>
       </c>
       <c r="Q36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,Q$35,$D$34)</f>
-        <v>30325160</v>
+        <v>30393432</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7558,27 +7558,27 @@
       </c>
       <c r="B37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,B$35,$D$34)</f>
-        <v>6596</v>
+        <v>6670.01</v>
       </c>
       <c r="C37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,C$35,$D$34)</f>
-        <v>6597.99</v>
+        <v>6671.01</v>
       </c>
       <c r="D37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,D$35,$D$34)</f>
-        <v>6593.27</v>
+        <v>6662.15</v>
       </c>
       <c r="E37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,E$35,$D$34)</f>
-        <v>6593.27</v>
+        <v>6664.13</v>
       </c>
       <c r="F37" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,F$35,$D$34)</f>
-        <v>43284.722222222219</v>
+        <v>43285.51666666667</v>
       </c>
       <c r="G37" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,G$35,$D$34)</f>
-        <v>43284.72291665509</v>
+        <v>43285.517361099533</v>
       </c>
       <c r="H37" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,H$35,$D$34)</f>
@@ -7586,19 +7586,19 @@
       </c>
       <c r="I37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,I$35,$D$34)</f>
-        <v>1797.6540783099999</v>
+        <v>67997.397360820003</v>
       </c>
       <c r="J37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,J$35,$D$34)</f>
-        <v>0.27246199999999998</v>
+        <v>10.200435000000001</v>
       </c>
       <c r="K37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,K$35,$D$34)</f>
-        <v>0.22354499999999999</v>
+        <v>2.0317949999999998</v>
       </c>
       <c r="L37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,L$35,$D$34)</f>
-        <v>1474.9476208200001</v>
+        <v>13547.573522049999</v>
       </c>
       <c r="M37" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,M$35,$D$34)</f>
@@ -7606,19 +7606,19 @@
       </c>
       <c r="N37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,N$35,$D$34)</f>
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="O37" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,O$35,$D$34)</f>
-        <v>43284.722259895832</v>
+        <v>43285.517102071761</v>
       </c>
       <c r="P37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,P$35,$D$34)</f>
-        <v>54784340</v>
+        <v>54910865</v>
       </c>
       <c r="Q37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,Q$35,$D$34)</f>
-        <v>54784346</v>
+        <v>54910928</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7627,27 +7627,27 @@
       </c>
       <c r="B38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,B$35,$D$34)</f>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
       </c>
       <c r="C38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,C$35,$D$34)</f>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
       </c>
       <c r="D38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,D$35,$D$34)</f>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
       </c>
       <c r="E38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,E$35,$D$34)</f>
-        <v>5.9399999999999999E-6</v>
+        <v>5.8900000000000004E-6</v>
       </c>
       <c r="F38" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,F$35,$D$34)</f>
-        <v>43284.722222222219</v>
+        <v>43285.51666666667</v>
       </c>
       <c r="G38" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,G$35,$D$34)</f>
-        <v>43284.72291665509</v>
+        <v>43285.517361099533</v>
       </c>
       <c r="H38" s="18" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,H$35,$D$34)</f>
@@ -7655,19 +7655,19 @@
       </c>
       <c r="I38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,I$35,$D$34)</f>
-        <v>1.352538E-2</v>
+        <v>0.18112928</v>
       </c>
       <c r="J38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,J$35,$D$34)</f>
-        <v>2277</v>
+        <v>30752</v>
       </c>
       <c r="K38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,K$35,$D$34)</f>
-        <v>2277</v>
+        <v>30752</v>
       </c>
       <c r="L38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,L$35,$D$34)</f>
-        <v>1.352538E-2</v>
+        <v>0.18112928</v>
       </c>
       <c r="M38" s="18" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,M$35,$D$34)</f>
@@ -7675,19 +7675,19 @@
       </c>
       <c r="N38" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,N$35,$D$34)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O38" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,O$35,$D$34)</f>
-        <v>43284.722241145835</v>
+        <v>43285.516921388888</v>
       </c>
       <c r="P38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,P$35,$D$34)</f>
-        <v>30862956</v>
+        <v>30882888</v>
       </c>
       <c r="Q38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,Q$35,$D$34)</f>
-        <v>30862956</v>
+        <v>30882892</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -8080,31 +8080,31 @@
       </c>
       <c r="B3" s="2">
         <f>RTD(progId,,GDAX,$A3,B$2)</f>
-        <v>468</v>
+        <v>471.76</v>
       </c>
       <c r="C3" s="2">
         <f>RTD(progId,,GDAX,$A3,C$2)</f>
-        <v>468.01</v>
+        <v>471.77</v>
       </c>
       <c r="D3" s="2">
         <f>RTD(progId,,GDAX,$A3,D$2)</f>
-        <v>468.01</v>
+        <v>471.77</v>
       </c>
       <c r="E3" s="2">
         <f>RTD(progId,,GDAX,$A3,E$2)</f>
-        <v>475.27</v>
+        <v>468.56</v>
       </c>
       <c r="F3" s="2">
         <f>RTD(progId,,GDAX,$A3,F$2)</f>
-        <v>486.76</v>
+        <v>482.01</v>
       </c>
       <c r="G3" s="2">
         <f>RTD(progId,,GDAX,$A3,G$2)</f>
-        <v>461.69</v>
+        <v>451.35</v>
       </c>
       <c r="H3" s="2">
         <f>RTD(progId,,GDAX,$A3,H$2)</f>
-        <v>68576.476604249998</v>
+        <v>64263.177474869997</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8113,31 +8113,31 @@
       </c>
       <c r="B4" s="2">
         <f>RTD(progId,,GDAX,$A4,B$2)</f>
-        <v>6596.21</v>
+        <v>6663.66</v>
       </c>
       <c r="C4" s="2">
         <f>RTD(progId,,GDAX,$A4,C$2)</f>
-        <v>6596.5</v>
+        <v>6663.67</v>
       </c>
       <c r="D4" s="2">
         <f>RTD(progId,,GDAX,$A4,D$2)</f>
-        <v>6596.5</v>
+        <v>6663.67</v>
       </c>
       <c r="E4" s="2">
         <f>RTD(progId,,GDAX,$A4,E$2)</f>
-        <v>6626.31</v>
+        <v>6589.99</v>
       </c>
       <c r="F4" s="2">
         <f>RTD(progId,,GDAX,$A4,F$2)</f>
-        <v>6673.99</v>
+        <v>6796.62</v>
       </c>
       <c r="G4" s="2">
         <f>RTD(progId,,GDAX,$A4,G$2)</f>
-        <v>6535</v>
+        <v>6411.51</v>
       </c>
       <c r="H4" s="2">
         <f>RTD(progId,,GDAX,$A4,H$2)</f>
-        <v>6147.1162924800001</v>
+        <v>7532.5732854899998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to latestes Binance.net
</commit_message>
<xml_diff>
--- a/doc/crypto.xlsx
+++ b/doc/crypto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\Crypto\crypto-rtd\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6FE897-269A-4AAF-9B6C-4DEE6E248649}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B31F1DC-6A60-4BE4-B498-8D5E580CA2B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12225" tabRatio="245" xr2:uid="{FA204BA2-54FD-4EAD-B49B-FB8867D94DC8}"/>
   </bookViews>
@@ -31,6 +31,11 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2400,7 +2405,7 @@
   <volType type="realTimeData">
     <main first="crypto">
       <tp>
-        <v>30240</v>
+        <v>47488</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -2408,7 +2413,7 @@
         <tr r="O11" s="1"/>
       </tp>
       <tp>
-        <v>35.743519800000001</v>
+        <v>6.2586106099999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2417,7 +2422,7 @@
         <tr r="I32" s="1"/>
       </tp>
       <tp>
-        <v>0.18112928</v>
+        <v>6.7387999999999997E-4</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2434,7 +2439,7 @@
         <tr r="N19" s="1"/>
       </tp>
       <tp>
-        <v>6691.01</v>
+        <v>8180</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2443,7 +2448,7 @@
         <tr r="C31" s="1"/>
       </tp>
       <tp>
-        <v>6671.01</v>
+        <v>8160.23</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2452,7 +2457,7 @@
         <tr r="C37" s="1"/>
       </tp>
       <tp>
-        <v>474.62</v>
+        <v>457.02</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2461,7 +2466,7 @@
         <tr r="C30" s="1"/>
       </tp>
       <tp>
-        <v>472.62</v>
+        <v>456.39</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2470,7 +2475,7 @@
         <tr r="C36" s="1"/>
       </tp>
       <tp>
-        <v>473.21</v>
+        <v>456.19</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2479,7 +2484,7 @@
         <tr r="B30" s="1"/>
       </tp>
       <tp>
-        <v>472.61</v>
+        <v>456.31</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2488,7 +2493,7 @@
         <tr r="B36" s="1"/>
       </tp>
       <tp>
-        <v>6683.77</v>
+        <v>8171.4</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2497,7 +2502,7 @@
         <tr r="B31" s="1"/>
       </tp>
       <tp>
-        <v>6670.01</v>
+        <v>8153.35</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2506,7 +2511,7 @@
         <tr r="B37" s="1"/>
       </tp>
       <tp>
-        <v>4014</v>
+        <v>1959</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2515,7 +2520,7 @@
         <tr r="N31" s="1"/>
       </tp>
       <tp>
-        <v>64</v>
+        <v>35</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2524,7 +2529,7 @@
         <tr r="N37" s="1"/>
       </tp>
       <tp>
-        <v>2114</v>
+        <v>1121</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2533,7 +2538,7 @@
         <tr r="N30" s="1"/>
       </tp>
       <tp>
-        <v>26</v>
+        <v>21</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2542,7 +2547,7 @@
         <tr r="N36" s="1"/>
       </tp>
       <tp>
-        <v>-1.6900000000000001E-3</v>
+        <v>-6.3420000000000004E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -2550,7 +2555,7 @@
         <tr r="P11" s="1"/>
       </tp>
       <tp>
-        <v>30879</v>
+        <v>34493</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -2558,7 +2563,7 @@
         <tr r="O10" s="1"/>
       </tp>
       <tp>
-        <v>471.77</v>
+        <v>456.79</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -2566,7 +2571,7 @@
         <tr r="C3" s="2"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -2574,7 +2579,7 @@
         <tr r="P18" s="1"/>
       </tp>
       <tp>
-        <v>471.76</v>
+        <v>456.78</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -2582,7 +2587,7 @@
         <tr r="B3" s="2"/>
       </tp>
       <tp>
-        <v>6663.66</v>
+        <v>8153.52</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -2590,7 +2595,7 @@
         <tr r="B4" s="2"/>
       </tp>
       <tp>
-        <v>43285.51666666667</v>
+        <v>43311.845833333333</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2599,7 +2604,7 @@
         <tr r="F38" s="1"/>
       </tp>
       <tp>
-        <v>43285.5</v>
+        <v>43311.833333333336</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2608,7 +2613,7 @@
         <tr r="F32" s="1"/>
       </tp>
       <tp>
-        <v>-2.121E-2</v>
+        <v>-1.6719999999999999E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -2616,7 +2621,7 @@
         <tr r="P10" s="1"/>
       </tp>
       <tp>
-        <v>6663.67</v>
+        <v>8153.53</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -2648,7 +2653,7 @@
         <tr r="T16" s="1"/>
       </tp>
       <tp>
-        <v>4.7629999999999999E-2</v>
+        <v>-3.295E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -2664,7 +2669,7 @@
         <tr r="T18" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -2672,7 +2677,7 @@
         <tr r="P16" s="1"/>
       </tp>
       <tp>
-        <v>6411.51</v>
+        <v>7850</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -2680,7 +2685,7 @@
         <tr r="G4" s="2"/>
       </tp>
       <tp>
-        <v>30882892</v>
+        <v>32003158</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2689,7 +2694,7 @@
         <tr r="Q38" s="1"/>
       </tp>
       <tp>
-        <v>30882892</v>
+        <v>32003158</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2698,7 +2703,7 @@
         <tr r="Q32" s="1"/>
       </tp>
       <tp>
-        <v>6.88591</v>
+        <v>6.8019699999999998</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2707,7 +2712,7 @@
         <tr r="K36" s="1"/>
       </tp>
       <tp>
-        <v>1193.0365300000001</v>
+        <v>1061.29333</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2716,7 +2721,7 @@
         <tr r="K30" s="1"/>
       </tp>
       <tp>
-        <v>2.0317949999999998</v>
+        <v>1.619294</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2725,7 +2730,7 @@
         <tr r="K37" s="1"/>
       </tp>
       <tp>
-        <v>366.14173099999999</v>
+        <v>194.972328</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2734,7 +2739,7 @@
         <tr r="K31" s="1"/>
       </tp>
       <tp>
-        <v>54910928</v>
+        <v>60065180</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2743,7 +2748,7 @@
         <tr r="Q37" s="1"/>
       </tp>
       <tp>
-        <v>54910928</v>
+        <v>60065180</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -2784,7 +2789,7 @@
         <tr r="N21" s="1"/>
       </tp>
       <tp>
-        <v>51127</v>
+        <v>34468</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -2792,7 +2797,7 @@
         <tr r="O9" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -2800,7 +2805,7 @@
         <tr r="P15" s="1"/>
       </tp>
       <tp>
-        <v>451.35</v>
+        <v>446</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -2808,7 +2813,7 @@
         <tr r="G3" s="2"/>
       </tp>
       <tp>
-        <v>30393432</v>
+        <v>33094463</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2817,7 +2822,7 @@
         <tr r="Q30" s="1"/>
       </tp>
       <tp>
-        <v>30393432</v>
+        <v>33094463</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -2826,7 +2831,7 @@
         <tr r="Q36" s="1"/>
       </tp>
       <tp>
-        <v>5.4349999999999997E-3</v>
+        <v>3.8899999999999998E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -2834,7 +2839,7 @@
         <tr r="B9" s="1"/>
       </tp>
       <tp>
-        <v>5.7699999999999998E-6</v>
+        <v>4.3599999999999998E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -2842,7 +2847,7 @@
         <tr r="B11" s="1"/>
       </tp>
       <tp>
-        <v>7.3490000000000003E-5</v>
+        <v>5.4190000000000001E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -2850,7 +2855,7 @@
         <tr r="B10" s="1"/>
       </tp>
       <tp t="s">
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -2858,7 +2863,7 @@
         <tr r="U19" s="1"/>
       </tp>
       <tp t="s">
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -2866,7 +2871,7 @@
         <tr r="U21" s="1"/>
       </tp>
       <tp t="s">
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -2882,7 +2887,7 @@
         <tr r="N20" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -2898,7 +2903,7 @@
         <tr r="S18" s="1"/>
       </tp>
       <tp>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4299999999999999E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2907,7 +2912,7 @@
         <tr r="B38" s="1"/>
       </tp>
       <tp>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2931,8 +2936,8 @@
         <stp>Spread</stp>
         <tr r="J11" s="1"/>
       </tp>
-      <tp>
-        <v>377</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -2940,7 +2945,7 @@
         <tr r="J20" s="1"/>
       </tp>
       <tp>
-        <v>5</v>
+        <v>3</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2949,7 +2954,7 @@
         <tr r="N38" s="1"/>
       </tp>
       <tp>
-        <v>500</v>
+        <v>240</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2958,7 +2963,7 @@
         <tr r="N32" s="1"/>
       </tp>
       <tp>
-        <v>14554128</v>
+        <v>15655775</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -2966,7 +2971,7 @@
         <tr r="H19" s="1"/>
       </tp>
       <tp>
-        <v>3086</v>
+        <v>639</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -2974,7 +2979,7 @@
         <tr r="H10" s="1"/>
       </tp>
       <tp>
-        <v>14130749.716714</v>
+        <v>14185322.523376999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -2982,7 +2987,7 @@
         <tr r="N8" s="1"/>
       </tp>
       <tp>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2991,7 +2996,7 @@
         <tr r="C38" s="1"/>
       </tp>
       <tp>
-        <v>5.9100000000000002E-6</v>
+        <v>4.4599999999999996E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -2999,8 +3004,8 @@
         <stp>5</stp>
         <tr r="C32" s="1"/>
       </tp>
-      <tp t="b">
-        <v>0</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3008,7 +3013,7 @@
         <tr r="K20" s="1"/>
       </tp>
       <tp>
-        <v>1035439</v>
+        <v>104282</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3016,7 +3021,7 @@
         <tr r="H11" s="1"/>
       </tp>
       <tp>
-        <v>6.58</v>
+        <v>4.1500000000000004</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3024,7 +3029,7 @@
         <tr r="L9" s="1"/>
       </tp>
       <tp>
-        <v>7.0000000000000005E-8</v>
+        <v>5.9999999999999995E-8</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3032,7 +3037,7 @@
         <tr r="J10" s="1"/>
       </tp>
       <tp>
-        <v>2.6858599999999999</v>
+        <v>2.2699999999999999E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -3040,7 +3045,7 @@
         <tr r="L5" s="1"/>
       </tp>
       <tp>
-        <v>0.56000000000000005</v>
+        <v>2.0000000000000001E-4</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -3048,15 +3053,15 @@
         <tr r="L7" s="1"/>
       </tp>
       <tp>
-        <v>0.26262600000000003</v>
+        <v>0.209645</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
         <stp>ASK_SIZE</stp>
         <tr r="L6" s="1"/>
       </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+      <tp>
+        <v>4787.5</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3064,7 +3069,7 @@
         <tr r="J18" s="1"/>
       </tp>
       <tp>
-        <v>2358.1084988900002</v>
+        <v>2832.6466749199999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3072,7 +3077,7 @@
         <tr r="N11" s="1"/>
       </tp>
       <tp>
-        <v>2711.1513072399998</v>
+        <v>2097.0739247000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3080,7 +3085,7 @@
         <tr r="N10" s="1"/>
       </tp>
       <tp>
-        <v>0.91744999999999999</v>
+        <v>0.48276000000000002</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3088,7 +3093,7 @@
         <tr r="J15" s="1"/>
       </tp>
       <tp>
-        <v>0.109002</v>
+        <v>4.1603000000000001E-2</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3096,7 +3101,7 @@
         <tr r="J16" s="1"/>
       </tp>
       <tp>
-        <v>2.5009299999999999</v>
+        <v>1.0522</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3104,7 +3109,7 @@
         <tr r="J17" s="1"/>
       </tp>
       <tp>
-        <v>0.57014500000000001</v>
+        <v>0.5</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3113,7 +3118,7 @@
         <tr r="E23" s="1"/>
       </tp>
       <tp>
-        <v>0.01</v>
+        <v>0.1012</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3122,7 +3127,7 @@
         <tr r="E24" s="1"/>
       </tp>
       <tp>
-        <v>0.49435000000000001</v>
+        <v>0.310498</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3131,7 +3136,7 @@
         <tr r="E19" s="1"/>
       </tp>
       <tp>
-        <v>9.4730999999999996E-2</v>
+        <v>0.19</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3140,7 +3145,7 @@
         <tr r="E20" s="1"/>
       </tp>
       <tp>
-        <v>7.5079999999999999E-3</v>
+        <v>0.35439999999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3149,7 +3154,7 @@
         <tr r="E21" s="1"/>
       </tp>
       <tp>
-        <v>0.66981900000000005</v>
+        <v>0.21632699999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3158,7 +3163,7 @@
         <tr r="E22" s="1"/>
       </tp>
       <tp>
-        <v>2.0254000000000001E-2</v>
+        <v>0.63443899999999998</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3167,7 +3172,7 @@
         <tr r="E15" s="1"/>
       </tp>
       <tp>
-        <v>0.35168100000000002</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3176,7 +3181,7 @@
         <tr r="E16" s="1"/>
       </tp>
       <tp>
-        <v>4.7935999999999999E-2</v>
+        <v>0.34868500000000002</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3185,7 +3190,7 @@
         <tr r="E17" s="1"/>
       </tp>
       <tp>
-        <v>5.6000000000000001E-2</v>
+        <v>1.6038E-2</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3194,7 +3199,7 @@
         <tr r="E18" s="1"/>
       </tp>
       <tp>
-        <v>500</v>
+        <v>10</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3202,15 +3207,15 @@
         <tr r="J21" s="1"/>
       </tp>
       <tp>
-        <v>3292</v>
+        <v>44.7</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
         <stp>ASK_SIZE</stp>
         <tr r="L8" s="1"/>
       </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+      <tp>
+        <v>43311.84629065972</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3218,7 +3223,7 @@
         <tr r="L18" s="1"/>
       </tp>
       <tp>
-        <v>43285.516921724535</v>
+        <v>43311.846334247683</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3226,7 +3231,7 @@
         <tr r="L17" s="1"/>
       </tp>
       <tp>
-        <v>43285.517101666665</v>
+        <v>43311.846317650467</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3234,7 +3239,7 @@
         <tr r="L15" s="1"/>
       </tp>
       <tp>
-        <v>43285.517102048609</v>
+        <v>43311.846355023146</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3242,7 +3247,7 @@
         <tr r="L16" s="1"/>
       </tp>
       <tp t="s">
-        <v>Server error: {"code":-2015,"msg":"Invalid API-key, IP, or permissions for action."}</v>
+        <v>Invalid API-key, IP, or permissions for action.</v>
         <stp/>
         <stp>BINANCE_HISTORY</stp>
         <stp>ETHUSDT</stp>
@@ -3250,8 +3255,8 @@
         <stp>10</stp>
         <tr r="G24" s="1"/>
       </tp>
-      <tp>
-        <v>18596602</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -3259,7 +3264,7 @@
         <tr r="H20" s="1"/>
       </tp>
       <tp>
-        <v>471.3</v>
+        <v>456.29</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3268,7 +3273,7 @@
         <tr r="E36" s="1"/>
       </tp>
       <tp>
-        <v>471.3</v>
+        <v>456.29</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3293,7 +3298,7 @@
         <tr r="S16" s="1"/>
       </tp>
       <tp>
-        <v>73326</v>
+        <v>1629845</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3301,7 +3306,7 @@
         <tr r="L11" s="1"/>
       </tp>
       <tp>
-        <v>1.537E-2</v>
+        <v>1.70052</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -3309,7 +3314,7 @@
         <tr r="H7" s="1"/>
       </tp>
       <tp>
-        <v>6.7424999999999999E-2</v>
+        <v>7.6309999999999998E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -3317,7 +3322,7 @@
         <tr r="H6" s="1"/>
       </tp>
       <tp>
-        <v>2.4573100000000001</v>
+        <v>2.7384599999999999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -3325,7 +3330,7 @@
         <tr r="H5" s="1"/>
       </tp>
       <tp>
-        <v>0.03</v>
+        <v>18.25</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3333,7 +3338,7 @@
         <tr r="H9" s="1"/>
       </tp>
       <tp>
-        <v>191494800.14948204</v>
+        <v>307914890.48390466</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -3341,7 +3346,7 @@
         <tr r="N6" s="1"/>
       </tp>
       <tp>
-        <v>11444940.7380598</v>
+        <v>11879122.185702</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -3349,7 +3354,7 @@
         <tr r="N7" s="1"/>
       </tp>
       <tp>
-        <v>6902.4</v>
+        <v>56.1</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -3357,7 +3362,7 @@
         <tr r="H8" s="1"/>
       </tp>
       <tp>
-        <v>15.4</v>
+        <v>0.54</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -3365,7 +3370,7 @@
         <tr r="J19" s="1"/>
       </tp>
       <tp>
-        <v>6664.13</v>
+        <v>8152.02</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3374,7 +3379,7 @@
         <tr r="E37" s="1"/>
       </tp>
       <tp>
-        <v>6664.13</v>
+        <v>8152.02</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3391,7 +3396,7 @@
         <tr r="K19" s="1"/>
       </tp>
       <tp>
-        <v>43285.517097245371</v>
+        <v>43311.846329664353</v>
         <stp/>
         <stp>CLOCK</stp>
         <tr r="T4" s="1"/>
@@ -3405,7 +3410,7 @@
         <tr r="J9" s="1"/>
       </tp>
       <tp>
-        <v>2043046</v>
+        <v>445703</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3414,7 +3419,7 @@
         <tr r="K32" s="1"/>
       </tp>
       <tp>
-        <v>30752</v>
+        <v>52</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3423,7 +3428,7 @@
         <tr r="K38" s="1"/>
       </tp>
       <tp>
-        <v>3.8E-3</v>
+        <v>0.5</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3432,7 +3437,7 @@
         <tr r="A23" s="1"/>
       </tp>
       <tp>
-        <v>0.97992699999999999</v>
+        <v>0.77</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3441,7 +3446,7 @@
         <tr r="A24" s="1"/>
       </tp>
       <tp>
-        <v>9.0060000000000001E-2</v>
+        <v>6.1339999999999997E-3</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3450,7 +3455,7 @@
         <tr r="A19" s="1"/>
       </tp>
       <tp>
-        <v>4.0910000000000002</v>
+        <v>6.7230259999999999</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3459,7 +3464,7 @@
         <tr r="A20" s="1"/>
       </tp>
       <tp>
-        <v>0.109</v>
+        <v>0.99</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3468,7 +3473,7 @@
         <tr r="A21" s="1"/>
       </tp>
       <tp>
-        <v>4.413157</v>
+        <v>0.231682</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3477,7 +3482,7 @@
         <tr r="A22" s="1"/>
       </tp>
       <tp>
-        <v>1.992E-2</v>
+        <v>0.79360200000000003</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3486,7 +3491,7 @@
         <tr r="A15" s="1"/>
       </tp>
       <tp>
-        <v>0.98658500000000005</v>
+        <v>7.6309999999999998E-3</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3495,7 +3500,7 @@
         <tr r="A16" s="1"/>
       </tp>
       <tp>
-        <v>2.9922629999999999</v>
+        <v>0.5</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3504,7 +3509,7 @@
         <tr r="A17" s="1"/>
       </tp>
       <tp>
-        <v>5.6000000000000001E-2</v>
+        <v>3.4143300000000001</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -3513,7 +3518,7 @@
         <tr r="A18" s="1"/>
       </tp>
       <tp>
-        <v>7532.5732854899998</v>
+        <v>10179.092113299999</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -3521,7 +3526,7 @@
         <tr r="H4" s="2"/>
       </tp>
       <tp>
-        <v>64263.177474869997</v>
+        <v>49281.142481360002</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -3554,8 +3559,8 @@
         <stp>5</stp>
         <tr r="H31" s="1"/>
       </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+      <tp>
+        <v>1939683</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3563,14 +3568,14 @@
         <tr r="H18" s="1"/>
       </tp>
       <tp>
-        <v>-443</v>
+        <v>-230</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>DRIFT</stp>
         <tr r="T5" s="1"/>
       </tp>
       <tp>
-        <v>48377931</v>
+        <v>53127003</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -3578,7 +3583,7 @@
         <tr r="H16" s="1"/>
       </tp>
       <tp>
-        <v>7533270</v>
+        <v>8202329</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -3586,7 +3591,7 @@
         <tr r="H17" s="1"/>
       </tp>
       <tp>
-        <v>27105497</v>
+        <v>29601071</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -3594,7 +3599,7 @@
         <tr r="H15" s="1"/>
       </tp>
       <tp>
-        <v>2938.16672982</v>
+        <v>1298.85586367</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3602,7 +3607,7 @@
         <tr r="N9" s="1"/>
       </tp>
       <tp>
-        <v>19233907</v>
+        <v>19966248</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -3628,7 +3633,7 @@
         <tr r="H30" s="1"/>
       </tp>
       <tp>
-        <v>56432388.176379703</v>
+        <v>80652609.0343173</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -3636,7 +3641,7 @@
         <tr r="N5" s="1"/>
       </tp>
       <tp>
-        <v>2199</v>
+        <v>2890</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3644,7 +3649,7 @@
         <tr r="L10" s="1"/>
       </tp>
       <tp>
-        <v>43285.516620439812</v>
+        <v>43311.84597584491</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>EXCHANGE_TIME</stp>
@@ -3659,7 +3664,7 @@
         <tr r="Q18" s="1"/>
       </tp>
       <tp t="s">
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3675,7 +3680,7 @@
         <tr r="Q19" s="1"/>
       </tp>
       <tp>
-        <v>457</v>
+        <v>446.1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -3691,7 +3696,7 @@
         <tr r="R17" s="1"/>
       </tp>
       <tp>
-        <v>26.591799999999999</v>
+        <v>12.380129999999999</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3700,7 +3705,7 @@
         <tr r="J36" s="1"/>
       </tp>
       <tp>
-        <v>2463.4826800000001</v>
+        <v>1966.45597</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3717,7 +3722,7 @@
         <tr r="O21" s="1"/>
       </tp>
       <tp>
-        <v>5.8799999999999996E-6</v>
+        <v>4.4299999999999999E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3725,7 +3730,7 @@
         <tr r="I11" s="1"/>
       </tp>
       <tp>
-        <v>7.4190000000000006E-5</v>
+        <v>5.4629999999999997E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3733,7 +3738,7 @@
         <tr r="I10" s="1"/>
       </tp>
       <tp>
-        <v>5.8050000000000003E-3</v>
+        <v>3.9329999999999999E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3765,7 +3770,7 @@
         <tr r="Q17" s="1"/>
       </tp>
       <tp>
-        <v>6441.11</v>
+        <v>7866</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3773,7 +3778,7 @@
         <tr r="B6" s="1"/>
       </tp>
       <tp>
-        <v>5.8069999999999997E-3</v>
+        <v>3.934E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -3781,7 +3786,7 @@
         <tr r="K9" s="1"/>
       </tp>
       <tp>
-        <v>7.428E-5</v>
+        <v>5.469E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -3789,7 +3794,7 @@
         <tr r="K10" s="1"/>
       </tp>
       <tp>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -3797,7 +3802,7 @@
         <tr r="K11" s="1"/>
       </tp>
       <tp t="s">
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3812,8 +3817,8 @@
         <stp>QUOTE_ASSET_PRECISION</stp>
         <tr r="S19" s="1"/>
       </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+      <tp>
+        <v>0.44630999999999998</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -3821,7 +3826,7 @@
         <tr r="I18" s="1"/>
       </tp>
       <tp>
-        <v>0.50654999999999994</v>
+        <v>0.45621</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -3829,7 +3834,7 @@
         <tr r="C8" s="1"/>
       </tp>
       <tp>
-        <v>43285.517102071761</v>
+        <v>43311.846345601851</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3838,7 +3843,7 @@
         <tr r="O37" s="1"/>
       </tp>
       <tp>
-        <v>43285.517102083337</v>
+        <v>43311.84634556713</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3847,7 +3852,7 @@
         <tr r="O31" s="1"/>
       </tp>
       <tp>
-        <v>43285.517101504629</v>
+        <v>43311.846317685187</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3856,7 +3861,7 @@
         <tr r="O36" s="1"/>
       </tp>
       <tp>
-        <v>43285.517101504629</v>
+        <v>43311.846317685187</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -3865,7 +3870,7 @@
         <tr r="O30" s="1"/>
       </tp>
       <tp>
-        <v>83.64</v>
+        <v>79.760000000000005</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3873,7 +3878,7 @@
         <tr r="B7" s="1"/>
       </tp>
       <tp>
-        <v>717.961096</v>
+        <v>388.666763</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3882,7 +3887,7 @@
         <tr r="J31" s="1"/>
       </tp>
       <tp>
-        <v>10.200435000000001</v>
+        <v>3.721597</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -3891,7 +3896,7 @@
         <tr r="J37" s="1"/>
       </tp>
       <tp>
-        <v>6.1910000000000003E-3</v>
+        <v>4.1399999999999996E-3</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3899,7 +3904,7 @@
         <tr r="C9" s="1"/>
       </tp>
       <tp t="s">
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3907,7 +3912,7 @@
         <tr r="U17" s="1"/>
       </tp>
       <tp>
-        <v>6062958</v>
+        <v>1409501</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3916,7 +3921,7 @@
         <tr r="J32" s="1"/>
       </tp>
       <tp>
-        <v>30752</v>
+        <v>152</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -3941,7 +3946,7 @@
         <tr r="R16" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -3949,7 +3954,7 @@
         <tr r="P21" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -3957,7 +3962,7 @@
         <tr r="P20" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>neobtc</stp>
@@ -3965,7 +3970,7 @@
         <tr r="P19" s="1"/>
       </tp>
       <tp>
-        <v>6784.92</v>
+        <v>8273</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>btcusdt</stp>
@@ -3973,7 +3978,7 @@
         <tr r="C6" s="1"/>
       </tp>
       <tp>
-        <v>89.01</v>
+        <v>84.62</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ltcusdt</stp>
@@ -3981,7 +3986,7 @@
         <tr r="C7" s="1"/>
       </tp>
       <tp>
-        <v>482.7</v>
+        <v>469.79</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>ethusdt</stp>
@@ -4065,7 +4070,7 @@
         <tr r="T20" s="1"/>
       </tp>
       <tp>
-        <v>54910865</v>
+        <v>60065146</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4074,7 +4079,7 @@
         <tr r="P37" s="1"/>
       </tp>
       <tp>
-        <v>54906915</v>
+        <v>60063222</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4083,7 +4088,7 @@
         <tr r="P31" s="1"/>
       </tp>
       <tp>
-        <v>30393407</v>
+        <v>33094443</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4092,7 +4097,7 @@
         <tr r="P36" s="1"/>
       </tp>
       <tp>
-        <v>30391319</v>
+        <v>33093343</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4101,7 +4106,7 @@
         <tr r="P30" s="1"/>
       </tp>
       <tp>
-        <v>399604654</v>
+        <v>620653152</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -4109,7 +4114,7 @@
         <tr r="M11" s="1"/>
       </tp>
       <tp>
-        <v>36351363</v>
+        <v>37988898</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -4117,7 +4122,7 @@
         <tr r="M10" s="1"/>
       </tp>
       <tp>
-        <v>506889</v>
+        <v>324679.78999999998</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4125,7 +4130,7 @@
         <tr r="M9" s="1"/>
       </tp>
       <tp>
-        <v>43285.541666655095</v>
+        <v>43311.874999988424</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4134,7 +4139,7 @@
         <tr r="G30" s="1"/>
       </tp>
       <tp>
-        <v>43285.517361099533</v>
+        <v>43311.846527766204</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4143,7 +4148,7 @@
         <tr r="G36" s="1"/>
       </tp>
       <tp>
-        <v>43285.541666655095</v>
+        <v>43311.874999988424</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4152,7 +4157,7 @@
         <tr r="G31" s="1"/>
       </tp>
       <tp>
-        <v>43285.517361099533</v>
+        <v>43311.846527766204</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4161,7 +4166,7 @@
         <tr r="G37" s="1"/>
       </tp>
       <tp>
-        <v>5.9900000000000002E-6</v>
+        <v>4.8300000000000003E-6</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>trxbtc</stp>
@@ -4169,7 +4174,7 @@
         <tr r="C11" s="1"/>
       </tp>
       <tp>
-        <v>5.8799999999999996E-6</v>
+        <v>4.4299999999999999E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4178,7 +4183,7 @@
         <tr r="D32" s="1"/>
       </tp>
       <tp>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4299999999999999E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4205,7 +4210,7 @@
         <tr r="H32" s="1"/>
       </tp>
       <tp>
-        <v>20628</v>
+        <v>23655</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4213,7 +4218,7 @@
         <tr r="O7" s="1"/>
       </tp>
       <tp>
-        <v>168939</v>
+        <v>199972</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4221,7 +4226,7 @@
         <tr r="O6" s="1"/>
       </tp>
       <tp>
-        <v>92427</v>
+        <v>100596</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4229,7 +4234,7 @@
         <tr r="O5" s="1"/>
       </tp>
       <tp>
-        <v>17606</v>
+        <v>17556</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4237,7 +4242,7 @@
         <tr r="O8" s="1"/>
       </tp>
       <tp>
-        <v>6650.93</v>
+        <v>8130.32</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4246,7 +4251,7 @@
         <tr r="D31" s="1"/>
       </tp>
       <tp>
-        <v>6662.15</v>
+        <v>8150.55</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4255,7 +4260,7 @@
         <tr r="D37" s="1"/>
       </tp>
       <tp>
-        <v>5.3299999999999997E-3</v>
+        <v>-3.8700000000000002E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4263,7 +4268,7 @@
         <tr r="P7" s="1"/>
       </tp>
       <tp>
-        <v>6.2899999999999996E-3</v>
+        <v>-1.244E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4271,7 +4276,7 @@
         <tr r="P5" s="1"/>
       </tp>
       <tp>
-        <v>1.191E-2</v>
+        <v>5.7000000000000002E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4279,7 +4284,7 @@
         <tr r="P6" s="1"/>
       </tp>
       <tp>
-        <v>-9.2899999999999996E-3</v>
+        <v>-1.099E-2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4287,7 +4292,7 @@
         <tr r="P8" s="1"/>
       </tp>
       <tp>
-        <v>6664.13</v>
+        <v>8152.02</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>btcusdt</stp>
@@ -4295,7 +4300,7 @@
         <tr r="I16" s="1"/>
       </tp>
       <tp>
-        <v>86.86</v>
+        <v>82.47</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4319,7 +4324,7 @@
         <tr r="R18" s="1"/>
       </tp>
       <tp>
-        <v>471.3</v>
+        <v>456.29</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4328,7 +4333,7 @@
         <tr r="D36" s="1"/>
       </tp>
       <tp>
-        <v>471.03</v>
+        <v>454.1</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4369,7 +4374,7 @@
         <tr r="Q21" s="1"/>
       </tp>
       <tp>
-        <v>0.47800999999999999</v>
+        <v>0.43381999999999998</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4377,7 +4382,7 @@
         <tr r="B8" s="1"/>
       </tp>
       <tp t="s">
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpusdt</stp>
@@ -4385,7 +4390,7 @@
         <tr r="U18" s="1"/>
       </tp>
       <tp>
-        <v>7.6240000000000002E-5</v>
+        <v>5.5899999999999997E-5</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp>xrpbtc</stp>
@@ -4425,7 +4430,7 @@
         <tr r="N17" s="1"/>
       </tp>
       <tp>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4434,7 +4439,7 @@
         <tr r="E38" s="1"/>
       </tp>
       <tp>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4443,7 +4448,7 @@
         <tr r="E32" s="1"/>
       </tp>
       <tp>
-        <v>13547.573522049999</v>
+        <v>13210.08758555</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4452,7 +4457,7 @@
         <tr r="L37" s="1"/>
       </tp>
       <tp>
-        <v>2447502.1504584299</v>
+        <v>1590078.60588646</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4461,7 +4466,7 @@
         <tr r="L31" s="1"/>
       </tp>
       <tp>
-        <v>3252.4823544999999</v>
+        <v>3104.2154962</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4470,7 +4475,7 @@
         <tr r="L36" s="1"/>
       </tp>
       <tp>
-        <v>564552.89316370001</v>
+        <v>484055.28109459998</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4503,7 +4508,7 @@
         <tr r="O15" s="1"/>
       </tp>
       <tp>
-        <v>471.3</v>
+        <v>456.29</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ethusdt</stp>
@@ -4511,7 +4516,7 @@
         <tr r="I15" s="1"/>
       </tp>
       <tp>
-        <v>132521.51637999999</v>
+        <v>143669.38344999999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4519,7 +4524,7 @@
         <tr r="M7" s="1"/>
       </tp>
       <tp>
-        <v>0.49421999999999999</v>
+        <v>0.44571</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4527,7 +4532,7 @@
         <tr r="I8" s="1"/>
       </tp>
       <tp>
-        <v>43285.51666666667</v>
+        <v>43311.845833333333</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4536,7 +4541,7 @@
         <tr r="F36" s="1"/>
       </tp>
       <tp>
-        <v>43285.5</v>
+        <v>43311.833333333336</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4545,7 +4550,7 @@
         <tr r="F30" s="1"/>
       </tp>
       <tp>
-        <v>86.41</v>
+        <v>82.77</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4553,7 +4558,7 @@
         <tr r="D7" s="1"/>
       </tp>
       <tp>
-        <v>6591.31</v>
+        <v>8113.99</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4561,7 +4566,7 @@
         <tr r="D6" s="1"/>
       </tp>
       <tp>
-        <v>43285.517102199075</v>
+        <v>43311.846354965281</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4569,7 +4574,7 @@
         <tr r="L19" s="1"/>
       </tp>
       <tp>
-        <v>5.5440000000000003E-3</v>
+        <v>4.0679999999999996E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4577,7 +4582,7 @@
         <tr r="G9" s="1"/>
       </tp>
       <tp>
-        <v>469.52</v>
+        <v>462.04</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4585,7 +4590,7 @@
         <tr r="G5" s="1"/>
       </tp>
       <tp>
-        <v>0.49541000000000002</v>
+        <v>0.44630999999999998</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4593,7 +4598,7 @@
         <tr r="K8" s="1"/>
       </tp>
       <tp>
-        <v>6589.41</v>
+        <v>8113.99</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4601,7 +4606,7 @@
         <tr r="G6" s="1"/>
       </tp>
       <tp>
-        <v>86.38</v>
+        <v>82.79</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4609,7 +4614,7 @@
         <tr r="G7" s="1"/>
       </tp>
       <tp t="b">
-        <v>0</v>
+        <v>1</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>ltcusdt</stp>
@@ -4632,8 +4637,8 @@
         <stp>BUYER_IS_MAKER</stp>
         <tr r="K15" s="1"/>
       </tp>
-      <tp t="s">
-        <v>&lt;?&gt;</v>
+      <tp t="b">
+        <v>0</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpusdt</stp>
@@ -4641,7 +4646,7 @@
         <tr r="K18" s="1"/>
       </tp>
       <tp>
-        <v>482.01</v>
+        <v>469</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4649,7 +4654,7 @@
         <tr r="F3" s="2"/>
       </tp>
       <tp>
-        <v>6796.62</v>
+        <v>8274.92</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4657,7 +4662,7 @@
         <tr r="F4" s="2"/>
       </tp>
       <tp>
-        <v>0.49940000000000001</v>
+        <v>0.45061000000000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4665,7 +4670,7 @@
         <tr r="G8" s="1"/>
       </tp>
       <tp>
-        <v>43285.51666666667</v>
+        <v>43311.845833333333</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4674,7 +4679,7 @@
         <tr r="F37" s="1"/>
       </tp>
       <tp>
-        <v>43285.5</v>
+        <v>43311.833333333336</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4683,7 +4688,7 @@
         <tr r="F31" s="1"/>
       </tp>
       <tp>
-        <v>-1.66E-6</v>
+        <v>-9.5999999999999991E-7</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -4691,7 +4696,7 @@
         <tr r="Q10" s="1"/>
       </tp>
       <tp>
-        <v>469.12</v>
+        <v>462.04</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4699,7 +4704,7 @@
         <tr r="D5" s="1"/>
       </tp>
       <tp>
-        <v>120420.34009</v>
+        <v>175756.00234000001</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4707,7 +4712,7 @@
         <tr r="M5" s="1"/>
       </tp>
       <tp>
-        <v>5.5380000000000004E-3</v>
+        <v>4.0699999999999998E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4733,7 +4738,7 @@
         <tr r="M32" s="1"/>
       </tp>
       <tp>
-        <v>-1E-8</v>
+        <v>-2.9999999999999999E-7</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -4741,7 +4746,7 @@
         <tr r="Q11" s="1"/>
       </tp>
       <tp>
-        <v>4797712.7030429197</v>
+        <v>3169220.3606163301</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4750,7 +4755,7 @@
         <tr r="I31" s="1"/>
       </tp>
       <tp>
-        <v>67997.397360820003</v>
+        <v>30346.96819467</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>btcusdt</stp>
@@ -4759,7 +4764,7 @@
         <tr r="I37" s="1"/>
       </tp>
       <tp>
-        <v>1165600.1691212</v>
+        <v>896475.9274096</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4768,7 +4773,7 @@
         <tr r="I30" s="1"/>
       </tp>
       <tp>
-        <v>12544.048344999999</v>
+        <v>5649.5433349000004</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>ethusdt</stp>
@@ -4777,7 +4782,7 @@
         <tr r="I36" s="1"/>
       </tp>
       <tp>
-        <v>471.77</v>
+        <v>456.79</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -4785,7 +4790,7 @@
         <tr r="D3" s="2"/>
       </tp>
       <tp>
-        <v>6663.67</v>
+        <v>8153.52</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
@@ -4793,7 +4798,7 @@
         <tr r="D4" s="2"/>
       </tp>
       <tp>
-        <v>5.7980000000000002E-3</v>
+        <v>3.9329999999999999E-3</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>neobtc</stp>
@@ -4801,7 +4806,7 @@
         <tr r="I19" s="1"/>
       </tp>
       <tp>
-        <v>43285.516921388888</v>
+        <v>43311.846323900463</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4810,7 +4815,7 @@
         <tr r="O32" s="1"/>
       </tp>
       <tp>
-        <v>43285.516921388888</v>
+        <v>43311.846323900463</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4819,7 +4824,7 @@
         <tr r="O38" s="1"/>
       </tp>
       <tp>
-        <v>29075.271000000001</v>
+        <v>38006.927171000003</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4834,7 +4839,7 @@
         <tr r="T7" s="1"/>
       </tp>
       <tp>
-        <v>0.46</v>
+        <v>-0.32</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4842,7 +4847,7 @@
         <tr r="Q7" s="1"/>
       </tp>
       <tp>
-        <v>72.8</v>
+        <v>46.2</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4850,7 +4855,7 @@
         <tr r="Q6" s="1"/>
       </tp>
       <tp>
-        <v>2.63E-4</v>
+        <v>-1.35E-4</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>neobtc</stp>
@@ -4858,7 +4863,7 @@
         <tr r="Q9" s="1"/>
       </tp>
       <tp>
-        <v>2.91</v>
+        <v>-5.82</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4866,7 +4871,7 @@
         <tr r="Q5" s="1"/>
       </tp>
       <tp>
-        <v>0.49924000000000002</v>
+        <v>0.45127</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4874,7 +4879,7 @@
         <tr r="D8" s="1"/>
       </tp>
       <tp>
-        <v>0.15</v>
+        <v>0.02</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4882,7 +4887,7 @@
         <tr r="J7" s="1"/>
       </tp>
       <tp>
-        <v>5.72</v>
+        <v>8.1999999999999993</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -4890,7 +4895,7 @@
         <tr r="J6" s="1"/>
       </tp>
       <tp>
-        <v>0.51</v>
+        <v>0.18</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -4898,7 +4903,7 @@
         <tr r="J5" s="1"/>
       </tp>
       <tp>
-        <v>1.1800000000000001E-3</v>
+        <v>5.9000000000000003E-4</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4906,7 +4911,7 @@
         <tr r="J8" s="1"/>
       </tp>
       <tp>
-        <v>43285.517361099533</v>
+        <v>43311.846527766204</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4915,7 +4920,7 @@
         <tr r="G38" s="1"/>
       </tp>
       <tp>
-        <v>43285.541666655095</v>
+        <v>43311.874999988424</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4924,7 +4929,7 @@
         <tr r="G32" s="1"/>
       </tp>
       <tp>
-        <v>30882393</v>
+        <v>32002919</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4933,7 +4938,7 @@
         <tr r="P32" s="1"/>
       </tp>
       <tp>
-        <v>30882888</v>
+        <v>32003156</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -4942,7 +4947,7 @@
         <tr r="P38" s="1"/>
       </tp>
       <tp>
-        <v>86.7</v>
+        <v>82.46</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4950,7 +4955,7 @@
         <tr r="I7" s="1"/>
       </tp>
       <tp>
-        <v>28720303.899999999</v>
+        <v>31623342.399999999</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4958,7 +4963,7 @@
         <tr r="M8" s="1"/>
       </tp>
       <tp>
-        <v>7.5850000000000001E-5</v>
+        <v>5.5590000000000001E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -4966,7 +4971,7 @@
         <tr r="G10" s="1"/>
       </tp>
       <tp>
-        <v>43285.516921377312</v>
+        <v>43311.84632384259</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
@@ -4974,7 +4979,7 @@
         <tr r="L21" s="1"/>
       </tp>
       <tp>
-        <v>-4.64E-3</v>
+        <v>-4.3E-3</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpusdt</stp>
@@ -4982,7 +4987,7 @@
         <tr r="Q8" s="1"/>
       </tp>
       <tp>
-        <v>86.85</v>
+        <v>82.48</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ltcusdt</stp>
@@ -4990,7 +4995,7 @@
         <tr r="K7" s="1"/>
       </tp>
       <tp t="s">
-        <v>["ETHBTC","LTCBTC","BNBBTC","NEOBTC","QTUMETH","EOSETH","SNTETH","BNTETH","BCCBTC","GASBTC","BNBETH","BTCUSDT","ETHUSDT","HSRBTC","OAXETH","DNTETH","MCOETH","ICNETH","MCOBTC","WTCBTC","WTCETH","LRCBTC","LRCETH","QTUMBTC","YOYOBTC","OMGBTC","OMGETH","ZRXBTC","ZRXETH","STRATBTC","STRATETH","SNGLSBTC","SNGLSETH","BQXBTC","BQXETH","KNCBTC","KNCETH","FUNBTC","FUNETH","SNMBTC","SNMETH","NEOETH","IOTABTC","IOTAETH","LINKBTC","LINKETH","XVGBTC","XVGETH","SALTBTC","SALTETH","MDABTC","MDAETH","MTLBTC","MTLETH","SUBBTC","SUBETH","EOSBTC","SNTBTC","ETCETH","ETCBTC","MTHBTC","MTHETH","ENGBTC","ENGETH","DNTBTC","ZECBTC","ZECETH","BNTBTC","ASTBTC","ASTETH","DASHBTC","DASHETH","OAXBTC","ICNBTC","BTGBTC","BTGETH","EVXBTC","EVXETH","REQBTC","REQETH","VIBBTC","VIBETH","HSRETH","TRXBTC","TRXETH","POWRBTC","POWRETH","ARKBTC","ARKETH","YOYOETH","XRPBTC","XRPETH","MODBTC","MODETH","ENJBTC","ENJETH","STORJBTC","STORJETH","BNBUSDT","VENBNB","YOYOBNB","POWRBNB","VENBTC","VENETH","KMDBTC","KMDETH","NULSBNB","RCNBTC","RCNETH","RCNBNB","NULSBTC","NULSETH","RDNBTC","RDNETH","RDNBNB","XMRBTC","XMRETH","DLTBNB","WTCBNB","DLTBTC","DLTETH","AMBBTC","AMBETH","AMBBNB","BCCETH","BCCUSDT","BCCBNB","BATBTC","BATETH","BATBNB","BCPTBTC","BCPTETH","BCPTBNB","ARNBTC","ARNETH","GVTBTC","GVTETH","CDTBTC","CDTETH","GXSBTC","GXSETH","NEOUSDT","NEOBNB","POEBTC","POEETH","QSPBTC","QSPETH","QSPBNB","BTSBTC","BTSETH","BTSBNB","XZCBTC","XZCETH","XZCBNB","LSKBTC","LSKETH","LSKBNB","TNTBTC","TNTETH","FUELBTC","FUELETH","MANABTC","MANAETH","BCDBTC","BCDETH","DGDBTC","DGDETH","IOTABNB","ADXBTC","ADXETH","ADXBNB","ADABTC","ADAETH","PPTBTC","PPTETH","CMTBTC","CMTETH","CMTBNB","XLMBTC","XLMETH","XLMBNB","CNDBTC","CNDETH","CNDBNB","LENDBTC","LENDETH","WABIBTC","WABIETH","WABIBNB","LTCETH","LTCUSDT","LTCBNB","TNBBTC","TNBETH","WAVESBTC","WAVESETH","WAVESBNB","GTOBTC","GTOETH","GTOBNB","ICXBTC","ICXETH","ICXBNB","OSTBTC","OSTETH","OSTBNB","ELFBTC","ELFETH","AIONBTC","AIONETH","AIONBNB","NEBLBTC","NEBLETH","NEBLBNB","BRDBTC","BRDETH","BRDBNB","MCOBNB","EDOBTC","EDOETH","WINGSBTC","WINGSETH","NAVBTC","NAVETH","NAVBNB","LUNBTC","LUNETH","TRIGBTC","TRIGETH","TRIGBNB","APPCBTC","APPCETH","APPCBNB","VIBEBTC","VIBEETH","RLCBTC","RLCETH","RLCBNB","INSBTC","INSETH","PIVXBTC","PIVXETH","PIVXBNB","IOSTBTC","IOSTETH","CHATBTC","CHATETH","STEEMBTC","STEEMETH","STEEMBNB","NANOBTC","NANOETH","NANOBNB","VIABTC","VIAETH","VIABNB","BLZBTC","BLZETH","BLZBNB","AEBTC","AEETH","AEBNB","RPXBTC","RPXETH","RPXBNB","NCASHBTC","NCASHETH","NCASHBNB","POABTC","POAETH","POABNB","ZILBTC","ZILETH","ZILBNB","ONTBTC","ONTETH","ONTBNB","STORMBTC","STORMETH","STORMBNB","QTUMBNB","QTUMUSDT","XEMBTC","XEMETH","XEMBNB","WANBTC","WANETH","WANBNB","WPRBTC","WPRETH","QLCBTC","QLCETH","SYSBTC","SYSETH","SYSBNB","QLCBNB","GRSBTC","GRSETH","ADAUSDT","ADABNB","CLOAKBTC","CLOAKETH","GNTBTC","GNTETH","GNTBNB","LOOMBTC","LOOMETH","LOOMBNB","XRPUSDT","BCNBTC","BCNETH","BCNBNB","REPBTC","REPETH","REPBNB","TUSDBTC","TUSDETH","TUSDBNB","ZENBTC","ZENETH","ZENBNB","SKYBTC","SKYETH","SKYBNB","EOSUSDT","EOSBNB","CVCBTC","CVCETH","CVCBNB","THETABTC","THETAETH","THETABNB","XRPBNB","TUSDUSDT","IOTAUSDT","XLMUSDT","IOTXBTC","IOTXETH","QKCBTC","QKCETH","AGIBTC","AGIETH","AGIBNB","NXSBTC","NXSETH","NXSBNB","ENJBNB","DATABTC","DATAETH","ONTUSDT","TRXUSDT","ETCUSDT","ETCBNB","ICXUSDT","SCBTC","SCETH","SCBNB","NPXSBTC","NPXSETH","VENUSDT","KEYBTC","KEYETH","NASBTC","NASETH","NASBNB"]</v>
+        <v>["ETHBTC","LTCBTC","BNBBTC","NEOBTC","QTUMETH","EOSETH","SNTETH","BNTETH","BCCBTC","GASBTC","BNBETH","BTCUSDT","ETHUSDT","HSRBTC","OAXETH","DNTETH","MCOETH","ICNETH","MCOBTC","WTCBTC","WTCETH","LRCBTC","LRCETH","QTUMBTC","YOYOBTC","OMGBTC","OMGETH","ZRXBTC","ZRXETH","STRATBTC","STRATETH","SNGLSBTC","SNGLSETH","BQXBTC","BQXETH","KNCBTC","KNCETH","FUNBTC","FUNETH","SNMBTC","SNMETH","NEOETH","IOTABTC","IOTAETH","LINKBTC","LINKETH","XVGBTC","XVGETH","SALTBTC","SALTETH","MDABTC","MDAETH","MTLBTC","MTLETH","SUBBTC","SUBETH","EOSBTC","SNTBTC","ETCETH","ETCBTC","MTHBTC","MTHETH","ENGBTC","ENGETH","DNTBTC","ZECBTC","ZECETH","BNTBTC","ASTBTC","ASTETH","DASHBTC","DASHETH","OAXBTC","ICNBTC","BTGBTC","BTGETH","EVXBTC","EVXETH","REQBTC","REQETH","VIBBTC","VIBETH","HSRETH","TRXBTC","TRXETH","POWRBTC","POWRETH","ARKBTC","ARKETH","YOYOETH","XRPBTC","XRPETH","MODBTC","MODETH","ENJBTC","ENJETH","STORJBTC","STORJETH","BNBUSDT","VENBNB","YOYOBNB","POWRBNB","VENBTC","VENETH","KMDBTC","KMDETH","NULSBNB","RCNBTC","RCNETH","RCNBNB","NULSBTC","NULSETH","RDNBTC","RDNETH","RDNBNB","XMRBTC","XMRETH","DLTBNB","WTCBNB","DLTBTC","DLTETH","AMBBTC","AMBETH","AMBBNB","BCCETH","BCCUSDT","BCCBNB","BATBTC","BATETH","BATBNB","BCPTBTC","BCPTETH","BCPTBNB","ARNBTC","ARNETH","GVTBTC","GVTETH","CDTBTC","CDTETH","GXSBTC","GXSETH","NEOUSDT","NEOBNB","POEBTC","POEETH","QSPBTC","QSPETH","QSPBNB","BTSBTC","BTSETH","BTSBNB","XZCBTC","XZCETH","XZCBNB","LSKBTC","LSKETH","LSKBNB","TNTBTC","TNTETH","FUELBTC","FUELETH","MANABTC","MANAETH","BCDBTC","BCDETH","DGDBTC","DGDETH","IOTABNB","ADXBTC","ADXETH","ADXBNB","ADABTC","ADAETH","PPTBTC","PPTETH","CMTBTC","CMTETH","CMTBNB","XLMBTC","XLMETH","XLMBNB","CNDBTC","CNDETH","CNDBNB","LENDBTC","LENDETH","WABIBTC","WABIETH","WABIBNB","LTCETH","LTCUSDT","LTCBNB","TNBBTC","TNBETH","WAVESBTC","WAVESETH","WAVESBNB","GTOBTC","GTOETH","GTOBNB","ICXBTC","ICXETH","ICXBNB","OSTBTC","OSTETH","OSTBNB","ELFBTC","ELFETH","AIONBTC","AIONETH","AIONBNB","NEBLBTC","NEBLETH","NEBLBNB","BRDBTC","BRDETH","BRDBNB","MCOBNB","EDOBTC","EDOETH","WINGSBTC","WINGSETH","NAVBTC","NAVETH","NAVBNB","LUNBTC","LUNETH","TRIGBTC","TRIGETH","TRIGBNB","APPCBTC","APPCETH","APPCBNB","VIBEBTC","VIBEETH","RLCBTC","RLCETH","RLCBNB","INSBTC","INSETH","PIVXBTC","PIVXETH","PIVXBNB","IOSTBTC","IOSTETH","CHATBTC","CHATETH","STEEMBTC","STEEMETH","STEEMBNB","NANOBTC","NANOETH","NANOBNB","VIABTC","VIAETH","VIABNB","BLZBTC","BLZETH","BLZBNB","AEBTC","AEETH","AEBNB","RPXBTC","RPXETH","RPXBNB","NCASHBTC","NCASHETH","NCASHBNB","POABTC","POAETH","POABNB","ZILBTC","ZILETH","ZILBNB","ONTBTC","ONTETH","ONTBNB","STORMBTC","STORMETH","STORMBNB","QTUMBNB","QTUMUSDT","XEMBTC","XEMETH","XEMBNB","WANBTC","WANETH","WANBNB","WPRBTC","WPRETH","QLCBTC","QLCETH","SYSBTC","SYSETH","SYSBNB","QLCBNB","GRSBTC","GRSETH","ADAUSDT","ADABNB","CLOAKBTC","CLOAKETH","GNTBTC","GNTETH","GNTBNB","LOOMBTC","LOOMETH","LOOMBNB","XRPUSDT","BCNBTC","BCNETH","BCNBNB","REPBTC","REPETH","REPBNB","TUSDBTC","TUSDETH","TUSDBNB","ZENBTC","ZENETH","ZENBNB","SKYBTC","SKYETH","SKYBNB","EOSUSDT","EOSBNB","CVCBTC","CVCETH","CVCBNB","THETABTC","THETAETH","THETABNB","XRPBNB","TUSDUSDT","IOTAUSDT","XLMUSDT","IOTXBTC","IOTXETH","QKCBTC","QKCETH","AGIBTC","AGIETH","AGIBNB","NXSBTC","NXSETH","NXSBNB","ENJBNB","DATABTC","DATAETH","ONTUSDT","TRXUSDT","ETCUSDT","ETCBNB","ICXUSDT","SCBTC","SCETH","SCBNB","NPXSBTC","NPXSETH","VENUSDT","KEYBTC","KEYETH","NASBTC","NASETH","NASBNB","MFTBTC","MFTETH","MFTBNB","DENTBTC","DENTETH","ARDRBTC","ARDRETH","ARDRBNB","NULSUSDT","HOTBTC","HOTETH","VETBTC","VETETH","VETUSDT","VETBNB","DOCKBTC","DOCKETH"]</v>
         <stp/>
         <stp>BINANCE</stp>
         <stp/>
@@ -4998,7 +5003,7 @@
         <tr r="T8" s="1"/>
       </tp>
       <tp>
-        <v>12.049877589999999</v>
+        <v>1.9841261400000001</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5007,7 +5012,7 @@
         <tr r="L32" s="1"/>
       </tp>
       <tp>
-        <v>0.18112928</v>
+        <v>2.3088000000000001E-4</v>
         <stp/>
         <stp>BINANCE_CANDLE</stp>
         <stp>trxbtc</stp>
@@ -5016,15 +5021,15 @@
         <tr r="L38" s="1"/>
       </tp>
       <tp>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>trxbtc</stp>
         <stp>PRICE</stp>
         <tr r="I21" s="1"/>
       </tp>
-      <tp>
-        <v>7.4259999999999997E-5</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -5032,7 +5037,7 @@
         <tr r="I20" s="1"/>
       </tp>
       <tp>
-        <v>6669.86</v>
+        <v>8160.19</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -5040,7 +5045,7 @@
         <tr r="K6" s="1"/>
       </tp>
       <tp>
-        <v>5.9000000000000003E-6</v>
+        <v>4.7199999999999997E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -5048,7 +5053,7 @@
         <tr r="G11" s="1"/>
       </tp>
       <tp>
-        <v>6664.1</v>
+        <v>8152.02</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>btcusdt</stp>
@@ -5056,7 +5061,7 @@
         <tr r="I6" s="1"/>
       </tp>
       <tp>
-        <v>5.9000000000000003E-6</v>
+        <v>4.7299999999999996E-6</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>trxbtc</stp>
@@ -5064,7 +5069,7 @@
         <tr r="D11" s="1"/>
       </tp>
       <tp>
-        <v>7.5820000000000003E-5</v>
+        <v>5.5630000000000001E-5</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>xrpbtc</stp>
@@ -5072,7 +5077,7 @@
         <tr r="D10" s="1"/>
       </tp>
       <tp>
-        <v>6662.15</v>
+        <v>8150.5</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5081,7 +5086,7 @@
         <tr r="B19" s="1"/>
       </tp>
       <tp>
-        <v>6661.45</v>
+        <v>8150</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5090,7 +5095,7 @@
         <tr r="B20" s="1"/>
       </tp>
       <tp>
-        <v>6661.02</v>
+        <v>8149.92</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5099,7 +5104,7 @@
         <tr r="B21" s="1"/>
       </tp>
       <tp>
-        <v>6660.61</v>
+        <v>8148.8</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5108,7 +5113,7 @@
         <tr r="B22" s="1"/>
       </tp>
       <tp>
-        <v>6665</v>
+        <v>8152.02</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5117,7 +5122,7 @@
         <tr r="B15" s="1"/>
       </tp>
       <tp>
-        <v>6664.77</v>
+        <v>8151.99</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5126,7 +5131,7 @@
         <tr r="B16" s="1"/>
       </tp>
       <tp>
-        <v>6664.13</v>
+        <v>8151.79</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5135,7 +5140,7 @@
         <tr r="B17" s="1"/>
       </tp>
       <tp>
-        <v>6663.73</v>
+        <v>8150.55</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5144,7 +5149,7 @@
         <tr r="B18" s="1"/>
       </tp>
       <tp>
-        <v>6660.53</v>
+        <v>8147.78</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5153,7 +5158,7 @@
         <tr r="B23" s="1"/>
       </tp>
       <tp>
-        <v>6660</v>
+        <v>8147.56</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5162,7 +5167,7 @@
         <tr r="B24" s="1"/>
       </tp>
       <tp>
-        <v>468.56</v>
+        <v>461.8</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>ETH-USD</stp>
@@ -5170,7 +5175,7 @@
         <tr r="E3" s="2"/>
       </tp>
       <tp>
-        <v>471.53</v>
+        <v>456.28</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -5178,15 +5183,15 @@
         <tr r="I5" s="1"/>
       </tp>
       <tp>
-        <v>6589.99</v>
+        <v>8105.01</v>
         <stp/>
         <stp>GDAX</stp>
         <stp>BTC-USD</stp>
         <stp>open_24h</stp>
         <tr r="E4" s="2"/>
       </tp>
-      <tp>
-        <v>43285.517003391207</v>
+      <tp t="s">
+        <v>&lt;?&gt;</v>
         <stp/>
         <stp>BINANCE_TRADE</stp>
         <stp>xrpbtc</stp>
@@ -5194,7 +5199,7 @@
         <tr r="L20" s="1"/>
       </tp>
       <tp>
-        <v>6669.87</v>
+        <v>8164.28</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5203,7 +5208,7 @@
         <tr r="D24" s="1"/>
       </tp>
       <tp>
-        <v>6669.86</v>
+        <v>8162.46</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5212,7 +5217,7 @@
         <tr r="D23" s="1"/>
       </tp>
       <tp>
-        <v>6668.74</v>
+        <v>8160.21</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5221,7 +5226,7 @@
         <tr r="D18" s="1"/>
       </tp>
       <tp>
-        <v>6668</v>
+        <v>8160.11</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5230,7 +5235,7 @@
         <tr r="D17" s="1"/>
       </tp>
       <tp>
-        <v>6667.97</v>
+        <v>8160.09</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5239,7 +5244,7 @@
         <tr r="D16" s="1"/>
       </tp>
       <tp>
-        <v>6667.96</v>
+        <v>8160.08</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5248,7 +5253,7 @@
         <tr r="D15" s="1"/>
       </tp>
       <tp>
-        <v>6669.51</v>
+        <v>8162</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5257,7 +5262,7 @@
         <tr r="D22" s="1"/>
       </tp>
       <tp>
-        <v>6669</v>
+        <v>8161.99</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5266,7 +5271,7 @@
         <tr r="D21" s="1"/>
       </tp>
       <tp>
-        <v>6668.91</v>
+        <v>8160.76</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5275,7 +5280,7 @@
         <tr r="D20" s="1"/>
       </tp>
       <tp>
-        <v>6668.78</v>
+        <v>8160.23</v>
         <stp/>
         <stp>BINANCE_DEPTH</stp>
         <stp>btcusdt</stp>
@@ -5284,7 +5289,7 @@
         <tr r="D19" s="1"/>
       </tp>
       <tp>
-        <v>472.03</v>
+        <v>456.46</v>
         <stp/>
         <stp>BINANCE_24H</stp>
         <stp>ethusdt</stp>
@@ -5923,7 +5928,7 @@
       </c>
       <c r="T4" s="37">
         <f>RTD(progId,,"CLOCK")</f>
-        <v>43285.517097245371</v>
+        <v>43311.846329664353</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5932,66 +5937,66 @@
       </c>
       <c r="B5" s="2">
         <f>RTD(progId,,BINANCE,$A5,B$4)</f>
-        <v>457</v>
+        <v>446.1</v>
       </c>
       <c r="C5" s="2">
         <f>RTD(progId,,BINANCE,$A5,C$4)</f>
-        <v>482.7</v>
+        <v>469.79</v>
       </c>
       <c r="D5" s="2">
         <f>RTD(progId,,BINANCE_24H,$A5,D$4)</f>
-        <v>469.12</v>
+        <v>462.04</v>
       </c>
       <c r="G5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,G$4)</f>
-        <v>469.52</v>
+        <v>462.04</v>
       </c>
       <c r="H5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,H$4)</f>
-        <v>2.4573100000000001</v>
+        <v>2.7384599999999999</v>
       </c>
       <c r="I5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,I$4)</f>
-        <v>471.53</v>
+        <v>456.28</v>
       </c>
       <c r="J5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,J$4)</f>
-        <v>0.51</v>
+        <v>0.18</v>
       </c>
       <c r="K5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,K$4)</f>
-        <v>472.03</v>
+        <v>456.46</v>
       </c>
       <c r="L5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,L$4)</f>
-        <v>2.6858599999999999</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="M5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,M$4)</f>
-        <v>120420.34009</v>
+        <v>175756.00234000001</v>
       </c>
       <c r="N5" s="42">
         <f>RTD(progId,,BINANCE_24H,$A5,N$4)</f>
-        <v>56432388.176379703</v>
+        <v>80652609.0343173</v>
       </c>
       <c r="O5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,O$4)</f>
-        <v>92427</v>
+        <v>100596</v>
       </c>
       <c r="P5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,P$4)</f>
-        <v>6.2899999999999996E-3</v>
+        <v>-1.244E-2</v>
       </c>
       <c r="Q5" s="40">
         <f>RTD(progId,,BINANCE_24H,$A5,Q$4)</f>
-        <v>2.91</v>
+        <v>-5.82</v>
       </c>
       <c r="S5" s="38" t="s">
         <v>61</v>
       </c>
       <c r="T5" s="36">
         <f>RTD(progId,,BINANCE,S5)</f>
-        <v>-443</v>
+        <v>-230</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -6000,66 +6005,66 @@
       </c>
       <c r="B6" s="2">
         <f>RTD(progId,,BINANCE,$A6,B$4)</f>
-        <v>6441.11</v>
+        <v>7866</v>
       </c>
       <c r="C6" s="2">
         <f>RTD(progId,,BINANCE,$A6,C$4)</f>
-        <v>6784.92</v>
+        <v>8273</v>
       </c>
       <c r="D6" s="2">
         <f>RTD(progId,,BINANCE_24H,$A6,D$4)</f>
-        <v>6591.31</v>
+        <v>8113.99</v>
       </c>
       <c r="G6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,G$4)</f>
-        <v>6589.41</v>
+        <v>8113.99</v>
       </c>
       <c r="H6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,H$4)</f>
-        <v>6.7424999999999999E-2</v>
+        <v>7.6309999999999998E-3</v>
       </c>
       <c r="I6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,I$4)</f>
-        <v>6664.1</v>
+        <v>8152.02</v>
       </c>
       <c r="J6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,J$4)</f>
-        <v>5.72</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="K6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,K$4)</f>
-        <v>6669.86</v>
+        <v>8160.19</v>
       </c>
       <c r="L6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,L$4)</f>
-        <v>0.26262600000000003</v>
+        <v>0.209645</v>
       </c>
       <c r="M6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,M$4)</f>
-        <v>29075.271000000001</v>
+        <v>38006.927171000003</v>
       </c>
       <c r="N6" s="42">
         <f>RTD(progId,,BINANCE_24H,$A6,N$4)</f>
-        <v>191494800.14948204</v>
+        <v>307914890.48390466</v>
       </c>
       <c r="O6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,O$4)</f>
-        <v>168939</v>
+        <v>199972</v>
       </c>
       <c r="P6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,P$4)</f>
-        <v>1.191E-2</v>
+        <v>5.7000000000000002E-3</v>
       </c>
       <c r="Q6" s="40">
         <f>RTD(progId,,BINANCE_24H,$A6,Q$4)</f>
-        <v>72.8</v>
+        <v>46.2</v>
       </c>
       <c r="S6" s="38" t="s">
         <v>62</v>
       </c>
       <c r="T6" s="37">
         <f>RTD(progId,,BINANCE,S6)</f>
-        <v>43285.516620439812</v>
+        <v>43311.84597584491</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -6068,59 +6073,59 @@
       </c>
       <c r="B7" s="2">
         <f>RTD(progId,,BINANCE,$A7,B$4)</f>
-        <v>83.64</v>
+        <v>79.760000000000005</v>
       </c>
       <c r="C7" s="2">
         <f>RTD(progId,,BINANCE,$A7,C$4)</f>
-        <v>89.01</v>
+        <v>84.62</v>
       </c>
       <c r="D7" s="2">
         <f>RTD(progId,,BINANCE_24H,$A7,D$4)</f>
-        <v>86.41</v>
+        <v>82.77</v>
       </c>
       <c r="G7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,G$4)</f>
-        <v>86.38</v>
+        <v>82.79</v>
       </c>
       <c r="H7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,H$4)</f>
-        <v>1.537E-2</v>
+        <v>1.70052</v>
       </c>
       <c r="I7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,I$4)</f>
-        <v>86.7</v>
+        <v>82.46</v>
       </c>
       <c r="J7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,J$4)</f>
-        <v>0.15</v>
+        <v>0.02</v>
       </c>
       <c r="K7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,K$4)</f>
-        <v>86.85</v>
+        <v>82.48</v>
       </c>
       <c r="L7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,L$4)</f>
-        <v>0.56000000000000005</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="M7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,M$4)</f>
-        <v>132521.51637999999</v>
+        <v>143669.38344999999</v>
       </c>
       <c r="N7" s="42">
         <f>RTD(progId,,BINANCE_24H,$A7,N$4)</f>
-        <v>11444940.7380598</v>
+        <v>11879122.185702</v>
       </c>
       <c r="O7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,O$4)</f>
-        <v>20628</v>
+        <v>23655</v>
       </c>
       <c r="P7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,P$4)</f>
-        <v>5.3299999999999997E-3</v>
+        <v>-3.8700000000000002E-3</v>
       </c>
       <c r="Q7" s="40">
         <f>RTD(progId,,BINANCE_24H,$A7,Q$4)</f>
-        <v>0.46</v>
+        <v>-0.32</v>
       </c>
       <c r="S7" s="38" t="s">
         <v>63</v>
@@ -6136,66 +6141,66 @@
       </c>
       <c r="B8" s="2">
         <f>RTD(progId,,BINANCE,$A8,B$4)</f>
-        <v>0.47800999999999999</v>
+        <v>0.43381999999999998</v>
       </c>
       <c r="C8" s="2">
         <f>RTD(progId,,BINANCE,$A8,C$4)</f>
-        <v>0.50654999999999994</v>
+        <v>0.45621</v>
       </c>
       <c r="D8" s="2">
         <f>RTD(progId,,BINANCE_24H,$A8,D$4)</f>
-        <v>0.49924000000000002</v>
+        <v>0.45127</v>
       </c>
       <c r="G8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,G$4)</f>
-        <v>0.49940000000000001</v>
+        <v>0.45061000000000001</v>
       </c>
       <c r="H8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,H$4)</f>
-        <v>6902.4</v>
+        <v>56.1</v>
       </c>
       <c r="I8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,I$4)</f>
-        <v>0.49421999999999999</v>
+        <v>0.44571</v>
       </c>
       <c r="J8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,J$4)</f>
-        <v>1.1800000000000001E-3</v>
+        <v>5.9000000000000003E-4</v>
       </c>
       <c r="K8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,K$4)</f>
-        <v>0.49541000000000002</v>
+        <v>0.44630999999999998</v>
       </c>
       <c r="L8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,L$4)</f>
-        <v>3292</v>
+        <v>44.7</v>
       </c>
       <c r="M8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,M$4)</f>
-        <v>28720303.899999999</v>
+        <v>31623342.399999999</v>
       </c>
       <c r="N8" s="42">
         <f>RTD(progId,,BINANCE_24H,$A8,N$4)</f>
-        <v>14130749.716714</v>
+        <v>14185322.523376999</v>
       </c>
       <c r="O8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,O$4)</f>
-        <v>17606</v>
+        <v>17556</v>
       </c>
       <c r="P8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,P$4)</f>
-        <v>-9.2899999999999996E-3</v>
+        <v>-1.099E-2</v>
       </c>
       <c r="Q8" s="40">
         <f>RTD(progId,,BINANCE_24H,$A8,Q$4)</f>
-        <v>-4.64E-3</v>
+        <v>-4.3E-3</v>
       </c>
       <c r="S8" s="38" t="s">
         <v>64</v>
       </c>
       <c r="T8" s="36" t="str">
         <f>RTD(progId,,BINANCE,,S8)</f>
-        <v>["ETHBTC","LTCBTC","BNBBTC","NEOBTC","QTUMETH","EOSETH","SNTETH","BNTETH","BCCBTC","GASBTC","BNBETH","BTCUSDT","ETHUSDT","HSRBTC","OAXETH","DNTETH","MCOETH","ICNETH","MCOBTC","WTCBTC","WTCETH","LRCBTC","LRCETH","QTUMBTC","YOYOBTC","OMGBTC","OMGETH","ZRXBTC","ZRXETH","STRATBTC","STRATETH","SNGLSBTC","SNGLSETH","BQXBTC","BQXETH","KNCBTC","KNCETH","FUNBTC","FUNETH","SNMBTC","SNMETH","NEOETH","IOTABTC","IOTAETH","LINKBTC","LINKETH","XVGBTC","XVGETH","SALTBTC","SALTETH","MDABTC","MDAETH","MTLBTC","MTLETH","SUBBTC","SUBETH","EOSBTC","SNTBTC","ETCETH","ETCBTC","MTHBTC","MTHETH","ENGBTC","ENGETH","DNTBTC","ZECBTC","ZECETH","BNTBTC","ASTBTC","ASTETH","DASHBTC","DASHETH","OAXBTC","ICNBTC","BTGBTC","BTGETH","EVXBTC","EVXETH","REQBTC","REQETH","VIBBTC","VIBETH","HSRETH","TRXBTC","TRXETH","POWRBTC","POWRETH","ARKBTC","ARKETH","YOYOETH","XRPBTC","XRPETH","MODBTC","MODETH","ENJBTC","ENJETH","STORJBTC","STORJETH","BNBUSDT","VENBNB","YOYOBNB","POWRBNB","VENBTC","VENETH","KMDBTC","KMDETH","NULSBNB","RCNBTC","RCNETH","RCNBNB","NULSBTC","NULSETH","RDNBTC","RDNETH","RDNBNB","XMRBTC","XMRETH","DLTBNB","WTCBNB","DLTBTC","DLTETH","AMBBTC","AMBETH","AMBBNB","BCCETH","BCCUSDT","BCCBNB","BATBTC","BATETH","BATBNB","BCPTBTC","BCPTETH","BCPTBNB","ARNBTC","ARNETH","GVTBTC","GVTETH","CDTBTC","CDTETH","GXSBTC","GXSETH","NEOUSDT","NEOBNB","POEBTC","POEETH","QSPBTC","QSPETH","QSPBNB","BTSBTC","BTSETH","BTSBNB","XZCBTC","XZCETH","XZCBNB","LSKBTC","LSKETH","LSKBNB","TNTBTC","TNTETH","FUELBTC","FUELETH","MANABTC","MANAETH","BCDBTC","BCDETH","DGDBTC","DGDETH","IOTABNB","ADXBTC","ADXETH","ADXBNB","ADABTC","ADAETH","PPTBTC","PPTETH","CMTBTC","CMTETH","CMTBNB","XLMBTC","XLMETH","XLMBNB","CNDBTC","CNDETH","CNDBNB","LENDBTC","LENDETH","WABIBTC","WABIETH","WABIBNB","LTCETH","LTCUSDT","LTCBNB","TNBBTC","TNBETH","WAVESBTC","WAVESETH","WAVESBNB","GTOBTC","GTOETH","GTOBNB","ICXBTC","ICXETH","ICXBNB","OSTBTC","OSTETH","OSTBNB","ELFBTC","ELFETH","AIONBTC","AIONETH","AIONBNB","NEBLBTC","NEBLETH","NEBLBNB","BRDBTC","BRDETH","BRDBNB","MCOBNB","EDOBTC","EDOETH","WINGSBTC","WINGSETH","NAVBTC","NAVETH","NAVBNB","LUNBTC","LUNETH","TRIGBTC","TRIGETH","TRIGBNB","APPCBTC","APPCETH","APPCBNB","VIBEBTC","VIBEETH","RLCBTC","RLCETH","RLCBNB","INSBTC","INSETH","PIVXBTC","PIVXETH","PIVXBNB","IOSTBTC","IOSTETH","CHATBTC","CHATETH","STEEMBTC","STEEMETH","STEEMBNB","NANOBTC","NANOETH","NANOBNB","VIABTC","VIAETH","VIABNB","BLZBTC","BLZETH","BLZBNB","AEBTC","AEETH","AEBNB","RPXBTC","RPXETH","RPXBNB","NCASHBTC","NCASHETH","NCASHBNB","POABTC","POAETH","POABNB","ZILBTC","ZILETH","ZILBNB","ONTBTC","ONTETH","ONTBNB","STORMBTC","STORMETH","STORMBNB","QTUMBNB","QTUMUSDT","XEMBTC","XEMETH","XEMBNB","WANBTC","WANETH","WANBNB","WPRBTC","WPRETH","QLCBTC","QLCETH","SYSBTC","SYSETH","SYSBNB","QLCBNB","GRSBTC","GRSETH","ADAUSDT","ADABNB","CLOAKBTC","CLOAKETH","GNTBTC","GNTETH","GNTBNB","LOOMBTC","LOOMETH","LOOMBNB","XRPUSDT","BCNBTC","BCNETH","BCNBNB","REPBTC","REPETH","REPBNB","TUSDBTC","TUSDETH","TUSDBNB","ZENBTC","ZENETH","ZENBNB","SKYBTC","SKYETH","SKYBNB","EOSUSDT","EOSBNB","CVCBTC","CVCETH","CVCBNB","THETABTC","THETAETH","THETABNB","XRPBNB","TUSDUSDT","IOTAUSDT","XLMUSDT","IOTXBTC","IOTXETH","QKCBTC","QKCETH","AGIBTC","AGIETH","AGIBNB","NXSBTC","NXSETH","NXSBNB","ENJBNB","DATABTC","DATAETH","ONTUSDT","TRXUSDT","ETCUSDT","ETCBNB","ICXUSDT","SCBTC","SCETH","SCBNB","NPXSBTC","NPXSETH","VENUSDT","KEYBTC","KEYETH","NASBTC","NASETH","NASBNB"]</v>
+        <v>["ETHBTC","LTCBTC","BNBBTC","NEOBTC","QTUMETH","EOSETH","SNTETH","BNTETH","BCCBTC","GASBTC","BNBETH","BTCUSDT","ETHUSDT","HSRBTC","OAXETH","DNTETH","MCOETH","ICNETH","MCOBTC","WTCBTC","WTCETH","LRCBTC","LRCETH","QTUMBTC","YOYOBTC","OMGBTC","OMGETH","ZRXBTC","ZRXETH","STRATBTC","STRATETH","SNGLSBTC","SNGLSETH","BQXBTC","BQXETH","KNCBTC","KNCETH","FUNBTC","FUNETH","SNMBTC","SNMETH","NEOETH","IOTABTC","IOTAETH","LINKBTC","LINKETH","XVGBTC","XVGETH","SALTBTC","SALTETH","MDABTC","MDAETH","MTLBTC","MTLETH","SUBBTC","SUBETH","EOSBTC","SNTBTC","ETCETH","ETCBTC","MTHBTC","MTHETH","ENGBTC","ENGETH","DNTBTC","ZECBTC","ZECETH","BNTBTC","ASTBTC","ASTETH","DASHBTC","DASHETH","OAXBTC","ICNBTC","BTGBTC","BTGETH","EVXBTC","EVXETH","REQBTC","REQETH","VIBBTC","VIBETH","HSRETH","TRXBTC","TRXETH","POWRBTC","POWRETH","ARKBTC","ARKETH","YOYOETH","XRPBTC","XRPETH","MODBTC","MODETH","ENJBTC","ENJETH","STORJBTC","STORJETH","BNBUSDT","VENBNB","YOYOBNB","POWRBNB","VENBTC","VENETH","KMDBTC","KMDETH","NULSBNB","RCNBTC","RCNETH","RCNBNB","NULSBTC","NULSETH","RDNBTC","RDNETH","RDNBNB","XMRBTC","XMRETH","DLTBNB","WTCBNB","DLTBTC","DLTETH","AMBBTC","AMBETH","AMBBNB","BCCETH","BCCUSDT","BCCBNB","BATBTC","BATETH","BATBNB","BCPTBTC","BCPTETH","BCPTBNB","ARNBTC","ARNETH","GVTBTC","GVTETH","CDTBTC","CDTETH","GXSBTC","GXSETH","NEOUSDT","NEOBNB","POEBTC","POEETH","QSPBTC","QSPETH","QSPBNB","BTSBTC","BTSETH","BTSBNB","XZCBTC","XZCETH","XZCBNB","LSKBTC","LSKETH","LSKBNB","TNTBTC","TNTETH","FUELBTC","FUELETH","MANABTC","MANAETH","BCDBTC","BCDETH","DGDBTC","DGDETH","IOTABNB","ADXBTC","ADXETH","ADXBNB","ADABTC","ADAETH","PPTBTC","PPTETH","CMTBTC","CMTETH","CMTBNB","XLMBTC","XLMETH","XLMBNB","CNDBTC","CNDETH","CNDBNB","LENDBTC","LENDETH","WABIBTC","WABIETH","WABIBNB","LTCETH","LTCUSDT","LTCBNB","TNBBTC","TNBETH","WAVESBTC","WAVESETH","WAVESBNB","GTOBTC","GTOETH","GTOBNB","ICXBTC","ICXETH","ICXBNB","OSTBTC","OSTETH","OSTBNB","ELFBTC","ELFETH","AIONBTC","AIONETH","AIONBNB","NEBLBTC","NEBLETH","NEBLBNB","BRDBTC","BRDETH","BRDBNB","MCOBNB","EDOBTC","EDOETH","WINGSBTC","WINGSETH","NAVBTC","NAVETH","NAVBNB","LUNBTC","LUNETH","TRIGBTC","TRIGETH","TRIGBNB","APPCBTC","APPCETH","APPCBNB","VIBEBTC","VIBEETH","RLCBTC","RLCETH","RLCBNB","INSBTC","INSETH","PIVXBTC","PIVXETH","PIVXBNB","IOSTBTC","IOSTETH","CHATBTC","CHATETH","STEEMBTC","STEEMETH","STEEMBNB","NANOBTC","NANOETH","NANOBNB","VIABTC","VIAETH","VIABNB","BLZBTC","BLZETH","BLZBNB","AEBTC","AEETH","AEBNB","RPXBTC","RPXETH","RPXBNB","NCASHBTC","NCASHETH","NCASHBNB","POABTC","POAETH","POABNB","ZILBTC","ZILETH","ZILBNB","ONTBTC","ONTETH","ONTBNB","STORMBTC","STORMETH","STORMBNB","QTUMBNB","QTUMUSDT","XEMBTC","XEMETH","XEMBNB","WANBTC","WANETH","WANBNB","WPRBTC","WPRETH","QLCBTC","QLCETH","SYSBTC","SYSETH","SYSBNB","QLCBNB","GRSBTC","GRSETH","ADAUSDT","ADABNB","CLOAKBTC","CLOAKETH","GNTBTC","GNTETH","GNTBNB","LOOMBTC","LOOMETH","LOOMBNB","XRPUSDT","BCNBTC","BCNETH","BCNBNB","REPBTC","REPETH","REPBNB","TUSDBTC","TUSDETH","TUSDBNB","ZENBTC","ZENETH","ZENBNB","SKYBTC","SKYETH","SKYBNB","EOSUSDT","EOSBNB","CVCBTC","CVCETH","CVCBNB","THETABTC","THETAETH","THETABNB","XRPBNB","TUSDUSDT","IOTAUSDT","XLMUSDT","IOTXBTC","IOTXETH","QKCBTC","QKCETH","AGIBTC","AGIETH","AGIBNB","NXSBTC","NXSETH","NXSBNB","ENJBNB","DATABTC","DATAETH","ONTUSDT","TRXUSDT","ETCUSDT","ETCBNB","ICXUSDT","SCBTC","SCETH","SCBNB","NPXSBTC","NPXSETH","VENUSDT","KEYBTC","KEYETH","NASBTC","NASETH","NASBNB","MFTBTC","MFTETH","MFTBNB","DENTBTC","DENTETH","ARDRBTC","ARDRETH","ARDRBNB","NULSUSDT","HOTBTC","HOTETH","VETBTC","VETETH","VETUSDT","VETBNB","DOCKBTC","DOCKETH"]</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -6204,27 +6209,27 @@
       </c>
       <c r="B9" s="2">
         <f>RTD(progId,,BINANCE,$A9,B$4)</f>
-        <v>5.4349999999999997E-3</v>
+        <v>3.8899999999999998E-3</v>
       </c>
       <c r="C9" s="2">
         <f>RTD(progId,,BINANCE,$A9,C$4)</f>
-        <v>6.1910000000000003E-3</v>
+        <v>4.1399999999999996E-3</v>
       </c>
       <c r="D9" s="2">
         <f>RTD(progId,,BINANCE_24H,$A9,D$4)</f>
-        <v>5.5380000000000004E-3</v>
+        <v>4.0699999999999998E-3</v>
       </c>
       <c r="G9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,G$4)</f>
-        <v>5.5440000000000003E-3</v>
+        <v>4.0679999999999996E-3</v>
       </c>
       <c r="H9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,H$4)</f>
-        <v>0.03</v>
+        <v>18.25</v>
       </c>
       <c r="I9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,I$4)</f>
-        <v>5.8050000000000003E-3</v>
+        <v>3.9329999999999999E-3</v>
       </c>
       <c r="J9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,J$4)</f>
@@ -6232,31 +6237,31 @@
       </c>
       <c r="K9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,K$4)</f>
-        <v>5.8069999999999997E-3</v>
+        <v>3.934E-3</v>
       </c>
       <c r="L9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,L$4)</f>
-        <v>6.58</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="M9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,M$4)</f>
-        <v>506889</v>
+        <v>324679.78999999998</v>
       </c>
       <c r="N9" s="42">
         <f>RTD(progId,,BINANCE_24H,$A9,N$4)</f>
-        <v>2938.16672982</v>
+        <v>1298.85586367</v>
       </c>
       <c r="O9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,O$4)</f>
-        <v>51127</v>
+        <v>34468</v>
       </c>
       <c r="P9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,P$4)</f>
-        <v>4.7629999999999999E-2</v>
+        <v>-3.295E-2</v>
       </c>
       <c r="Q9" s="40">
         <f>RTD(progId,,BINANCE_24H,$A9,Q$4)</f>
-        <v>2.63E-4</v>
+        <v>-1.35E-4</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6265,59 +6270,59 @@
       </c>
       <c r="B10" s="2">
         <f>RTD(progId,,BINANCE,$A10,B$4)</f>
-        <v>7.3490000000000003E-5</v>
+        <v>5.4190000000000001E-5</v>
       </c>
       <c r="C10" s="2">
         <f>RTD(progId,,BINANCE,$A10,C$4)</f>
-        <v>7.6240000000000002E-5</v>
+        <v>5.5899999999999997E-5</v>
       </c>
       <c r="D10" s="2">
         <f>RTD(progId,,BINANCE_24H,$A10,D$4)</f>
-        <v>7.5820000000000003E-5</v>
+        <v>5.5630000000000001E-5</v>
       </c>
       <c r="G10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,G$4)</f>
-        <v>7.5850000000000001E-5</v>
+        <v>5.5590000000000001E-5</v>
       </c>
       <c r="H10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,H$4)</f>
-        <v>3086</v>
+        <v>639</v>
       </c>
       <c r="I10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,I$4)</f>
-        <v>7.4190000000000006E-5</v>
+        <v>5.4629999999999997E-5</v>
       </c>
       <c r="J10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,J$4)</f>
-        <v>7.0000000000000005E-8</v>
+        <v>5.9999999999999995E-8</v>
       </c>
       <c r="K10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,K$4)</f>
-        <v>7.428E-5</v>
+        <v>5.469E-5</v>
       </c>
       <c r="L10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,L$4)</f>
-        <v>2199</v>
+        <v>2890</v>
       </c>
       <c r="M10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,M$4)</f>
-        <v>36351363</v>
+        <v>37988898</v>
       </c>
       <c r="N10" s="42">
         <f>RTD(progId,,BINANCE_24H,$A10,N$4)</f>
-        <v>2711.1513072399998</v>
+        <v>2097.0739247000001</v>
       </c>
       <c r="O10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,O$4)</f>
-        <v>30879</v>
+        <v>34493</v>
       </c>
       <c r="P10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,P$4)</f>
-        <v>-2.121E-2</v>
+        <v>-1.6719999999999999E-2</v>
       </c>
       <c r="Q10" s="40">
         <f>RTD(progId,,BINANCE_24H,$A10,Q$4)</f>
-        <v>-1.66E-6</v>
+        <v>-9.5999999999999991E-7</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6326,27 +6331,27 @@
       </c>
       <c r="B11" s="2">
         <f>RTD(progId,,BINANCE,$A11,B$4)</f>
-        <v>5.7699999999999998E-6</v>
+        <v>4.3599999999999998E-6</v>
       </c>
       <c r="C11" s="2">
         <f>RTD(progId,,BINANCE,$A11,C$4)</f>
-        <v>5.9900000000000002E-6</v>
+        <v>4.8300000000000003E-6</v>
       </c>
       <c r="D11" s="2">
         <f>RTD(progId,,BINANCE_24H,$A11,D$4)</f>
-        <v>5.9000000000000003E-6</v>
+        <v>4.7299999999999996E-6</v>
       </c>
       <c r="G11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,G$4)</f>
-        <v>5.9000000000000003E-6</v>
+        <v>4.7199999999999997E-6</v>
       </c>
       <c r="H11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,H$4)</f>
-        <v>1035439</v>
+        <v>104282</v>
       </c>
       <c r="I11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,I$4)</f>
-        <v>5.8799999999999996E-6</v>
+        <v>4.4299999999999999E-6</v>
       </c>
       <c r="J11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,J$4)</f>
@@ -6354,31 +6359,31 @@
       </c>
       <c r="K11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,K$4)</f>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
       </c>
       <c r="L11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,L$4)</f>
-        <v>73326</v>
+        <v>1629845</v>
       </c>
       <c r="M11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,M$4)</f>
-        <v>399604654</v>
+        <v>620653152</v>
       </c>
       <c r="N11" s="42">
         <f>RTD(progId,,BINANCE_24H,$A11,N$4)</f>
-        <v>2358.1084988900002</v>
+        <v>2832.6466749199999</v>
       </c>
       <c r="O11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,O$4)</f>
-        <v>30240</v>
+        <v>47488</v>
       </c>
       <c r="P11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,P$4)</f>
-        <v>-1.6900000000000001E-3</v>
+        <v>-6.3420000000000004E-2</v>
       </c>
       <c r="Q11" s="40">
         <f>RTD(progId,,BINANCE_24H,$A11,Q$4)</f>
-        <v>-1E-8</v>
+        <v>-2.9999999999999999E-7</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6466,22 +6471,22 @@
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C15)</f>
-        <v>1.992E-2</v>
+        <v>0.79360200000000003</v>
       </c>
       <c r="B15" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C15)</f>
-        <v>6665</v>
+        <v>8152.02</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
       </c>
       <c r="D15" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C15)</f>
-        <v>6667.96</v>
+        <v>8160.08</v>
       </c>
       <c r="E15" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C15)</f>
-        <v>2.0254000000000001E-2</v>
+        <v>0.63443899999999998</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
@@ -6489,15 +6494,15 @@
       </c>
       <c r="H15" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G15,H$14)</f>
-        <v>27105497</v>
+        <v>29601071</v>
       </c>
       <c r="I15" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G15,I$14)</f>
-        <v>471.3</v>
+        <v>456.29</v>
       </c>
       <c r="J15" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G15,J$14)</f>
-        <v>0.91744999999999999</v>
+        <v>0.48276000000000002</v>
       </c>
       <c r="K15" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G15,K$14)</f>
@@ -6505,7 +6510,7 @@
       </c>
       <c r="L15" s="28">
         <f>RTD(progId,,BINACE_TRADE,$G15,L$14)</f>
-        <v>43285.517101666665</v>
+        <v>43311.846317650467</v>
       </c>
       <c r="N15" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G15,N$14)</f>
@@ -6517,7 +6522,7 @@
       </c>
       <c r="P15" s="36" t="b">
         <f>RTD(progId,,BINANCE,$G15,P$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G15,Q$14)</f>
@@ -6537,17 +6542,17 @@
       </c>
       <c r="U15" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G15,U$14)</f>
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C16)</f>
-        <v>0.98658500000000005</v>
+        <v>7.6309999999999998E-3</v>
       </c>
       <c r="B16" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C16)</f>
-        <v>6664.77</v>
+        <v>8151.99</v>
       </c>
       <c r="C16" s="8">
         <f>C15+1</f>
@@ -6555,11 +6560,11 @@
       </c>
       <c r="D16" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C16)</f>
-        <v>6667.97</v>
+        <v>8160.09</v>
       </c>
       <c r="E16" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C16)</f>
-        <v>0.35168100000000002</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
@@ -6567,15 +6572,15 @@
       </c>
       <c r="H16" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G16,H$14)</f>
-        <v>48377931</v>
+        <v>53127003</v>
       </c>
       <c r="I16" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G16,I$14)</f>
-        <v>6664.13</v>
+        <v>8152.02</v>
       </c>
       <c r="J16" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G16,J$14)</f>
-        <v>0.109002</v>
+        <v>4.1603000000000001E-2</v>
       </c>
       <c r="K16" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G16,K$14)</f>
@@ -6583,7 +6588,7 @@
       </c>
       <c r="L16" s="28">
         <f>RTD(progId,,BINACE_TRADE,$G16,L$14)</f>
-        <v>43285.517102048609</v>
+        <v>43311.846355023146</v>
       </c>
       <c r="N16" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G16,N$14)</f>
@@ -6595,7 +6600,7 @@
       </c>
       <c r="P16" s="36" t="b">
         <f>RTD(progId,,BINANCE,$G16,P$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G16,Q$14)</f>
@@ -6615,17 +6620,17 @@
       </c>
       <c r="U16" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G16,U$14)</f>
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C17)</f>
-        <v>2.9922629999999999</v>
+        <v>0.5</v>
       </c>
       <c r="B17" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C17)</f>
-        <v>6664.13</v>
+        <v>8151.79</v>
       </c>
       <c r="C17" s="8">
         <f t="shared" ref="C17:C24" si="0">C16+1</f>
@@ -6633,11 +6638,11 @@
       </c>
       <c r="D17" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C17)</f>
-        <v>6668</v>
+        <v>8160.11</v>
       </c>
       <c r="E17" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C17)</f>
-        <v>4.7935999999999999E-2</v>
+        <v>0.34868500000000002</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
@@ -6645,23 +6650,23 @@
       </c>
       <c r="H17" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G17,H$14)</f>
-        <v>7533270</v>
+        <v>8202329</v>
       </c>
       <c r="I17" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G17,I$14)</f>
-        <v>86.86</v>
+        <v>82.47</v>
       </c>
       <c r="J17" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G17,J$14)</f>
-        <v>2.5009299999999999</v>
+        <v>1.0522</v>
       </c>
       <c r="K17" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G17,K$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G17,L$14)</f>
-        <v>43285.516921724535</v>
+        <v>43311.846334247683</v>
       </c>
       <c r="N17" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G17,N$14)</f>
@@ -6673,7 +6678,7 @@
       </c>
       <c r="P17" s="36" t="b">
         <f>RTD(progId,,BINANCE,$G17,P$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G17,Q$14)</f>
@@ -6693,17 +6698,17 @@
       </c>
       <c r="U17" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G17,U$14)</f>
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C18)</f>
-        <v>5.6000000000000001E-2</v>
+        <v>3.4143300000000001</v>
       </c>
       <c r="B18" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C18)</f>
-        <v>6663.73</v>
+        <v>8150.55</v>
       </c>
       <c r="C18" s="8">
         <f t="shared" si="0"/>
@@ -6711,35 +6716,35 @@
       </c>
       <c r="D18" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C18)</f>
-        <v>6668.74</v>
+        <v>8160.21</v>
       </c>
       <c r="E18" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C18)</f>
-        <v>5.6000000000000001E-2</v>
+        <v>1.6038E-2</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="13" t="str">
+      <c r="H18" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G18,H$14)</f>
-        <v>&lt;?&gt;</v>
-      </c>
-      <c r="I18" s="13" t="str">
+        <v>1939683</v>
+      </c>
+      <c r="I18" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G18,I$14)</f>
-        <v>&lt;?&gt;</v>
-      </c>
-      <c r="J18" s="13" t="str">
+        <v>0.44630999999999998</v>
+      </c>
+      <c r="J18" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G18,J$14)</f>
-        <v>&lt;?&gt;</v>
-      </c>
-      <c r="K18" s="13" t="str">
+        <v>4787.5</v>
+      </c>
+      <c r="K18" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G18,K$14)</f>
-        <v>&lt;?&gt;</v>
-      </c>
-      <c r="L18" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="L18" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G18,L$14)</f>
-        <v>&lt;?&gt;</v>
+        <v>43311.84629065972</v>
       </c>
       <c r="N18" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G18,N$14)</f>
@@ -6751,7 +6756,7 @@
       </c>
       <c r="P18" s="36" t="b">
         <f>RTD(progId,,BINANCE,$G18,P$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G18,Q$14)</f>
@@ -6771,17 +6776,17 @@
       </c>
       <c r="U18" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G18,U$14)</f>
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C19)</f>
-        <v>9.0060000000000001E-2</v>
+        <v>6.1339999999999997E-3</v>
       </c>
       <c r="B19" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C19)</f>
-        <v>6662.15</v>
+        <v>8150.5</v>
       </c>
       <c r="C19" s="8">
         <f t="shared" si="0"/>
@@ -6789,11 +6794,11 @@
       </c>
       <c r="D19" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C19)</f>
-        <v>6668.78</v>
+        <v>8160.23</v>
       </c>
       <c r="E19" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C19)</f>
-        <v>0.49435000000000001</v>
+        <v>0.310498</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
@@ -6801,15 +6806,15 @@
       </c>
       <c r="H19" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G19,H$14)</f>
-        <v>14554128</v>
+        <v>15655775</v>
       </c>
       <c r="I19" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G19,I$14)</f>
-        <v>5.7980000000000002E-3</v>
+        <v>3.9329999999999999E-3</v>
       </c>
       <c r="J19" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G19,J$14)</f>
-        <v>15.4</v>
+        <v>0.54</v>
       </c>
       <c r="K19" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G19,K$14)</f>
@@ -6817,7 +6822,7 @@
       </c>
       <c r="L19" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G19,L$14)</f>
-        <v>43285.517102199075</v>
+        <v>43311.846354965281</v>
       </c>
       <c r="N19" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G19,N$14)</f>
@@ -6829,7 +6834,7 @@
       </c>
       <c r="P19" s="36" t="b">
         <f>RTD(progId,,BINANCE,$G19,P$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G19,Q$14)</f>
@@ -6849,17 +6854,17 @@
       </c>
       <c r="U19" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G19,U$14)</f>
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C20)</f>
-        <v>4.0910000000000002</v>
+        <v>6.7230259999999999</v>
       </c>
       <c r="B20" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C20)</f>
-        <v>6661.45</v>
+        <v>8150</v>
       </c>
       <c r="C20" s="8">
         <f t="shared" si="0"/>
@@ -6867,35 +6872,35 @@
       </c>
       <c r="D20" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C20)</f>
-        <v>6668.91</v>
+        <v>8160.76</v>
       </c>
       <c r="E20" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C20)</f>
-        <v>9.4730999999999996E-2</v>
+        <v>0.19</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="13" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G20,H$14)</f>
-        <v>18596602</v>
-      </c>
-      <c r="I20" s="13">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="I20" s="13" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G20,I$14)</f>
-        <v>7.4259999999999997E-5</v>
-      </c>
-      <c r="J20" s="13">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="J20" s="13" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G20,J$14)</f>
-        <v>377</v>
-      </c>
-      <c r="K20" s="13" t="b">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="K20" s="13" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G20,K$14)</f>
-        <v>0</v>
-      </c>
-      <c r="L20" s="29">
+        <v>&lt;?&gt;</v>
+      </c>
+      <c r="L20" s="29" t="str">
         <f>RTD(progId,,BINACE_TRADE,$G20,L$14)</f>
-        <v>43285.517003391207</v>
+        <v>&lt;?&gt;</v>
       </c>
       <c r="N20" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G20,N$14)</f>
@@ -6907,7 +6912,7 @@
       </c>
       <c r="P20" s="36" t="b">
         <f>RTD(progId,,BINANCE,$G20,P$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G20,Q$14)</f>
@@ -6927,17 +6932,17 @@
       </c>
       <c r="U20" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G20,U$14)</f>
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C21)</f>
-        <v>0.109</v>
+        <v>0.99</v>
       </c>
       <c r="B21" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C21)</f>
-        <v>6661.02</v>
+        <v>8149.92</v>
       </c>
       <c r="C21" s="8">
         <f t="shared" si="0"/>
@@ -6945,11 +6950,11 @@
       </c>
       <c r="D21" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C21)</f>
-        <v>6669</v>
+        <v>8161.99</v>
       </c>
       <c r="E21" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C21)</f>
-        <v>7.5079999999999999E-3</v>
+        <v>0.35439999999999999</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
@@ -6957,15 +6962,15 @@
       </c>
       <c r="H21" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G21,H$14)</f>
-        <v>19233907</v>
+        <v>19966248</v>
       </c>
       <c r="I21" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G21,I$14)</f>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
       </c>
       <c r="J21" s="13">
         <f>RTD(progId,,BINACE_TRADE,$G21,J$14)</f>
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="K21" s="13" t="b">
         <f>RTD(progId,,BINACE_TRADE,$G21,K$14)</f>
@@ -6973,7 +6978,7 @@
       </c>
       <c r="L21" s="29">
         <f>RTD(progId,,BINACE_TRADE,$G21,L$14)</f>
-        <v>43285.516921377312</v>
+        <v>43311.84632384259</v>
       </c>
       <c r="N21" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G21,N$14)</f>
@@ -6985,7 +6990,7 @@
       </c>
       <c r="P21" s="36" t="b">
         <f>RTD(progId,,BINANCE,$G21,P$14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G21,Q$14)</f>
@@ -7005,17 +7010,17 @@
       </c>
       <c r="U21" s="36" t="str">
         <f>RTD(progId,,BINANCE,$G21,U$14)</f>
-        <v>Limit|LimitMaker|Market|StopLossLimit|TakeProfitLimit|</v>
+        <v>[0,6,1,3,5]</v>
       </c>
     </row>
     <row r="22" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C22)</f>
-        <v>4.413157</v>
+        <v>0.231682</v>
       </c>
       <c r="B22" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C22)</f>
-        <v>6660.61</v>
+        <v>8148.8</v>
       </c>
       <c r="C22" s="8">
         <f t="shared" si="0"/>
@@ -7023,21 +7028,21 @@
       </c>
       <c r="D22" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C22)</f>
-        <v>6669.51</v>
+        <v>8162</v>
       </c>
       <c r="E22" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C22)</f>
-        <v>0.66981900000000005</v>
+        <v>0.21632699999999999</v>
       </c>
     </row>
     <row r="23" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C23)</f>
-        <v>3.8E-3</v>
+        <v>0.5</v>
       </c>
       <c r="B23" s="15">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C23)</f>
-        <v>6660.53</v>
+        <v>8147.78</v>
       </c>
       <c r="C23" s="8">
         <f t="shared" si="0"/>
@@ -7045,11 +7050,11 @@
       </c>
       <c r="D23" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C23)</f>
-        <v>6669.86</v>
+        <v>8162.46</v>
       </c>
       <c r="E23" s="16">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C23)</f>
-        <v>0.57014500000000001</v>
+        <v>0.5</v>
       </c>
       <c r="G23" s="34" t="s">
         <v>55</v>
@@ -7065,11 +7070,11 @@
     <row r="24" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="31">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,A$14,$C24)</f>
-        <v>0.97992699999999999</v>
+        <v>0.77</v>
       </c>
       <c r="B24" s="31">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,B$14,$C24)</f>
-        <v>6660</v>
+        <v>8147.56</v>
       </c>
       <c r="C24" s="32">
         <f t="shared" si="0"/>
@@ -7077,38 +7082,38 @@
       </c>
       <c r="D24" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,D$14,$C24)</f>
-        <v>6669.87</v>
+        <v>8164.28</v>
       </c>
       <c r="E24" s="33">
         <f>RTD(progId,,BINANCE_DEPTH,$C$14,E$14,$C24)</f>
-        <v>0.01</v>
+        <v>0.1012</v>
       </c>
       <c r="G24" s="35" t="str">
         <f>RTD(progId,,BINANCE_HISTORY,J23,"a,b,c",10)</f>
-        <v>Server error: {"code":-2015,"msg":"Invalid API-key, IP, or permissions for action."}</v>
+        <v>Invalid API-key, IP, or permissions for action.</v>
       </c>
       <c r="H24"/>
     </row>
     <row r="25" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <f>SUM(Table3[BID_DEPTH_SIZE])</f>
-        <v>13.741712000000001</v>
+        <v>13.936404999999999</v>
       </c>
       <c r="B25" s="14">
         <f>SUMPRODUCT(Table3[BID_DEPTH_SIZE],Table3[BID_DEPTH])</f>
-        <v>91546.105255410002</v>
+        <v>113582.74894182998</v>
       </c>
       <c r="C25" s="39">
         <f>B25-D25</f>
-        <v>76057.582041400005</v>
+        <v>83619.399682839983</v>
       </c>
       <c r="D25" s="14">
         <f>SUMPRODUCT(Table3[ASK_DEPTH_SIZE],Table3[ASK_DEPTH])</f>
-        <v>15488.523214010002</v>
+        <v>29963.349258989998</v>
       </c>
       <c r="E25" s="12">
         <f>SUM(Table3[ASK_DEPTH_SIZE])</f>
-        <v>2.3224239999999998</v>
+        <v>3.6715870000000002</v>
       </c>
       <c r="F25" s="9"/>
       <c r="H25" s="1"/>
@@ -7119,14 +7124,14 @@
     <row r="26" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="30">
         <f>B15-B24</f>
-        <v>5</v>
+        <v>4.4600000000000364</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D26" s="30">
         <f>D15-D24</f>
-        <v>-1.9099999999998545</v>
+        <v>-4.1999999999998181</v>
       </c>
       <c r="F26" s="9"/>
       <c r="I26" s="4"/>
@@ -7212,27 +7217,27 @@
       </c>
       <c r="B30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,B$29,$D$28)</f>
-        <v>473.21</v>
+        <v>456.19</v>
       </c>
       <c r="C30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,C$29,$D$28)</f>
-        <v>474.62</v>
+        <v>457.02</v>
       </c>
       <c r="D30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,D$29,$D$28)</f>
-        <v>471.03</v>
+        <v>454.1</v>
       </c>
       <c r="E30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,E$29,$D$28)</f>
-        <v>471.3</v>
+        <v>456.29</v>
       </c>
       <c r="F30" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,F$29,$D$28)</f>
-        <v>43285.5</v>
+        <v>43311.833333333336</v>
       </c>
       <c r="G30" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,G$29,$D$28)</f>
-        <v>43285.541666655095</v>
+        <v>43311.874999988424</v>
       </c>
       <c r="H30" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,H$29,$D$28)</f>
@@ -7240,19 +7245,19 @@
       </c>
       <c r="I30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,I$29,$D$28)</f>
-        <v>1165600.1691212</v>
+        <v>896475.9274096</v>
       </c>
       <c r="J30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,J$29,$D$28)</f>
-        <v>2463.4826800000001</v>
+        <v>1966.45597</v>
       </c>
       <c r="K30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,K$29,$D$28)</f>
-        <v>1193.0365300000001</v>
+        <v>1061.29333</v>
       </c>
       <c r="L30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,L$29,$D$28)</f>
-        <v>564552.89316370001</v>
+        <v>484055.28109459998</v>
       </c>
       <c r="M30" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,M$29,$D$28)</f>
@@ -7260,19 +7265,19 @@
       </c>
       <c r="N30" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,N$29,$D$28)</f>
-        <v>2114</v>
+        <v>1121</v>
       </c>
       <c r="O30" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,O$29,$D$28)</f>
-        <v>43285.517101504629</v>
+        <v>43311.846317685187</v>
       </c>
       <c r="P30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,P$29,$D$28)</f>
-        <v>30391319</v>
+        <v>33093343</v>
       </c>
       <c r="Q30" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A30,Q$29,$D$28)</f>
-        <v>30393432</v>
+        <v>33094463</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -7281,27 +7286,27 @@
       </c>
       <c r="B31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,B$29,$D$28)</f>
-        <v>6683.77</v>
+        <v>8171.4</v>
       </c>
       <c r="C31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,C$29,$D$28)</f>
-        <v>6691.01</v>
+        <v>8180</v>
       </c>
       <c r="D31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,D$29,$D$28)</f>
-        <v>6650.93</v>
+        <v>8130.32</v>
       </c>
       <c r="E31" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,E$29,$D$28)</f>
-        <v>6664.13</v>
+        <v>8152.02</v>
       </c>
       <c r="F31" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,F$29,$D$28)</f>
-        <v>43285.5</v>
+        <v>43311.833333333336</v>
       </c>
       <c r="G31" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,G$29,$D$28)</f>
-        <v>43285.541666655095</v>
+        <v>43311.874999988424</v>
       </c>
       <c r="H31" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,H$29,$D$28)</f>
@@ -7309,19 +7314,19 @@
       </c>
       <c r="I31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,I$29,$D$28)</f>
-        <v>4797712.7030429197</v>
+        <v>3169220.3606163301</v>
       </c>
       <c r="J31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,J$29,$D$28)</f>
-        <v>717.961096</v>
+        <v>388.666763</v>
       </c>
       <c r="K31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,K$29,$D$28)</f>
-        <v>366.14173099999999</v>
+        <v>194.972328</v>
       </c>
       <c r="L31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,L$29,$D$28)</f>
-        <v>2447502.1504584299</v>
+        <v>1590078.60588646</v>
       </c>
       <c r="M31" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,M$29,$D$28)</f>
@@ -7329,19 +7334,19 @@
       </c>
       <c r="N31" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,N$29,$D$28)</f>
-        <v>4014</v>
+        <v>1959</v>
       </c>
       <c r="O31" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,O$29,$D$28)</f>
-        <v>43285.517102083337</v>
+        <v>43311.84634556713</v>
       </c>
       <c r="P31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,P$29,$D$28)</f>
-        <v>54906915</v>
+        <v>60063222</v>
       </c>
       <c r="Q31" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A31,Q$29,$D$28)</f>
-        <v>54910928</v>
+        <v>60065180</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -7350,27 +7355,27 @@
       </c>
       <c r="B32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,B$29,$D$28)</f>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
       </c>
       <c r="C32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,C$29,$D$28)</f>
-        <v>5.9100000000000002E-6</v>
+        <v>4.4599999999999996E-6</v>
       </c>
       <c r="D32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,D$29,$D$28)</f>
-        <v>5.8799999999999996E-6</v>
+        <v>4.4299999999999999E-6</v>
       </c>
       <c r="E32" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,E$29,$D$28)</f>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
       </c>
       <c r="F32" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,F$29,$D$28)</f>
-        <v>43285.5</v>
+        <v>43311.833333333336</v>
       </c>
       <c r="G32" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,G$29,$D$28)</f>
-        <v>43285.541666655095</v>
+        <v>43311.874999988424</v>
       </c>
       <c r="H32" s="18" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,H$29,$D$28)</f>
@@ -7378,19 +7383,19 @@
       </c>
       <c r="I32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,I$29,$D$28)</f>
-        <v>35.743519800000001</v>
+        <v>6.2586106099999999</v>
       </c>
       <c r="J32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,J$29,$D$28)</f>
-        <v>6062958</v>
+        <v>1409501</v>
       </c>
       <c r="K32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,K$29,$D$28)</f>
-        <v>2043046</v>
+        <v>445703</v>
       </c>
       <c r="L32" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,L$29,$D$28)</f>
-        <v>12.049877589999999</v>
+        <v>1.9841261400000001</v>
       </c>
       <c r="M32" s="18" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,M$29,$D$28)</f>
@@ -7398,19 +7403,19 @@
       </c>
       <c r="N32" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,N$29,$D$28)</f>
-        <v>500</v>
+        <v>240</v>
       </c>
       <c r="O32" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,O$29,$D$28)</f>
-        <v>43285.516921388888</v>
+        <v>43311.846323900463</v>
       </c>
       <c r="P32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,P$29,$D$28)</f>
-        <v>30882393</v>
+        <v>32002919</v>
       </c>
       <c r="Q32" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A32,Q$29,$D$28)</f>
-        <v>30882892</v>
+        <v>32003158</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -7489,27 +7494,27 @@
       </c>
       <c r="B36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,B$35,$D$34)</f>
-        <v>472.61</v>
+        <v>456.31</v>
       </c>
       <c r="C36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,C$35,$D$34)</f>
-        <v>472.62</v>
+        <v>456.39</v>
       </c>
       <c r="D36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,D$35,$D$34)</f>
-        <v>471.3</v>
+        <v>456.29</v>
       </c>
       <c r="E36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,E$35,$D$34)</f>
-        <v>471.3</v>
+        <v>456.29</v>
       </c>
       <c r="F36" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,F$35,$D$34)</f>
-        <v>43285.51666666667</v>
+        <v>43311.845833333333</v>
       </c>
       <c r="G36" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,G$35,$D$34)</f>
-        <v>43285.517361099533</v>
+        <v>43311.846527766204</v>
       </c>
       <c r="H36" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,H$35,$D$34)</f>
@@ -7517,19 +7522,19 @@
       </c>
       <c r="I36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,I$35,$D$34)</f>
-        <v>12544.048344999999</v>
+        <v>5649.5433349000004</v>
       </c>
       <c r="J36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,J$35,$D$34)</f>
-        <v>26.591799999999999</v>
+        <v>12.380129999999999</v>
       </c>
       <c r="K36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,K$35,$D$34)</f>
-        <v>6.88591</v>
+        <v>6.8019699999999998</v>
       </c>
       <c r="L36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,L$35,$D$34)</f>
-        <v>3252.4823544999999</v>
+        <v>3104.2154962</v>
       </c>
       <c r="M36" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,M$35,$D$34)</f>
@@ -7537,19 +7542,19 @@
       </c>
       <c r="N36" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,N$35,$D$34)</f>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="O36" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,O$35,$D$34)</f>
-        <v>43285.517101504629</v>
+        <v>43311.846317685187</v>
       </c>
       <c r="P36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,P$35,$D$34)</f>
-        <v>30393407</v>
+        <v>33094443</v>
       </c>
       <c r="Q36" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A36,Q$35,$D$34)</f>
-        <v>30393432</v>
+        <v>33094463</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7558,27 +7563,27 @@
       </c>
       <c r="B37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,B$35,$D$34)</f>
-        <v>6670.01</v>
+        <v>8153.35</v>
       </c>
       <c r="C37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,C$35,$D$34)</f>
-        <v>6671.01</v>
+        <v>8160.23</v>
       </c>
       <c r="D37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,D$35,$D$34)</f>
-        <v>6662.15</v>
+        <v>8150.55</v>
       </c>
       <c r="E37" s="13">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,E$35,$D$34)</f>
-        <v>6664.13</v>
+        <v>8152.02</v>
       </c>
       <c r="F37" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,F$35,$D$34)</f>
-        <v>43285.51666666667</v>
+        <v>43311.845833333333</v>
       </c>
       <c r="G37" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,G$35,$D$34)</f>
-        <v>43285.517361099533</v>
+        <v>43311.846527766204</v>
       </c>
       <c r="H37" s="13" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,H$35,$D$34)</f>
@@ -7586,19 +7591,19 @@
       </c>
       <c r="I37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,I$35,$D$34)</f>
-        <v>67997.397360820003</v>
+        <v>30346.96819467</v>
       </c>
       <c r="J37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,J$35,$D$34)</f>
-        <v>10.200435000000001</v>
+        <v>3.721597</v>
       </c>
       <c r="K37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,K$35,$D$34)</f>
-        <v>2.0317949999999998</v>
+        <v>1.619294</v>
       </c>
       <c r="L37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,L$35,$D$34)</f>
-        <v>13547.573522049999</v>
+        <v>13210.08758555</v>
       </c>
       <c r="M37" s="13" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,M$35,$D$34)</f>
@@ -7606,19 +7611,19 @@
       </c>
       <c r="N37" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,N$35,$D$34)</f>
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="O37" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,O$35,$D$34)</f>
-        <v>43285.517102071761</v>
+        <v>43311.846345601851</v>
       </c>
       <c r="P37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,P$35,$D$34)</f>
-        <v>54910865</v>
+        <v>60065146</v>
       </c>
       <c r="Q37" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A37,Q$35,$D$34)</f>
-        <v>54910928</v>
+        <v>60065180</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7627,27 +7632,27 @@
       </c>
       <c r="B38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,B$35,$D$34)</f>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4299999999999999E-6</v>
       </c>
       <c r="C38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,C$35,$D$34)</f>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
       </c>
       <c r="D38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,D$35,$D$34)</f>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4299999999999999E-6</v>
       </c>
       <c r="E38" s="18">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,E$35,$D$34)</f>
-        <v>5.8900000000000004E-6</v>
+        <v>4.4399999999999998E-6</v>
       </c>
       <c r="F38" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,F$35,$D$34)</f>
-        <v>43285.51666666667</v>
+        <v>43311.845833333333</v>
       </c>
       <c r="G38" s="22">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,G$35,$D$34)</f>
-        <v>43285.517361099533</v>
+        <v>43311.846527766204</v>
       </c>
       <c r="H38" s="18" t="b">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,H$35,$D$34)</f>
@@ -7655,19 +7660,19 @@
       </c>
       <c r="I38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,I$35,$D$34)</f>
-        <v>0.18112928</v>
+        <v>6.7387999999999997E-4</v>
       </c>
       <c r="J38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,J$35,$D$34)</f>
-        <v>30752</v>
+        <v>152</v>
       </c>
       <c r="K38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,K$35,$D$34)</f>
-        <v>30752</v>
+        <v>52</v>
       </c>
       <c r="L38" s="24">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,L$35,$D$34)</f>
-        <v>0.18112928</v>
+        <v>2.3088000000000001E-4</v>
       </c>
       <c r="M38" s="18" t="str">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,M$35,$D$34)</f>
@@ -7675,19 +7680,19 @@
       </c>
       <c r="N38" s="25">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,N$35,$D$34)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O38" s="23">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,O$35,$D$34)</f>
-        <v>43285.516921388888</v>
+        <v>43311.846323900463</v>
       </c>
       <c r="P38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,P$35,$D$34)</f>
-        <v>30882888</v>
+        <v>32003156</v>
       </c>
       <c r="Q38" s="26">
         <f>RTD(progId,,BINANCE_CANDLE,$A38,Q$35,$D$34)</f>
-        <v>30882892</v>
+        <v>32003158</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -8080,31 +8085,31 @@
       </c>
       <c r="B3" s="2">
         <f>RTD(progId,,GDAX,$A3,B$2)</f>
-        <v>471.76</v>
+        <v>456.78</v>
       </c>
       <c r="C3" s="2">
         <f>RTD(progId,,GDAX,$A3,C$2)</f>
-        <v>471.77</v>
+        <v>456.79</v>
       </c>
       <c r="D3" s="2">
         <f>RTD(progId,,GDAX,$A3,D$2)</f>
-        <v>471.77</v>
+        <v>456.79</v>
       </c>
       <c r="E3" s="2">
         <f>RTD(progId,,GDAX,$A3,E$2)</f>
-        <v>468.56</v>
+        <v>461.8</v>
       </c>
       <c r="F3" s="2">
         <f>RTD(progId,,GDAX,$A3,F$2)</f>
-        <v>482.01</v>
+        <v>469</v>
       </c>
       <c r="G3" s="2">
         <f>RTD(progId,,GDAX,$A3,G$2)</f>
-        <v>451.35</v>
+        <v>446</v>
       </c>
       <c r="H3" s="2">
         <f>RTD(progId,,GDAX,$A3,H$2)</f>
-        <v>64263.177474869997</v>
+        <v>49281.142481360002</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -8113,31 +8118,31 @@
       </c>
       <c r="B4" s="2">
         <f>RTD(progId,,GDAX,$A4,B$2)</f>
-        <v>6663.66</v>
+        <v>8153.52</v>
       </c>
       <c r="C4" s="2">
         <f>RTD(progId,,GDAX,$A4,C$2)</f>
-        <v>6663.67</v>
+        <v>8153.53</v>
       </c>
       <c r="D4" s="2">
         <f>RTD(progId,,GDAX,$A4,D$2)</f>
-        <v>6663.67</v>
+        <v>8153.52</v>
       </c>
       <c r="E4" s="2">
         <f>RTD(progId,,GDAX,$A4,E$2)</f>
-        <v>6589.99</v>
+        <v>8105.01</v>
       </c>
       <c r="F4" s="2">
         <f>RTD(progId,,GDAX,$A4,F$2)</f>
-        <v>6796.62</v>
+        <v>8274.92</v>
       </c>
       <c r="G4" s="2">
         <f>RTD(progId,,GDAX,$A4,G$2)</f>
-        <v>6411.51</v>
+        <v>7850</v>
       </c>
       <c r="H4" s="2">
         <f>RTD(progId,,GDAX,$A4,H$2)</f>
-        <v>7532.5732854899998</v>
+        <v>10179.092113299999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>